<commit_message>
change pptx, change .xslx
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -401,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -503,6 +503,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1084,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1093,7 +1114,7 @@
     <col min="1" max="1" width="9.33203125" style="11" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="10" customWidth="1"/>
     <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="42" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
@@ -1189,7 +1210,7 @@
       <c r="C3" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="28"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="28"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -1211,7 +1232,7 @@
       <c r="C4" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="41"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
@@ -1279,7 +1300,7 @@
       <c r="C7" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="17"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
@@ -1306,7 +1327,7 @@
       <c r="C8" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="35"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
@@ -1318,7 +1339,7 @@
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>42</v>
       </c>
@@ -1328,7 +1349,7 @@
       <c r="C9" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="44" t="s">
         <v>96</v>
       </c>
       <c r="E9" s="19"/>
@@ -1362,7 +1383,7 @@
       <c r="C10" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="19"/>
+      <c r="D10" s="44"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19" t="s">
         <v>48</v>
@@ -1406,7 +1427,7 @@
       <c r="C12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="17"/>
+      <c r="D12" s="41"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
       <c r="G12" s="17"/>
@@ -1430,7 +1451,7 @@
       <c r="C13" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="19"/>
+      <c r="D13" s="44"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19" t="s">
         <v>49</v>
@@ -1462,7 +1483,7 @@
       <c r="C14" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="34"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
@@ -1484,7 +1505,7 @@
       <c r="C15" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="19"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19" t="s">
         <v>48</v>
@@ -1516,7 +1537,7 @@
       <c r="C16" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="19"/>
       <c r="F16" s="19" t="s">
         <v>50</v>
@@ -1548,7 +1569,7 @@
       <c r="C17" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="19"/>
       <c r="F17" s="19" t="s">
         <v>52</v>
@@ -1580,7 +1601,7 @@
       <c r="C18" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="19"/>
+      <c r="D18" s="44"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19" t="s">
         <v>50</v>
@@ -1612,7 +1633,7 @@
       <c r="C19" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D19" s="19"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="19"/>
       <c r="F19" s="19" t="s">
         <v>51</v>
@@ -1634,7 +1655,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="24">
         <v>3.5</v>
       </c>
@@ -1644,7 +1665,7 @@
       <c r="C20" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="44" t="s">
         <v>97</v>
       </c>
       <c r="E20" s="19"/>
@@ -1678,7 +1699,7 @@
       <c r="C21" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="22"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="22"/>
       <c r="F21" s="22" t="s">
         <v>52</v>
@@ -1736,7 +1757,7 @@
       <c r="C24" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="17"/>
+      <c r="D24" s="41"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -1786,7 +1807,7 @@
       <c r="C27" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D27" s="17"/>
+      <c r="D27" s="41"/>
       <c r="E27" s="17"/>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
@@ -1836,7 +1857,7 @@
       <c r="C30" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="17"/>
+      <c r="D30" s="41"/>
       <c r="E30" s="17"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>

</xml_diff>

<commit_message>
added descriptions / general stuff on the scrum excel file
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\03_Sem_HS\BTX8081_SoftwareEngineeringAndDesign\Eclipse\ch.bfh.btx8081.w2017.blue.git\trunk\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasch\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8892" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
   <si>
     <t>ID</t>
   </si>
@@ -165,27 +165,6 @@
     <t>Check Credentials</t>
   </si>
   <si>
-    <t>MVP Login</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Sascha</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>Michaela</t>
-  </si>
-  <si>
-    <t>Jemal</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
     <t>Miscellaneous</t>
   </si>
   <si>
@@ -316,12 +295,81 @@
   </si>
   <si>
     <t>Create the class model for drug in Java</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>odaoj1</t>
+  </si>
+  <si>
+    <t>Differents tasks, that we can't allocate in the following stories or tasks which influences all other stories</t>
+  </si>
+  <si>
+    <t>The first step for an HealthVisitor is to LogIn in the WebApp. A Login window is appearing, where the HV can enter his credentials. If the login is successful, it opens the patient view (story 2).</t>
+  </si>
+  <si>
+    <t>After the LogIn, the HV sees the complete list of all his patients. He can select a patient with clicking on its tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The core of the Application, the patient view is a semi-complete view of the patients personal data with a picture. The HV can look at their diagnosis and medication. There's a list of the goals as well. </t>
+  </si>
+  <si>
+    <t>The HV can add or modify objectives in the patient view with clicking on a existing object or the "add" button. A new view is opening with the data of the objective. A progress bar is showing the actual state of the objective. The HV can complete an objective.</t>
+  </si>
+  <si>
+    <t>If an objective exists, the HV can add an activity entry in it. This activity has a name, description and also a progress bar. The HV can complete an activity.</t>
+  </si>
+  <si>
+    <t>For every activity, the HV can record one or more activity records. This activity record shows the process of one attempt. In this formular, the HV documents the status of the patient before and after the activity. He discuss and documents if the activity was successful or not with the patient together. This leads into an valuation of the record.</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Presenter</t>
+  </si>
+  <si>
+    <t>Model, DB</t>
+  </si>
+  <si>
+    <t>DB Connect</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>DB, Model</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>VP Login</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Main View Container and shows the patient data like name, birthdate etc.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -401,7 +449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -525,6 +573,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -544,7 +594,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -619,6 +669,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -654,6 +721,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -829,28 +913,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -858,57 +946,72 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -916,26 +1019,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="15" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -949,30 +1052,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16"/>
+      <c r="E2" s="16">
+        <v>15</v>
+      </c>
       <c r="F2" s="16"/>
       <c r="G2" s="16">
         <v>0</v>
@@ -980,111 +1087,170 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C3" s="42" t="s">
+        <v>95</v>
+      </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8">
+        <v>15</v>
+      </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
+      <c r="C4" s="42" t="s">
+        <v>96</v>
+      </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>15</v>
+      </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8">
         <v>0</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
+      <c r="C5" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8">
+        <v>44</v>
+      </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="C6" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>20</v>
+      </c>
       <c r="F6" s="8"/>
       <c r="G6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="C7" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>20</v>
+      </c>
       <c r="F7" s="8"/>
       <c r="G7" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="17"/>
-      <c r="E8" s="31"/>
+      <c r="C8" s="42" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="31">
+        <v>30</v>
+      </c>
       <c r="F8" s="31"/>
       <c r="G8" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E9">
         <f>SUM(E2:E8)</f>
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="F9">
         <f>SUM(F2:F8)</f>
@@ -1097,36 +1263,36 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="42" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="42" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -1152,19 +1318,19 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>0.1</v>
       </c>
@@ -1172,15 +1338,17 @@
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D2" s="30"/>
-      <c r="E2" s="19"/>
+      <c r="E2" s="19" t="s">
+        <v>104</v>
+      </c>
       <c r="F2" s="19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="H2" s="19" t="s">
         <v>5</v>
@@ -1195,23 +1363,25 @@
       <c r="L2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="T2" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="W2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="28" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D3" s="40"/>
-      <c r="E3" s="28"/>
+      <c r="E3" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
@@ -1224,16 +1394,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4" s="41"/>
-      <c r="E4" s="17"/>
+      <c r="E4" s="17" t="s">
+        <v>106</v>
+      </c>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -1245,19 +1417,22 @@
       <c r="L4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="T4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>107</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1265,43 +1440,48 @@
       <c r="L5" t="s">
         <v>8</v>
       </c>
-      <c r="M5" t="s">
-        <v>80</v>
-      </c>
-      <c r="P5" t="s">
+      <c r="T5" t="s">
+        <v>73</v>
+      </c>
+      <c r="W5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>1.2</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
+      <c r="E6" t="s">
+        <v>111</v>
+      </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6" t="s">
         <v>8</v>
       </c>
-      <c r="M6" t="s">
+      <c r="T6" t="s">
         <v>17</v>
       </c>
-      <c r="P6" t="s">
+      <c r="W6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="23">
         <v>1.3</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="17" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="D7" s="41"/>
-      <c r="E7" s="17"/>
+      <c r="E7" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -1313,19 +1493,19 @@
       <c r="L7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="M7" t="s">
+      <c r="T7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B8" s="33">
         <v>1</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="35"/>
@@ -1333,13 +1513,13 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="36" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J8" s="35"/>
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
     </row>
-    <row r="9" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>42</v>
       </c>
@@ -1347,17 +1527,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9" s="19"/>
+        <v>89</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>16</v>
+      </c>
       <c r="F9" s="19" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>5</v>
@@ -1373,23 +1555,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B10" s="18">
         <v>1</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D10" s="44"/>
-      <c r="E10" s="19"/>
+      <c r="E10" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="F10" s="19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>5</v>
@@ -1405,12 +1589,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>2.2000000000000002</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1419,13 +1603,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" s="20"/>
       <c r="C12" s="17" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D12" s="41"/>
       <c r="E12" s="17"/>
@@ -1441,7 +1625,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>3.1</v>
       </c>
@@ -1449,15 +1633,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="19"/>
+        <v>75</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="F13" s="19" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>6</v>
@@ -1473,7 +1661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="37">
         <v>3.2</v>
       </c>
@@ -1481,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="34"/>
@@ -1489,13 +1677,13 @@
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
       <c r="I14" s="39" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>40</v>
       </c>
@@ -1503,15 +1691,17 @@
         <v>1</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D15" s="44"/>
-      <c r="E15" s="19"/>
+      <c r="E15" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="F15" s="19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>5</v>
@@ -1527,7 +1717,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>41</v>
       </c>
@@ -1535,15 +1725,17 @@
         <v>1</v>
       </c>
       <c r="C16" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="44"/>
+      <c r="E16" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>52</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>6</v>
@@ -1559,23 +1751,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B17" s="18">
         <v>1</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D17" s="44"/>
-      <c r="E17" s="19"/>
+      <c r="E17" s="19" t="s">
+        <v>102</v>
+      </c>
       <c r="F17" s="19" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>6</v>
@@ -1591,7 +1785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>3.3</v>
       </c>
@@ -1599,15 +1793,17 @@
         <v>1</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D18" s="44"/>
-      <c r="E18" s="19"/>
+      <c r="E18" s="19" t="s">
+        <v>103</v>
+      </c>
       <c r="F18" s="19" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>5</v>
@@ -1623,7 +1819,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>3.4</v>
       </c>
@@ -1631,15 +1827,17 @@
         <v>1</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D19" s="44"/>
-      <c r="E19" s="19"/>
+      <c r="E19" s="19" t="s">
+        <v>108</v>
+      </c>
       <c r="F19" s="19" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>6</v>
@@ -1655,7 +1853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>3.5</v>
       </c>
@@ -1663,17 +1861,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="19"/>
+        <v>90</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>101</v>
+      </c>
       <c r="F20" s="19" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>7</v>
@@ -1689,7 +1889,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>3.6</v>
       </c>
@@ -1697,15 +1897,17 @@
         <v>1</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D21" s="46"/>
-      <c r="E21" s="22"/>
+      <c r="E21" s="22" t="s">
+        <v>101</v>
+      </c>
       <c r="F21" s="22" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G21" s="22" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="H21" s="22" t="s">
         <v>7</v>
@@ -1721,12 +1923,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>4.0999999999999996</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>62</v>
+      </c>
+      <c r="E22" s="47" t="s">
+        <v>101</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1735,12 +1940,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>4.2</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>61</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>108</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1749,16 +1957,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="23">
         <v>4.3</v>
       </c>
       <c r="B24" s="20"/>
       <c r="C24" s="17" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D24" s="41"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="48" t="s">
+        <v>110</v>
+      </c>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
@@ -1771,12 +1981,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>5.0999999999999996</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>66</v>
+      </c>
+      <c r="E25" s="47" t="s">
+        <v>101</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1785,12 +1998,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>5.2</v>
       </c>
       <c r="C26" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="E26" s="47" t="s">
+        <v>108</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1799,16 +2015,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="23">
         <v>5.3</v>
       </c>
       <c r="B27" s="20"/>
       <c r="C27" s="17" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D27" s="41"/>
-      <c r="E27" s="17"/>
+      <c r="E27" s="17" t="s">
+        <v>110</v>
+      </c>
       <c r="F27" s="17"/>
       <c r="G27" s="17"/>
       <c r="H27" s="17"/>
@@ -1821,12 +2039,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>6.1</v>
       </c>
       <c r="C28" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>101</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -1835,12 +2056,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>6.2</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>69</v>
+      </c>
+      <c r="E29" s="47" t="s">
+        <v>112</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -1849,16 +2073,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="23">
         <v>6.3</v>
       </c>
       <c r="B30" s="20"/>
       <c r="C30" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D30" s="41"/>
-      <c r="E30" s="17"/>
+      <c r="E30" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -1871,9 +2097,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I31">
         <f>SUM(I2:I30)</f>
@@ -1888,9 +2114,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I32">
         <v>54</v>
@@ -1906,21 +2132,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -1934,10 +2160,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated scrum.xls with dwscriptions
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sasch\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -364,12 +359,21 @@
   </si>
   <si>
     <t>Main View Container and shows the patient data like name, birthdate etc.</t>
+  </si>
+  <si>
+    <t>Creation of interfacee and view class wich shows advanced patient info</t>
+  </si>
+  <si>
+    <t>Create Ojective and ObjectiveList Class and creating the corresponding relations in DB</t>
+  </si>
+  <si>
+    <t>Create the class for diagnosis in Java</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -577,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -594,9 +598,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -634,9 +638,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,26 +673,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -721,26 +708,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -913,7 +883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1006,12 +976,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1019,10 +989,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -1268,11 +1238,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1687,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>41</v>
       </c>
@@ -1727,7 +1697,9 @@
       <c r="C16" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="44"/>
+      <c r="D16" s="44" t="s">
+        <v>114</v>
+      </c>
       <c r="E16" s="19" t="s">
         <v>112</v>
       </c>
@@ -1785,7 +1757,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>3.3</v>
       </c>
@@ -1795,7 +1767,9 @@
       <c r="C18" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="44"/>
+      <c r="D18" s="44" t="s">
+        <v>115</v>
+      </c>
       <c r="E18" s="19" t="s">
         <v>103</v>
       </c>
@@ -1889,7 +1863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="25">
         <v>3.6</v>
       </c>
@@ -1899,7 +1873,9 @@
       <c r="C21" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="46" t="s">
+        <v>116</v>
+      </c>
       <c r="E21" s="22" t="s">
         <v>101</v>
       </c>
@@ -2132,7 +2108,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add infos to scrum.xlsx
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="118">
   <si>
     <t>ID</t>
   </si>
@@ -361,19 +366,22 @@
     <t>Main View Container and shows the patient data like name, birthdate etc.</t>
   </si>
   <si>
-    <t>Creation of interfacee and view class wich shows advanced patient info</t>
-  </si>
-  <si>
     <t>Create Ojective and ObjectiveList Class and creating the corresponding relations in DB</t>
   </si>
   <si>
     <t>Create the class for diagnosis in Java</t>
+  </si>
+  <si>
+    <t>Creation of interface and view class wich shows advanced patient info</t>
+  </si>
+  <si>
+    <t>Shows the objectiv (they can be created, opened or changed)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,12 +488,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -503,85 +505,107 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -598,9 +622,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -638,9 +662,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -673,9 +697,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,9 +749,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -883,7 +941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -976,12 +1034,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -989,16 +1047,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="15" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" customWidth="1"/>
@@ -1009,7 +1067,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1035,7 +1093,7 @@
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+      <c r="A2" s="13">
         <v>0</v>
       </c>
       <c r="B2" t="s">
@@ -1047,11 +1105,11 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="14">
         <v>15</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1062,13 +1120,13 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="18" t="s">
         <v>95</v>
       </c>
       <c r="D3" t="s">
@@ -1089,13 +1147,13 @@
       </c>
     </row>
     <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="18" t="s">
         <v>96</v>
       </c>
       <c r="D4" t="s">
@@ -1116,13 +1174,13 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="18" t="s">
         <v>97</v>
       </c>
       <c r="D5" t="s">
@@ -1143,13 +1201,13 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="18" t="s">
         <v>98</v>
       </c>
       <c r="D6" t="s">
@@ -1167,13 +1225,13 @@
       </c>
     </row>
     <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="18" t="s">
         <v>99</v>
       </c>
       <c r="D7" t="s">
@@ -1191,23 +1249,23 @@
       </c>
     </row>
     <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="17">
         <v>30</v>
       </c>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31">
+      <c r="F8" s="17"/>
+      <c r="G8" s="17">
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1238,32 +1296,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="42" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
@@ -1301,169 +1360,169 @@
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="24">
+      <c r="A2" s="19">
         <v>0.1</v>
       </c>
-      <c r="B2" s="18">
+      <c r="B2" s="20">
         <v>1</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="19" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="21">
         <v>2</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19">
-        <v>0</v>
-      </c>
-      <c r="L2" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="J2" s="21"/>
+      <c r="K2" s="21">
+        <v>0</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28" t="s">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="25"/>
+      <c r="E3" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28">
-        <v>0</v>
-      </c>
-      <c r="L3" s="28" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="41"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17">
-        <v>0</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28">
+        <v>0</v>
+      </c>
+      <c r="L4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W4" t="s">
+      <c r="W4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="11">
+      <c r="A5" s="30">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>8</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="11">
+      <c r="A6" s="30">
         <v>1.2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="23">
+      <c r="A7" s="26">
         <v>1.3</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="17" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="17" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17">
-        <v>0</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="T7" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28">
+        <v>0</v>
+      </c>
+      <c r="L7" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="T7" s="1" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1477,176 +1536,176 @@
       <c r="C8" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="36" t="s">
+      <c r="D8" s="35"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="20">
         <v>1</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="19" t="s">
+      <c r="F9" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="19">
+      <c r="I9" s="21">
         <v>5</v>
       </c>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19">
-        <v>0</v>
-      </c>
-      <c r="L9" s="19" t="s">
+      <c r="J9" s="21"/>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="20">
         <v>1</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="44"/>
-      <c r="E10" s="19" t="s">
+      <c r="D10" s="16"/>
+      <c r="E10" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="19" t="s">
+      <c r="H10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="21">
         <v>3</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19">
-        <v>0</v>
-      </c>
-      <c r="L10" s="19" t="s">
+      <c r="J10" s="21"/>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="11">
+      <c r="A11" s="30">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="23">
+      <c r="A12" s="26">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17">
-        <v>0</v>
-      </c>
-      <c r="L12" s="17" t="s">
+      <c r="D12" s="29"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28">
+        <v>0</v>
+      </c>
+      <c r="L12" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
+      <c r="A13" s="19">
         <v>3.1</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="20">
         <v>1</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="19">
+      <c r="I13" s="21">
         <v>9</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19">
-        <v>0</v>
-      </c>
-      <c r="L13" s="19" t="s">
+      <c r="J13" s="21"/>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="21" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="37">
+      <c r="A14" s="39">
         <v>3.2</v>
       </c>
-      <c r="B14" s="38">
+      <c r="B14" s="40">
         <v>1</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="45"/>
+      <c r="D14" s="41"/>
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="42" t="s">
         <v>84</v>
       </c>
       <c r="J14" s="34"/>
@@ -1654,447 +1713,449 @@
       <c r="L14" s="34"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="20">
         <v>1</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="19" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="19">
+      <c r="I15" s="21">
         <v>4</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19">
-        <v>0</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="J15" s="21"/>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="20">
         <v>1</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="21">
+        <v>4</v>
+      </c>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="20">
+        <v>1</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="21">
+        <v>3</v>
+      </c>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21">
+        <v>0</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>3.3</v>
+      </c>
+      <c r="B18" s="20">
+        <v>1</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="F16" s="19" t="s">
+      <c r="E18" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G18" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="21">
+        <v>5</v>
+      </c>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21">
+        <v>0</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>3.4</v>
+      </c>
+      <c r="B19" s="20">
+        <v>1</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="21">
+        <v>9</v>
+      </c>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21">
+        <v>0</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>3.5</v>
+      </c>
+      <c r="B20" s="20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="21">
+        <v>4</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21">
+        <v>0</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="43">
+        <v>3.6</v>
+      </c>
+      <c r="B21" s="44">
+        <v>1</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="H16" s="19" t="s">
+      <c r="G21" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="45">
         <v>6</v>
       </c>
-      <c r="I16" s="19">
-        <v>4</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19">
-        <v>0</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="18">
-        <v>1</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="19">
-        <v>3</v>
-      </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19">
-        <v>0</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="24">
-        <v>3.3</v>
-      </c>
-      <c r="B18" s="18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="I18" s="19">
-        <v>5</v>
-      </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19">
-        <v>0</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="24">
-        <v>3.4</v>
-      </c>
-      <c r="B19" s="18">
-        <v>1</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" s="44"/>
-      <c r="E19" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="I19" s="19">
-        <v>9</v>
-      </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19">
-        <v>0</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="B20" s="18">
-        <v>1</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="19">
-        <v>4</v>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19">
-        <v>0</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
-        <v>3.6</v>
-      </c>
-      <c r="B21" s="21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="46" t="s">
-        <v>116</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="22">
-        <v>6</v>
-      </c>
-      <c r="J21" s="22"/>
-      <c r="K21" s="22">
-        <v>0</v>
-      </c>
-      <c r="L21" s="22" t="s">
+      <c r="J21" s="45"/>
+      <c r="K21" s="45">
+        <v>0</v>
+      </c>
+      <c r="L21" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="11">
+      <c r="A22" s="30">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
       <c r="E22" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="11">
+      <c r="A23" s="30">
         <v>4.2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
       <c r="E23" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="23">
+      <c r="A24" s="26">
         <v>4.3</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="27"/>
+      <c r="C24" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="D24" s="41"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17">
-        <v>0</v>
-      </c>
-      <c r="L24" s="17" t="s">
+      <c r="F24" s="28"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28">
+        <v>0</v>
+      </c>
+      <c r="L24" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
+      <c r="A25" s="30">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E25" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
+      <c r="A26" s="30">
         <v>5.2</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>64</v>
       </c>
       <c r="E26" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="23">
+      <c r="A27" s="26">
         <v>5.3</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="17" t="s">
+      <c r="B27" s="27"/>
+      <c r="C27" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="41"/>
-      <c r="E27" s="17" t="s">
+      <c r="D27" s="29"/>
+      <c r="E27" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17">
-        <v>0</v>
-      </c>
-      <c r="L27" s="17" t="s">
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28">
+        <v>0</v>
+      </c>
+      <c r="L27" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="11">
+      <c r="A28" s="30">
         <v>6.1</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>67</v>
       </c>
       <c r="E28" s="47" t="s">
         <v>101</v>
       </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="11">
+      <c r="A29" s="30">
         <v>6.2</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E29" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="K29" s="1">
+        <v>0</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="23">
+      <c r="A30" s="26">
         <v>6.3</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="27"/>
+      <c r="C30" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="17" t="s">
+      <c r="D30" s="29"/>
+      <c r="E30" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17">
-        <v>0</v>
-      </c>
-      <c r="L30" s="17" t="s">
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28">
+        <v>0</v>
+      </c>
+      <c r="L30" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H31" t="s">
+      <c r="H31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="1">
         <f>SUM(I2:I30)</f>
         <v>54</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
         <f>SUM(J2:J30)</f>
         <v>0</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="1">
         <f>SUM(K2:K30)</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H32" t="s">
+      <c r="H32" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="1">
         <v>54</v>
       </c>
     </row>
@@ -2108,7 +2169,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
add discpritions in sprint backlog
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/ch.bfh.btx8081.w2017.blue.git/doc/04-ScrumSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-4800" windowWidth="51200" windowHeight="28340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,12 +17,20 @@
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -375,13 +383,22 @@
     <t>Creation of interface and view class wich shows advanced patient info</t>
   </si>
   <si>
-    <t>Shows the objectiv (they can be created, opened or changed)</t>
+    <t>Shows the objective (they can be created, opened or changed)</t>
+  </si>
+  <si>
+    <t>Creating a model for the Patient Info (may contain more informatino than just the patient model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create the Java patient model out of the DB </t>
+  </si>
+  <si>
+    <t>Create the presenter for the Patient Info (acts between View Interface and Model)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -452,7 +469,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -605,8 +622,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -622,7 +639,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -667,9 +684,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -697,31 +714,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -749,23 +749,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -941,21 +924,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -966,7 +949,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -977,7 +960,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -988,7 +971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -999,7 +982,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1010,7 +993,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1021,7 +1004,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1034,12 +1017,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1047,26 +1030,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1075,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1119,7 +1102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1146,7 +1129,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1173,7 +1156,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1200,7 +1183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1224,7 +1207,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1248,7 +1231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1272,7 +1255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>71</v>
       </c>
@@ -1296,32 +1279,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1359,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>0.1</v>
       </c>
@@ -1399,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>80</v>
       </c>
@@ -1423,7 +1406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>81</v>
       </c>
@@ -1453,7 +1436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>1.1000000000000001</v>
       </c>
@@ -1476,7 +1459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>1.2</v>
       </c>
@@ -1499,7 +1482,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>1.3</v>
       </c>
@@ -1526,7 +1509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>77</v>
       </c>
@@ -1548,7 +1531,7 @@
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:23" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>42</v>
       </c>
@@ -1576,7 +1559,9 @@
       <c r="I9" s="21">
         <v>5</v>
       </c>
-      <c r="J9" s="21"/>
+      <c r="J9" s="21">
+        <v>5</v>
+      </c>
       <c r="K9" s="21">
         <v>0</v>
       </c>
@@ -1584,7 +1569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>76</v>
       </c>
@@ -1594,7 +1579,9 @@
       <c r="C10" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D10" s="16"/>
+      <c r="D10" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="E10" s="21" t="s">
         <v>101</v>
       </c>
@@ -1610,7 +1597,9 @@
       <c r="I10" s="21">
         <v>3</v>
       </c>
-      <c r="J10" s="21"/>
+      <c r="J10" s="21">
+        <v>3</v>
+      </c>
       <c r="K10" s="21">
         <v>0</v>
       </c>
@@ -1618,7 +1607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>2.2000000000000002</v>
       </c>
@@ -1632,7 +1621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>2.2999999999999998</v>
       </c>
@@ -1654,7 +1643,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19">
         <v>3.1</v>
       </c>
@@ -1682,7 +1671,9 @@
       <c r="I13" s="21">
         <v>9</v>
       </c>
-      <c r="J13" s="21"/>
+      <c r="J13" s="21">
+        <v>9</v>
+      </c>
       <c r="K13" s="21">
         <v>0</v>
       </c>
@@ -1690,7 +1681,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="39">
         <v>3.2</v>
       </c>
@@ -1712,7 +1703,7 @@
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
@@ -1722,7 +1713,9 @@
       <c r="C15" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="D15" s="16"/>
+      <c r="D15" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="E15" s="21" t="s">
         <v>101</v>
       </c>
@@ -1738,7 +1731,9 @@
       <c r="I15" s="21">
         <v>4</v>
       </c>
-      <c r="J15" s="21"/>
+      <c r="J15" s="21">
+        <v>4</v>
+      </c>
       <c r="K15" s="21">
         <v>0</v>
       </c>
@@ -1746,7 +1741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>41</v>
       </c>
@@ -1774,7 +1769,9 @@
       <c r="I16" s="21">
         <v>4</v>
       </c>
-      <c r="J16" s="21"/>
+      <c r="J16" s="21">
+        <v>4</v>
+      </c>
       <c r="K16" s="21">
         <v>0</v>
       </c>
@@ -1782,7 +1779,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>87</v>
       </c>
@@ -1792,7 +1789,9 @@
       <c r="C17" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="16"/>
+      <c r="D17" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="E17" s="21" t="s">
         <v>102</v>
       </c>
@@ -1808,7 +1807,9 @@
       <c r="I17" s="21">
         <v>3</v>
       </c>
-      <c r="J17" s="21"/>
+      <c r="J17" s="21">
+        <v>3</v>
+      </c>
       <c r="K17" s="21">
         <v>0</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>3.3</v>
       </c>
@@ -1844,7 +1845,9 @@
       <c r="I18" s="21">
         <v>5</v>
       </c>
-      <c r="J18" s="21"/>
+      <c r="J18" s="21">
+        <v>5</v>
+      </c>
       <c r="K18" s="21">
         <v>0</v>
       </c>
@@ -1852,7 +1855,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>3.4</v>
       </c>
@@ -1880,7 +1883,9 @@
       <c r="I19" s="21">
         <v>9</v>
       </c>
-      <c r="J19" s="21"/>
+      <c r="J19" s="21">
+        <v>9</v>
+      </c>
       <c r="K19" s="21">
         <v>0</v>
       </c>
@@ -1888,7 +1893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>3.5</v>
       </c>
@@ -1916,7 +1921,9 @@
       <c r="I20" s="21">
         <v>4</v>
       </c>
-      <c r="J20" s="21"/>
+      <c r="J20" s="21">
+        <v>4</v>
+      </c>
       <c r="K20" s="21">
         <v>0</v>
       </c>
@@ -1924,7 +1931,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="43">
         <v>3.6</v>
       </c>
@@ -1952,7 +1959,9 @@
       <c r="I21" s="45">
         <v>6</v>
       </c>
-      <c r="J21" s="45"/>
+      <c r="J21" s="45">
+        <v>6</v>
+      </c>
       <c r="K21" s="45">
         <v>0</v>
       </c>
@@ -1960,7 +1969,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>4.0999999999999996</v>
       </c>
@@ -1977,7 +1986,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>4.2</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
         <v>4.3</v>
       </c>
@@ -2018,7 +2027,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
         <v>5.0999999999999996</v>
       </c>
@@ -2035,7 +2044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <v>5.2</v>
       </c>
@@ -2052,7 +2061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <v>5.3</v>
       </c>
@@ -2076,7 +2085,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <v>6.1</v>
       </c>
@@ -2093,7 +2102,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <v>6.2</v>
       </c>
@@ -2110,7 +2119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="26">
         <v>6.3</v>
       </c>
@@ -2134,7 +2143,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H31" s="1" t="s">
         <v>71</v>
       </c>
@@ -2144,14 +2153,14 @@
       </c>
       <c r="J31" s="1">
         <f>SUM(J2:J30)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="K31" s="1">
         <f>SUM(K2:K30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2169,21 +2178,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2197,10 +2206,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add first try of persistence
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -427,7 +427,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,6 +458,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -481,7 +493,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -590,9 +602,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -605,23 +614,50 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1285,8 +1321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1332,7 @@
     <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="45" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="7.83203125" style="1" customWidth="1"/>
@@ -1323,7 +1359,7 @@
       <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="44" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1345,45 +1381,44 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="19">
+    <row r="2" spans="1:23" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A2" s="49">
         <v>0.1</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="50">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="51" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="48">
         <v>2</v>
       </c>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21">
-        <v>0</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="K2" s="48">
+        <v>0</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="48" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1399,7 +1434,7 @@
       <c r="E3" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
       <c r="I3" s="24"/>
@@ -1423,7 +1458,7 @@
       <c r="E4" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="28"/>
+      <c r="F4" s="47"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
@@ -1499,7 +1534,7 @@
       <c r="E7" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="47"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
@@ -1526,7 +1561,7 @@
       </c>
       <c r="D8" s="35"/>
       <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="F8" s="46"/>
       <c r="G8" s="36"/>
       <c r="H8" s="36"/>
       <c r="I8" s="37" t="s">
@@ -1536,41 +1571,41 @@
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:23" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
+    <row r="9" spans="1:23" s="48" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A9" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="50">
         <v>1</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="48">
         <v>5</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="48">
         <v>5</v>
       </c>
-      <c r="K9" s="21">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21" t="s">
+      <c r="K9" s="48">
+        <v>0</v>
+      </c>
+      <c r="L9" s="48" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1590,7 +1625,7 @@
       <c r="E10" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="45" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="21" t="s">
@@ -1636,7 +1671,7 @@
       </c>
       <c r="D12" s="29"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
+      <c r="F12" s="47"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
@@ -1648,60 +1683,59 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="19">
+    <row r="13" spans="1:23" s="48" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="49">
         <v>3.1</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="50">
         <v>1</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="21" t="s">
+      <c r="H13" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="48">
         <v>9</v>
       </c>
-      <c r="J13" s="21">
+      <c r="J13" s="48">
         <v>9</v>
       </c>
-      <c r="K13" s="21">
-        <v>0</v>
-      </c>
-      <c r="L13" s="21" t="s">
+      <c r="K13" s="48">
+        <v>0</v>
+      </c>
+      <c r="L13" s="48" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A14" s="39">
+      <c r="A14" s="38">
         <v>3.2</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="39">
         <v>1</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D14" s="41"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="41" t="s">
         <v>84</v>
       </c>
       <c r="J14" s="34"/>
@@ -1724,7 +1758,7 @@
       <c r="E15" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="45" t="s">
         <v>25</v>
       </c>
       <c r="G15" s="21" t="s">
@@ -1762,7 +1796,7 @@
       <c r="E16" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="45" t="s">
         <v>28</v>
       </c>
       <c r="G16" s="21" t="s">
@@ -1800,7 +1834,7 @@
       <c r="E17" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="45" t="s">
         <v>93</v>
       </c>
       <c r="G17" s="21" t="s">
@@ -1822,79 +1856,79 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
+    <row r="18" spans="1:12" s="48" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A18" s="49">
         <v>3.3</v>
       </c>
-      <c r="B18" s="20">
+      <c r="B18" s="50">
         <v>1</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="H18" s="21" t="s">
+      <c r="H18" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="48">
         <v>5</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="48">
         <v>5</v>
       </c>
-      <c r="K18" s="21">
-        <v>0</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
+      <c r="K18" s="48">
+        <v>0</v>
+      </c>
+      <c r="L18" s="48" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="48" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="49">
         <v>3.4</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="50">
         <v>1</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H19" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="48">
         <v>9</v>
       </c>
-      <c r="J19" s="21">
+      <c r="J19" s="48">
         <v>9</v>
       </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-      <c r="L19" s="21" t="s">
+      <c r="K19" s="48">
+        <v>0</v>
+      </c>
+      <c r="L19" s="48" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1914,7 +1948,7 @@
       <c r="E20" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="45" t="s">
         <v>31</v>
       </c>
       <c r="G20" s="21" t="s">
@@ -1936,41 +1970,41 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A21" s="43">
+    <row r="21" spans="1:12" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="53">
         <v>3.6</v>
       </c>
-      <c r="B21" s="44">
+      <c r="B21" s="54">
         <v>1</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="55" t="s">
         <v>101</v>
       </c>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="H21" s="45" t="s">
+      <c r="H21" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="45">
+      <c r="I21" s="55">
         <v>6</v>
       </c>
-      <c r="J21" s="45">
+      <c r="J21" s="55">
         <v>6</v>
       </c>
-      <c r="K21" s="45">
-        <v>0</v>
-      </c>
-      <c r="L21" s="45" t="s">
+      <c r="K21" s="55">
+        <v>0</v>
+      </c>
+      <c r="L21" s="55" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1981,7 +2015,7 @@
       <c r="C22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="42" t="s">
         <v>101</v>
       </c>
       <c r="K22" s="1">
@@ -1998,7 +2032,7 @@
       <c r="C23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E23" s="47" t="s">
+      <c r="E23" s="42" t="s">
         <v>108</v>
       </c>
       <c r="K23" s="1">
@@ -2017,10 +2051,10 @@
         <v>63</v>
       </c>
       <c r="D24" s="29"/>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="47"/>
       <c r="G24" s="28"/>
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
@@ -2039,7 +2073,7 @@
       <c r="C25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="42" t="s">
         <v>101</v>
       </c>
       <c r="K25" s="1">
@@ -2056,7 +2090,7 @@
       <c r="C26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="47" t="s">
+      <c r="E26" s="42" t="s">
         <v>108</v>
       </c>
       <c r="K26" s="1">
@@ -2078,7 +2112,7 @@
       <c r="E27" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="28"/>
+      <c r="F27" s="47"/>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
@@ -2097,7 +2131,7 @@
       <c r="C28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="E28" s="42" t="s">
         <v>101</v>
       </c>
       <c r="K28" s="1">
@@ -2114,7 +2148,7 @@
       <c r="C29" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="47" t="s">
+      <c r="E29" s="42" t="s">
         <v>112</v>
       </c>
       <c r="K29" s="1">
@@ -2136,7 +2170,7 @@
       <c r="E30" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="47"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>

</xml_diff>

<commit_message>
updated my scrum entries
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/ch.bfh.btx8081.w2017.blue.git/doc/04-ScrumSetup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/sophobia/doc/04-ScrumSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="17540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:W32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1409,8 +1409,11 @@
       <c r="I2" s="48">
         <v>2</v>
       </c>
+      <c r="J2" s="48">
+        <v>8</v>
+      </c>
       <c r="K2" s="48">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L2" s="48" t="s">
         <v>8</v>
@@ -1638,10 +1641,10 @@
         <v>3</v>
       </c>
       <c r="J10" s="21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K10" s="21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L10" s="21" t="s">
         <v>8</v>
@@ -1771,7 +1774,7 @@
         <v>4</v>
       </c>
       <c r="J15" s="21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K15" s="21">
         <v>0</v>
@@ -2192,11 +2195,11 @@
       </c>
       <c r="J31" s="1">
         <f>SUM(J2:J30)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K31" s="1">
         <f>SUM(K2:K30)</f>
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added new model (does not work with db yet)
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/sophobia/doc/04-ScrumSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="17535" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId3"/>
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
+    <sheet name="ScrumMeeting" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="127">
   <si>
     <t>ID</t>
   </si>
@@ -399,13 +400,25 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Scrum Meetings</t>
+  </si>
+  <si>
+    <t>Persistence Klasse soweit abgeschlossen</t>
+  </si>
+  <si>
+    <t>Patiene Model muss noch ganz fertig gemacht werden, kann aber bereits gelesen und in DB geschrieben werden</t>
+  </si>
+  <si>
+    <t>Main View beinahe fertig, wird noch gerezised, bis jetzt noch Dummywerte für Patient -&gt; es muss noch ein richtiger Patient von der DB geholt werden</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +438,29 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="22"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -496,7 +532,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -662,10 +698,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -966,21 +1005,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -991,7 +1030,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1002,7 +1041,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1013,7 +1052,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1024,7 +1063,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1035,7 +1074,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1046,7 +1085,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1059,12 +1098,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1072,26 +1111,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1117,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1144,7 +1183,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1171,7 +1210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1198,7 +1237,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1225,7 +1264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1249,7 +1288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1273,7 +1312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1297,7 +1336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>71</v>
       </c>
@@ -1321,32 +1360,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="30" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="45" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="7.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="45" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="7.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="49">
         <v>0.1</v>
       </c>
@@ -1428,7 +1467,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>80</v>
       </c>
@@ -1452,7 +1491,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>81</v>
       </c>
@@ -1482,7 +1521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="30">
         <v>1.1000000000000001</v>
       </c>
@@ -1505,7 +1544,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="30">
         <v>1.2</v>
       </c>
@@ -1528,7 +1567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="26">
         <v>1.3</v>
       </c>
@@ -1555,7 +1594,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>77</v>
       </c>
@@ -1577,7 +1616,7 @@
       <c r="K8" s="36"/>
       <c r="L8" s="36"/>
     </row>
-    <row r="9" spans="1:23" s="48" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="48" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A9" s="49" t="s">
         <v>42</v>
       </c>
@@ -1615,7 +1654,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>76</v>
       </c>
@@ -1653,7 +1692,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="30">
         <v>2.2000000000000002</v>
       </c>
@@ -1667,7 +1706,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="26">
         <v>2.2999999999999998</v>
       </c>
@@ -1689,7 +1728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="48" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="48" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="49">
         <v>3.1</v>
       </c>
@@ -1727,7 +1766,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="38">
         <v>3.2</v>
       </c>
@@ -1748,7 +1787,7 @@
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
     </row>
-    <row r="15" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
         <v>40</v>
       </c>
@@ -1786,7 +1825,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
         <v>41</v>
       </c>
@@ -1824,7 +1863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
         <v>87</v>
       </c>
@@ -1862,7 +1901,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="48" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="48" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A18" s="49">
         <v>3.3</v>
       </c>
@@ -1900,7 +1939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="48" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="48" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="49">
         <v>3.4</v>
       </c>
@@ -1938,7 +1977,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>3.5</v>
       </c>
@@ -1976,7 +2015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="48" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="53">
         <v>3.6</v>
       </c>
@@ -2014,7 +2053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="30">
         <v>4.0999999999999996</v>
       </c>
@@ -2031,7 +2070,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="30">
         <v>4.2</v>
       </c>
@@ -2048,7 +2087,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="26">
         <v>4.3</v>
       </c>
@@ -2072,7 +2111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="30">
         <v>5.0999999999999996</v>
       </c>
@@ -2089,7 +2128,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="30">
         <v>5.2</v>
       </c>
@@ -2106,7 +2145,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="26">
         <v>5.3</v>
       </c>
@@ -2130,7 +2169,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="30">
         <v>6.1</v>
       </c>
@@ -2147,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="30">
         <v>6.2</v>
       </c>
@@ -2164,7 +2203,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="26">
         <v>6.3</v>
       </c>
@@ -2188,7 +2227,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H31" s="1" t="s">
         <v>71</v>
       </c>
@@ -2205,7 +2244,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="H32" s="1" t="s">
         <v>74</v>
       </c>
@@ -2223,21 +2262,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -2251,14 +2290,55 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="58" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="59">
+        <v>43069</v>
+      </c>
+      <c r="B7" s="57" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B8" s="57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="B9" s="57" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update scrum after scrum meeting
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -397,9 +397,6 @@
     <t>Create Persinstance Helper methods</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>Persistence Klasse soweit abgeschlossen</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t>Diagnosis View should look the same as medication.</t>
+  </si>
+  <si>
+    <t>pending</t>
   </si>
 </sst>
 </file>
@@ -1590,10 +1590,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>177</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>178</v>
       </c>
       <c r="D9" s="66" t="s">
         <v>6</v>
@@ -1610,10 +1610,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="69" t="s">
         <v>6</v>
@@ -1652,10 +1652,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1751,7 +1752,7 @@
         <v>12</v>
       </c>
       <c r="L2" s="52" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="T2" s="52" t="s">
         <v>16</v>
@@ -1760,7 +1761,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>78</v>
       </c>
@@ -1784,7 +1785,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
         <v>79</v>
       </c>
@@ -1814,7 +1815,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
         <v>1.1000000000000001</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24">
         <v>1.2</v>
       </c>
@@ -1860,7 +1861,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>1.3</v>
       </c>
@@ -1944,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="L9" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1982,7 +1983,7 @@
         <v>5</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -1996,10 +1997,10 @@
         <v>50</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E11" s="65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F11" s="65" t="s">
         <v>27</v>
@@ -2023,7 +2024,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="54" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="54" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="55">
         <v>2.2999999999999998</v>
       </c>
@@ -2082,7 +2083,7 @@
         <v>12</v>
       </c>
       <c r="L13" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -2129,13 +2130,13 @@
         <v>4</v>
       </c>
       <c r="J15" s="33">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K15" s="59">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L15" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:23" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -2173,7 +2174,7 @@
         <v>7</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -2208,27 +2209,27 @@
         <v>3</v>
       </c>
       <c r="K17" s="59">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B18" s="62">
         <v>2</v>
       </c>
       <c r="C18" s="63" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="71" t="s">
         <v>134</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="E18" s="63" t="s">
         <v>135</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>136</v>
       </c>
       <c r="F18" s="63" t="s">
         <v>28</v>
@@ -2249,21 +2250,21 @@
         <v>6</v>
       </c>
       <c r="L18" s="63" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="61" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B19" s="62">
         <v>2</v>
       </c>
       <c r="C19" s="63" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="71" t="s">
         <v>138</v>
-      </c>
-      <c r="D19" s="71" t="s">
-        <v>139</v>
       </c>
       <c r="E19" s="63" t="s">
         <v>99</v>
@@ -2284,10 +2285,10 @@
         <v>3</v>
       </c>
       <c r="K19" s="63">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L19" s="63" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.2">
@@ -2325,7 +2326,7 @@
         <v>5</v>
       </c>
       <c r="L20" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -2363,21 +2364,21 @@
         <v>7</v>
       </c>
       <c r="L21" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A22" s="61" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="62">
         <v>2</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" s="71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E22" s="63" t="s">
         <v>110</v>
@@ -2401,21 +2402,21 @@
         <v>0</v>
       </c>
       <c r="L22" s="63" t="s">
-        <v>8</v>
+        <v>183</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B23" s="62">
         <v>2</v>
       </c>
       <c r="C23" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23" s="71" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E23" s="63" t="s">
         <v>110</v>
@@ -2477,7 +2478,7 @@
         <v>0</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -2515,21 +2516,21 @@
         <v>0</v>
       </c>
       <c r="L25" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A26" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B26" s="32">
         <v>1</v>
       </c>
       <c r="C26" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="D26" s="34" t="s">
         <v>182</v>
-      </c>
-      <c r="D26" s="34" t="s">
-        <v>183</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>99</v>
@@ -2553,7 +2554,7 @@
         <v>0</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="74" customFormat="1" ht="75" x14ac:dyDescent="0.2">
@@ -2564,10 +2565,10 @@
         <v>2</v>
       </c>
       <c r="C27" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="75" t="s">
         <v>155</v>
-      </c>
-      <c r="D27" s="75" t="s">
-        <v>156</v>
       </c>
       <c r="E27" s="65" t="s">
         <v>99</v>
@@ -2585,16 +2586,16 @@
         <v>5</v>
       </c>
       <c r="J27" s="74">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K27" s="74">
         <v>0</v>
       </c>
       <c r="L27" s="74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24">
         <v>4.2</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>4.3</v>
       </c>
@@ -2635,7 +2636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="24">
         <v>5.0999999999999996</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="24">
         <v>5.2</v>
       </c>
@@ -2669,7 +2670,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>5.3</v>
       </c>
@@ -2693,7 +2694,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="24">
         <v>6.1</v>
       </c>
@@ -2710,7 +2711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="24">
         <v>6.2</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>6.3</v>
       </c>
@@ -2753,16 +2754,16 @@
     </row>
     <row r="36" spans="1:17" s="74" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A36" s="76" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B36" s="77">
         <v>2</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E36" s="65" t="s">
         <v>110</v>
@@ -2780,27 +2781,27 @@
         <v>3</v>
       </c>
       <c r="J36" s="65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K36" s="65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L36" s="65" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:17" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="76" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B37" s="77">
         <v>2</v>
       </c>
       <c r="C37" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D37" s="64" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E37" s="65" t="s">
         <v>110</v>
@@ -2824,21 +2825,21 @@
         <v>1</v>
       </c>
       <c r="L37" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B38" s="77">
         <v>2</v>
       </c>
       <c r="C38" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D38" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E38" s="65" t="s">
         <v>110</v>
@@ -2861,20 +2862,22 @@
       <c r="K38" s="65">
         <v>0</v>
       </c>
-      <c r="L38" s="65"/>
+      <c r="L38" s="65" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="39" spans="1:17" s="74" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="76" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B39" s="77">
         <v>2</v>
       </c>
       <c r="C39" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" s="64" t="s">
         <v>163</v>
-      </c>
-      <c r="D39" s="64" t="s">
-        <v>164</v>
       </c>
       <c r="E39" s="65" t="s">
         <v>110</v>
@@ -2901,19 +2904,19 @@
     </row>
     <row r="40" spans="1:17" s="74" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B40" s="77">
         <v>2</v>
       </c>
       <c r="C40" s="65" t="s">
+        <v>149</v>
+      </c>
+      <c r="D40" s="64" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="65" t="s">
         <v>150</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>152</v>
-      </c>
-      <c r="E40" s="65" t="s">
-        <v>151</v>
       </c>
       <c r="F40" s="65" t="s">
         <v>28</v>
@@ -2963,13 +2966,13 @@
       <c r="G43" s="18"/>
       <c r="H43" s="18"/>
       <c r="I43" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="J43" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="J43" s="18" t="s">
+      <c r="K43" s="18" t="s">
         <v>171</v>
-      </c>
-      <c r="K43" s="18" t="s">
-        <v>172</v>
       </c>
       <c r="L43" s="18" t="s">
         <v>27</v>
@@ -2992,10 +2995,10 @@
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E44" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G44" s="79" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H44" s="79"/>
       <c r="I44" s="1">
@@ -3004,11 +3007,11 @@
       </c>
       <c r="J44" s="1">
         <f>SUMIF(B2:B40,1,J2:J40)</f>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="K44" s="1">
         <f>SUMIF(B2:B40,1,K2:K40)</f>
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="L44" s="1">
         <f>SUMIFS(I2:I40,B2:B40,1,F2:F40,"gfels6")</f>
@@ -3037,10 +3040,10 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E45" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G45" s="79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H45" s="79"/>
       <c r="I45" s="1">
@@ -3049,11 +3052,11 @@
       </c>
       <c r="J45" s="1">
         <f>SUMIF(B2:B40,2,J2:J40)</f>
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="K45" s="1">
         <f>SUMIF(B2:B40,2,K2:K40)</f>
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="L45" s="1">
         <f>SUMIFS(I2:I40,B2:B40,2,F2:F40,"gfels6")</f>
@@ -3082,10 +3085,10 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E46" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G46" s="79" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H46" s="79"/>
       <c r="I46" s="1">
@@ -3126,7 +3129,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:L40"/>
+  <autoFilter ref="B1:L40">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:C7">
     <sortCondition ref="A2"/>
   </sortState>
@@ -3196,7 +3205,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.3">
@@ -3204,10 +3213,10 @@
         <v>14</v>
       </c>
       <c r="B7" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>141</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
@@ -3218,7 +3227,7 @@
         <v>43062</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="48"/>
@@ -3241,7 +3250,7 @@
         <v>43063</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="48"/>
       <c r="E9" s="48"/>
@@ -3264,7 +3273,7 @@
         <v>43069</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D10" s="48"/>
       <c r="E10" s="48"/>
@@ -3283,7 +3292,7 @@
       <c r="A11" s="49"/>
       <c r="B11" s="48"/>
       <c r="C11" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="48"/>
@@ -3302,7 +3311,7 @@
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D12" s="48"/>
       <c r="E12" s="48"/>
@@ -3325,7 +3334,7 @@
         <v>43070</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D13" s="48"/>
       <c r="E13" s="48"/>
@@ -3348,7 +3357,7 @@
         <v>43070</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
@@ -9027,15 +9036,15 @@
   <sheetData>
     <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="47" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="48"/>
       <c r="D4" s="48"/>
@@ -9052,7 +9061,7 @@
         <v>43070</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -9067,7 +9076,7 @@
     <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="48"/>
       <c r="B6" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="48"/>
       <c r="D6" s="48"/>
@@ -9082,7 +9091,7 @@
     <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="48"/>
       <c r="B7" s="48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="48"/>
       <c r="D7" s="48"/>

</xml_diff>

<commit_message>
update time sprint 1
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/sophobia/doc/04-ScrumSetup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\03_Sem_HS\BTX8081_SoftwareEngineeringAndDesign\Eclipse\ch.bfh.btx8081.w2017.blue.git\doc\04-ScrumSetup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -22,11 +22,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$40</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -952,8 +949,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1261,14 +1258,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1279,7 +1276,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1290,7 +1287,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1301,7 +1298,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1312,7 +1309,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1334,7 +1331,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1367,19 +1364,19 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1405,7 +1402,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1432,7 +1429,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1459,7 +1456,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1486,7 +1483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1513,7 +1510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1537,7 +1534,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1561,7 +1558,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1585,7 +1582,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1605,7 +1602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1627,7 +1624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>70</v>
       </c>
@@ -1652,34 +1649,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="24" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="30" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="8.1640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.109375" style="1"/>
+    <col min="16" max="16" width="8.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="52" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" s="52" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="50">
         <v>0.1</v>
       </c>
@@ -1761,7 +1758,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>78</v>
       </c>
@@ -1785,7 +1782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>79</v>
       </c>
@@ -1815,7 +1812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
         <v>1.1000000000000001</v>
       </c>
@@ -1838,7 +1835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24">
         <v>1.2</v>
       </c>
@@ -1861,7 +1858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="20">
         <v>1.3</v>
       </c>
@@ -1888,7 +1885,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>75</v>
       </c>
@@ -1910,7 +1907,7 @@
       <c r="K8" s="35"/>
       <c r="L8" s="35"/>
     </row>
-    <row r="9" spans="1:23" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>42</v>
       </c>
@@ -1939,16 +1936,16 @@
         <v>5</v>
       </c>
       <c r="J9" s="33">
-        <v>5</v>
-      </c>
-      <c r="K9" s="59">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="K9" s="33">
+        <v>3</v>
       </c>
       <c r="L9" s="33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="37" t="s">
         <v>74</v>
       </c>
@@ -1986,7 +1983,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" s="63" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="61">
         <v>2.2000000000000002</v>
       </c>
@@ -2024,7 +2021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="54" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" s="54" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55">
         <v>2.2999999999999998</v>
       </c>
@@ -2048,7 +2045,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="33" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" s="33" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37">
         <v>3.1</v>
       </c>
@@ -2086,7 +2083,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37">
         <v>3.2</v>
       </c>
@@ -2101,7 +2098,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="37" t="s">
         <v>40</v>
       </c>
@@ -2139,7 +2136,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" s="33" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A16" s="37" t="s">
         <v>41</v>
       </c>
@@ -2177,7 +2174,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="33" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="33" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A17" s="37" t="s">
         <v>85</v>
       </c>
@@ -2215,7 +2212,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="63" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="61" t="s">
         <v>132</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="63" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="61" t="s">
         <v>136</v>
       </c>
@@ -2291,7 +2288,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="33" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A20" s="37">
         <v>3.3</v>
       </c>
@@ -2329,7 +2326,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="37">
         <v>3.4</v>
       </c>
@@ -2367,7 +2364,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="63" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="63" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="61" t="s">
         <v>152</v>
       </c>
@@ -2405,7 +2402,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="63" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="63" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A23" s="61" t="s">
         <v>156</v>
       </c>
@@ -2443,7 +2440,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="37">
         <v>3.5</v>
       </c>
@@ -2474,14 +2471,14 @@
       <c r="J24" s="33">
         <v>4</v>
       </c>
-      <c r="K24" s="59">
-        <v>0</v>
+      <c r="K24" s="33">
+        <v>5</v>
       </c>
       <c r="L24" s="33" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="40">
         <v>3.6</v>
       </c>
@@ -2519,7 +2516,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="33" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="33" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A26" s="31" t="s">
         <v>180</v>
       </c>
@@ -2557,7 +2554,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="74" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="74" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A27" s="72">
         <v>4.0999999999999996</v>
       </c>
@@ -2595,7 +2592,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24">
         <v>4.2</v>
       </c>
@@ -2612,7 +2609,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>4.3</v>
       </c>
@@ -2636,7 +2633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24">
         <v>5.0999999999999996</v>
       </c>
@@ -2653,7 +2650,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24">
         <v>5.2</v>
       </c>
@@ -2670,7 +2667,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20">
         <v>5.3</v>
       </c>
@@ -2694,7 +2691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24">
         <v>6.1</v>
       </c>
@@ -2711,7 +2708,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24">
         <v>6.2</v>
       </c>
@@ -2728,7 +2725,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20">
         <v>6.3</v>
       </c>
@@ -2752,7 +2749,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="74" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" s="74" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" s="76" t="s">
         <v>130</v>
       </c>
@@ -2790,7 +2787,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="74" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="76" t="s">
         <v>145</v>
       </c>
@@ -2828,7 +2825,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="76" t="s">
         <v>148</v>
       </c>
@@ -2866,7 +2863,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="74" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" s="74" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="76" t="s">
         <v>161</v>
       </c>
@@ -2902,7 +2899,7 @@
       </c>
       <c r="L39" s="65"/>
     </row>
-    <row r="40" spans="1:17" s="74" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" s="74" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="76" t="s">
         <v>178</v>
       </c>
@@ -2940,7 +2937,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="17"/>
       <c r="C41" s="18"/>
@@ -2954,13 +2951,13 @@
       <c r="K41" s="18"/>
       <c r="L41" s="18"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="17"/>
       <c r="C42" s="18"/>
       <c r="D42" s="19"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E43" s="18"/>
       <c r="F43" s="26"/>
       <c r="G43" s="18"/>
@@ -2993,7 +2990,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E44" s="1" t="s">
         <v>172</v>
       </c>
@@ -3007,11 +3004,11 @@
       </c>
       <c r="J44" s="1">
         <f>SUMIF(B2:B40,1,J2:J40)</f>
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K44" s="1">
         <f>SUMIF(B2:B40,1,K2:K40)</f>
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="L44" s="1">
         <f>SUMIFS(I2:I40,B2:B40,1,F2:F40,"gfels6")</f>
@@ -3038,7 +3035,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E45" s="1" t="s">
         <v>173</v>
       </c>
@@ -3083,7 +3080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E46" s="1" t="s">
         <v>174</v>
       </c>
@@ -3157,14 +3154,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>21</v>
       </c>
@@ -3178,10 +3175,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -3198,17 +3195,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="28" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="46" t="s">
         <v>14</v>
       </c>
@@ -3219,7 +3216,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="48">
         <v>1</v>
       </c>
@@ -3242,7 +3239,7 @@
       <c r="N8" s="48"/>
       <c r="O8" s="48"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="48">
         <v>1</v>
       </c>
@@ -3265,7 +3262,7 @@
       <c r="N9" s="48"/>
       <c r="O9" s="48"/>
     </row>
-    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="49">
         <v>1</v>
       </c>
@@ -3288,7 +3285,7 @@
       <c r="N10" s="48"/>
       <c r="O10" s="48"/>
     </row>
-    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="49"/>
       <c r="B11" s="48"/>
       <c r="C11" s="48" t="s">
@@ -3307,7 +3304,7 @@
       <c r="N11" s="48"/>
       <c r="O11" s="48"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48" t="s">
@@ -3326,7 +3323,7 @@
       <c r="N12" s="48"/>
       <c r="O12" s="48"/>
     </row>
-    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="49">
         <v>1</v>
       </c>
@@ -3349,7 +3346,7 @@
       <c r="N13" s="48"/>
       <c r="O13" s="48"/>
     </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="49">
         <v>2</v>
       </c>
@@ -3372,7 +3369,7 @@
       <c r="N14" s="48"/>
       <c r="O14" s="48"/>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="49"/>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -3389,7 +3386,7 @@
       <c r="N15" s="48"/>
       <c r="O15" s="48"/>
     </row>
-    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="49"/>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -3406,7 +3403,7 @@
       <c r="N16" s="48"/>
       <c r="O16" s="48"/>
     </row>
-    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="49"/>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
@@ -3423,7 +3420,7 @@
       <c r="N17" s="48"/>
       <c r="O17" s="48"/>
     </row>
-    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="49"/>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -3440,7 +3437,7 @@
       <c r="N18" s="48"/>
       <c r="O18" s="48"/>
     </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="49"/>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>
@@ -3457,7 +3454,7 @@
       <c r="N19" s="48"/>
       <c r="O19" s="48"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A20" s="49"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -3474,7 +3471,7 @@
       <c r="N20" s="48"/>
       <c r="O20" s="48"/>
     </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="49"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -3491,7 +3488,7 @@
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
     </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="49"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -3508,7 +3505,7 @@
       <c r="N22" s="48"/>
       <c r="O22" s="48"/>
     </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="49"/>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -3525,7 +3522,7 @@
       <c r="N23" s="48"/>
       <c r="O23" s="48"/>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="49"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
@@ -3542,7 +3539,7 @@
       <c r="N24" s="48"/>
       <c r="O24" s="48"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="49"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
@@ -3559,7 +3556,7 @@
       <c r="N25" s="48"/>
       <c r="O25" s="48"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="49"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
@@ -3576,7 +3573,7 @@
       <c r="N26" s="48"/>
       <c r="O26" s="48"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="49"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
@@ -3593,7 +3590,7 @@
       <c r="N27" s="48"/>
       <c r="O27" s="48"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="49"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
@@ -3610,7 +3607,7 @@
       <c r="N28" s="48"/>
       <c r="O28" s="48"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A29" s="49"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
@@ -3627,7 +3624,7 @@
       <c r="N29" s="48"/>
       <c r="O29" s="48"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="49"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
@@ -3644,7 +3641,7 @@
       <c r="N30" s="48"/>
       <c r="O30" s="48"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="49"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
@@ -3661,7 +3658,7 @@
       <c r="N31" s="48"/>
       <c r="O31" s="48"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="49"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
@@ -3678,7 +3675,7 @@
       <c r="N32" s="48"/>
       <c r="O32" s="48"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="49"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -3695,7 +3692,7 @@
       <c r="N33" s="48"/>
       <c r="O33" s="48"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="49"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
@@ -3712,7 +3709,7 @@
       <c r="N34" s="48"/>
       <c r="O34" s="48"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="49"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -3729,7 +3726,7 @@
       <c r="N35" s="48"/>
       <c r="O35" s="48"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="49"/>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -3746,7 +3743,7 @@
       <c r="N36" s="48"/>
       <c r="O36" s="48"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="49"/>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
@@ -3763,7 +3760,7 @@
       <c r="N37" s="48"/>
       <c r="O37" s="48"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="49"/>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3780,7 +3777,7 @@
       <c r="N38" s="48"/>
       <c r="O38" s="48"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="49"/>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
@@ -3797,7 +3794,7 @@
       <c r="N39" s="48"/>
       <c r="O39" s="48"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="49"/>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
@@ -3814,7 +3811,7 @@
       <c r="N40" s="48"/>
       <c r="O40" s="48"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="49"/>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -3831,7 +3828,7 @@
       <c r="N41" s="48"/>
       <c r="O41" s="48"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A42" s="49"/>
       <c r="B42" s="48"/>
       <c r="C42" s="48"/>
@@ -3848,7 +3845,7 @@
       <c r="N42" s="48"/>
       <c r="O42" s="48"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A43" s="49"/>
       <c r="B43" s="48"/>
       <c r="C43" s="48"/>
@@ -3865,7 +3862,7 @@
       <c r="N43" s="48"/>
       <c r="O43" s="48"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A44" s="49"/>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
@@ -3882,7 +3879,7 @@
       <c r="N44" s="48"/>
       <c r="O44" s="48"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A45" s="49"/>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
@@ -3899,7 +3896,7 @@
       <c r="N45" s="48"/>
       <c r="O45" s="48"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A46" s="49"/>
       <c r="B46" s="48"/>
       <c r="C46" s="48"/>
@@ -3916,7 +3913,7 @@
       <c r="N46" s="48"/>
       <c r="O46" s="48"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A47" s="49"/>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
@@ -3933,7 +3930,7 @@
       <c r="N47" s="48"/>
       <c r="O47" s="48"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A48" s="49"/>
       <c r="B48" s="48"/>
       <c r="C48" s="48"/>
@@ -3950,7 +3947,7 @@
       <c r="N48" s="48"/>
       <c r="O48" s="48"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A49" s="49"/>
       <c r="B49" s="48"/>
       <c r="C49" s="48"/>
@@ -3967,7 +3964,7 @@
       <c r="N49" s="48"/>
       <c r="O49" s="48"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="49"/>
       <c r="B50" s="48"/>
       <c r="C50" s="48"/>
@@ -3984,7 +3981,7 @@
       <c r="N50" s="48"/>
       <c r="O50" s="48"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A51" s="49"/>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
@@ -4001,7 +3998,7 @@
       <c r="N51" s="48"/>
       <c r="O51" s="48"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="49"/>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
@@ -4018,7 +4015,7 @@
       <c r="N52" s="48"/>
       <c r="O52" s="48"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A53" s="49"/>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
@@ -4035,7 +4032,7 @@
       <c r="N53" s="48"/>
       <c r="O53" s="48"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A54" s="49"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
@@ -4052,7 +4049,7 @@
       <c r="N54" s="48"/>
       <c r="O54" s="48"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A55" s="49"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
@@ -4069,7 +4066,7 @@
       <c r="N55" s="48"/>
       <c r="O55" s="48"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A56" s="49"/>
       <c r="B56" s="48"/>
       <c r="C56" s="48"/>
@@ -4086,7 +4083,7 @@
       <c r="N56" s="48"/>
       <c r="O56" s="48"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A57" s="49"/>
       <c r="B57" s="48"/>
       <c r="C57" s="48"/>
@@ -4103,7 +4100,7 @@
       <c r="N57" s="48"/>
       <c r="O57" s="48"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A58" s="48"/>
       <c r="B58" s="48"/>
       <c r="C58" s="48"/>
@@ -4120,7 +4117,7 @@
       <c r="N58" s="48"/>
       <c r="O58" s="48"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A59" s="48"/>
       <c r="B59" s="48"/>
       <c r="C59" s="48"/>
@@ -4137,7 +4134,7 @@
       <c r="N59" s="48"/>
       <c r="O59" s="48"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A60" s="48"/>
       <c r="B60" s="48"/>
       <c r="C60" s="48"/>
@@ -4154,7 +4151,7 @@
       <c r="N60" s="48"/>
       <c r="O60" s="48"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A61" s="48"/>
       <c r="B61" s="48"/>
       <c r="C61" s="48"/>
@@ -4171,7 +4168,7 @@
       <c r="N61" s="48"/>
       <c r="O61" s="48"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A62" s="48"/>
       <c r="B62" s="48"/>
       <c r="C62" s="48"/>
@@ -4188,7 +4185,7 @@
       <c r="N62" s="48"/>
       <c r="O62" s="48"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A63" s="48"/>
       <c r="B63" s="48"/>
       <c r="C63" s="48"/>
@@ -4205,7 +4202,7 @@
       <c r="N63" s="48"/>
       <c r="O63" s="48"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A64" s="48"/>
       <c r="B64" s="48"/>
       <c r="C64" s="48"/>
@@ -4222,7 +4219,7 @@
       <c r="N64" s="48"/>
       <c r="O64" s="48"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A65" s="48"/>
       <c r="B65" s="48"/>
       <c r="C65" s="48"/>
@@ -4239,7 +4236,7 @@
       <c r="N65" s="48"/>
       <c r="O65" s="48"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A66" s="48"/>
       <c r="B66" s="48"/>
       <c r="C66" s="48"/>
@@ -4256,7 +4253,7 @@
       <c r="N66" s="48"/>
       <c r="O66" s="48"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A67" s="48"/>
       <c r="B67" s="48"/>
       <c r="C67" s="48"/>
@@ -4273,7 +4270,7 @@
       <c r="N67" s="48"/>
       <c r="O67" s="48"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A68" s="48"/>
       <c r="B68" s="48"/>
       <c r="C68" s="48"/>
@@ -4290,7 +4287,7 @@
       <c r="N68" s="48"/>
       <c r="O68" s="48"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A69" s="48"/>
       <c r="B69" s="48"/>
       <c r="C69" s="48"/>
@@ -4307,7 +4304,7 @@
       <c r="N69" s="48"/>
       <c r="O69" s="48"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A70" s="48"/>
       <c r="B70" s="48"/>
       <c r="C70" s="48"/>
@@ -4324,7 +4321,7 @@
       <c r="N70" s="48"/>
       <c r="O70" s="48"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A71" s="48"/>
       <c r="B71" s="48"/>
       <c r="C71" s="48"/>
@@ -4341,7 +4338,7 @@
       <c r="N71" s="48"/>
       <c r="O71" s="48"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A72" s="48"/>
       <c r="B72" s="48"/>
       <c r="C72" s="48"/>
@@ -4358,7 +4355,7 @@
       <c r="N72" s="48"/>
       <c r="O72" s="48"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A73" s="48"/>
       <c r="B73" s="48"/>
       <c r="C73" s="48"/>
@@ -4375,7 +4372,7 @@
       <c r="N73" s="48"/>
       <c r="O73" s="48"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A74" s="48"/>
       <c r="B74" s="48"/>
       <c r="C74" s="48"/>
@@ -4392,7 +4389,7 @@
       <c r="N74" s="48"/>
       <c r="O74" s="48"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A75" s="48"/>
       <c r="B75" s="48"/>
       <c r="C75" s="48"/>
@@ -4409,7 +4406,7 @@
       <c r="N75" s="48"/>
       <c r="O75" s="48"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A76" s="48"/>
       <c r="B76" s="48"/>
       <c r="C76" s="48"/>
@@ -4426,7 +4423,7 @@
       <c r="N76" s="48"/>
       <c r="O76" s="48"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A77" s="48"/>
       <c r="B77" s="48"/>
       <c r="C77" s="48"/>
@@ -4443,7 +4440,7 @@
       <c r="N77" s="48"/>
       <c r="O77" s="48"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A78" s="48"/>
       <c r="B78" s="48"/>
       <c r="C78" s="48"/>
@@ -4460,7 +4457,7 @@
       <c r="N78" s="48"/>
       <c r="O78" s="48"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A79" s="48"/>
       <c r="B79" s="48"/>
       <c r="C79" s="48"/>
@@ -4477,7 +4474,7 @@
       <c r="N79" s="48"/>
       <c r="O79" s="48"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A80" s="48"/>
       <c r="B80" s="48"/>
       <c r="C80" s="48"/>
@@ -4494,7 +4491,7 @@
       <c r="N80" s="48"/>
       <c r="O80" s="48"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A81" s="48"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
@@ -4511,7 +4508,7 @@
       <c r="N81" s="48"/>
       <c r="O81" s="48"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A82" s="48"/>
       <c r="B82" s="48"/>
       <c r="C82" s="48"/>
@@ -4528,7 +4525,7 @@
       <c r="N82" s="48"/>
       <c r="O82" s="48"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A83" s="48"/>
       <c r="B83" s="48"/>
       <c r="C83" s="48"/>
@@ -4545,7 +4542,7 @@
       <c r="N83" s="48"/>
       <c r="O83" s="48"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A84" s="48"/>
       <c r="B84" s="48"/>
       <c r="C84" s="48"/>
@@ -4562,7 +4559,7 @@
       <c r="N84" s="48"/>
       <c r="O84" s="48"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A85" s="48"/>
       <c r="B85" s="48"/>
       <c r="C85" s="48"/>
@@ -4579,7 +4576,7 @@
       <c r="N85" s="48"/>
       <c r="O85" s="48"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A86" s="48"/>
       <c r="B86" s="48"/>
       <c r="C86" s="48"/>
@@ -4596,7 +4593,7 @@
       <c r="N86" s="48"/>
       <c r="O86" s="48"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A87" s="48"/>
       <c r="B87" s="48"/>
       <c r="C87" s="48"/>
@@ -4613,7 +4610,7 @@
       <c r="N87" s="48"/>
       <c r="O87" s="48"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A88" s="48"/>
       <c r="B88" s="48"/>
       <c r="C88" s="48"/>
@@ -4630,7 +4627,7 @@
       <c r="N88" s="48"/>
       <c r="O88" s="48"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A89" s="48"/>
       <c r="B89" s="48"/>
       <c r="C89" s="48"/>
@@ -4647,7 +4644,7 @@
       <c r="N89" s="48"/>
       <c r="O89" s="48"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A90" s="48"/>
       <c r="B90" s="48"/>
       <c r="C90" s="48"/>
@@ -4664,7 +4661,7 @@
       <c r="N90" s="48"/>
       <c r="O90" s="48"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A91" s="48"/>
       <c r="B91" s="48"/>
       <c r="C91" s="48"/>
@@ -4681,7 +4678,7 @@
       <c r="N91" s="48"/>
       <c r="O91" s="48"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A92" s="48"/>
       <c r="B92" s="48"/>
       <c r="C92" s="48"/>
@@ -4698,7 +4695,7 @@
       <c r="N92" s="48"/>
       <c r="O92" s="48"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A93" s="48"/>
       <c r="B93" s="48"/>
       <c r="C93" s="48"/>
@@ -4715,7 +4712,7 @@
       <c r="N93" s="48"/>
       <c r="O93" s="48"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A94" s="48"/>
       <c r="B94" s="48"/>
       <c r="C94" s="48"/>
@@ -4732,7 +4729,7 @@
       <c r="N94" s="48"/>
       <c r="O94" s="48"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A95" s="48"/>
       <c r="B95" s="48"/>
       <c r="C95" s="48"/>
@@ -4749,7 +4746,7 @@
       <c r="N95" s="48"/>
       <c r="O95" s="48"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A96" s="48"/>
       <c r="B96" s="48"/>
       <c r="C96" s="48"/>
@@ -4766,7 +4763,7 @@
       <c r="N96" s="48"/>
       <c r="O96" s="48"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A97" s="48"/>
       <c r="B97" s="48"/>
       <c r="C97" s="48"/>
@@ -4783,7 +4780,7 @@
       <c r="N97" s="48"/>
       <c r="O97" s="48"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A98" s="48"/>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
@@ -4800,7 +4797,7 @@
       <c r="N98" s="48"/>
       <c r="O98" s="48"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A99" s="48"/>
       <c r="B99" s="48"/>
       <c r="C99" s="48"/>
@@ -4817,7 +4814,7 @@
       <c r="N99" s="48"/>
       <c r="O99" s="48"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A100" s="48"/>
       <c r="B100" s="48"/>
       <c r="C100" s="48"/>
@@ -4834,7 +4831,7 @@
       <c r="N100" s="48"/>
       <c r="O100" s="48"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A101" s="48"/>
       <c r="B101" s="48"/>
       <c r="C101" s="48"/>
@@ -4851,7 +4848,7 @@
       <c r="N101" s="48"/>
       <c r="O101" s="48"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A102" s="48"/>
       <c r="B102" s="48"/>
       <c r="C102" s="48"/>
@@ -4868,7 +4865,7 @@
       <c r="N102" s="48"/>
       <c r="O102" s="48"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A103" s="48"/>
       <c r="B103" s="48"/>
       <c r="C103" s="48"/>
@@ -4885,7 +4882,7 @@
       <c r="N103" s="48"/>
       <c r="O103" s="48"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A104" s="48"/>
       <c r="B104" s="48"/>
       <c r="C104" s="48"/>
@@ -4902,7 +4899,7 @@
       <c r="N104" s="48"/>
       <c r="O104" s="48"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A105" s="48"/>
       <c r="B105" s="48"/>
       <c r="C105" s="48"/>
@@ -4919,7 +4916,7 @@
       <c r="N105" s="48"/>
       <c r="O105" s="48"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A106" s="48"/>
       <c r="B106" s="48"/>
       <c r="C106" s="48"/>
@@ -4936,7 +4933,7 @@
       <c r="N106" s="48"/>
       <c r="O106" s="48"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A107" s="48"/>
       <c r="B107" s="48"/>
       <c r="C107" s="48"/>
@@ -4953,7 +4950,7 @@
       <c r="N107" s="48"/>
       <c r="O107" s="48"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A108" s="48"/>
       <c r="B108" s="48"/>
       <c r="C108" s="48"/>
@@ -4970,7 +4967,7 @@
       <c r="N108" s="48"/>
       <c r="O108" s="48"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A109" s="48"/>
       <c r="B109" s="48"/>
       <c r="C109" s="48"/>
@@ -4987,7 +4984,7 @@
       <c r="N109" s="48"/>
       <c r="O109" s="48"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A110" s="48"/>
       <c r="B110" s="48"/>
       <c r="C110" s="48"/>
@@ -5004,7 +5001,7 @@
       <c r="N110" s="48"/>
       <c r="O110" s="48"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A111" s="48"/>
       <c r="B111" s="48"/>
       <c r="C111" s="48"/>
@@ -5021,7 +5018,7 @@
       <c r="N111" s="48"/>
       <c r="O111" s="48"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A112" s="48"/>
       <c r="B112" s="48"/>
       <c r="C112" s="48"/>
@@ -5038,7 +5035,7 @@
       <c r="N112" s="48"/>
       <c r="O112" s="48"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A113" s="48"/>
       <c r="B113" s="48"/>
       <c r="C113" s="48"/>
@@ -5055,7 +5052,7 @@
       <c r="N113" s="48"/>
       <c r="O113" s="48"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A114" s="48"/>
       <c r="B114" s="48"/>
       <c r="C114" s="48"/>
@@ -5072,7 +5069,7 @@
       <c r="N114" s="48"/>
       <c r="O114" s="48"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A115" s="48"/>
       <c r="B115" s="48"/>
       <c r="C115" s="48"/>
@@ -5089,7 +5086,7 @@
       <c r="N115" s="48"/>
       <c r="O115" s="48"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A116" s="48"/>
       <c r="B116" s="48"/>
       <c r="C116" s="48"/>
@@ -5106,7 +5103,7 @@
       <c r="N116" s="48"/>
       <c r="O116" s="48"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A117" s="48"/>
       <c r="B117" s="48"/>
       <c r="C117" s="48"/>
@@ -5123,7 +5120,7 @@
       <c r="N117" s="48"/>
       <c r="O117" s="48"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A118" s="48"/>
       <c r="B118" s="48"/>
       <c r="C118" s="48"/>
@@ -5140,7 +5137,7 @@
       <c r="N118" s="48"/>
       <c r="O118" s="48"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A119" s="48"/>
       <c r="B119" s="48"/>
       <c r="C119" s="48"/>
@@ -5157,7 +5154,7 @@
       <c r="N119" s="48"/>
       <c r="O119" s="48"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A120" s="48"/>
       <c r="B120" s="48"/>
       <c r="C120" s="48"/>
@@ -5174,7 +5171,7 @@
       <c r="N120" s="48"/>
       <c r="O120" s="48"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A121" s="48"/>
       <c r="B121" s="48"/>
       <c r="C121" s="48"/>
@@ -5191,7 +5188,7 @@
       <c r="N121" s="48"/>
       <c r="O121" s="48"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A122" s="48"/>
       <c r="B122" s="48"/>
       <c r="C122" s="48"/>
@@ -5208,7 +5205,7 @@
       <c r="N122" s="48"/>
       <c r="O122" s="48"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A123" s="48"/>
       <c r="B123" s="48"/>
       <c r="C123" s="48"/>
@@ -5225,7 +5222,7 @@
       <c r="N123" s="48"/>
       <c r="O123" s="48"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A124" s="48"/>
       <c r="B124" s="48"/>
       <c r="C124" s="48"/>
@@ -5242,7 +5239,7 @@
       <c r="N124" s="48"/>
       <c r="O124" s="48"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A125" s="48"/>
       <c r="B125" s="48"/>
       <c r="C125" s="48"/>
@@ -5259,7 +5256,7 @@
       <c r="N125" s="48"/>
       <c r="O125" s="48"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A126" s="48"/>
       <c r="B126" s="48"/>
       <c r="C126" s="48"/>
@@ -5276,7 +5273,7 @@
       <c r="N126" s="48"/>
       <c r="O126" s="48"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A127" s="48"/>
       <c r="B127" s="48"/>
       <c r="C127" s="48"/>
@@ -5293,7 +5290,7 @@
       <c r="N127" s="48"/>
       <c r="O127" s="48"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A128" s="48"/>
       <c r="B128" s="48"/>
       <c r="C128" s="48"/>
@@ -5310,7 +5307,7 @@
       <c r="N128" s="48"/>
       <c r="O128" s="48"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A129" s="48"/>
       <c r="B129" s="48"/>
       <c r="C129" s="48"/>
@@ -5327,7 +5324,7 @@
       <c r="N129" s="48"/>
       <c r="O129" s="48"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A130" s="48"/>
       <c r="B130" s="48"/>
       <c r="C130" s="48"/>
@@ -5344,7 +5341,7 @@
       <c r="N130" s="48"/>
       <c r="O130" s="48"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A131" s="48"/>
       <c r="B131" s="48"/>
       <c r="C131" s="48"/>
@@ -5361,7 +5358,7 @@
       <c r="N131" s="48"/>
       <c r="O131" s="48"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A132" s="48"/>
       <c r="B132" s="48"/>
       <c r="C132" s="48"/>
@@ -5378,7 +5375,7 @@
       <c r="N132" s="48"/>
       <c r="O132" s="48"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A133" s="48"/>
       <c r="B133" s="48"/>
       <c r="C133" s="48"/>
@@ -5395,7 +5392,7 @@
       <c r="N133" s="48"/>
       <c r="O133" s="48"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A134" s="48"/>
       <c r="B134" s="48"/>
       <c r="C134" s="48"/>
@@ -5412,7 +5409,7 @@
       <c r="N134" s="48"/>
       <c r="O134" s="48"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A135" s="48"/>
       <c r="B135" s="48"/>
       <c r="C135" s="48"/>
@@ -5429,7 +5426,7 @@
       <c r="N135" s="48"/>
       <c r="O135" s="48"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A136" s="48"/>
       <c r="B136" s="48"/>
       <c r="C136" s="48"/>
@@ -5446,7 +5443,7 @@
       <c r="N136" s="48"/>
       <c r="O136" s="48"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A137" s="48"/>
       <c r="B137" s="48"/>
       <c r="C137" s="48"/>
@@ -5463,7 +5460,7 @@
       <c r="N137" s="48"/>
       <c r="O137" s="48"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A138" s="48"/>
       <c r="B138" s="48"/>
       <c r="C138" s="48"/>
@@ -5480,7 +5477,7 @@
       <c r="N138" s="48"/>
       <c r="O138" s="48"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A139" s="48"/>
       <c r="B139" s="48"/>
       <c r="C139" s="48"/>
@@ -5497,7 +5494,7 @@
       <c r="N139" s="48"/>
       <c r="O139" s="48"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A140" s="48"/>
       <c r="B140" s="48"/>
       <c r="C140" s="48"/>
@@ -5514,7 +5511,7 @@
       <c r="N140" s="48"/>
       <c r="O140" s="48"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A141" s="48"/>
       <c r="B141" s="48"/>
       <c r="C141" s="48"/>
@@ -5531,7 +5528,7 @@
       <c r="N141" s="48"/>
       <c r="O141" s="48"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A142" s="48"/>
       <c r="B142" s="48"/>
       <c r="C142" s="48"/>
@@ -5548,7 +5545,7 @@
       <c r="N142" s="48"/>
       <c r="O142" s="48"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A143" s="48"/>
       <c r="B143" s="48"/>
       <c r="C143" s="48"/>
@@ -5565,7 +5562,7 @@
       <c r="N143" s="48"/>
       <c r="O143" s="48"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A144" s="48"/>
       <c r="B144" s="48"/>
       <c r="C144" s="48"/>
@@ -5582,7 +5579,7 @@
       <c r="N144" s="48"/>
       <c r="O144" s="48"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A145" s="48"/>
       <c r="B145" s="48"/>
       <c r="C145" s="48"/>
@@ -5599,7 +5596,7 @@
       <c r="N145" s="48"/>
       <c r="O145" s="48"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A146" s="48"/>
       <c r="B146" s="48"/>
       <c r="C146" s="48"/>
@@ -5616,7 +5613,7 @@
       <c r="N146" s="48"/>
       <c r="O146" s="48"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A147" s="48"/>
       <c r="B147" s="48"/>
       <c r="C147" s="48"/>
@@ -5633,7 +5630,7 @@
       <c r="N147" s="48"/>
       <c r="O147" s="48"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A148" s="48"/>
       <c r="B148" s="48"/>
       <c r="C148" s="48"/>
@@ -5650,7 +5647,7 @@
       <c r="N148" s="48"/>
       <c r="O148" s="48"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A149" s="48"/>
       <c r="B149" s="48"/>
       <c r="C149" s="48"/>
@@ -5667,7 +5664,7 @@
       <c r="N149" s="48"/>
       <c r="O149" s="48"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A150" s="48"/>
       <c r="B150" s="48"/>
       <c r="C150" s="48"/>
@@ -5684,7 +5681,7 @@
       <c r="N150" s="48"/>
       <c r="O150" s="48"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A151" s="48"/>
       <c r="B151" s="48"/>
       <c r="C151" s="48"/>
@@ -5701,7 +5698,7 @@
       <c r="N151" s="48"/>
       <c r="O151" s="48"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A152" s="48"/>
       <c r="B152" s="48"/>
       <c r="C152" s="48"/>
@@ -5718,7 +5715,7 @@
       <c r="N152" s="48"/>
       <c r="O152" s="48"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A153" s="48"/>
       <c r="B153" s="48"/>
       <c r="C153" s="48"/>
@@ -5735,7 +5732,7 @@
       <c r="N153" s="48"/>
       <c r="O153" s="48"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A154" s="48"/>
       <c r="B154" s="48"/>
       <c r="C154" s="48"/>
@@ -5752,7 +5749,7 @@
       <c r="N154" s="48"/>
       <c r="O154" s="48"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A155" s="48"/>
       <c r="B155" s="48"/>
       <c r="C155" s="48"/>
@@ -5769,7 +5766,7 @@
       <c r="N155" s="48"/>
       <c r="O155" s="48"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A156" s="48"/>
       <c r="B156" s="48"/>
       <c r="C156" s="48"/>
@@ -5786,7 +5783,7 @@
       <c r="N156" s="48"/>
       <c r="O156" s="48"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A157" s="48"/>
       <c r="B157" s="48"/>
       <c r="C157" s="48"/>
@@ -5803,7 +5800,7 @@
       <c r="N157" s="48"/>
       <c r="O157" s="48"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A158" s="48"/>
       <c r="B158" s="48"/>
       <c r="C158" s="48"/>
@@ -5820,7 +5817,7 @@
       <c r="N158" s="48"/>
       <c r="O158" s="48"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A159" s="48"/>
       <c r="B159" s="48"/>
       <c r="C159" s="48"/>
@@ -5837,7 +5834,7 @@
       <c r="N159" s="48"/>
       <c r="O159" s="48"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A160" s="48"/>
       <c r="B160" s="48"/>
       <c r="C160" s="48"/>
@@ -5854,7 +5851,7 @@
       <c r="N160" s="48"/>
       <c r="O160" s="48"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A161" s="48"/>
       <c r="B161" s="48"/>
       <c r="C161" s="48"/>
@@ -5871,7 +5868,7 @@
       <c r="N161" s="48"/>
       <c r="O161" s="48"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A162" s="48"/>
       <c r="B162" s="48"/>
       <c r="C162" s="48"/>
@@ -5888,7 +5885,7 @@
       <c r="N162" s="48"/>
       <c r="O162" s="48"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A163" s="48"/>
       <c r="B163" s="48"/>
       <c r="C163" s="48"/>
@@ -5905,7 +5902,7 @@
       <c r="N163" s="48"/>
       <c r="O163" s="48"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A164" s="48"/>
       <c r="B164" s="48"/>
       <c r="C164" s="48"/>
@@ -5922,7 +5919,7 @@
       <c r="N164" s="48"/>
       <c r="O164" s="48"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A165" s="48"/>
       <c r="B165" s="48"/>
       <c r="C165" s="48"/>
@@ -5939,7 +5936,7 @@
       <c r="N165" s="48"/>
       <c r="O165" s="48"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A166" s="48"/>
       <c r="B166" s="48"/>
       <c r="C166" s="48"/>
@@ -5956,7 +5953,7 @@
       <c r="N166" s="48"/>
       <c r="O166" s="48"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A167" s="48"/>
       <c r="B167" s="48"/>
       <c r="C167" s="48"/>
@@ -5973,7 +5970,7 @@
       <c r="N167" s="48"/>
       <c r="O167" s="48"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A168" s="48"/>
       <c r="B168" s="48"/>
       <c r="C168" s="48"/>
@@ -5990,7 +5987,7 @@
       <c r="N168" s="48"/>
       <c r="O168" s="48"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A169" s="48"/>
       <c r="B169" s="48"/>
       <c r="C169" s="48"/>
@@ -6007,7 +6004,7 @@
       <c r="N169" s="48"/>
       <c r="O169" s="48"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A170" s="48"/>
       <c r="B170" s="48"/>
       <c r="C170" s="48"/>
@@ -6024,7 +6021,7 @@
       <c r="N170" s="48"/>
       <c r="O170" s="48"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A171" s="48"/>
       <c r="B171" s="48"/>
       <c r="C171" s="48"/>
@@ -6041,7 +6038,7 @@
       <c r="N171" s="48"/>
       <c r="O171" s="48"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A172" s="48"/>
       <c r="B172" s="48"/>
       <c r="C172" s="48"/>
@@ -6058,7 +6055,7 @@
       <c r="N172" s="48"/>
       <c r="O172" s="48"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A173" s="48"/>
       <c r="B173" s="48"/>
       <c r="C173" s="48"/>
@@ -6075,7 +6072,7 @@
       <c r="N173" s="48"/>
       <c r="O173" s="48"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A174" s="48"/>
       <c r="B174" s="48"/>
       <c r="C174" s="48"/>
@@ -6092,7 +6089,7 @@
       <c r="N174" s="48"/>
       <c r="O174" s="48"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A175" s="48"/>
       <c r="B175" s="48"/>
       <c r="C175" s="48"/>
@@ -6109,7 +6106,7 @@
       <c r="N175" s="48"/>
       <c r="O175" s="48"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A176" s="48"/>
       <c r="B176" s="48"/>
       <c r="C176" s="48"/>
@@ -6126,7 +6123,7 @@
       <c r="N176" s="48"/>
       <c r="O176" s="48"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A177" s="48"/>
       <c r="B177" s="48"/>
       <c r="C177" s="48"/>
@@ -6143,7 +6140,7 @@
       <c r="N177" s="48"/>
       <c r="O177" s="48"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A178" s="48"/>
       <c r="B178" s="48"/>
       <c r="C178" s="48"/>
@@ -6160,7 +6157,7 @@
       <c r="N178" s="48"/>
       <c r="O178" s="48"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A179" s="48"/>
       <c r="B179" s="48"/>
       <c r="C179" s="48"/>
@@ -6177,7 +6174,7 @@
       <c r="N179" s="48"/>
       <c r="O179" s="48"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A180" s="48"/>
       <c r="B180" s="48"/>
       <c r="C180" s="48"/>
@@ -6194,7 +6191,7 @@
       <c r="N180" s="48"/>
       <c r="O180" s="48"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A181" s="48"/>
       <c r="B181" s="48"/>
       <c r="C181" s="48"/>
@@ -6211,7 +6208,7 @@
       <c r="N181" s="48"/>
       <c r="O181" s="48"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A182" s="48"/>
       <c r="B182" s="48"/>
       <c r="C182" s="48"/>
@@ -6228,7 +6225,7 @@
       <c r="N182" s="48"/>
       <c r="O182" s="48"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A183" s="48"/>
       <c r="B183" s="48"/>
       <c r="C183" s="48"/>
@@ -6245,7 +6242,7 @@
       <c r="N183" s="48"/>
       <c r="O183" s="48"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A184" s="48"/>
       <c r="B184" s="48"/>
       <c r="C184" s="48"/>
@@ -6262,7 +6259,7 @@
       <c r="N184" s="48"/>
       <c r="O184" s="48"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A185" s="48"/>
       <c r="B185" s="48"/>
       <c r="C185" s="48"/>
@@ -6279,7 +6276,7 @@
       <c r="N185" s="48"/>
       <c r="O185" s="48"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A186" s="48"/>
       <c r="B186" s="48"/>
       <c r="C186" s="48"/>
@@ -6296,7 +6293,7 @@
       <c r="N186" s="48"/>
       <c r="O186" s="48"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A187" s="48"/>
       <c r="B187" s="48"/>
       <c r="C187" s="48"/>
@@ -6313,7 +6310,7 @@
       <c r="N187" s="48"/>
       <c r="O187" s="48"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A188" s="48"/>
       <c r="B188" s="48"/>
       <c r="C188" s="48"/>
@@ -6330,7 +6327,7 @@
       <c r="N188" s="48"/>
       <c r="O188" s="48"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A189" s="48"/>
       <c r="B189" s="48"/>
       <c r="C189" s="48"/>
@@ -6347,7 +6344,7 @@
       <c r="N189" s="48"/>
       <c r="O189" s="48"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A190" s="48"/>
       <c r="B190" s="48"/>
       <c r="C190" s="48"/>
@@ -6364,7 +6361,7 @@
       <c r="N190" s="48"/>
       <c r="O190" s="48"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A191" s="48"/>
       <c r="B191" s="48"/>
       <c r="C191" s="48"/>
@@ -6381,7 +6378,7 @@
       <c r="N191" s="48"/>
       <c r="O191" s="48"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A192" s="48"/>
       <c r="B192" s="48"/>
       <c r="C192" s="48"/>
@@ -6398,7 +6395,7 @@
       <c r="N192" s="48"/>
       <c r="O192" s="48"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A193" s="48"/>
       <c r="B193" s="48"/>
       <c r="C193" s="48"/>
@@ -6415,7 +6412,7 @@
       <c r="N193" s="48"/>
       <c r="O193" s="48"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A194" s="48"/>
       <c r="B194" s="48"/>
       <c r="C194" s="48"/>
@@ -6432,7 +6429,7 @@
       <c r="N194" s="48"/>
       <c r="O194" s="48"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A195" s="48"/>
       <c r="B195" s="48"/>
       <c r="C195" s="48"/>
@@ -6449,7 +6446,7 @@
       <c r="N195" s="48"/>
       <c r="O195" s="48"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A196" s="48"/>
       <c r="B196" s="48"/>
       <c r="C196" s="48"/>
@@ -6466,7 +6463,7 @@
       <c r="N196" s="48"/>
       <c r="O196" s="48"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A197" s="48"/>
       <c r="B197" s="48"/>
       <c r="C197" s="48"/>
@@ -6483,7 +6480,7 @@
       <c r="N197" s="48"/>
       <c r="O197" s="48"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A198" s="48"/>
       <c r="B198" s="48"/>
       <c r="C198" s="48"/>
@@ -6500,7 +6497,7 @@
       <c r="N198" s="48"/>
       <c r="O198" s="48"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A199" s="48"/>
       <c r="B199" s="48"/>
       <c r="C199" s="48"/>
@@ -6517,7 +6514,7 @@
       <c r="N199" s="48"/>
       <c r="O199" s="48"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A200" s="48"/>
       <c r="B200" s="48"/>
       <c r="C200" s="48"/>
@@ -6534,7 +6531,7 @@
       <c r="N200" s="48"/>
       <c r="O200" s="48"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A201" s="48"/>
       <c r="B201" s="48"/>
       <c r="C201" s="48"/>
@@ -6551,7 +6548,7 @@
       <c r="N201" s="48"/>
       <c r="O201" s="48"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A202" s="48"/>
       <c r="B202" s="48"/>
       <c r="C202" s="48"/>
@@ -6568,7 +6565,7 @@
       <c r="N202" s="48"/>
       <c r="O202" s="48"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A203" s="48"/>
       <c r="B203" s="48"/>
       <c r="C203" s="48"/>
@@ -6585,7 +6582,7 @@
       <c r="N203" s="48"/>
       <c r="O203" s="48"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A204" s="48"/>
       <c r="B204" s="48"/>
       <c r="C204" s="48"/>
@@ -6602,7 +6599,7 @@
       <c r="N204" s="48"/>
       <c r="O204" s="48"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A205" s="48"/>
       <c r="B205" s="48"/>
       <c r="C205" s="48"/>
@@ -6619,7 +6616,7 @@
       <c r="N205" s="48"/>
       <c r="O205" s="48"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A206" s="48"/>
       <c r="B206" s="48"/>
       <c r="C206" s="48"/>
@@ -6636,7 +6633,7 @@
       <c r="N206" s="48"/>
       <c r="O206" s="48"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A207" s="48"/>
       <c r="B207" s="48"/>
       <c r="C207" s="48"/>
@@ -6653,7 +6650,7 @@
       <c r="N207" s="48"/>
       <c r="O207" s="48"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A208" s="48"/>
       <c r="B208" s="48"/>
       <c r="C208" s="48"/>
@@ -6670,7 +6667,7 @@
       <c r="N208" s="48"/>
       <c r="O208" s="48"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A209" s="48"/>
       <c r="B209" s="48"/>
       <c r="C209" s="48"/>
@@ -6687,7 +6684,7 @@
       <c r="N209" s="48"/>
       <c r="O209" s="48"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A210" s="48"/>
       <c r="B210" s="48"/>
       <c r="C210" s="48"/>
@@ -6704,7 +6701,7 @@
       <c r="N210" s="48"/>
       <c r="O210" s="48"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A211" s="48"/>
       <c r="B211" s="48"/>
       <c r="C211" s="48"/>
@@ -6721,7 +6718,7 @@
       <c r="N211" s="48"/>
       <c r="O211" s="48"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A212" s="48"/>
       <c r="B212" s="48"/>
       <c r="C212" s="48"/>
@@ -6738,7 +6735,7 @@
       <c r="N212" s="48"/>
       <c r="O212" s="48"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A213" s="48"/>
       <c r="B213" s="48"/>
       <c r="C213" s="48"/>
@@ -6755,7 +6752,7 @@
       <c r="N213" s="48"/>
       <c r="O213" s="48"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A214" s="48"/>
       <c r="B214" s="48"/>
       <c r="C214" s="48"/>
@@ -6772,7 +6769,7 @@
       <c r="N214" s="48"/>
       <c r="O214" s="48"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A215" s="48"/>
       <c r="B215" s="48"/>
       <c r="C215" s="48"/>
@@ -6789,7 +6786,7 @@
       <c r="N215" s="48"/>
       <c r="O215" s="48"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A216" s="48"/>
       <c r="B216" s="48"/>
       <c r="C216" s="48"/>
@@ -6806,7 +6803,7 @@
       <c r="N216" s="48"/>
       <c r="O216" s="48"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A217" s="48"/>
       <c r="B217" s="48"/>
       <c r="C217" s="48"/>
@@ -6823,7 +6820,7 @@
       <c r="N217" s="48"/>
       <c r="O217" s="48"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A218" s="48"/>
       <c r="B218" s="48"/>
       <c r="C218" s="48"/>
@@ -6840,7 +6837,7 @@
       <c r="N218" s="48"/>
       <c r="O218" s="48"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A219" s="48"/>
       <c r="B219" s="48"/>
       <c r="C219" s="48"/>
@@ -6857,7 +6854,7 @@
       <c r="N219" s="48"/>
       <c r="O219" s="48"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A220" s="48"/>
       <c r="B220" s="48"/>
       <c r="C220" s="48"/>
@@ -6874,7 +6871,7 @@
       <c r="N220" s="48"/>
       <c r="O220" s="48"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A221" s="48"/>
       <c r="B221" s="48"/>
       <c r="C221" s="48"/>
@@ -6891,7 +6888,7 @@
       <c r="N221" s="48"/>
       <c r="O221" s="48"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A222" s="48"/>
       <c r="B222" s="48"/>
       <c r="C222" s="48"/>
@@ -6908,7 +6905,7 @@
       <c r="N222" s="48"/>
       <c r="O222" s="48"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A223" s="48"/>
       <c r="B223" s="48"/>
       <c r="C223" s="48"/>
@@ -6925,7 +6922,7 @@
       <c r="N223" s="48"/>
       <c r="O223" s="48"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A224" s="48"/>
       <c r="B224" s="48"/>
       <c r="C224" s="48"/>
@@ -6942,7 +6939,7 @@
       <c r="N224" s="48"/>
       <c r="O224" s="48"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A225" s="48"/>
       <c r="B225" s="48"/>
       <c r="C225" s="48"/>
@@ -6959,7 +6956,7 @@
       <c r="N225" s="48"/>
       <c r="O225" s="48"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A226" s="48"/>
       <c r="B226" s="48"/>
       <c r="C226" s="48"/>
@@ -6976,7 +6973,7 @@
       <c r="N226" s="48"/>
       <c r="O226" s="48"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A227" s="48"/>
       <c r="B227" s="48"/>
       <c r="C227" s="48"/>
@@ -6993,7 +6990,7 @@
       <c r="N227" s="48"/>
       <c r="O227" s="48"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A228" s="48"/>
       <c r="B228" s="48"/>
       <c r="C228" s="48"/>
@@ -7010,7 +7007,7 @@
       <c r="N228" s="48"/>
       <c r="O228" s="48"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A229" s="48"/>
       <c r="B229" s="48"/>
       <c r="C229" s="48"/>
@@ -7027,7 +7024,7 @@
       <c r="N229" s="48"/>
       <c r="O229" s="48"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A230" s="48"/>
       <c r="B230" s="48"/>
       <c r="C230" s="48"/>
@@ -7044,7 +7041,7 @@
       <c r="N230" s="48"/>
       <c r="O230" s="48"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A231" s="48"/>
       <c r="B231" s="48"/>
       <c r="C231" s="48"/>
@@ -7061,7 +7058,7 @@
       <c r="N231" s="48"/>
       <c r="O231" s="48"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A232" s="48"/>
       <c r="B232" s="48"/>
       <c r="C232" s="48"/>
@@ -7078,7 +7075,7 @@
       <c r="N232" s="48"/>
       <c r="O232" s="48"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A233" s="48"/>
       <c r="B233" s="48"/>
       <c r="C233" s="48"/>
@@ -7095,7 +7092,7 @@
       <c r="N233" s="48"/>
       <c r="O233" s="48"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A234" s="48"/>
       <c r="B234" s="48"/>
       <c r="C234" s="48"/>
@@ -7112,7 +7109,7 @@
       <c r="N234" s="48"/>
       <c r="O234" s="48"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A235" s="48"/>
       <c r="B235" s="48"/>
       <c r="C235" s="48"/>
@@ -7129,7 +7126,7 @@
       <c r="N235" s="48"/>
       <c r="O235" s="48"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A236" s="48"/>
       <c r="B236" s="48"/>
       <c r="C236" s="48"/>
@@ -7146,7 +7143,7 @@
       <c r="N236" s="48"/>
       <c r="O236" s="48"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A237" s="48"/>
       <c r="B237" s="48"/>
       <c r="C237" s="48"/>
@@ -7163,7 +7160,7 @@
       <c r="N237" s="48"/>
       <c r="O237" s="48"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A238" s="48"/>
       <c r="B238" s="48"/>
       <c r="C238" s="48"/>
@@ -7180,7 +7177,7 @@
       <c r="N238" s="48"/>
       <c r="O238" s="48"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A239" s="48"/>
       <c r="B239" s="48"/>
       <c r="C239" s="48"/>
@@ -7197,7 +7194,7 @@
       <c r="N239" s="48"/>
       <c r="O239" s="48"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A240" s="48"/>
       <c r="B240" s="48"/>
       <c r="C240" s="48"/>
@@ -7214,7 +7211,7 @@
       <c r="N240" s="48"/>
       <c r="O240" s="48"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A241" s="48"/>
       <c r="B241" s="48"/>
       <c r="C241" s="48"/>
@@ -7231,7 +7228,7 @@
       <c r="N241" s="48"/>
       <c r="O241" s="48"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A242" s="48"/>
       <c r="B242" s="48"/>
       <c r="C242" s="48"/>
@@ -7248,7 +7245,7 @@
       <c r="N242" s="48"/>
       <c r="O242" s="48"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A243" s="48"/>
       <c r="B243" s="48"/>
       <c r="C243" s="48"/>
@@ -7265,7 +7262,7 @@
       <c r="N243" s="48"/>
       <c r="O243" s="48"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A244" s="48"/>
       <c r="B244" s="48"/>
       <c r="C244" s="48"/>
@@ -7282,7 +7279,7 @@
       <c r="N244" s="48"/>
       <c r="O244" s="48"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A245" s="48"/>
       <c r="B245" s="48"/>
       <c r="C245" s="48"/>
@@ -7299,7 +7296,7 @@
       <c r="N245" s="48"/>
       <c r="O245" s="48"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A246" s="48"/>
       <c r="B246" s="48"/>
       <c r="C246" s="48"/>
@@ -7316,7 +7313,7 @@
       <c r="N246" s="48"/>
       <c r="O246" s="48"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A247" s="48"/>
       <c r="B247" s="48"/>
       <c r="C247" s="48"/>
@@ -7333,7 +7330,7 @@
       <c r="N247" s="48"/>
       <c r="O247" s="48"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A248" s="48"/>
       <c r="B248" s="48"/>
       <c r="C248" s="48"/>
@@ -7350,7 +7347,7 @@
       <c r="N248" s="48"/>
       <c r="O248" s="48"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A249" s="48"/>
       <c r="B249" s="48"/>
       <c r="C249" s="48"/>
@@ -7367,7 +7364,7 @@
       <c r="N249" s="48"/>
       <c r="O249" s="48"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A250" s="48"/>
       <c r="B250" s="48"/>
       <c r="C250" s="48"/>
@@ -7384,7 +7381,7 @@
       <c r="N250" s="48"/>
       <c r="O250" s="48"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A251" s="48"/>
       <c r="B251" s="48"/>
       <c r="C251" s="48"/>
@@ -7401,7 +7398,7 @@
       <c r="N251" s="48"/>
       <c r="O251" s="48"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A252" s="48"/>
       <c r="B252" s="48"/>
       <c r="C252" s="48"/>
@@ -7418,7 +7415,7 @@
       <c r="N252" s="48"/>
       <c r="O252" s="48"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A253" s="48"/>
       <c r="B253" s="48"/>
       <c r="C253" s="48"/>
@@ -7435,7 +7432,7 @@
       <c r="N253" s="48"/>
       <c r="O253" s="48"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A254" s="48"/>
       <c r="B254" s="48"/>
       <c r="C254" s="48"/>
@@ -7452,7 +7449,7 @@
       <c r="N254" s="48"/>
       <c r="O254" s="48"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A255" s="48"/>
       <c r="B255" s="48"/>
       <c r="C255" s="48"/>
@@ -7469,7 +7466,7 @@
       <c r="N255" s="48"/>
       <c r="O255" s="48"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A256" s="48"/>
       <c r="B256" s="48"/>
       <c r="C256" s="48"/>
@@ -7486,7 +7483,7 @@
       <c r="N256" s="48"/>
       <c r="O256" s="48"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A257" s="48"/>
       <c r="B257" s="48"/>
       <c r="C257" s="48"/>
@@ -7503,7 +7500,7 @@
       <c r="N257" s="48"/>
       <c r="O257" s="48"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A258" s="48"/>
       <c r="B258" s="48"/>
       <c r="C258" s="48"/>
@@ -7520,7 +7517,7 @@
       <c r="N258" s="48"/>
       <c r="O258" s="48"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A259" s="48"/>
       <c r="B259" s="48"/>
       <c r="C259" s="48"/>
@@ -7537,7 +7534,7 @@
       <c r="N259" s="48"/>
       <c r="O259" s="48"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A260" s="48"/>
       <c r="B260" s="48"/>
       <c r="C260" s="48"/>
@@ -7554,7 +7551,7 @@
       <c r="N260" s="48"/>
       <c r="O260" s="48"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A261" s="48"/>
       <c r="B261" s="48"/>
       <c r="C261" s="48"/>
@@ -7571,7 +7568,7 @@
       <c r="N261" s="48"/>
       <c r="O261" s="48"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A262" s="48"/>
       <c r="B262" s="48"/>
       <c r="C262" s="48"/>
@@ -7588,7 +7585,7 @@
       <c r="N262" s="48"/>
       <c r="O262" s="48"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A263" s="48"/>
       <c r="B263" s="48"/>
       <c r="C263" s="48"/>
@@ -7605,7 +7602,7 @@
       <c r="N263" s="48"/>
       <c r="O263" s="48"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A264" s="48"/>
       <c r="B264" s="48"/>
       <c r="C264" s="48"/>
@@ -7622,7 +7619,7 @@
       <c r="N264" s="48"/>
       <c r="O264" s="48"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A265" s="48"/>
       <c r="B265" s="48"/>
       <c r="C265" s="48"/>
@@ -7639,7 +7636,7 @@
       <c r="N265" s="48"/>
       <c r="O265" s="48"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A266" s="48"/>
       <c r="B266" s="48"/>
       <c r="C266" s="48"/>
@@ -7656,7 +7653,7 @@
       <c r="N266" s="48"/>
       <c r="O266" s="48"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A267" s="48"/>
       <c r="B267" s="48"/>
       <c r="C267" s="48"/>
@@ -7673,7 +7670,7 @@
       <c r="N267" s="48"/>
       <c r="O267" s="48"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A268" s="48"/>
       <c r="B268" s="48"/>
       <c r="C268" s="48"/>
@@ -7690,7 +7687,7 @@
       <c r="N268" s="48"/>
       <c r="O268" s="48"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A269" s="48"/>
       <c r="B269" s="48"/>
       <c r="C269" s="48"/>
@@ -7707,7 +7704,7 @@
       <c r="N269" s="48"/>
       <c r="O269" s="48"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A270" s="48"/>
       <c r="B270" s="48"/>
       <c r="C270" s="48"/>
@@ -7724,7 +7721,7 @@
       <c r="N270" s="48"/>
       <c r="O270" s="48"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A271" s="48"/>
       <c r="B271" s="48"/>
       <c r="C271" s="48"/>
@@ -7741,7 +7738,7 @@
       <c r="N271" s="48"/>
       <c r="O271" s="48"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A272" s="48"/>
       <c r="B272" s="48"/>
       <c r="C272" s="48"/>
@@ -7758,7 +7755,7 @@
       <c r="N272" s="48"/>
       <c r="O272" s="48"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A273" s="48"/>
       <c r="B273" s="48"/>
       <c r="C273" s="48"/>
@@ -7775,7 +7772,7 @@
       <c r="N273" s="48"/>
       <c r="O273" s="48"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A274" s="48"/>
       <c r="B274" s="48"/>
       <c r="C274" s="48"/>
@@ -7792,7 +7789,7 @@
       <c r="N274" s="48"/>
       <c r="O274" s="48"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A275" s="48"/>
       <c r="B275" s="48"/>
       <c r="C275" s="48"/>
@@ -7809,7 +7806,7 @@
       <c r="N275" s="48"/>
       <c r="O275" s="48"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A276" s="48"/>
       <c r="B276" s="48"/>
       <c r="C276" s="48"/>
@@ -7826,7 +7823,7 @@
       <c r="N276" s="48"/>
       <c r="O276" s="48"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A277" s="48"/>
       <c r="B277" s="48"/>
       <c r="C277" s="48"/>
@@ -7843,7 +7840,7 @@
       <c r="N277" s="48"/>
       <c r="O277" s="48"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A278" s="48"/>
       <c r="B278" s="48"/>
       <c r="C278" s="48"/>
@@ -7860,7 +7857,7 @@
       <c r="N278" s="48"/>
       <c r="O278" s="48"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A279" s="48"/>
       <c r="B279" s="48"/>
       <c r="C279" s="48"/>
@@ -7877,7 +7874,7 @@
       <c r="N279" s="48"/>
       <c r="O279" s="48"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A280" s="48"/>
       <c r="B280" s="48"/>
       <c r="C280" s="48"/>
@@ -7894,7 +7891,7 @@
       <c r="N280" s="48"/>
       <c r="O280" s="48"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A281" s="48"/>
       <c r="B281" s="48"/>
       <c r="C281" s="48"/>
@@ -7911,7 +7908,7 @@
       <c r="N281" s="48"/>
       <c r="O281" s="48"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A282" s="48"/>
       <c r="B282" s="48"/>
       <c r="C282" s="48"/>
@@ -7928,7 +7925,7 @@
       <c r="N282" s="48"/>
       <c r="O282" s="48"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A283" s="48"/>
       <c r="B283" s="48"/>
       <c r="C283" s="48"/>
@@ -7945,7 +7942,7 @@
       <c r="N283" s="48"/>
       <c r="O283" s="48"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A284" s="48"/>
       <c r="B284" s="48"/>
       <c r="C284" s="48"/>
@@ -7962,7 +7959,7 @@
       <c r="N284" s="48"/>
       <c r="O284" s="48"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A285" s="48"/>
       <c r="B285" s="48"/>
       <c r="C285" s="48"/>
@@ -7979,7 +7976,7 @@
       <c r="N285" s="48"/>
       <c r="O285" s="48"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A286" s="48"/>
       <c r="B286" s="48"/>
       <c r="C286" s="48"/>
@@ -7996,7 +7993,7 @@
       <c r="N286" s="48"/>
       <c r="O286" s="48"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A287" s="48"/>
       <c r="B287" s="48"/>
       <c r="C287" s="48"/>
@@ -8013,7 +8010,7 @@
       <c r="N287" s="48"/>
       <c r="O287" s="48"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A288" s="48"/>
       <c r="B288" s="48"/>
       <c r="C288" s="48"/>
@@ -8030,7 +8027,7 @@
       <c r="N288" s="48"/>
       <c r="O288" s="48"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A289" s="48"/>
       <c r="B289" s="48"/>
       <c r="C289" s="48"/>
@@ -8047,7 +8044,7 @@
       <c r="N289" s="48"/>
       <c r="O289" s="48"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A290" s="48"/>
       <c r="B290" s="48"/>
       <c r="C290" s="48"/>
@@ -8064,7 +8061,7 @@
       <c r="N290" s="48"/>
       <c r="O290" s="48"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A291" s="48"/>
       <c r="B291" s="48"/>
       <c r="C291" s="48"/>
@@ -8081,7 +8078,7 @@
       <c r="N291" s="48"/>
       <c r="O291" s="48"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A292" s="48"/>
       <c r="B292" s="48"/>
       <c r="C292" s="48"/>
@@ -8098,7 +8095,7 @@
       <c r="N292" s="48"/>
       <c r="O292" s="48"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A293" s="48"/>
       <c r="B293" s="48"/>
       <c r="C293" s="48"/>
@@ -8115,7 +8112,7 @@
       <c r="N293" s="48"/>
       <c r="O293" s="48"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A294" s="48"/>
       <c r="B294" s="48"/>
       <c r="C294" s="48"/>
@@ -8132,7 +8129,7 @@
       <c r="N294" s="48"/>
       <c r="O294" s="48"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A295" s="48"/>
       <c r="B295" s="48"/>
       <c r="C295" s="48"/>
@@ -8149,7 +8146,7 @@
       <c r="N295" s="48"/>
       <c r="O295" s="48"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A296" s="48"/>
       <c r="B296" s="48"/>
       <c r="C296" s="48"/>
@@ -8166,7 +8163,7 @@
       <c r="N296" s="48"/>
       <c r="O296" s="48"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A297" s="48"/>
       <c r="B297" s="48"/>
       <c r="C297" s="48"/>
@@ -8183,7 +8180,7 @@
       <c r="N297" s="48"/>
       <c r="O297" s="48"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A298" s="48"/>
       <c r="B298" s="48"/>
       <c r="C298" s="48"/>
@@ -8200,7 +8197,7 @@
       <c r="N298" s="48"/>
       <c r="O298" s="48"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A299" s="48"/>
       <c r="B299" s="48"/>
       <c r="C299" s="48"/>
@@ -8217,7 +8214,7 @@
       <c r="N299" s="48"/>
       <c r="O299" s="48"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A300" s="48"/>
       <c r="B300" s="48"/>
       <c r="C300" s="48"/>
@@ -8234,7 +8231,7 @@
       <c r="N300" s="48"/>
       <c r="O300" s="48"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A301" s="48"/>
       <c r="B301" s="48"/>
       <c r="C301" s="48"/>
@@ -8251,7 +8248,7 @@
       <c r="N301" s="48"/>
       <c r="O301" s="48"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A302" s="48"/>
       <c r="B302" s="48"/>
       <c r="C302" s="48"/>
@@ -8268,7 +8265,7 @@
       <c r="N302" s="48"/>
       <c r="O302" s="48"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A303" s="48"/>
       <c r="B303" s="48"/>
       <c r="C303" s="48"/>
@@ -8285,7 +8282,7 @@
       <c r="N303" s="48"/>
       <c r="O303" s="48"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A304" s="48"/>
       <c r="B304" s="48"/>
       <c r="C304" s="48"/>
@@ -8302,7 +8299,7 @@
       <c r="N304" s="48"/>
       <c r="O304" s="48"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A305" s="48"/>
       <c r="B305" s="48"/>
       <c r="C305" s="48"/>
@@ -8319,7 +8316,7 @@
       <c r="N305" s="48"/>
       <c r="O305" s="48"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A306" s="48"/>
       <c r="B306" s="48"/>
       <c r="C306" s="48"/>
@@ -8336,7 +8333,7 @@
       <c r="N306" s="48"/>
       <c r="O306" s="48"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A307" s="48"/>
       <c r="B307" s="48"/>
       <c r="C307" s="48"/>
@@ -8353,7 +8350,7 @@
       <c r="N307" s="48"/>
       <c r="O307" s="48"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A308" s="48"/>
       <c r="B308" s="48"/>
       <c r="C308" s="48"/>
@@ -8370,7 +8367,7 @@
       <c r="N308" s="48"/>
       <c r="O308" s="48"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A309" s="48"/>
       <c r="B309" s="48"/>
       <c r="C309" s="48"/>
@@ -8387,7 +8384,7 @@
       <c r="N309" s="48"/>
       <c r="O309" s="48"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A310" s="48"/>
       <c r="B310" s="48"/>
       <c r="C310" s="48"/>
@@ -8404,7 +8401,7 @@
       <c r="N310" s="48"/>
       <c r="O310" s="48"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A311" s="48"/>
       <c r="B311" s="48"/>
       <c r="C311" s="48"/>
@@ -8421,7 +8418,7 @@
       <c r="N311" s="48"/>
       <c r="O311" s="48"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A312" s="48"/>
       <c r="B312" s="48"/>
       <c r="C312" s="48"/>
@@ -8438,7 +8435,7 @@
       <c r="N312" s="48"/>
       <c r="O312" s="48"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A313" s="48"/>
       <c r="B313" s="48"/>
       <c r="C313" s="48"/>
@@ -8455,7 +8452,7 @@
       <c r="N313" s="48"/>
       <c r="O313" s="48"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A314" s="48"/>
       <c r="B314" s="48"/>
       <c r="C314" s="48"/>
@@ -8472,7 +8469,7 @@
       <c r="N314" s="48"/>
       <c r="O314" s="48"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A315" s="48"/>
       <c r="B315" s="48"/>
       <c r="C315" s="48"/>
@@ -8489,7 +8486,7 @@
       <c r="N315" s="48"/>
       <c r="O315" s="48"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A316" s="48"/>
       <c r="B316" s="48"/>
       <c r="C316" s="48"/>
@@ -8506,7 +8503,7 @@
       <c r="N316" s="48"/>
       <c r="O316" s="48"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A317" s="48"/>
       <c r="B317" s="48"/>
       <c r="C317" s="48"/>
@@ -8523,7 +8520,7 @@
       <c r="N317" s="48"/>
       <c r="O317" s="48"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A318" s="48"/>
       <c r="B318" s="48"/>
       <c r="C318" s="48"/>
@@ -8540,7 +8537,7 @@
       <c r="N318" s="48"/>
       <c r="O318" s="48"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A319" s="48"/>
       <c r="B319" s="48"/>
       <c r="C319" s="48"/>
@@ -8557,7 +8554,7 @@
       <c r="N319" s="48"/>
       <c r="O319" s="48"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A320" s="48"/>
       <c r="B320" s="48"/>
       <c r="C320" s="48"/>
@@ -8574,7 +8571,7 @@
       <c r="N320" s="48"/>
       <c r="O320" s="48"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A321" s="48"/>
       <c r="B321" s="48"/>
       <c r="C321" s="48"/>
@@ -8591,7 +8588,7 @@
       <c r="N321" s="48"/>
       <c r="O321" s="48"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A322" s="48"/>
       <c r="B322" s="48"/>
       <c r="C322" s="48"/>
@@ -8608,7 +8605,7 @@
       <c r="N322" s="48"/>
       <c r="O322" s="48"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A323" s="48"/>
       <c r="B323" s="48"/>
       <c r="C323" s="48"/>
@@ -8625,7 +8622,7 @@
       <c r="N323" s="48"/>
       <c r="O323" s="48"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A324" s="48"/>
       <c r="B324" s="48"/>
       <c r="C324" s="48"/>
@@ -8642,7 +8639,7 @@
       <c r="N324" s="48"/>
       <c r="O324" s="48"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A325" s="48"/>
       <c r="B325" s="48"/>
       <c r="C325" s="48"/>
@@ -8659,7 +8656,7 @@
       <c r="N325" s="48"/>
       <c r="O325" s="48"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A326" s="48"/>
       <c r="B326" s="48"/>
       <c r="C326" s="48"/>
@@ -8676,7 +8673,7 @@
       <c r="N326" s="48"/>
       <c r="O326" s="48"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A327" s="48"/>
       <c r="B327" s="48"/>
       <c r="C327" s="48"/>
@@ -8693,7 +8690,7 @@
       <c r="N327" s="48"/>
       <c r="O327" s="48"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A328" s="48"/>
       <c r="B328" s="48"/>
       <c r="C328" s="48"/>
@@ -8710,7 +8707,7 @@
       <c r="N328" s="48"/>
       <c r="O328" s="48"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A329" s="48"/>
       <c r="B329" s="48"/>
       <c r="C329" s="48"/>
@@ -8727,7 +8724,7 @@
       <c r="N329" s="48"/>
       <c r="O329" s="48"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A330" s="48"/>
       <c r="B330" s="48"/>
       <c r="C330" s="48"/>
@@ -8744,7 +8741,7 @@
       <c r="N330" s="48"/>
       <c r="O330" s="48"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A331" s="48"/>
       <c r="B331" s="48"/>
       <c r="C331" s="48"/>
@@ -8761,7 +8758,7 @@
       <c r="N331" s="48"/>
       <c r="O331" s="48"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A332" s="48"/>
       <c r="B332" s="48"/>
       <c r="C332" s="48"/>
@@ -8778,7 +8775,7 @@
       <c r="N332" s="48"/>
       <c r="O332" s="48"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A333" s="48"/>
       <c r="B333" s="48"/>
       <c r="C333" s="48"/>
@@ -8795,7 +8792,7 @@
       <c r="N333" s="48"/>
       <c r="O333" s="48"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A334" s="48"/>
       <c r="B334" s="48"/>
       <c r="C334" s="48"/>
@@ -8812,7 +8809,7 @@
       <c r="N334" s="48"/>
       <c r="O334" s="48"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A335" s="48"/>
       <c r="B335" s="48"/>
       <c r="C335" s="48"/>
@@ -8829,7 +8826,7 @@
       <c r="N335" s="48"/>
       <c r="O335" s="48"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A336" s="48"/>
       <c r="B336" s="48"/>
       <c r="C336" s="48"/>
@@ -8846,7 +8843,7 @@
       <c r="N336" s="48"/>
       <c r="O336" s="48"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A337" s="48"/>
       <c r="B337" s="48"/>
       <c r="C337" s="48"/>
@@ -8863,7 +8860,7 @@
       <c r="N337" s="48"/>
       <c r="O337" s="48"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A338" s="48"/>
       <c r="B338" s="48"/>
       <c r="C338" s="48"/>
@@ -8880,7 +8877,7 @@
       <c r="N338" s="48"/>
       <c r="O338" s="48"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A339" s="48"/>
       <c r="B339" s="48"/>
       <c r="C339" s="48"/>
@@ -8897,7 +8894,7 @@
       <c r="N339" s="48"/>
       <c r="O339" s="48"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A340" s="48"/>
       <c r="B340" s="48"/>
       <c r="C340" s="48"/>
@@ -8914,7 +8911,7 @@
       <c r="N340" s="48"/>
       <c r="O340" s="48"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A341" s="48"/>
       <c r="B341" s="48"/>
       <c r="C341" s="48"/>
@@ -8931,7 +8928,7 @@
       <c r="N341" s="48"/>
       <c r="O341" s="48"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A342" s="48"/>
       <c r="B342" s="48"/>
       <c r="C342" s="48"/>
@@ -8948,7 +8945,7 @@
       <c r="N342" s="48"/>
       <c r="O342" s="48"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A343" s="48"/>
       <c r="B343" s="48"/>
       <c r="C343" s="48"/>
@@ -8965,7 +8962,7 @@
       <c r="N343" s="48"/>
       <c r="O343" s="48"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A344" s="48"/>
       <c r="B344" s="48"/>
       <c r="C344" s="48"/>
@@ -8982,7 +8979,7 @@
       <c r="N344" s="48"/>
       <c r="O344" s="48"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A345" s="48"/>
       <c r="B345" s="48"/>
       <c r="C345" s="48"/>
@@ -8999,7 +8996,7 @@
       <c r="N345" s="48"/>
       <c r="O345" s="48"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A346" s="48"/>
       <c r="B346" s="48"/>
       <c r="C346" s="48"/>
@@ -9029,17 +9026,17 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="47" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="45" t="s">
         <v>140</v>
       </c>
@@ -9056,7 +9053,7 @@
       <c r="J4" s="48"/>
       <c r="K4" s="48"/>
     </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="29">
         <v>43070</v>
       </c>
@@ -9073,7 +9070,7 @@
       <c r="J5" s="48"/>
       <c r="K5" s="48"/>
     </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="48"/>
       <c r="B6" s="48" t="s">
         <v>126</v>
@@ -9088,7 +9085,7 @@
       <c r="J6" s="48"/>
       <c r="K6" s="48"/>
     </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="48"/>
       <c r="B7" s="48" t="s">
         <v>127</v>
@@ -9103,7 +9100,7 @@
       <c r="J7" s="48"/>
       <c r="K7" s="48"/>
     </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="48"/>
       <c r="B8" s="48"/>
       <c r="C8" s="48"/>
@@ -9116,7 +9113,7 @@
       <c r="J8" s="48"/>
       <c r="K8" s="48"/>
     </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="48"/>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -9129,7 +9126,7 @@
       <c r="J9" s="48"/>
       <c r="K9" s="48"/>
     </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="48"/>
       <c r="B10" s="48"/>
       <c r="C10" s="48"/>
@@ -9142,7 +9139,7 @@
       <c r="J10" s="48"/>
       <c r="K10" s="48"/>
     </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="48"/>
       <c r="B11" s="48"/>
       <c r="C11" s="48"/>
@@ -9155,7 +9152,7 @@
       <c r="J11" s="48"/>
       <c r="K11" s="48"/>
     </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="48"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48"/>
@@ -9168,7 +9165,7 @@
       <c r="J12" s="48"/>
       <c r="K12" s="48"/>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="48"/>
       <c r="B13" s="48"/>
       <c r="C13" s="48"/>
@@ -9181,7 +9178,7 @@
       <c r="J13" s="48"/>
       <c r="K13" s="48"/>
     </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="48"/>
       <c r="B14" s="48"/>
       <c r="C14" s="48"/>
@@ -9194,7 +9191,7 @@
       <c r="J14" s="48"/>
       <c r="K14" s="48"/>
     </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="48"/>
       <c r="B15" s="48"/>
       <c r="C15" s="48"/>
@@ -9207,7 +9204,7 @@
       <c r="J15" s="48"/>
       <c r="K15" s="48"/>
     </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="48"/>
       <c r="B16" s="48"/>
       <c r="C16" s="48"/>
@@ -9220,7 +9217,7 @@
       <c r="J16" s="48"/>
       <c r="K16" s="48"/>
     </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="48"/>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
@@ -9233,7 +9230,7 @@
       <c r="J17" s="48"/>
       <c r="K17" s="48"/>
     </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="48"/>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -9246,7 +9243,7 @@
       <c r="J18" s="48"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="48"/>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>

</xml_diff>

<commit_message>
update scrum and some files
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -514,12 +514,6 @@
     <t>7.4</t>
   </si>
   <si>
-    <t>Themeing</t>
-  </si>
-  <si>
-    <t>Theming all over the place.</t>
-  </si>
-  <si>
     <t>Add Fake history</t>
   </si>
   <si>
@@ -583,10 +577,16 @@
     <t>0.4</t>
   </si>
   <si>
-    <t>NavitatorView</t>
-  </si>
-  <si>
     <t>Add Navigation in view so switch between different panes is possible.</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Fixing PatientView / Presenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are some misconcepts in PatientView and Presenter. </t>
   </si>
 </sst>
 </file>
@@ -908,9 +908,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -958,6 +955,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1599,10 +1599,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" s="61" t="s">
         <v>6</v>
@@ -1619,10 +1619,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D10" s="64" t="s">
         <v>6</v>
@@ -1664,8 +1664,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1726,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="52" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="50">
         <v>0.1</v>
       </c>
@@ -1812,42 +1812,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+    <row r="5" spans="1:12" s="68" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A5" s="66" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="67">
+        <v>2</v>
+      </c>
+      <c r="C5" s="68" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="68">
-        <v>2</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="69" t="s">
+      <c r="D5" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="69" t="s">
+      <c r="F5" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="69" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="69" t="s">
+      <c r="H5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="69">
+      <c r="I5" s="68">
         <v>4</v>
       </c>
-      <c r="J5" s="69">
+      <c r="J5" s="68">
         <v>0</v>
       </c>
-      <c r="K5" s="69">
+      <c r="K5" s="68">
         <v>0</v>
       </c>
-      <c r="L5" s="69" t="s">
-        <v>180</v>
+      <c r="L5" s="68" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -1908,7 +1908,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>72</v>
       </c>
@@ -1930,7 +1930,7 @@
       <c r="K9" s="35"/>
       <c r="L9" s="35"/>
     </row>
-    <row r="10" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="33" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>41</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="33" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>71</v>
       </c>
@@ -2006,41 +2006,41 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="76">
+    <row r="12" spans="1:12" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A12" s="75">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B12" s="77">
+      <c r="B12" s="76">
         <v>2</v>
       </c>
-      <c r="C12" s="75" t="s">
+      <c r="C12" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="78" t="s">
-        <v>172</v>
-      </c>
-      <c r="E12" s="79" t="s">
+      <c r="D12" s="77" t="s">
+        <v>170</v>
+      </c>
+      <c r="E12" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="F12" s="79" t="s">
+      <c r="F12" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="79" t="s">
+      <c r="G12" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="79" t="s">
+      <c r="H12" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="79">
+      <c r="I12" s="78">
         <v>8</v>
       </c>
-      <c r="J12" s="75">
+      <c r="J12" s="74">
         <v>0</v>
       </c>
-      <c r="K12" s="75">
+      <c r="K12" s="74">
         <v>0</v>
       </c>
-      <c r="L12" s="79" t="s">
+      <c r="L12" s="78" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2068,7 +2068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="33" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="33" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="37">
         <v>3.1</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="37">
         <v>3.2</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="33" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="37" t="s">
         <v>39</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="33" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="37" t="s">
         <v>40</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="33" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="37" t="s">
         <v>82</v>
       </c>
@@ -2235,83 +2235,83 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A19" s="76" t="s">
+    <row r="19" spans="1:12" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A19" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="B19" s="77">
+      <c r="B19" s="76">
         <v>2</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="E19" s="75" t="s">
+      <c r="E19" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="F19" s="75" t="s">
+      <c r="F19" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="75" t="s">
+      <c r="G19" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="I19" s="75">
+      <c r="I19" s="74">
         <v>6</v>
       </c>
-      <c r="J19" s="75">
+      <c r="J19" s="74">
         <v>6</v>
       </c>
-      <c r="K19" s="75">
+      <c r="K19" s="74">
         <v>6</v>
       </c>
-      <c r="L19" s="75" t="s">
+      <c r="L19" s="74" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A20" s="76" t="s">
+    <row r="20" spans="1:12" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A20" s="75" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="77">
+      <c r="B20" s="76">
         <v>2</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="D20" s="80" t="s">
+      <c r="D20" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="75" t="s">
+      <c r="E20" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="75" t="s">
+      <c r="F20" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="75" t="s">
+      <c r="G20" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="75" t="s">
+      <c r="H20" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="75">
+      <c r="I20" s="74">
         <v>4</v>
       </c>
-      <c r="J20" s="75">
+      <c r="J20" s="74">
         <v>3</v>
       </c>
-      <c r="K20" s="75">
+      <c r="K20" s="74">
         <v>3</v>
       </c>
-      <c r="L20" s="75" t="s">
+      <c r="L20" s="74" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="33" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="37">
         <v>3.3</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="37">
         <v>3.4</v>
       </c>
@@ -2387,83 +2387,83 @@
         <v>121</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="75" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A23" s="76" t="s">
+    <row r="23" spans="1:12" s="74" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A23" s="75" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="77">
+      <c r="B23" s="76">
         <v>2</v>
       </c>
-      <c r="C23" s="79" t="s">
+      <c r="C23" s="78" t="s">
         <v>155</v>
       </c>
-      <c r="D23" s="80" t="s">
+      <c r="D23" s="79" t="s">
         <v>157</v>
       </c>
-      <c r="E23" s="75" t="s">
+      <c r="E23" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F23" s="75" t="s">
+      <c r="F23" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="H23" s="75" t="s">
+      <c r="H23" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="75">
+      <c r="I23" s="74">
         <v>9</v>
       </c>
-      <c r="J23" s="75">
+      <c r="J23" s="74">
         <v>8</v>
       </c>
-      <c r="K23" s="75">
+      <c r="K23" s="74">
         <v>8</v>
       </c>
-      <c r="L23" s="75" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="75" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="76" t="s">
+      <c r="L23" s="74" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A24" s="75" t="s">
         <v>153</v>
       </c>
-      <c r="B24" s="77">
+      <c r="B24" s="76">
         <v>2</v>
       </c>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="78" t="s">
         <v>154</v>
       </c>
-      <c r="D24" s="80" t="s">
+      <c r="D24" s="79" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="75" t="s">
+      <c r="E24" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="75" t="s">
+      <c r="F24" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="75" t="s">
+      <c r="G24" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="H24" s="75" t="s">
+      <c r="H24" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="75">
+      <c r="I24" s="74">
         <v>7</v>
       </c>
-      <c r="J24" s="75">
+      <c r="J24" s="74">
         <v>0</v>
       </c>
-      <c r="K24" s="75">
+      <c r="K24" s="74">
         <v>0</v>
       </c>
-      <c r="L24" s="75" t="s">
+      <c r="L24" s="74" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="33" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="37">
         <v>3.5</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="33" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="40">
         <v>3.6</v>
       </c>
@@ -2539,80 +2539,80 @@
         <v>121</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="75" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A27" s="71" t="s">
+    <row r="27" spans="1:12" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A27" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="B27" s="71">
+        <v>2</v>
+      </c>
+      <c r="C27" s="72" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="73" t="s">
         <v>177</v>
       </c>
-      <c r="B27" s="72">
+      <c r="E27" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="72" t="s">
+        <v>24</v>
+      </c>
+      <c r="H27" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="I27" s="72">
+        <v>12</v>
+      </c>
+      <c r="J27" s="72">
+        <v>0</v>
+      </c>
+      <c r="K27" s="72">
+        <v>0</v>
+      </c>
+      <c r="L27" s="72" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" s="68" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A28" s="66">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B28" s="67">
         <v>2</v>
       </c>
-      <c r="C27" s="73" t="s">
+      <c r="C28" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="69" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="68" t="s">
+        <v>28</v>
+      </c>
+      <c r="H28" s="68" t="s">
+        <v>5</v>
+      </c>
+      <c r="I28" s="68">
+        <v>5</v>
+      </c>
+      <c r="J28" s="68">
+        <v>5</v>
+      </c>
+      <c r="K28" s="68">
+        <v>0</v>
+      </c>
+      <c r="L28" s="68" t="s">
         <v>178</v>
-      </c>
-      <c r="D27" s="74" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="F27" s="73" t="s">
-        <v>88</v>
-      </c>
-      <c r="G27" s="73" t="s">
-        <v>24</v>
-      </c>
-      <c r="H27" s="73" t="s">
-        <v>6</v>
-      </c>
-      <c r="I27" s="73">
-        <v>12</v>
-      </c>
-      <c r="J27" s="73">
-        <v>0</v>
-      </c>
-      <c r="K27" s="73">
-        <v>0</v>
-      </c>
-      <c r="L27" s="73" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A28" s="67">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="B28" s="68">
-        <v>2</v>
-      </c>
-      <c r="C28" s="69" t="s">
-        <v>151</v>
-      </c>
-      <c r="D28" s="70" t="s">
-        <v>152</v>
-      </c>
-      <c r="E28" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>30</v>
-      </c>
-      <c r="G28" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="H28" s="69" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" s="69">
-        <v>5</v>
-      </c>
-      <c r="J28" s="69">
-        <v>5</v>
-      </c>
-      <c r="K28" s="69">
-        <v>0</v>
-      </c>
-      <c r="L28" s="69" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
@@ -2772,191 +2772,191 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="81" t="s">
+    <row r="37" spans="1:17" s="68" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A37" s="80" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="82">
+      <c r="B37" s="81">
         <v>2</v>
       </c>
-      <c r="C37" s="79" t="s">
+      <c r="C37" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="78" t="s">
+      <c r="D37" s="77" t="s">
         <v>150</v>
       </c>
-      <c r="E37" s="79" t="s">
+      <c r="E37" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="79" t="s">
+      <c r="F37" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="G37" s="79" t="s">
+      <c r="G37" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="H37" s="79" t="s">
+      <c r="H37" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="I37" s="79">
+      <c r="I37" s="78">
         <v>3</v>
       </c>
-      <c r="J37" s="79">
+      <c r="J37" s="78">
         <v>2</v>
       </c>
-      <c r="K37" s="79">
+      <c r="K37" s="78">
         <v>2</v>
       </c>
-      <c r="L37" s="79" t="s">
+      <c r="L37" s="78" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="69" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" s="81" t="s">
+    <row r="38" spans="1:17" s="68" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A38" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="82">
+      <c r="B38" s="81">
         <v>2</v>
       </c>
-      <c r="C38" s="79" t="s">
+      <c r="C38" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="D38" s="78" t="s">
-        <v>162</v>
-      </c>
-      <c r="E38" s="79" t="s">
+      <c r="D38" s="77" t="s">
+        <v>160</v>
+      </c>
+      <c r="E38" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="79" t="s">
+      <c r="F38" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G38" s="69" t="s">
+      <c r="G38" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="H38" s="79" t="s">
+      <c r="H38" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="I38" s="79">
+      <c r="I38" s="78">
         <v>2</v>
       </c>
-      <c r="J38" s="79">
+      <c r="J38" s="78">
         <v>1</v>
       </c>
-      <c r="K38" s="79">
+      <c r="K38" s="78">
         <v>1</v>
       </c>
-      <c r="L38" s="79" t="s">
+      <c r="L38" s="78" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="81" t="s">
+    <row r="39" spans="1:17" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="80" t="s">
         <v>145</v>
       </c>
-      <c r="B39" s="82">
+      <c r="B39" s="81">
         <v>2</v>
       </c>
-      <c r="C39" s="79" t="s">
+      <c r="C39" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="D39" s="78" t="s">
-        <v>161</v>
-      </c>
-      <c r="E39" s="79" t="s">
+      <c r="D39" s="77" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="79" t="s">
+      <c r="F39" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G39" s="79" t="s">
+      <c r="G39" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H39" s="79" t="s">
+      <c r="H39" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="79">
+      <c r="I39" s="78">
         <v>4</v>
       </c>
-      <c r="J39" s="79">
+      <c r="J39" s="78">
         <v>0</v>
       </c>
-      <c r="K39" s="79">
+      <c r="K39" s="78">
         <v>0</v>
       </c>
-      <c r="L39" s="79" t="s">
+      <c r="L39" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="81" t="s">
+    <row r="40" spans="1:17" s="68" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+      <c r="A40" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="82">
+      <c r="B40" s="81">
         <v>2</v>
       </c>
-      <c r="C40" s="79" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="78" t="s">
-        <v>160</v>
-      </c>
-      <c r="E40" s="79" t="s">
+      <c r="C40" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="77" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="79" t="s">
+      <c r="F40" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="G40" s="75" t="s">
+      <c r="H40" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I40" s="78">
+        <v>8</v>
+      </c>
+      <c r="J40" s="78">
+        <v>0</v>
+      </c>
+      <c r="K40" s="78">
+        <v>0</v>
+      </c>
+      <c r="L40" s="78"/>
+    </row>
+    <row r="41" spans="1:17" s="68" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B41" s="81">
+        <v>2</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="D41" s="77" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" s="78" t="s">
+        <v>147</v>
+      </c>
+      <c r="F41" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="H40" s="79" t="s">
-        <v>6</v>
-      </c>
-      <c r="I40" s="79">
+      <c r="G41" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I41" s="78">
         <v>8</v>
       </c>
-      <c r="J40" s="79">
-        <v>0</v>
-      </c>
-      <c r="K40" s="79">
-        <v>0</v>
-      </c>
-      <c r="L40" s="79"/>
-    </row>
-    <row r="41" spans="1:17" s="69" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="81" t="s">
-        <v>175</v>
-      </c>
-      <c r="B41" s="82">
-        <v>2</v>
-      </c>
-      <c r="C41" s="79" t="s">
-        <v>146</v>
-      </c>
-      <c r="D41" s="78" t="s">
-        <v>148</v>
-      </c>
-      <c r="E41" s="79" t="s">
-        <v>147</v>
-      </c>
-      <c r="F41" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="G41" s="79" t="s">
-        <v>24</v>
-      </c>
-      <c r="H41" s="79" t="s">
-        <v>5</v>
-      </c>
-      <c r="I41" s="79">
+      <c r="J41" s="78">
         <v>8</v>
       </c>
-      <c r="J41" s="79">
+      <c r="K41" s="78">
         <v>8</v>
       </c>
-      <c r="K41" s="79">
-        <v>8</v>
-      </c>
-      <c r="L41" s="79" t="s">
+      <c r="L41" s="78" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2986,13 +2986,13 @@
       <c r="G44" s="18"/>
       <c r="H44" s="18"/>
       <c r="I44" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J44" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="K44" s="18" t="s">
         <v>166</v>
-      </c>
-      <c r="J44" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>168</v>
       </c>
       <c r="L44" s="18" t="s">
         <v>26</v>
@@ -3015,12 +3015,12 @@
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E45" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G45" s="66" t="s">
-        <v>163</v>
-      </c>
-      <c r="H45" s="66"/>
+        <v>167</v>
+      </c>
+      <c r="G45" s="82" t="s">
+        <v>161</v>
+      </c>
+      <c r="H45" s="82"/>
       <c r="I45" s="1">
         <f>SUMIF(B2:B41,1,I2:I41)</f>
         <v>54</v>
@@ -3060,12 +3060,12 @@
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E46" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G46" s="66" t="s">
-        <v>164</v>
-      </c>
-      <c r="H46" s="66"/>
+        <v>168</v>
+      </c>
+      <c r="G46" s="82" t="s">
+        <v>162</v>
+      </c>
+      <c r="H46" s="82"/>
       <c r="I46" s="1">
         <f>SUMIF(B2:B41,2,I2:I41)</f>
         <v>80</v>
@@ -3080,7 +3080,7 @@
       </c>
       <c r="L46" s="1">
         <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"gfels6")</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="M46" s="1">
         <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"ziegm")</f>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="N46" s="1">
         <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"jntme")</f>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O46" s="1">
         <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"kybup1")</f>
@@ -3105,12 +3105,12 @@
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E47" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="G47" s="66" t="s">
-        <v>165</v>
-      </c>
-      <c r="H47" s="66"/>
+        <v>169</v>
+      </c>
+      <c r="G47" s="82" t="s">
+        <v>163</v>
+      </c>
+      <c r="H47" s="82"/>
       <c r="I47" s="1">
         <f>SUMIF(B2:B41,3,I2:I41)</f>
         <v>0</v>
@@ -3151,9 +3151,9 @@
   </sheetData>
   <autoFilter ref="B1:L41">
     <filterColumn colId="0">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters>
+        <filter val="2"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:C7">

</xml_diff>

<commit_message>
Timeplanning in Scrum.xlsx (ziegm, petim)
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1363,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1655,8 +1655,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P46" sqref="P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2407,10 +2407,10 @@
         <v>9</v>
       </c>
       <c r="J23" s="72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K23" s="72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L23" s="72" t="s">
         <v>175</v>
@@ -2445,13 +2445,13 @@
         <v>7</v>
       </c>
       <c r="J24" s="72">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K24" s="72">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L24" s="72" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="33" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
@@ -2600,7 +2600,7 @@
         <v>5</v>
       </c>
       <c r="K28" s="66">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L28" s="66" t="s">
         <v>175</v>
@@ -3071,11 +3071,11 @@
       </c>
       <c r="J46" s="1">
         <f>SUMIF(B2:B41,2,J2:J41)</f>
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="K46" s="1">
         <f>SUMIF(B2:B41,2,K2:K41)</f>
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="L46" s="1">
         <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"gfels6")</f>

</xml_diff>

<commit_message>
added some fancypants stuff in scrum file
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programmierung\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23250" windowHeight="13170" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$41</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -579,16 +584,13 @@
   </si>
   <si>
     <t>actual h</t>
-  </si>
-  <si>
-    <t>planed hours per user</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -658,6 +660,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -691,7 +701,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -717,12 +727,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -942,9 +1023,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1246,18 +1360,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1271,7 +1385,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1282,7 +1396,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1293,7 +1407,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1304,7 +1418,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1315,7 +1429,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1326,7 +1440,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1339,12 +1453,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1352,23 +1466,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1577,7 +1691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1597,7 +1711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1619,7 +1733,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>68</v>
       </c>
@@ -1643,32 +1757,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="32.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="30" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.109375" style="1"/>
-    <col min="16" max="16" width="8.109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="30" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="8.140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1747,7 +1861,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>74</v>
       </c>
@@ -1771,7 +1885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>75</v>
       </c>
@@ -1833,7 +1947,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>1.1000000000000001</v>
       </c>
@@ -1850,7 +1964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>1.2</v>
       </c>
@@ -1867,7 +1981,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>1.3</v>
       </c>
@@ -1891,7 +2005,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="33" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>71</v>
       </c>
@@ -2027,7 +2141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="54" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="54" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55">
         <v>2.2999999999999998</v>
       </c>
@@ -2089,7 +2203,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="33" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="33" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37">
         <v>3.2</v>
       </c>
@@ -2598,7 +2712,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="24">
         <v>4.2</v>
       </c>
@@ -2615,7 +2729,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="20">
         <v>4.3</v>
       </c>
@@ -2639,7 +2753,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24">
         <v>5.0999999999999996</v>
       </c>
@@ -2656,7 +2770,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24">
         <v>5.2</v>
       </c>
@@ -2673,7 +2787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20">
         <v>5.3</v>
       </c>
@@ -2697,7 +2811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="24">
         <v>6.1</v>
       </c>
@@ -2714,7 +2828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="24">
         <v>6.2</v>
       </c>
@@ -2731,7 +2845,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20">
         <v>6.3</v>
       </c>
@@ -2831,7 +2945,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="66" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="78" t="s">
         <v>144</v>
       </c>
@@ -2863,7 +2977,7 @@
         <v>4</v>
       </c>
       <c r="K39" s="76">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L39" s="76" t="s">
         <v>8</v>
@@ -2943,7 +3057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="17"/>
       <c r="C42" s="18"/>
@@ -2957,21 +3071,19 @@
       <c r="K42" s="18"/>
       <c r="L42" s="18"/>
     </row>
-    <row r="43" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="16"/>
       <c r="B43" s="17"/>
       <c r="C43" s="18"/>
       <c r="D43" s="19"/>
-      <c r="L43" s="80" t="s">
-        <v>184</v>
-      </c>
+      <c r="L43" s="80"/>
       <c r="M43" s="80"/>
       <c r="N43" s="80"/>
       <c r="O43" s="80"/>
       <c r="P43" s="80"/>
       <c r="Q43" s="80"/>
     </row>
-    <row r="44" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E44" s="18"/>
       <c r="F44" s="26"/>
       <c r="G44" s="18"/>
@@ -2985,26 +3097,9 @@
       <c r="K44" s="18" t="s">
         <v>183</v>
       </c>
-      <c r="L44" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+      <c r="L44" s="18"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E45" s="1" t="s">
         <v>164</v>
       </c>
@@ -3024,32 +3119,8 @@
         <f>SUMIF(B2:B41,1,K2:K41)</f>
         <v>69</v>
       </c>
-      <c r="L45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"gfels6")</f>
-        <v>9</v>
-      </c>
-      <c r="M45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"ziegm")</f>
-        <v>9</v>
-      </c>
-      <c r="N45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"jntme")</f>
-        <v>9</v>
-      </c>
-      <c r="O45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"kybup1")</f>
-        <v>9</v>
-      </c>
-      <c r="P45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"petim1")</f>
-        <v>9</v>
-      </c>
-      <c r="Q45" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,1,F2:F41,"odaoj1")</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E46" s="1" t="s">
         <v>165</v>
       </c>
@@ -3067,34 +3138,10 @@
       </c>
       <c r="K46" s="1">
         <f>SUMIF(B2:B41,2,K2:K41)</f>
-        <v>61</v>
-      </c>
-      <c r="L46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"gfels6")</f>
-        <v>14</v>
-      </c>
-      <c r="M46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"ziegm")</f>
-        <v>12</v>
-      </c>
-      <c r="N46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"jntme")</f>
-        <v>14</v>
-      </c>
-      <c r="O46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"kybup1")</f>
-        <v>14</v>
-      </c>
-      <c r="P46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"petim1")</f>
-        <v>12</v>
-      </c>
-      <c r="Q46" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,2,F2:F41,"odaoj1")</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E47" s="1" t="s">
         <v>166</v>
       </c>
@@ -3114,33 +3161,384 @@
         <f>SUMIF(B2:B41,3,K2:K41)</f>
         <v>0</v>
       </c>
-      <c r="L47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"gfels6")</f>
+    </row>
+    <row r="50" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G51" s="81" t="s">
+        <v>54</v>
+      </c>
+      <c r="H51" s="82"/>
+      <c r="I51" s="82"/>
+      <c r="J51" s="82"/>
+      <c r="K51" s="82"/>
+      <c r="L51" s="82"/>
+      <c r="M51" s="82"/>
+      <c r="N51" s="83"/>
+    </row>
+    <row r="52" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G52" s="84"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J52" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L52" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M52" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N52" s="85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G53" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="H53" s="87"/>
+      <c r="I53" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"gfels6")</f>
+        <v>9</v>
+      </c>
+      <c r="J53" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"ziegm")</f>
+        <v>9</v>
+      </c>
+      <c r="K53" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"jntme")</f>
+        <v>9</v>
+      </c>
+      <c r="L53" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"kybup1")</f>
+        <v>9</v>
+      </c>
+      <c r="M53" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"petim1")</f>
+        <v>9</v>
+      </c>
+      <c r="N53" s="85">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,1,$F$2:$F$41,"odaoj1")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G54" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="H54" s="87"/>
+      <c r="I54" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"gfels6")</f>
+        <v>14</v>
+      </c>
+      <c r="J54" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"ziegm")</f>
+        <v>12</v>
+      </c>
+      <c r="K54" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"jntme")</f>
+        <v>14</v>
+      </c>
+      <c r="L54" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"kybup1")</f>
+        <v>14</v>
+      </c>
+      <c r="M54" s="18">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"petim1")</f>
+        <v>12</v>
+      </c>
+      <c r="N54" s="85">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,2,$F$2:$F$41,"odaoj1")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G55" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="H55" s="89"/>
+      <c r="I55" s="90">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"gfels6")</f>
         <v>0</v>
       </c>
-      <c r="M47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"ziegm")</f>
+      <c r="J55" s="90">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"ziegm")</f>
         <v>0</v>
       </c>
-      <c r="N47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"jntme")</f>
+      <c r="K55" s="90">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"jntme")</f>
         <v>0</v>
       </c>
-      <c r="O47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"kybup1")</f>
+      <c r="L55" s="90">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"kybup1")</f>
         <v>0</v>
       </c>
-      <c r="P47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"petim1")</f>
+      <c r="M55" s="90">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"petim1")</f>
         <v>0</v>
       </c>
-      <c r="Q47" s="1">
-        <f>SUMIFS(I2:I41,B2:B41,3,F2:F41,"odaoj1")</f>
+      <c r="N55" s="91">
+        <f>SUMIFS(I$2:I$41,$B$2:$B$41,3,$F$2:$F$41,"odaoj1")</f>
         <v>0</v>
       </c>
     </row>
+    <row r="56" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G57" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="H57" s="82"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="82"/>
+      <c r="K57" s="82"/>
+      <c r="L57" s="82"/>
+      <c r="M57" s="82"/>
+      <c r="N57" s="83"/>
+    </row>
+    <row r="58" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G58" s="84"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J58" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K58" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L58" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M58" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N58" s="85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G59" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="H59" s="87"/>
+      <c r="I59" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"gfels6")</f>
+        <v>11</v>
+      </c>
+      <c r="J59" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"ziegm")</f>
+        <v>9</v>
+      </c>
+      <c r="K59" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"jntme")</f>
+        <v>18</v>
+      </c>
+      <c r="L59" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"kybup1")</f>
+        <v>9</v>
+      </c>
+      <c r="M59" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"petim1")</f>
+        <v>7</v>
+      </c>
+      <c r="N59" s="85">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,1,$F$2:$F$41,"odaoj1")</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G60" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="H60" s="87"/>
+      <c r="I60" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"gfels6")</f>
+        <v>13</v>
+      </c>
+      <c r="J60" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"ziegm")</f>
+        <v>12</v>
+      </c>
+      <c r="K60" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"jntme")</f>
+        <v>3</v>
+      </c>
+      <c r="L60" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"kybup1")</f>
+        <v>14</v>
+      </c>
+      <c r="M60" s="18">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"petim1")</f>
+        <v>12</v>
+      </c>
+      <c r="N60" s="85">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,2,$F$2:$F$41,"odaoj1")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G61" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="H61" s="89"/>
+      <c r="I61" s="90">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"gfels6")</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="90">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"ziegm")</f>
+        <v>0</v>
+      </c>
+      <c r="K61" s="90">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"jntme")</f>
+        <v>0</v>
+      </c>
+      <c r="L61" s="90">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"kybup1")</f>
+        <v>0</v>
+      </c>
+      <c r="M61" s="90">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"petim1")</f>
+        <v>0</v>
+      </c>
+      <c r="N61" s="91">
+        <f>SUMIFS(J$2:J$41,$B$2:$B$41,3,$F$2:$F$41,"odaoj1")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G63" s="81" t="s">
+        <v>56</v>
+      </c>
+      <c r="H63" s="82"/>
+      <c r="I63" s="82"/>
+      <c r="J63" s="82"/>
+      <c r="K63" s="82"/>
+      <c r="L63" s="82"/>
+      <c r="M63" s="82"/>
+      <c r="N63" s="83"/>
+    </row>
+    <row r="64" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G64" s="84"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J64" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="K64" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="L64" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="M64" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N64" s="85" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G65" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="H65" s="87"/>
+      <c r="I65" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"gfels6")</f>
+        <v>12</v>
+      </c>
+      <c r="J65" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"ziegm")</f>
+        <v>7</v>
+      </c>
+      <c r="K65" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"jntme")</f>
+        <v>22</v>
+      </c>
+      <c r="L65" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"kybup1")</f>
+        <v>12</v>
+      </c>
+      <c r="M65" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"petim1")</f>
+        <v>8</v>
+      </c>
+      <c r="N65" s="85">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,1,$F$2:$F$41,"odaoj1")</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G66" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="H66" s="87"/>
+      <c r="I66" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"gfels6")</f>
+        <v>9</v>
+      </c>
+      <c r="J66" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"ziegm")</f>
+        <v>12</v>
+      </c>
+      <c r="K66" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"jntme")</f>
+        <v>3</v>
+      </c>
+      <c r="L66" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"kybup1")</f>
+        <v>15</v>
+      </c>
+      <c r="M66" s="18">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"petim1")</f>
+        <v>13</v>
+      </c>
+      <c r="N66" s="85">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,2,$F$2:$F$41,"odaoj1")</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G67" s="88" t="s">
+        <v>162</v>
+      </c>
+      <c r="H67" s="89"/>
+      <c r="I67" s="90">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"gfels6")</f>
+        <v>0</v>
+      </c>
+      <c r="J67" s="90">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"ziegm")</f>
+        <v>0</v>
+      </c>
+      <c r="K67" s="90">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"jntme")</f>
+        <v>0</v>
+      </c>
+      <c r="L67" s="90">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"kybup1")</f>
+        <v>0</v>
+      </c>
+      <c r="M67" s="90">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"petim1")</f>
+        <v>0</v>
+      </c>
+      <c r="N67" s="91">
+        <f>SUMIFS(K$2:K$41,$B$2:$B$41,3,$F$2:$F$41,"odaoj1")</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="B1:L41">
+  <autoFilter ref="B1:L41" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="2"/>
@@ -3150,7 +3548,19 @@
   <sortState ref="A2:C7">
     <sortCondition ref="A2"/>
   </sortState>
-  <mergeCells count="4">
+  <mergeCells count="16">
+    <mergeCell ref="G51:N51"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G57:N57"/>
+    <mergeCell ref="G59:H59"/>
+    <mergeCell ref="G60:H60"/>
+    <mergeCell ref="G61:H61"/>
+    <mergeCell ref="G63:N63"/>
+    <mergeCell ref="G65:H65"/>
+    <mergeCell ref="G66:H66"/>
+    <mergeCell ref="G67:H67"/>
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G46:H46"/>
     <mergeCell ref="G47:H47"/>
@@ -3162,21 +3572,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -3190,10 +3600,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -3203,16 +3613,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O346"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
@@ -3254,7 +3664,7 @@
       <c r="N8" s="48"/>
       <c r="O8" s="48"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="48">
         <v>1</v>
       </c>
@@ -3319,7 +3729,7 @@
       <c r="N11" s="48"/>
       <c r="O11" s="48"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="49"/>
       <c r="B12" s="48"/>
       <c r="C12" s="48" t="s">
@@ -3469,7 +3879,7 @@
       <c r="N19" s="48"/>
       <c r="O19" s="48"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="49"/>
       <c r="B20" s="48"/>
       <c r="C20" s="48"/>
@@ -3486,7 +3896,7 @@
       <c r="N20" s="48"/>
       <c r="O20" s="48"/>
     </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="49"/>
       <c r="B21" s="48"/>
       <c r="C21" s="48"/>
@@ -3503,7 +3913,7 @@
       <c r="N21" s="48"/>
       <c r="O21" s="48"/>
     </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="49"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -3520,7 +3930,7 @@
       <c r="N22" s="48"/>
       <c r="O22" s="48"/>
     </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="49"/>
       <c r="B23" s="48"/>
       <c r="C23" s="48"/>
@@ -3537,7 +3947,7 @@
       <c r="N23" s="48"/>
       <c r="O23" s="48"/>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="49"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
@@ -3554,7 +3964,7 @@
       <c r="N24" s="48"/>
       <c r="O24" s="48"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="49"/>
       <c r="B25" s="48"/>
       <c r="C25" s="48"/>
@@ -3571,7 +3981,7 @@
       <c r="N25" s="48"/>
       <c r="O25" s="48"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="49"/>
       <c r="B26" s="48"/>
       <c r="C26" s="48"/>
@@ -3588,7 +3998,7 @@
       <c r="N26" s="48"/>
       <c r="O26" s="48"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="49"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
@@ -3605,7 +4015,7 @@
       <c r="N27" s="48"/>
       <c r="O27" s="48"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="49"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
@@ -3622,7 +4032,7 @@
       <c r="N28" s="48"/>
       <c r="O28" s="48"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="49"/>
       <c r="B29" s="48"/>
       <c r="C29" s="48"/>
@@ -3639,7 +4049,7 @@
       <c r="N29" s="48"/>
       <c r="O29" s="48"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="49"/>
       <c r="B30" s="48"/>
       <c r="C30" s="48"/>
@@ -3656,7 +4066,7 @@
       <c r="N30" s="48"/>
       <c r="O30" s="48"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="49"/>
       <c r="B31" s="48"/>
       <c r="C31" s="48"/>
@@ -3673,7 +4083,7 @@
       <c r="N31" s="48"/>
       <c r="O31" s="48"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="49"/>
       <c r="B32" s="48"/>
       <c r="C32" s="48"/>
@@ -3690,7 +4100,7 @@
       <c r="N32" s="48"/>
       <c r="O32" s="48"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="49"/>
       <c r="B33" s="48"/>
       <c r="C33" s="48"/>
@@ -3707,7 +4117,7 @@
       <c r="N33" s="48"/>
       <c r="O33" s="48"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="49"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
@@ -3724,7 +4134,7 @@
       <c r="N34" s="48"/>
       <c r="O34" s="48"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="49"/>
       <c r="B35" s="48"/>
       <c r="C35" s="48"/>
@@ -3741,7 +4151,7 @@
       <c r="N35" s="48"/>
       <c r="O35" s="48"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="49"/>
       <c r="B36" s="48"/>
       <c r="C36" s="48"/>
@@ -3758,7 +4168,7 @@
       <c r="N36" s="48"/>
       <c r="O36" s="48"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="49"/>
       <c r="B37" s="48"/>
       <c r="C37" s="48"/>
@@ -3775,7 +4185,7 @@
       <c r="N37" s="48"/>
       <c r="O37" s="48"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="49"/>
       <c r="B38" s="48"/>
       <c r="C38" s="48"/>
@@ -3792,7 +4202,7 @@
       <c r="N38" s="48"/>
       <c r="O38" s="48"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="49"/>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
@@ -3809,7 +4219,7 @@
       <c r="N39" s="48"/>
       <c r="O39" s="48"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="49"/>
       <c r="B40" s="48"/>
       <c r="C40" s="48"/>
@@ -3826,7 +4236,7 @@
       <c r="N40" s="48"/>
       <c r="O40" s="48"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="49"/>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -3843,7 +4253,7 @@
       <c r="N41" s="48"/>
       <c r="O41" s="48"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="49"/>
       <c r="B42" s="48"/>
       <c r="C42" s="48"/>
@@ -3860,7 +4270,7 @@
       <c r="N42" s="48"/>
       <c r="O42" s="48"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="49"/>
       <c r="B43" s="48"/>
       <c r="C43" s="48"/>
@@ -3877,7 +4287,7 @@
       <c r="N43" s="48"/>
       <c r="O43" s="48"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="49"/>
       <c r="B44" s="48"/>
       <c r="C44" s="48"/>
@@ -3894,7 +4304,7 @@
       <c r="N44" s="48"/>
       <c r="O44" s="48"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="49"/>
       <c r="B45" s="48"/>
       <c r="C45" s="48"/>
@@ -3911,7 +4321,7 @@
       <c r="N45" s="48"/>
       <c r="O45" s="48"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="49"/>
       <c r="B46" s="48"/>
       <c r="C46" s="48"/>
@@ -3928,7 +4338,7 @@
       <c r="N46" s="48"/>
       <c r="O46" s="48"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="49"/>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
@@ -3945,7 +4355,7 @@
       <c r="N47" s="48"/>
       <c r="O47" s="48"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="49"/>
       <c r="B48" s="48"/>
       <c r="C48" s="48"/>
@@ -3962,7 +4372,7 @@
       <c r="N48" s="48"/>
       <c r="O48" s="48"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="49"/>
       <c r="B49" s="48"/>
       <c r="C49" s="48"/>
@@ -3979,7 +4389,7 @@
       <c r="N49" s="48"/>
       <c r="O49" s="48"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="49"/>
       <c r="B50" s="48"/>
       <c r="C50" s="48"/>
@@ -3996,7 +4406,7 @@
       <c r="N50" s="48"/>
       <c r="O50" s="48"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="49"/>
       <c r="B51" s="48"/>
       <c r="C51" s="48"/>
@@ -4013,7 +4423,7 @@
       <c r="N51" s="48"/>
       <c r="O51" s="48"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="49"/>
       <c r="B52" s="48"/>
       <c r="C52" s="48"/>
@@ -4030,7 +4440,7 @@
       <c r="N52" s="48"/>
       <c r="O52" s="48"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="49"/>
       <c r="B53" s="48"/>
       <c r="C53" s="48"/>
@@ -4047,7 +4457,7 @@
       <c r="N53" s="48"/>
       <c r="O53" s="48"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="49"/>
       <c r="B54" s="48"/>
       <c r="C54" s="48"/>
@@ -4064,7 +4474,7 @@
       <c r="N54" s="48"/>
       <c r="O54" s="48"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="49"/>
       <c r="B55" s="48"/>
       <c r="C55" s="48"/>
@@ -4081,7 +4491,7 @@
       <c r="N55" s="48"/>
       <c r="O55" s="48"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="49"/>
       <c r="B56" s="48"/>
       <c r="C56" s="48"/>
@@ -4098,7 +4508,7 @@
       <c r="N56" s="48"/>
       <c r="O56" s="48"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="49"/>
       <c r="B57" s="48"/>
       <c r="C57" s="48"/>
@@ -4115,7 +4525,7 @@
       <c r="N57" s="48"/>
       <c r="O57" s="48"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="48"/>
       <c r="B58" s="48"/>
       <c r="C58" s="48"/>
@@ -4132,7 +4542,7 @@
       <c r="N58" s="48"/>
       <c r="O58" s="48"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="48"/>
       <c r="B59" s="48"/>
       <c r="C59" s="48"/>
@@ -4149,7 +4559,7 @@
       <c r="N59" s="48"/>
       <c r="O59" s="48"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="48"/>
       <c r="B60" s="48"/>
       <c r="C60" s="48"/>
@@ -4166,7 +4576,7 @@
       <c r="N60" s="48"/>
       <c r="O60" s="48"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="48"/>
       <c r="B61" s="48"/>
       <c r="C61" s="48"/>
@@ -4183,7 +4593,7 @@
       <c r="N61" s="48"/>
       <c r="O61" s="48"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="48"/>
       <c r="B62" s="48"/>
       <c r="C62" s="48"/>
@@ -4200,7 +4610,7 @@
       <c r="N62" s="48"/>
       <c r="O62" s="48"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="48"/>
       <c r="B63" s="48"/>
       <c r="C63" s="48"/>
@@ -4217,7 +4627,7 @@
       <c r="N63" s="48"/>
       <c r="O63" s="48"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A64" s="48"/>
       <c r="B64" s="48"/>
       <c r="C64" s="48"/>
@@ -4234,7 +4644,7 @@
       <c r="N64" s="48"/>
       <c r="O64" s="48"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A65" s="48"/>
       <c r="B65" s="48"/>
       <c r="C65" s="48"/>
@@ -4251,7 +4661,7 @@
       <c r="N65" s="48"/>
       <c r="O65" s="48"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="48"/>
       <c r="B66" s="48"/>
       <c r="C66" s="48"/>
@@ -4268,7 +4678,7 @@
       <c r="N66" s="48"/>
       <c r="O66" s="48"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A67" s="48"/>
       <c r="B67" s="48"/>
       <c r="C67" s="48"/>
@@ -4285,7 +4695,7 @@
       <c r="N67" s="48"/>
       <c r="O67" s="48"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="48"/>
       <c r="B68" s="48"/>
       <c r="C68" s="48"/>
@@ -4302,7 +4712,7 @@
       <c r="N68" s="48"/>
       <c r="O68" s="48"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="48"/>
       <c r="B69" s="48"/>
       <c r="C69" s="48"/>
@@ -4319,7 +4729,7 @@
       <c r="N69" s="48"/>
       <c r="O69" s="48"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="48"/>
       <c r="B70" s="48"/>
       <c r="C70" s="48"/>
@@ -4336,7 +4746,7 @@
       <c r="N70" s="48"/>
       <c r="O70" s="48"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="48"/>
       <c r="B71" s="48"/>
       <c r="C71" s="48"/>
@@ -4353,7 +4763,7 @@
       <c r="N71" s="48"/>
       <c r="O71" s="48"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="48"/>
       <c r="B72" s="48"/>
       <c r="C72" s="48"/>
@@ -4370,7 +4780,7 @@
       <c r="N72" s="48"/>
       <c r="O72" s="48"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="48"/>
       <c r="B73" s="48"/>
       <c r="C73" s="48"/>
@@ -4387,7 +4797,7 @@
       <c r="N73" s="48"/>
       <c r="O73" s="48"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="48"/>
       <c r="B74" s="48"/>
       <c r="C74" s="48"/>
@@ -4404,7 +4814,7 @@
       <c r="N74" s="48"/>
       <c r="O74" s="48"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A75" s="48"/>
       <c r="B75" s="48"/>
       <c r="C75" s="48"/>
@@ -4421,7 +4831,7 @@
       <c r="N75" s="48"/>
       <c r="O75" s="48"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="48"/>
       <c r="B76" s="48"/>
       <c r="C76" s="48"/>
@@ -4438,7 +4848,7 @@
       <c r="N76" s="48"/>
       <c r="O76" s="48"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A77" s="48"/>
       <c r="B77" s="48"/>
       <c r="C77" s="48"/>
@@ -4455,7 +4865,7 @@
       <c r="N77" s="48"/>
       <c r="O77" s="48"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A78" s="48"/>
       <c r="B78" s="48"/>
       <c r="C78" s="48"/>
@@ -4472,7 +4882,7 @@
       <c r="N78" s="48"/>
       <c r="O78" s="48"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="48"/>
       <c r="B79" s="48"/>
       <c r="C79" s="48"/>
@@ -4489,7 +4899,7 @@
       <c r="N79" s="48"/>
       <c r="O79" s="48"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A80" s="48"/>
       <c r="B80" s="48"/>
       <c r="C80" s="48"/>
@@ -4506,7 +4916,7 @@
       <c r="N80" s="48"/>
       <c r="O80" s="48"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="48"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
@@ -4523,7 +4933,7 @@
       <c r="N81" s="48"/>
       <c r="O81" s="48"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A82" s="48"/>
       <c r="B82" s="48"/>
       <c r="C82" s="48"/>
@@ -4540,7 +4950,7 @@
       <c r="N82" s="48"/>
       <c r="O82" s="48"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="48"/>
       <c r="B83" s="48"/>
       <c r="C83" s="48"/>
@@ -4557,7 +4967,7 @@
       <c r="N83" s="48"/>
       <c r="O83" s="48"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="48"/>
       <c r="B84" s="48"/>
       <c r="C84" s="48"/>
@@ -4574,7 +4984,7 @@
       <c r="N84" s="48"/>
       <c r="O84" s="48"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="48"/>
       <c r="B85" s="48"/>
       <c r="C85" s="48"/>
@@ -4591,7 +5001,7 @@
       <c r="N85" s="48"/>
       <c r="O85" s="48"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A86" s="48"/>
       <c r="B86" s="48"/>
       <c r="C86" s="48"/>
@@ -4608,7 +5018,7 @@
       <c r="N86" s="48"/>
       <c r="O86" s="48"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A87" s="48"/>
       <c r="B87" s="48"/>
       <c r="C87" s="48"/>
@@ -4625,7 +5035,7 @@
       <c r="N87" s="48"/>
       <c r="O87" s="48"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="48"/>
       <c r="B88" s="48"/>
       <c r="C88" s="48"/>
@@ -4642,7 +5052,7 @@
       <c r="N88" s="48"/>
       <c r="O88" s="48"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A89" s="48"/>
       <c r="B89" s="48"/>
       <c r="C89" s="48"/>
@@ -4659,7 +5069,7 @@
       <c r="N89" s="48"/>
       <c r="O89" s="48"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="48"/>
       <c r="B90" s="48"/>
       <c r="C90" s="48"/>
@@ -4676,7 +5086,7 @@
       <c r="N90" s="48"/>
       <c r="O90" s="48"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A91" s="48"/>
       <c r="B91" s="48"/>
       <c r="C91" s="48"/>
@@ -4693,7 +5103,7 @@
       <c r="N91" s="48"/>
       <c r="O91" s="48"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="48"/>
       <c r="B92" s="48"/>
       <c r="C92" s="48"/>
@@ -4710,7 +5120,7 @@
       <c r="N92" s="48"/>
       <c r="O92" s="48"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="48"/>
       <c r="B93" s="48"/>
       <c r="C93" s="48"/>
@@ -4727,7 +5137,7 @@
       <c r="N93" s="48"/>
       <c r="O93" s="48"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A94" s="48"/>
       <c r="B94" s="48"/>
       <c r="C94" s="48"/>
@@ -4744,7 +5154,7 @@
       <c r="N94" s="48"/>
       <c r="O94" s="48"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="48"/>
       <c r="B95" s="48"/>
       <c r="C95" s="48"/>
@@ -4761,7 +5171,7 @@
       <c r="N95" s="48"/>
       <c r="O95" s="48"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A96" s="48"/>
       <c r="B96" s="48"/>
       <c r="C96" s="48"/>
@@ -4778,7 +5188,7 @@
       <c r="N96" s="48"/>
       <c r="O96" s="48"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A97" s="48"/>
       <c r="B97" s="48"/>
       <c r="C97" s="48"/>
@@ -4795,7 +5205,7 @@
       <c r="N97" s="48"/>
       <c r="O97" s="48"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="48"/>
       <c r="B98" s="48"/>
       <c r="C98" s="48"/>
@@ -4812,7 +5222,7 @@
       <c r="N98" s="48"/>
       <c r="O98" s="48"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="48"/>
       <c r="B99" s="48"/>
       <c r="C99" s="48"/>
@@ -4829,7 +5239,7 @@
       <c r="N99" s="48"/>
       <c r="O99" s="48"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="48"/>
       <c r="B100" s="48"/>
       <c r="C100" s="48"/>
@@ -4846,7 +5256,7 @@
       <c r="N100" s="48"/>
       <c r="O100" s="48"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A101" s="48"/>
       <c r="B101" s="48"/>
       <c r="C101" s="48"/>
@@ -4863,7 +5273,7 @@
       <c r="N101" s="48"/>
       <c r="O101" s="48"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A102" s="48"/>
       <c r="B102" s="48"/>
       <c r="C102" s="48"/>
@@ -4880,7 +5290,7 @@
       <c r="N102" s="48"/>
       <c r="O102" s="48"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A103" s="48"/>
       <c r="B103" s="48"/>
       <c r="C103" s="48"/>
@@ -4897,7 +5307,7 @@
       <c r="N103" s="48"/>
       <c r="O103" s="48"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A104" s="48"/>
       <c r="B104" s="48"/>
       <c r="C104" s="48"/>
@@ -4914,7 +5324,7 @@
       <c r="N104" s="48"/>
       <c r="O104" s="48"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A105" s="48"/>
       <c r="B105" s="48"/>
       <c r="C105" s="48"/>
@@ -4931,7 +5341,7 @@
       <c r="N105" s="48"/>
       <c r="O105" s="48"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A106" s="48"/>
       <c r="B106" s="48"/>
       <c r="C106" s="48"/>
@@ -4948,7 +5358,7 @@
       <c r="N106" s="48"/>
       <c r="O106" s="48"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A107" s="48"/>
       <c r="B107" s="48"/>
       <c r="C107" s="48"/>
@@ -4965,7 +5375,7 @@
       <c r="N107" s="48"/>
       <c r="O107" s="48"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A108" s="48"/>
       <c r="B108" s="48"/>
       <c r="C108" s="48"/>
@@ -4982,7 +5392,7 @@
       <c r="N108" s="48"/>
       <c r="O108" s="48"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A109" s="48"/>
       <c r="B109" s="48"/>
       <c r="C109" s="48"/>
@@ -4999,7 +5409,7 @@
       <c r="N109" s="48"/>
       <c r="O109" s="48"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A110" s="48"/>
       <c r="B110" s="48"/>
       <c r="C110" s="48"/>
@@ -5016,7 +5426,7 @@
       <c r="N110" s="48"/>
       <c r="O110" s="48"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A111" s="48"/>
       <c r="B111" s="48"/>
       <c r="C111" s="48"/>
@@ -5033,7 +5443,7 @@
       <c r="N111" s="48"/>
       <c r="O111" s="48"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A112" s="48"/>
       <c r="B112" s="48"/>
       <c r="C112" s="48"/>
@@ -5050,7 +5460,7 @@
       <c r="N112" s="48"/>
       <c r="O112" s="48"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="48"/>
       <c r="B113" s="48"/>
       <c r="C113" s="48"/>
@@ -5067,7 +5477,7 @@
       <c r="N113" s="48"/>
       <c r="O113" s="48"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A114" s="48"/>
       <c r="B114" s="48"/>
       <c r="C114" s="48"/>
@@ -5084,7 +5494,7 @@
       <c r="N114" s="48"/>
       <c r="O114" s="48"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A115" s="48"/>
       <c r="B115" s="48"/>
       <c r="C115" s="48"/>
@@ -5101,7 +5511,7 @@
       <c r="N115" s="48"/>
       <c r="O115" s="48"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A116" s="48"/>
       <c r="B116" s="48"/>
       <c r="C116" s="48"/>
@@ -5118,7 +5528,7 @@
       <c r="N116" s="48"/>
       <c r="O116" s="48"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A117" s="48"/>
       <c r="B117" s="48"/>
       <c r="C117" s="48"/>
@@ -5135,7 +5545,7 @@
       <c r="N117" s="48"/>
       <c r="O117" s="48"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A118" s="48"/>
       <c r="B118" s="48"/>
       <c r="C118" s="48"/>
@@ -5152,7 +5562,7 @@
       <c r="N118" s="48"/>
       <c r="O118" s="48"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A119" s="48"/>
       <c r="B119" s="48"/>
       <c r="C119" s="48"/>
@@ -5169,7 +5579,7 @@
       <c r="N119" s="48"/>
       <c r="O119" s="48"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A120" s="48"/>
       <c r="B120" s="48"/>
       <c r="C120" s="48"/>
@@ -5186,7 +5596,7 @@
       <c r="N120" s="48"/>
       <c r="O120" s="48"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A121" s="48"/>
       <c r="B121" s="48"/>
       <c r="C121" s="48"/>
@@ -5203,7 +5613,7 @@
       <c r="N121" s="48"/>
       <c r="O121" s="48"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A122" s="48"/>
       <c r="B122" s="48"/>
       <c r="C122" s="48"/>
@@ -5220,7 +5630,7 @@
       <c r="N122" s="48"/>
       <c r="O122" s="48"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A123" s="48"/>
       <c r="B123" s="48"/>
       <c r="C123" s="48"/>
@@ -5237,7 +5647,7 @@
       <c r="N123" s="48"/>
       <c r="O123" s="48"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A124" s="48"/>
       <c r="B124" s="48"/>
       <c r="C124" s="48"/>
@@ -5254,7 +5664,7 @@
       <c r="N124" s="48"/>
       <c r="O124" s="48"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A125" s="48"/>
       <c r="B125" s="48"/>
       <c r="C125" s="48"/>
@@ -5271,7 +5681,7 @@
       <c r="N125" s="48"/>
       <c r="O125" s="48"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A126" s="48"/>
       <c r="B126" s="48"/>
       <c r="C126" s="48"/>
@@ -5288,7 +5698,7 @@
       <c r="N126" s="48"/>
       <c r="O126" s="48"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A127" s="48"/>
       <c r="B127" s="48"/>
       <c r="C127" s="48"/>
@@ -5305,7 +5715,7 @@
       <c r="N127" s="48"/>
       <c r="O127" s="48"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A128" s="48"/>
       <c r="B128" s="48"/>
       <c r="C128" s="48"/>
@@ -5322,7 +5732,7 @@
       <c r="N128" s="48"/>
       <c r="O128" s="48"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="48"/>
       <c r="B129" s="48"/>
       <c r="C129" s="48"/>
@@ -5339,7 +5749,7 @@
       <c r="N129" s="48"/>
       <c r="O129" s="48"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A130" s="48"/>
       <c r="B130" s="48"/>
       <c r="C130" s="48"/>
@@ -5356,7 +5766,7 @@
       <c r="N130" s="48"/>
       <c r="O130" s="48"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A131" s="48"/>
       <c r="B131" s="48"/>
       <c r="C131" s="48"/>
@@ -5373,7 +5783,7 @@
       <c r="N131" s="48"/>
       <c r="O131" s="48"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A132" s="48"/>
       <c r="B132" s="48"/>
       <c r="C132" s="48"/>
@@ -5390,7 +5800,7 @@
       <c r="N132" s="48"/>
       <c r="O132" s="48"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A133" s="48"/>
       <c r="B133" s="48"/>
       <c r="C133" s="48"/>
@@ -5407,7 +5817,7 @@
       <c r="N133" s="48"/>
       <c r="O133" s="48"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A134" s="48"/>
       <c r="B134" s="48"/>
       <c r="C134" s="48"/>
@@ -5424,7 +5834,7 @@
       <c r="N134" s="48"/>
       <c r="O134" s="48"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A135" s="48"/>
       <c r="B135" s="48"/>
       <c r="C135" s="48"/>
@@ -5441,7 +5851,7 @@
       <c r="N135" s="48"/>
       <c r="O135" s="48"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A136" s="48"/>
       <c r="B136" s="48"/>
       <c r="C136" s="48"/>
@@ -5458,7 +5868,7 @@
       <c r="N136" s="48"/>
       <c r="O136" s="48"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A137" s="48"/>
       <c r="B137" s="48"/>
       <c r="C137" s="48"/>
@@ -5475,7 +5885,7 @@
       <c r="N137" s="48"/>
       <c r="O137" s="48"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A138" s="48"/>
       <c r="B138" s="48"/>
       <c r="C138" s="48"/>
@@ -5492,7 +5902,7 @@
       <c r="N138" s="48"/>
       <c r="O138" s="48"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A139" s="48"/>
       <c r="B139" s="48"/>
       <c r="C139" s="48"/>
@@ -5509,7 +5919,7 @@
       <c r="N139" s="48"/>
       <c r="O139" s="48"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A140" s="48"/>
       <c r="B140" s="48"/>
       <c r="C140" s="48"/>
@@ -5526,7 +5936,7 @@
       <c r="N140" s="48"/>
       <c r="O140" s="48"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A141" s="48"/>
       <c r="B141" s="48"/>
       <c r="C141" s="48"/>
@@ -5543,7 +5953,7 @@
       <c r="N141" s="48"/>
       <c r="O141" s="48"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A142" s="48"/>
       <c r="B142" s="48"/>
       <c r="C142" s="48"/>
@@ -5560,7 +5970,7 @@
       <c r="N142" s="48"/>
       <c r="O142" s="48"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A143" s="48"/>
       <c r="B143" s="48"/>
       <c r="C143" s="48"/>
@@ -5577,7 +5987,7 @@
       <c r="N143" s="48"/>
       <c r="O143" s="48"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A144" s="48"/>
       <c r="B144" s="48"/>
       <c r="C144" s="48"/>
@@ -5594,7 +6004,7 @@
       <c r="N144" s="48"/>
       <c r="O144" s="48"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A145" s="48"/>
       <c r="B145" s="48"/>
       <c r="C145" s="48"/>
@@ -5611,7 +6021,7 @@
       <c r="N145" s="48"/>
       <c r="O145" s="48"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A146" s="48"/>
       <c r="B146" s="48"/>
       <c r="C146" s="48"/>
@@ -5628,7 +6038,7 @@
       <c r="N146" s="48"/>
       <c r="O146" s="48"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A147" s="48"/>
       <c r="B147" s="48"/>
       <c r="C147" s="48"/>
@@ -5645,7 +6055,7 @@
       <c r="N147" s="48"/>
       <c r="O147" s="48"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A148" s="48"/>
       <c r="B148" s="48"/>
       <c r="C148" s="48"/>
@@ -5662,7 +6072,7 @@
       <c r="N148" s="48"/>
       <c r="O148" s="48"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A149" s="48"/>
       <c r="B149" s="48"/>
       <c r="C149" s="48"/>
@@ -5679,7 +6089,7 @@
       <c r="N149" s="48"/>
       <c r="O149" s="48"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A150" s="48"/>
       <c r="B150" s="48"/>
       <c r="C150" s="48"/>
@@ -5696,7 +6106,7 @@
       <c r="N150" s="48"/>
       <c r="O150" s="48"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A151" s="48"/>
       <c r="B151" s="48"/>
       <c r="C151" s="48"/>
@@ -5713,7 +6123,7 @@
       <c r="N151" s="48"/>
       <c r="O151" s="48"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A152" s="48"/>
       <c r="B152" s="48"/>
       <c r="C152" s="48"/>
@@ -5730,7 +6140,7 @@
       <c r="N152" s="48"/>
       <c r="O152" s="48"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A153" s="48"/>
       <c r="B153" s="48"/>
       <c r="C153" s="48"/>
@@ -5747,7 +6157,7 @@
       <c r="N153" s="48"/>
       <c r="O153" s="48"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A154" s="48"/>
       <c r="B154" s="48"/>
       <c r="C154" s="48"/>
@@ -5764,7 +6174,7 @@
       <c r="N154" s="48"/>
       <c r="O154" s="48"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A155" s="48"/>
       <c r="B155" s="48"/>
       <c r="C155" s="48"/>
@@ -5781,7 +6191,7 @@
       <c r="N155" s="48"/>
       <c r="O155" s="48"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A156" s="48"/>
       <c r="B156" s="48"/>
       <c r="C156" s="48"/>
@@ -5798,7 +6208,7 @@
       <c r="N156" s="48"/>
       <c r="O156" s="48"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A157" s="48"/>
       <c r="B157" s="48"/>
       <c r="C157" s="48"/>
@@ -5815,7 +6225,7 @@
       <c r="N157" s="48"/>
       <c r="O157" s="48"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A158" s="48"/>
       <c r="B158" s="48"/>
       <c r="C158" s="48"/>
@@ -5832,7 +6242,7 @@
       <c r="N158" s="48"/>
       <c r="O158" s="48"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A159" s="48"/>
       <c r="B159" s="48"/>
       <c r="C159" s="48"/>
@@ -5849,7 +6259,7 @@
       <c r="N159" s="48"/>
       <c r="O159" s="48"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A160" s="48"/>
       <c r="B160" s="48"/>
       <c r="C160" s="48"/>
@@ -5866,7 +6276,7 @@
       <c r="N160" s="48"/>
       <c r="O160" s="48"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A161" s="48"/>
       <c r="B161" s="48"/>
       <c r="C161" s="48"/>
@@ -5883,7 +6293,7 @@
       <c r="N161" s="48"/>
       <c r="O161" s="48"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A162" s="48"/>
       <c r="B162" s="48"/>
       <c r="C162" s="48"/>
@@ -5900,7 +6310,7 @@
       <c r="N162" s="48"/>
       <c r="O162" s="48"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A163" s="48"/>
       <c r="B163" s="48"/>
       <c r="C163" s="48"/>
@@ -5917,7 +6327,7 @@
       <c r="N163" s="48"/>
       <c r="O163" s="48"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A164" s="48"/>
       <c r="B164" s="48"/>
       <c r="C164" s="48"/>
@@ -5934,7 +6344,7 @@
       <c r="N164" s="48"/>
       <c r="O164" s="48"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A165" s="48"/>
       <c r="B165" s="48"/>
       <c r="C165" s="48"/>
@@ -5951,7 +6361,7 @@
       <c r="N165" s="48"/>
       <c r="O165" s="48"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A166" s="48"/>
       <c r="B166" s="48"/>
       <c r="C166" s="48"/>
@@ -5968,7 +6378,7 @@
       <c r="N166" s="48"/>
       <c r="O166" s="48"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A167" s="48"/>
       <c r="B167" s="48"/>
       <c r="C167" s="48"/>
@@ -5985,7 +6395,7 @@
       <c r="N167" s="48"/>
       <c r="O167" s="48"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A168" s="48"/>
       <c r="B168" s="48"/>
       <c r="C168" s="48"/>
@@ -6002,7 +6412,7 @@
       <c r="N168" s="48"/>
       <c r="O168" s="48"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A169" s="48"/>
       <c r="B169" s="48"/>
       <c r="C169" s="48"/>
@@ -6019,7 +6429,7 @@
       <c r="N169" s="48"/>
       <c r="O169" s="48"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A170" s="48"/>
       <c r="B170" s="48"/>
       <c r="C170" s="48"/>
@@ -6036,7 +6446,7 @@
       <c r="N170" s="48"/>
       <c r="O170" s="48"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A171" s="48"/>
       <c r="B171" s="48"/>
       <c r="C171" s="48"/>
@@ -6053,7 +6463,7 @@
       <c r="N171" s="48"/>
       <c r="O171" s="48"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A172" s="48"/>
       <c r="B172" s="48"/>
       <c r="C172" s="48"/>
@@ -6070,7 +6480,7 @@
       <c r="N172" s="48"/>
       <c r="O172" s="48"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A173" s="48"/>
       <c r="B173" s="48"/>
       <c r="C173" s="48"/>
@@ -6087,7 +6497,7 @@
       <c r="N173" s="48"/>
       <c r="O173" s="48"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A174" s="48"/>
       <c r="B174" s="48"/>
       <c r="C174" s="48"/>
@@ -6104,7 +6514,7 @@
       <c r="N174" s="48"/>
       <c r="O174" s="48"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A175" s="48"/>
       <c r="B175" s="48"/>
       <c r="C175" s="48"/>
@@ -6121,7 +6531,7 @@
       <c r="N175" s="48"/>
       <c r="O175" s="48"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A176" s="48"/>
       <c r="B176" s="48"/>
       <c r="C176" s="48"/>
@@ -6138,7 +6548,7 @@
       <c r="N176" s="48"/>
       <c r="O176" s="48"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A177" s="48"/>
       <c r="B177" s="48"/>
       <c r="C177" s="48"/>
@@ -6155,7 +6565,7 @@
       <c r="N177" s="48"/>
       <c r="O177" s="48"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A178" s="48"/>
       <c r="B178" s="48"/>
       <c r="C178" s="48"/>
@@ -6172,7 +6582,7 @@
       <c r="N178" s="48"/>
       <c r="O178" s="48"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A179" s="48"/>
       <c r="B179" s="48"/>
       <c r="C179" s="48"/>
@@ -6189,7 +6599,7 @@
       <c r="N179" s="48"/>
       <c r="O179" s="48"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A180" s="48"/>
       <c r="B180" s="48"/>
       <c r="C180" s="48"/>
@@ -6206,7 +6616,7 @@
       <c r="N180" s="48"/>
       <c r="O180" s="48"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A181" s="48"/>
       <c r="B181" s="48"/>
       <c r="C181" s="48"/>
@@ -6223,7 +6633,7 @@
       <c r="N181" s="48"/>
       <c r="O181" s="48"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A182" s="48"/>
       <c r="B182" s="48"/>
       <c r="C182" s="48"/>
@@ -6240,7 +6650,7 @@
       <c r="N182" s="48"/>
       <c r="O182" s="48"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A183" s="48"/>
       <c r="B183" s="48"/>
       <c r="C183" s="48"/>
@@ -6257,7 +6667,7 @@
       <c r="N183" s="48"/>
       <c r="O183" s="48"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A184" s="48"/>
       <c r="B184" s="48"/>
       <c r="C184" s="48"/>
@@ -6274,7 +6684,7 @@
       <c r="N184" s="48"/>
       <c r="O184" s="48"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A185" s="48"/>
       <c r="B185" s="48"/>
       <c r="C185" s="48"/>
@@ -6291,7 +6701,7 @@
       <c r="N185" s="48"/>
       <c r="O185" s="48"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A186" s="48"/>
       <c r="B186" s="48"/>
       <c r="C186" s="48"/>
@@ -6308,7 +6718,7 @@
       <c r="N186" s="48"/>
       <c r="O186" s="48"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A187" s="48"/>
       <c r="B187" s="48"/>
       <c r="C187" s="48"/>
@@ -6325,7 +6735,7 @@
       <c r="N187" s="48"/>
       <c r="O187" s="48"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A188" s="48"/>
       <c r="B188" s="48"/>
       <c r="C188" s="48"/>
@@ -6342,7 +6752,7 @@
       <c r="N188" s="48"/>
       <c r="O188" s="48"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A189" s="48"/>
       <c r="B189" s="48"/>
       <c r="C189" s="48"/>
@@ -6359,7 +6769,7 @@
       <c r="N189" s="48"/>
       <c r="O189" s="48"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A190" s="48"/>
       <c r="B190" s="48"/>
       <c r="C190" s="48"/>
@@ -6376,7 +6786,7 @@
       <c r="N190" s="48"/>
       <c r="O190" s="48"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A191" s="48"/>
       <c r="B191" s="48"/>
       <c r="C191" s="48"/>
@@ -6393,7 +6803,7 @@
       <c r="N191" s="48"/>
       <c r="O191" s="48"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A192" s="48"/>
       <c r="B192" s="48"/>
       <c r="C192" s="48"/>
@@ -6410,7 +6820,7 @@
       <c r="N192" s="48"/>
       <c r="O192" s="48"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A193" s="48"/>
       <c r="B193" s="48"/>
       <c r="C193" s="48"/>
@@ -6427,7 +6837,7 @@
       <c r="N193" s="48"/>
       <c r="O193" s="48"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A194" s="48"/>
       <c r="B194" s="48"/>
       <c r="C194" s="48"/>
@@ -6444,7 +6854,7 @@
       <c r="N194" s="48"/>
       <c r="O194" s="48"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A195" s="48"/>
       <c r="B195" s="48"/>
       <c r="C195" s="48"/>
@@ -6461,7 +6871,7 @@
       <c r="N195" s="48"/>
       <c r="O195" s="48"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A196" s="48"/>
       <c r="B196" s="48"/>
       <c r="C196" s="48"/>
@@ -6478,7 +6888,7 @@
       <c r="N196" s="48"/>
       <c r="O196" s="48"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A197" s="48"/>
       <c r="B197" s="48"/>
       <c r="C197" s="48"/>
@@ -6495,7 +6905,7 @@
       <c r="N197" s="48"/>
       <c r="O197" s="48"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A198" s="48"/>
       <c r="B198" s="48"/>
       <c r="C198" s="48"/>
@@ -6512,7 +6922,7 @@
       <c r="N198" s="48"/>
       <c r="O198" s="48"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A199" s="48"/>
       <c r="B199" s="48"/>
       <c r="C199" s="48"/>
@@ -6529,7 +6939,7 @@
       <c r="N199" s="48"/>
       <c r="O199" s="48"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A200" s="48"/>
       <c r="B200" s="48"/>
       <c r="C200" s="48"/>
@@ -6546,7 +6956,7 @@
       <c r="N200" s="48"/>
       <c r="O200" s="48"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A201" s="48"/>
       <c r="B201" s="48"/>
       <c r="C201" s="48"/>
@@ -6563,7 +6973,7 @@
       <c r="N201" s="48"/>
       <c r="O201" s="48"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A202" s="48"/>
       <c r="B202" s="48"/>
       <c r="C202" s="48"/>
@@ -6580,7 +6990,7 @@
       <c r="N202" s="48"/>
       <c r="O202" s="48"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A203" s="48"/>
       <c r="B203" s="48"/>
       <c r="C203" s="48"/>
@@ -6597,7 +7007,7 @@
       <c r="N203" s="48"/>
       <c r="O203" s="48"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A204" s="48"/>
       <c r="B204" s="48"/>
       <c r="C204" s="48"/>
@@ -6614,7 +7024,7 @@
       <c r="N204" s="48"/>
       <c r="O204" s="48"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A205" s="48"/>
       <c r="B205" s="48"/>
       <c r="C205" s="48"/>
@@ -6631,7 +7041,7 @@
       <c r="N205" s="48"/>
       <c r="O205" s="48"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A206" s="48"/>
       <c r="B206" s="48"/>
       <c r="C206" s="48"/>
@@ -6648,7 +7058,7 @@
       <c r="N206" s="48"/>
       <c r="O206" s="48"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A207" s="48"/>
       <c r="B207" s="48"/>
       <c r="C207" s="48"/>
@@ -6665,7 +7075,7 @@
       <c r="N207" s="48"/>
       <c r="O207" s="48"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A208" s="48"/>
       <c r="B208" s="48"/>
       <c r="C208" s="48"/>
@@ -6682,7 +7092,7 @@
       <c r="N208" s="48"/>
       <c r="O208" s="48"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A209" s="48"/>
       <c r="B209" s="48"/>
       <c r="C209" s="48"/>
@@ -6699,7 +7109,7 @@
       <c r="N209" s="48"/>
       <c r="O209" s="48"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A210" s="48"/>
       <c r="B210" s="48"/>
       <c r="C210" s="48"/>
@@ -6716,7 +7126,7 @@
       <c r="N210" s="48"/>
       <c r="O210" s="48"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A211" s="48"/>
       <c r="B211" s="48"/>
       <c r="C211" s="48"/>
@@ -6733,7 +7143,7 @@
       <c r="N211" s="48"/>
       <c r="O211" s="48"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A212" s="48"/>
       <c r="B212" s="48"/>
       <c r="C212" s="48"/>
@@ -6750,7 +7160,7 @@
       <c r="N212" s="48"/>
       <c r="O212" s="48"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A213" s="48"/>
       <c r="B213" s="48"/>
       <c r="C213" s="48"/>
@@ -6767,7 +7177,7 @@
       <c r="N213" s="48"/>
       <c r="O213" s="48"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A214" s="48"/>
       <c r="B214" s="48"/>
       <c r="C214" s="48"/>
@@ -6784,7 +7194,7 @@
       <c r="N214" s="48"/>
       <c r="O214" s="48"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A215" s="48"/>
       <c r="B215" s="48"/>
       <c r="C215" s="48"/>
@@ -6801,7 +7211,7 @@
       <c r="N215" s="48"/>
       <c r="O215" s="48"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A216" s="48"/>
       <c r="B216" s="48"/>
       <c r="C216" s="48"/>
@@ -6818,7 +7228,7 @@
       <c r="N216" s="48"/>
       <c r="O216" s="48"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A217" s="48"/>
       <c r="B217" s="48"/>
       <c r="C217" s="48"/>
@@ -6835,7 +7245,7 @@
       <c r="N217" s="48"/>
       <c r="O217" s="48"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A218" s="48"/>
       <c r="B218" s="48"/>
       <c r="C218" s="48"/>
@@ -6852,7 +7262,7 @@
       <c r="N218" s="48"/>
       <c r="O218" s="48"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A219" s="48"/>
       <c r="B219" s="48"/>
       <c r="C219" s="48"/>
@@ -6869,7 +7279,7 @@
       <c r="N219" s="48"/>
       <c r="O219" s="48"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A220" s="48"/>
       <c r="B220" s="48"/>
       <c r="C220" s="48"/>
@@ -6886,7 +7296,7 @@
       <c r="N220" s="48"/>
       <c r="O220" s="48"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="48"/>
       <c r="B221" s="48"/>
       <c r="C221" s="48"/>
@@ -6903,7 +7313,7 @@
       <c r="N221" s="48"/>
       <c r="O221" s="48"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A222" s="48"/>
       <c r="B222" s="48"/>
       <c r="C222" s="48"/>
@@ -6920,7 +7330,7 @@
       <c r="N222" s="48"/>
       <c r="O222" s="48"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A223" s="48"/>
       <c r="B223" s="48"/>
       <c r="C223" s="48"/>
@@ -6937,7 +7347,7 @@
       <c r="N223" s="48"/>
       <c r="O223" s="48"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A224" s="48"/>
       <c r="B224" s="48"/>
       <c r="C224" s="48"/>
@@ -6954,7 +7364,7 @@
       <c r="N224" s="48"/>
       <c r="O224" s="48"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A225" s="48"/>
       <c r="B225" s="48"/>
       <c r="C225" s="48"/>
@@ -6971,7 +7381,7 @@
       <c r="N225" s="48"/>
       <c r="O225" s="48"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A226" s="48"/>
       <c r="B226" s="48"/>
       <c r="C226" s="48"/>
@@ -6988,7 +7398,7 @@
       <c r="N226" s="48"/>
       <c r="O226" s="48"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A227" s="48"/>
       <c r="B227" s="48"/>
       <c r="C227" s="48"/>
@@ -7005,7 +7415,7 @@
       <c r="N227" s="48"/>
       <c r="O227" s="48"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A228" s="48"/>
       <c r="B228" s="48"/>
       <c r="C228" s="48"/>
@@ -7022,7 +7432,7 @@
       <c r="N228" s="48"/>
       <c r="O228" s="48"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A229" s="48"/>
       <c r="B229" s="48"/>
       <c r="C229" s="48"/>
@@ -7039,7 +7449,7 @@
       <c r="N229" s="48"/>
       <c r="O229" s="48"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A230" s="48"/>
       <c r="B230" s="48"/>
       <c r="C230" s="48"/>
@@ -7056,7 +7466,7 @@
       <c r="N230" s="48"/>
       <c r="O230" s="48"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A231" s="48"/>
       <c r="B231" s="48"/>
       <c r="C231" s="48"/>
@@ -7073,7 +7483,7 @@
       <c r="N231" s="48"/>
       <c r="O231" s="48"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A232" s="48"/>
       <c r="B232" s="48"/>
       <c r="C232" s="48"/>
@@ -7090,7 +7500,7 @@
       <c r="N232" s="48"/>
       <c r="O232" s="48"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A233" s="48"/>
       <c r="B233" s="48"/>
       <c r="C233" s="48"/>
@@ -7107,7 +7517,7 @@
       <c r="N233" s="48"/>
       <c r="O233" s="48"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A234" s="48"/>
       <c r="B234" s="48"/>
       <c r="C234" s="48"/>
@@ -7124,7 +7534,7 @@
       <c r="N234" s="48"/>
       <c r="O234" s="48"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A235" s="48"/>
       <c r="B235" s="48"/>
       <c r="C235" s="48"/>
@@ -7141,7 +7551,7 @@
       <c r="N235" s="48"/>
       <c r="O235" s="48"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A236" s="48"/>
       <c r="B236" s="48"/>
       <c r="C236" s="48"/>
@@ -7158,7 +7568,7 @@
       <c r="N236" s="48"/>
       <c r="O236" s="48"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A237" s="48"/>
       <c r="B237" s="48"/>
       <c r="C237" s="48"/>
@@ -7175,7 +7585,7 @@
       <c r="N237" s="48"/>
       <c r="O237" s="48"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A238" s="48"/>
       <c r="B238" s="48"/>
       <c r="C238" s="48"/>
@@ -7192,7 +7602,7 @@
       <c r="N238" s="48"/>
       <c r="O238" s="48"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A239" s="48"/>
       <c r="B239" s="48"/>
       <c r="C239" s="48"/>
@@ -7209,7 +7619,7 @@
       <c r="N239" s="48"/>
       <c r="O239" s="48"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A240" s="48"/>
       <c r="B240" s="48"/>
       <c r="C240" s="48"/>
@@ -7226,7 +7636,7 @@
       <c r="N240" s="48"/>
       <c r="O240" s="48"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A241" s="48"/>
       <c r="B241" s="48"/>
       <c r="C241" s="48"/>
@@ -7243,7 +7653,7 @@
       <c r="N241" s="48"/>
       <c r="O241" s="48"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A242" s="48"/>
       <c r="B242" s="48"/>
       <c r="C242" s="48"/>
@@ -7260,7 +7670,7 @@
       <c r="N242" s="48"/>
       <c r="O242" s="48"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A243" s="48"/>
       <c r="B243" s="48"/>
       <c r="C243" s="48"/>
@@ -7277,7 +7687,7 @@
       <c r="N243" s="48"/>
       <c r="O243" s="48"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A244" s="48"/>
       <c r="B244" s="48"/>
       <c r="C244" s="48"/>
@@ -7294,7 +7704,7 @@
       <c r="N244" s="48"/>
       <c r="O244" s="48"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A245" s="48"/>
       <c r="B245" s="48"/>
       <c r="C245" s="48"/>
@@ -7311,7 +7721,7 @@
       <c r="N245" s="48"/>
       <c r="O245" s="48"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A246" s="48"/>
       <c r="B246" s="48"/>
       <c r="C246" s="48"/>
@@ -7328,7 +7738,7 @@
       <c r="N246" s="48"/>
       <c r="O246" s="48"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A247" s="48"/>
       <c r="B247" s="48"/>
       <c r="C247" s="48"/>
@@ -7345,7 +7755,7 @@
       <c r="N247" s="48"/>
       <c r="O247" s="48"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A248" s="48"/>
       <c r="B248" s="48"/>
       <c r="C248" s="48"/>
@@ -7362,7 +7772,7 @@
       <c r="N248" s="48"/>
       <c r="O248" s="48"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A249" s="48"/>
       <c r="B249" s="48"/>
       <c r="C249" s="48"/>
@@ -7379,7 +7789,7 @@
       <c r="N249" s="48"/>
       <c r="O249" s="48"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A250" s="48"/>
       <c r="B250" s="48"/>
       <c r="C250" s="48"/>
@@ -7396,7 +7806,7 @@
       <c r="N250" s="48"/>
       <c r="O250" s="48"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A251" s="48"/>
       <c r="B251" s="48"/>
       <c r="C251" s="48"/>
@@ -7413,7 +7823,7 @@
       <c r="N251" s="48"/>
       <c r="O251" s="48"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A252" s="48"/>
       <c r="B252" s="48"/>
       <c r="C252" s="48"/>
@@ -7430,7 +7840,7 @@
       <c r="N252" s="48"/>
       <c r="O252" s="48"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A253" s="48"/>
       <c r="B253" s="48"/>
       <c r="C253" s="48"/>
@@ -7447,7 +7857,7 @@
       <c r="N253" s="48"/>
       <c r="O253" s="48"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A254" s="48"/>
       <c r="B254" s="48"/>
       <c r="C254" s="48"/>
@@ -7464,7 +7874,7 @@
       <c r="N254" s="48"/>
       <c r="O254" s="48"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A255" s="48"/>
       <c r="B255" s="48"/>
       <c r="C255" s="48"/>
@@ -7481,7 +7891,7 @@
       <c r="N255" s="48"/>
       <c r="O255" s="48"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A256" s="48"/>
       <c r="B256" s="48"/>
       <c r="C256" s="48"/>
@@ -7498,7 +7908,7 @@
       <c r="N256" s="48"/>
       <c r="O256" s="48"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A257" s="48"/>
       <c r="B257" s="48"/>
       <c r="C257" s="48"/>
@@ -7515,7 +7925,7 @@
       <c r="N257" s="48"/>
       <c r="O257" s="48"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A258" s="48"/>
       <c r="B258" s="48"/>
       <c r="C258" s="48"/>
@@ -7532,7 +7942,7 @@
       <c r="N258" s="48"/>
       <c r="O258" s="48"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A259" s="48"/>
       <c r="B259" s="48"/>
       <c r="C259" s="48"/>
@@ -7549,7 +7959,7 @@
       <c r="N259" s="48"/>
       <c r="O259" s="48"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A260" s="48"/>
       <c r="B260" s="48"/>
       <c r="C260" s="48"/>
@@ -7566,7 +7976,7 @@
       <c r="N260" s="48"/>
       <c r="O260" s="48"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A261" s="48"/>
       <c r="B261" s="48"/>
       <c r="C261" s="48"/>
@@ -7583,7 +7993,7 @@
       <c r="N261" s="48"/>
       <c r="O261" s="48"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A262" s="48"/>
       <c r="B262" s="48"/>
       <c r="C262" s="48"/>
@@ -7600,7 +8010,7 @@
       <c r="N262" s="48"/>
       <c r="O262" s="48"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A263" s="48"/>
       <c r="B263" s="48"/>
       <c r="C263" s="48"/>
@@ -7617,7 +8027,7 @@
       <c r="N263" s="48"/>
       <c r="O263" s="48"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A264" s="48"/>
       <c r="B264" s="48"/>
       <c r="C264" s="48"/>
@@ -7634,7 +8044,7 @@
       <c r="N264" s="48"/>
       <c r="O264" s="48"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A265" s="48"/>
       <c r="B265" s="48"/>
       <c r="C265" s="48"/>
@@ -7651,7 +8061,7 @@
       <c r="N265" s="48"/>
       <c r="O265" s="48"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A266" s="48"/>
       <c r="B266" s="48"/>
       <c r="C266" s="48"/>
@@ -7668,7 +8078,7 @@
       <c r="N266" s="48"/>
       <c r="O266" s="48"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A267" s="48"/>
       <c r="B267" s="48"/>
       <c r="C267" s="48"/>
@@ -7685,7 +8095,7 @@
       <c r="N267" s="48"/>
       <c r="O267" s="48"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A268" s="48"/>
       <c r="B268" s="48"/>
       <c r="C268" s="48"/>
@@ -7702,7 +8112,7 @@
       <c r="N268" s="48"/>
       <c r="O268" s="48"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A269" s="48"/>
       <c r="B269" s="48"/>
       <c r="C269" s="48"/>
@@ -7719,7 +8129,7 @@
       <c r="N269" s="48"/>
       <c r="O269" s="48"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A270" s="48"/>
       <c r="B270" s="48"/>
       <c r="C270" s="48"/>
@@ -7736,7 +8146,7 @@
       <c r="N270" s="48"/>
       <c r="O270" s="48"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A271" s="48"/>
       <c r="B271" s="48"/>
       <c r="C271" s="48"/>
@@ -7753,7 +8163,7 @@
       <c r="N271" s="48"/>
       <c r="O271" s="48"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A272" s="48"/>
       <c r="B272" s="48"/>
       <c r="C272" s="48"/>
@@ -7770,7 +8180,7 @@
       <c r="N272" s="48"/>
       <c r="O272" s="48"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A273" s="48"/>
       <c r="B273" s="48"/>
       <c r="C273" s="48"/>
@@ -7787,7 +8197,7 @@
       <c r="N273" s="48"/>
       <c r="O273" s="48"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A274" s="48"/>
       <c r="B274" s="48"/>
       <c r="C274" s="48"/>
@@ -7804,7 +8214,7 @@
       <c r="N274" s="48"/>
       <c r="O274" s="48"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A275" s="48"/>
       <c r="B275" s="48"/>
       <c r="C275" s="48"/>
@@ -7821,7 +8231,7 @@
       <c r="N275" s="48"/>
       <c r="O275" s="48"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A276" s="48"/>
       <c r="B276" s="48"/>
       <c r="C276" s="48"/>
@@ -7838,7 +8248,7 @@
       <c r="N276" s="48"/>
       <c r="O276" s="48"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A277" s="48"/>
       <c r="B277" s="48"/>
       <c r="C277" s="48"/>
@@ -7855,7 +8265,7 @@
       <c r="N277" s="48"/>
       <c r="O277" s="48"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A278" s="48"/>
       <c r="B278" s="48"/>
       <c r="C278" s="48"/>
@@ -7872,7 +8282,7 @@
       <c r="N278" s="48"/>
       <c r="O278" s="48"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A279" s="48"/>
       <c r="B279" s="48"/>
       <c r="C279" s="48"/>
@@ -7889,7 +8299,7 @@
       <c r="N279" s="48"/>
       <c r="O279" s="48"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A280" s="48"/>
       <c r="B280" s="48"/>
       <c r="C280" s="48"/>
@@ -7906,7 +8316,7 @@
       <c r="N280" s="48"/>
       <c r="O280" s="48"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A281" s="48"/>
       <c r="B281" s="48"/>
       <c r="C281" s="48"/>
@@ -7923,7 +8333,7 @@
       <c r="N281" s="48"/>
       <c r="O281" s="48"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A282" s="48"/>
       <c r="B282" s="48"/>
       <c r="C282" s="48"/>
@@ -7940,7 +8350,7 @@
       <c r="N282" s="48"/>
       <c r="O282" s="48"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A283" s="48"/>
       <c r="B283" s="48"/>
       <c r="C283" s="48"/>
@@ -7957,7 +8367,7 @@
       <c r="N283" s="48"/>
       <c r="O283" s="48"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A284" s="48"/>
       <c r="B284" s="48"/>
       <c r="C284" s="48"/>
@@ -7974,7 +8384,7 @@
       <c r="N284" s="48"/>
       <c r="O284" s="48"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A285" s="48"/>
       <c r="B285" s="48"/>
       <c r="C285" s="48"/>
@@ -7991,7 +8401,7 @@
       <c r="N285" s="48"/>
       <c r="O285" s="48"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A286" s="48"/>
       <c r="B286" s="48"/>
       <c r="C286" s="48"/>
@@ -8008,7 +8418,7 @@
       <c r="N286" s="48"/>
       <c r="O286" s="48"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A287" s="48"/>
       <c r="B287" s="48"/>
       <c r="C287" s="48"/>
@@ -8025,7 +8435,7 @@
       <c r="N287" s="48"/>
       <c r="O287" s="48"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A288" s="48"/>
       <c r="B288" s="48"/>
       <c r="C288" s="48"/>
@@ -8042,7 +8452,7 @@
       <c r="N288" s="48"/>
       <c r="O288" s="48"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A289" s="48"/>
       <c r="B289" s="48"/>
       <c r="C289" s="48"/>
@@ -8059,7 +8469,7 @@
       <c r="N289" s="48"/>
       <c r="O289" s="48"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A290" s="48"/>
       <c r="B290" s="48"/>
       <c r="C290" s="48"/>
@@ -8076,7 +8486,7 @@
       <c r="N290" s="48"/>
       <c r="O290" s="48"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A291" s="48"/>
       <c r="B291" s="48"/>
       <c r="C291" s="48"/>
@@ -8093,7 +8503,7 @@
       <c r="N291" s="48"/>
       <c r="O291" s="48"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A292" s="48"/>
       <c r="B292" s="48"/>
       <c r="C292" s="48"/>
@@ -8110,7 +8520,7 @@
       <c r="N292" s="48"/>
       <c r="O292" s="48"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A293" s="48"/>
       <c r="B293" s="48"/>
       <c r="C293" s="48"/>
@@ -8127,7 +8537,7 @@
       <c r="N293" s="48"/>
       <c r="O293" s="48"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A294" s="48"/>
       <c r="B294" s="48"/>
       <c r="C294" s="48"/>
@@ -8144,7 +8554,7 @@
       <c r="N294" s="48"/>
       <c r="O294" s="48"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A295" s="48"/>
       <c r="B295" s="48"/>
       <c r="C295" s="48"/>
@@ -8161,7 +8571,7 @@
       <c r="N295" s="48"/>
       <c r="O295" s="48"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A296" s="48"/>
       <c r="B296" s="48"/>
       <c r="C296" s="48"/>
@@ -8178,7 +8588,7 @@
       <c r="N296" s="48"/>
       <c r="O296" s="48"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A297" s="48"/>
       <c r="B297" s="48"/>
       <c r="C297" s="48"/>
@@ -8195,7 +8605,7 @@
       <c r="N297" s="48"/>
       <c r="O297" s="48"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A298" s="48"/>
       <c r="B298" s="48"/>
       <c r="C298" s="48"/>
@@ -8212,7 +8622,7 @@
       <c r="N298" s="48"/>
       <c r="O298" s="48"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A299" s="48"/>
       <c r="B299" s="48"/>
       <c r="C299" s="48"/>
@@ -8229,7 +8639,7 @@
       <c r="N299" s="48"/>
       <c r="O299" s="48"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A300" s="48"/>
       <c r="B300" s="48"/>
       <c r="C300" s="48"/>
@@ -8246,7 +8656,7 @@
       <c r="N300" s="48"/>
       <c r="O300" s="48"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A301" s="48"/>
       <c r="B301" s="48"/>
       <c r="C301" s="48"/>
@@ -8263,7 +8673,7 @@
       <c r="N301" s="48"/>
       <c r="O301" s="48"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A302" s="48"/>
       <c r="B302" s="48"/>
       <c r="C302" s="48"/>
@@ -8280,7 +8690,7 @@
       <c r="N302" s="48"/>
       <c r="O302" s="48"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A303" s="48"/>
       <c r="B303" s="48"/>
       <c r="C303" s="48"/>
@@ -8297,7 +8707,7 @@
       <c r="N303" s="48"/>
       <c r="O303" s="48"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A304" s="48"/>
       <c r="B304" s="48"/>
       <c r="C304" s="48"/>
@@ -8314,7 +8724,7 @@
       <c r="N304" s="48"/>
       <c r="O304" s="48"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A305" s="48"/>
       <c r="B305" s="48"/>
       <c r="C305" s="48"/>
@@ -8331,7 +8741,7 @@
       <c r="N305" s="48"/>
       <c r="O305" s="48"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A306" s="48"/>
       <c r="B306" s="48"/>
       <c r="C306" s="48"/>
@@ -8348,7 +8758,7 @@
       <c r="N306" s="48"/>
       <c r="O306" s="48"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A307" s="48"/>
       <c r="B307" s="48"/>
       <c r="C307" s="48"/>
@@ -8365,7 +8775,7 @@
       <c r="N307" s="48"/>
       <c r="O307" s="48"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A308" s="48"/>
       <c r="B308" s="48"/>
       <c r="C308" s="48"/>
@@ -8382,7 +8792,7 @@
       <c r="N308" s="48"/>
       <c r="O308" s="48"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A309" s="48"/>
       <c r="B309" s="48"/>
       <c r="C309" s="48"/>
@@ -8399,7 +8809,7 @@
       <c r="N309" s="48"/>
       <c r="O309" s="48"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A310" s="48"/>
       <c r="B310" s="48"/>
       <c r="C310" s="48"/>
@@ -8416,7 +8826,7 @@
       <c r="N310" s="48"/>
       <c r="O310" s="48"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A311" s="48"/>
       <c r="B311" s="48"/>
       <c r="C311" s="48"/>
@@ -8433,7 +8843,7 @@
       <c r="N311" s="48"/>
       <c r="O311" s="48"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A312" s="48"/>
       <c r="B312" s="48"/>
       <c r="C312" s="48"/>
@@ -8450,7 +8860,7 @@
       <c r="N312" s="48"/>
       <c r="O312" s="48"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A313" s="48"/>
       <c r="B313" s="48"/>
       <c r="C313" s="48"/>
@@ -8467,7 +8877,7 @@
       <c r="N313" s="48"/>
       <c r="O313" s="48"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A314" s="48"/>
       <c r="B314" s="48"/>
       <c r="C314" s="48"/>
@@ -8484,7 +8894,7 @@
       <c r="N314" s="48"/>
       <c r="O314" s="48"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A315" s="48"/>
       <c r="B315" s="48"/>
       <c r="C315" s="48"/>
@@ -8501,7 +8911,7 @@
       <c r="N315" s="48"/>
       <c r="O315" s="48"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A316" s="48"/>
       <c r="B316" s="48"/>
       <c r="C316" s="48"/>
@@ -8518,7 +8928,7 @@
       <c r="N316" s="48"/>
       <c r="O316" s="48"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A317" s="48"/>
       <c r="B317" s="48"/>
       <c r="C317" s="48"/>
@@ -8535,7 +8945,7 @@
       <c r="N317" s="48"/>
       <c r="O317" s="48"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A318" s="48"/>
       <c r="B318" s="48"/>
       <c r="C318" s="48"/>
@@ -8552,7 +8962,7 @@
       <c r="N318" s="48"/>
       <c r="O318" s="48"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A319" s="48"/>
       <c r="B319" s="48"/>
       <c r="C319" s="48"/>
@@ -8569,7 +8979,7 @@
       <c r="N319" s="48"/>
       <c r="O319" s="48"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A320" s="48"/>
       <c r="B320" s="48"/>
       <c r="C320" s="48"/>
@@ -8586,7 +8996,7 @@
       <c r="N320" s="48"/>
       <c r="O320" s="48"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A321" s="48"/>
       <c r="B321" s="48"/>
       <c r="C321" s="48"/>
@@ -8603,7 +9013,7 @@
       <c r="N321" s="48"/>
       <c r="O321" s="48"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A322" s="48"/>
       <c r="B322" s="48"/>
       <c r="C322" s="48"/>
@@ -8620,7 +9030,7 @@
       <c r="N322" s="48"/>
       <c r="O322" s="48"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A323" s="48"/>
       <c r="B323" s="48"/>
       <c r="C323" s="48"/>
@@ -8637,7 +9047,7 @@
       <c r="N323" s="48"/>
       <c r="O323" s="48"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A324" s="48"/>
       <c r="B324" s="48"/>
       <c r="C324" s="48"/>
@@ -8654,7 +9064,7 @@
       <c r="N324" s="48"/>
       <c r="O324" s="48"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A325" s="48"/>
       <c r="B325" s="48"/>
       <c r="C325" s="48"/>
@@ -8671,7 +9081,7 @@
       <c r="N325" s="48"/>
       <c r="O325" s="48"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A326" s="48"/>
       <c r="B326" s="48"/>
       <c r="C326" s="48"/>
@@ -8688,7 +9098,7 @@
       <c r="N326" s="48"/>
       <c r="O326" s="48"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A327" s="48"/>
       <c r="B327" s="48"/>
       <c r="C327" s="48"/>
@@ -8705,7 +9115,7 @@
       <c r="N327" s="48"/>
       <c r="O327" s="48"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A328" s="48"/>
       <c r="B328" s="48"/>
       <c r="C328" s="48"/>
@@ -8722,7 +9132,7 @@
       <c r="N328" s="48"/>
       <c r="O328" s="48"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A329" s="48"/>
       <c r="B329" s="48"/>
       <c r="C329" s="48"/>
@@ -8739,7 +9149,7 @@
       <c r="N329" s="48"/>
       <c r="O329" s="48"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A330" s="48"/>
       <c r="B330" s="48"/>
       <c r="C330" s="48"/>
@@ -8756,7 +9166,7 @@
       <c r="N330" s="48"/>
       <c r="O330" s="48"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A331" s="48"/>
       <c r="B331" s="48"/>
       <c r="C331" s="48"/>
@@ -8773,7 +9183,7 @@
       <c r="N331" s="48"/>
       <c r="O331" s="48"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A332" s="48"/>
       <c r="B332" s="48"/>
       <c r="C332" s="48"/>
@@ -8790,7 +9200,7 @@
       <c r="N332" s="48"/>
       <c r="O332" s="48"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A333" s="48"/>
       <c r="B333" s="48"/>
       <c r="C333" s="48"/>
@@ -8807,7 +9217,7 @@
       <c r="N333" s="48"/>
       <c r="O333" s="48"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A334" s="48"/>
       <c r="B334" s="48"/>
       <c r="C334" s="48"/>
@@ -8824,7 +9234,7 @@
       <c r="N334" s="48"/>
       <c r="O334" s="48"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A335" s="48"/>
       <c r="B335" s="48"/>
       <c r="C335" s="48"/>
@@ -8841,7 +9251,7 @@
       <c r="N335" s="48"/>
       <c r="O335" s="48"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A336" s="48"/>
       <c r="B336" s="48"/>
       <c r="C336" s="48"/>
@@ -8858,7 +9268,7 @@
       <c r="N336" s="48"/>
       <c r="O336" s="48"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A337" s="48"/>
       <c r="B337" s="48"/>
       <c r="C337" s="48"/>
@@ -8875,7 +9285,7 @@
       <c r="N337" s="48"/>
       <c r="O337" s="48"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A338" s="48"/>
       <c r="B338" s="48"/>
       <c r="C338" s="48"/>
@@ -8892,7 +9302,7 @@
       <c r="N338" s="48"/>
       <c r="O338" s="48"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A339" s="48"/>
       <c r="B339" s="48"/>
       <c r="C339" s="48"/>
@@ -8909,7 +9319,7 @@
       <c r="N339" s="48"/>
       <c r="O339" s="48"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A340" s="48"/>
       <c r="B340" s="48"/>
       <c r="C340" s="48"/>
@@ -8926,7 +9336,7 @@
       <c r="N340" s="48"/>
       <c r="O340" s="48"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A341" s="48"/>
       <c r="B341" s="48"/>
       <c r="C341" s="48"/>
@@ -8943,7 +9353,7 @@
       <c r="N341" s="48"/>
       <c r="O341" s="48"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A342" s="48"/>
       <c r="B342" s="48"/>
       <c r="C342" s="48"/>
@@ -8960,7 +9370,7 @@
       <c r="N342" s="48"/>
       <c r="O342" s="48"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A343" s="48"/>
       <c r="B343" s="48"/>
       <c r="C343" s="48"/>
@@ -8977,7 +9387,7 @@
       <c r="N343" s="48"/>
       <c r="O343" s="48"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A344" s="48"/>
       <c r="B344" s="48"/>
       <c r="C344" s="48"/>
@@ -8994,7 +9404,7 @@
       <c r="N344" s="48"/>
       <c r="O344" s="48"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A345" s="48"/>
       <c r="B345" s="48"/>
       <c r="C345" s="48"/>
@@ -9011,7 +9421,7 @@
       <c r="N345" s="48"/>
       <c r="O345" s="48"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A346" s="48"/>
       <c r="B346" s="48"/>
       <c r="C346" s="48"/>
@@ -9034,14 +9444,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
@@ -9232,7 +9642,7 @@
       <c r="J16" s="48"/>
       <c r="K16" s="48"/>
     </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="48"/>
       <c r="B17" s="48"/>
       <c r="C17" s="48"/>
@@ -9245,7 +9655,7 @@
       <c r="J17" s="48"/>
       <c r="K17" s="48"/>
     </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="48"/>
       <c r="B18" s="48"/>
       <c r="C18" s="48"/>
@@ -9258,7 +9668,7 @@
       <c r="J18" s="48"/>
       <c r="K18" s="48"/>
     </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="48"/>
       <c r="B19" s="48"/>
       <c r="C19" s="48"/>

</xml_diff>

<commit_message>
fixed a bug on the ObjectiveViewImpl and added effort to scrum.xlsx
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1660" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="40000" yWindow="-9680" windowWidth="28800" windowHeight="17540" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -1134,30 +1134,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1229,6 +1205,30 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1936,7 +1936,7 @@
   <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2035,56 +2035,56 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="82" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
+    <row r="3" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="80" t="s">
+      <c r="B3" s="71"/>
+      <c r="C3" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="80" t="s">
+      <c r="D3" s="73"/>
+      <c r="E3" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80">
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72">
         <v>0</v>
       </c>
-      <c r="L3" s="80" t="s">
+      <c r="L3" s="72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="86" customFormat="1" ht="90" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="s">
+    <row r="4" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+      <c r="A4" s="79" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="88">
+      <c r="B4" s="80">
         <v>3</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="78" t="s">
         <v>186</v>
       </c>
-      <c r="D4" s="89" t="s">
+      <c r="D4" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="86" t="s">
+      <c r="H4" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="86">
+      <c r="J4" s="78">
         <v>0</v>
       </c>
-      <c r="K4" s="86">
+      <c r="K4" s="78">
         <v>0</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="78" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2126,103 +2126,103 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A6" s="87" t="s">
+    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A6" s="79" t="s">
         <v>219</v>
       </c>
-      <c r="B6" s="88">
+      <c r="B6" s="80">
         <v>3</v>
       </c>
-      <c r="C6" s="86" t="s">
+      <c r="C6" s="78" t="s">
         <v>185</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="E6" s="90" t="s">
+      <c r="E6" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="86" t="s">
+      <c r="G6" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="86">
+      <c r="I6" s="78">
         <v>4</v>
       </c>
-      <c r="J6" s="86">
+      <c r="J6" s="78">
         <v>0</v>
       </c>
-      <c r="K6" s="86">
+      <c r="K6" s="78">
         <v>0</v>
       </c>
-      <c r="L6" s="86" t="s">
+      <c r="L6" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="82" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="83">
+    <row r="7" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="75">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B7" s="84"/>
-      <c r="C7" s="82" t="s">
+      <c r="B7" s="76"/>
+      <c r="C7" s="74" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="82" t="s">
+      <c r="D7" s="77"/>
+      <c r="E7" s="74" t="s">
         <v>91</v>
       </c>
-      <c r="K7" s="82">
+      <c r="K7" s="74">
         <v>0</v>
       </c>
-      <c r="L7" s="82" t="s">
+      <c r="L7" s="74" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="82" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="83">
+    <row r="8" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="75">
         <v>1.2</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="82" t="s">
+      <c r="B8" s="76"/>
+      <c r="C8" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="82" t="s">
+      <c r="D8" s="77"/>
+      <c r="E8" s="74" t="s">
         <v>95</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="74">
         <v>0</v>
       </c>
-      <c r="L8" s="82" t="s">
+      <c r="L8" s="74" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="82" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="78">
+    <row r="9" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="70">
         <v>1.3</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="80" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="72" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="80" t="s">
+      <c r="D9" s="73"/>
+      <c r="E9" s="72" t="s">
         <v>94</v>
       </c>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80">
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72">
         <v>0</v>
       </c>
-      <c r="L9" s="80" t="s">
+      <c r="L9" s="72" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2355,22 +2355,22 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="100" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="98">
+    <row r="14" spans="1:12" s="92" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="90">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100" t="s">
+      <c r="B14" s="91"/>
+      <c r="C14" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="101"/>
-      <c r="H14" s="100" t="s">
+      <c r="D14" s="93"/>
+      <c r="H14" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="K14" s="100">
+      <c r="K14" s="92">
         <v>0</v>
       </c>
-      <c r="L14" s="80" t="s">
+      <c r="L14" s="72" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2959,449 +2959,449 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A31" s="87" t="s">
+    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A31" s="79" t="s">
         <v>221</v>
       </c>
-      <c r="B31" s="88">
+      <c r="B31" s="80">
         <v>3</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="D31" s="89" t="s">
+      <c r="D31" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="E31" s="90" t="s">
+      <c r="E31" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="F31" s="86" t="s">
+      <c r="F31" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="86" t="s">
+      <c r="G31" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="86" t="s">
+      <c r="H31" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I31" s="86">
+      <c r="I31" s="78">
         <v>3</v>
       </c>
-      <c r="J31" s="86">
+      <c r="J31" s="78">
+        <v>3</v>
+      </c>
+      <c r="K31" s="78">
+        <v>3</v>
+      </c>
+      <c r="L31" s="78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A32" s="79" t="s">
+        <v>220</v>
+      </c>
+      <c r="B32" s="80">
+        <v>3</v>
+      </c>
+      <c r="C32" s="78" t="s">
+        <v>172</v>
+      </c>
+      <c r="D32" s="81" t="s">
+        <v>194</v>
+      </c>
+      <c r="E32" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="G32" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="78">
+        <v>3</v>
+      </c>
+      <c r="J32" s="78">
+        <v>3</v>
+      </c>
+      <c r="K32" s="78">
+        <v>3</v>
+      </c>
+      <c r="L32" s="78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A33" s="79" t="s">
+        <v>222</v>
+      </c>
+      <c r="B33" s="80">
+        <v>3</v>
+      </c>
+      <c r="C33" s="78" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="81" t="s">
+        <v>196</v>
+      </c>
+      <c r="E33" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="78" t="s">
+        <v>24</v>
+      </c>
+      <c r="G33" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="78">
+        <v>2</v>
+      </c>
+      <c r="J33" s="78">
         <v>0</v>
       </c>
-      <c r="K31" s="86">
+      <c r="K33" s="78">
         <v>0</v>
       </c>
-      <c r="L31" s="86" t="s">
+      <c r="L33" s="78" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A32" s="87" t="s">
-        <v>220</v>
-      </c>
-      <c r="B32" s="88">
+    <row r="34" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A34" s="79" t="s">
+        <v>223</v>
+      </c>
+      <c r="B34" s="80">
         <v>3</v>
       </c>
-      <c r="C32" s="86" t="s">
-        <v>172</v>
-      </c>
-      <c r="D32" s="89" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="90" t="s">
+      <c r="C34" s="78" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="81" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="F32" s="86" t="s">
+      <c r="F34" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="G34" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="78">
+        <v>4</v>
+      </c>
+      <c r="J34" s="78">
+        <v>0</v>
+      </c>
+      <c r="K34" s="78">
+        <v>0</v>
+      </c>
+      <c r="L34" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="B35" s="80">
+        <v>3</v>
+      </c>
+      <c r="C35" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="D35" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="E35" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="G35" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I35" s="78">
+        <v>4</v>
+      </c>
+      <c r="J35" s="78">
+        <v>0</v>
+      </c>
+      <c r="K35" s="78">
+        <v>0</v>
+      </c>
+      <c r="L35" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="79" t="s">
+        <v>225</v>
+      </c>
+      <c r="B36" s="80">
+        <v>3</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" s="81" t="s">
+        <v>199</v>
+      </c>
+      <c r="E36" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="78" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G32" s="86" t="s">
+      <c r="H36" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="78">
+        <v>3</v>
+      </c>
+      <c r="J36" s="78">
+        <v>0</v>
+      </c>
+      <c r="K36" s="78">
+        <v>0</v>
+      </c>
+      <c r="L36" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A37" s="79"/>
+      <c r="B37" s="80">
+        <v>3</v>
+      </c>
+      <c r="C37" s="82" t="s">
+        <v>177</v>
+      </c>
+      <c r="D37" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="E37" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="78" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="78">
+        <v>4</v>
+      </c>
+      <c r="J37" s="78">
+        <v>0</v>
+      </c>
+      <c r="K37" s="78">
+        <v>0</v>
+      </c>
+      <c r="L37" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A38" s="79"/>
+      <c r="B38" s="80">
+        <v>3</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>180</v>
+      </c>
+      <c r="D38" s="81" t="s">
+        <v>203</v>
+      </c>
+      <c r="E38" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F38" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="86" t="s">
+      <c r="G38" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="H38" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="86">
+      <c r="I38" s="78">
+        <v>4</v>
+      </c>
+      <c r="J38" s="78">
+        <v>0</v>
+      </c>
+      <c r="K38" s="78">
+        <v>0</v>
+      </c>
+      <c r="L38" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A39" s="79" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="80">
         <v>3</v>
       </c>
-      <c r="J32" s="86">
+      <c r="C39" s="78" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="81" t="s">
+        <v>204</v>
+      </c>
+      <c r="E39" s="82" t="s">
+        <v>86</v>
+      </c>
+      <c r="F39" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="H39" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" s="78">
+        <v>2</v>
+      </c>
+      <c r="J39" s="78">
         <v>0</v>
       </c>
-      <c r="K32" s="86">
+      <c r="K39" s="78">
         <v>0</v>
       </c>
-      <c r="L32" s="86" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A33" s="87" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" s="88">
+      <c r="L39" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A40" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" s="80">
         <v>3</v>
       </c>
-      <c r="C33" s="86" t="s">
-        <v>173</v>
-      </c>
-      <c r="D33" s="89" t="s">
-        <v>196</v>
-      </c>
-      <c r="E33" s="90" t="s">
+      <c r="C40" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="81" t="s">
+        <v>205</v>
+      </c>
+      <c r="E40" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="F33" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="G33" s="86" t="s">
+      <c r="F40" s="78" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="78">
+        <v>4</v>
+      </c>
+      <c r="J40" s="78">
+        <v>0</v>
+      </c>
+      <c r="K40" s="78">
+        <v>0</v>
+      </c>
+      <c r="L40" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A41" s="79" t="s">
+        <v>214</v>
+      </c>
+      <c r="B41" s="80">
+        <v>3</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" s="81" t="s">
+        <v>206</v>
+      </c>
+      <c r="E41" s="82" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H33" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I33" s="86">
-        <v>2</v>
-      </c>
-      <c r="J33" s="86">
+      <c r="G41" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="H41" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I41" s="78">
+        <v>3</v>
+      </c>
+      <c r="J41" s="78">
         <v>0</v>
       </c>
-      <c r="K33" s="86">
+      <c r="K41" s="78">
         <v>0</v>
       </c>
-      <c r="L33" s="86" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A34" s="87" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" s="88">
+      <c r="L41" s="78" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A42" s="79" t="s">
+        <v>215</v>
+      </c>
+      <c r="B42" s="80">
         <v>3</v>
       </c>
-      <c r="C34" s="86" t="s">
-        <v>175</v>
-      </c>
-      <c r="D34" s="89" t="s">
-        <v>197</v>
-      </c>
-      <c r="E34" s="90" t="s">
+      <c r="C42" s="78" t="s">
+        <v>182</v>
+      </c>
+      <c r="D42" s="81" t="s">
+        <v>207</v>
+      </c>
+      <c r="E42" s="82" t="s">
         <v>92</v>
       </c>
-      <c r="F34" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="G34" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="H34" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I34" s="86">
+      <c r="H42" s="78" t="s">
+        <v>6</v>
+      </c>
+      <c r="I42" s="78">
         <v>4</v>
       </c>
-      <c r="J34" s="86">
+      <c r="J42" s="78">
         <v>0</v>
       </c>
-      <c r="K34" s="86">
+      <c r="K42" s="78">
         <v>0</v>
       </c>
-      <c r="L34" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="86" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="87" t="s">
-        <v>224</v>
-      </c>
-      <c r="B35" s="88">
-        <v>3</v>
-      </c>
-      <c r="C35" s="86" t="s">
-        <v>178</v>
-      </c>
-      <c r="D35" s="89" t="s">
-        <v>198</v>
-      </c>
-      <c r="E35" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" s="86">
-        <v>4</v>
-      </c>
-      <c r="J35" s="86">
-        <v>0</v>
-      </c>
-      <c r="K35" s="86">
-        <v>0</v>
-      </c>
-      <c r="L35" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="86" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="87" t="s">
-        <v>225</v>
-      </c>
-      <c r="B36" s="88">
-        <v>3</v>
-      </c>
-      <c r="C36" s="86" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="89" t="s">
-        <v>199</v>
-      </c>
-      <c r="E36" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="G36" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="H36" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I36" s="86">
-        <v>3</v>
-      </c>
-      <c r="J36" s="86">
-        <v>0</v>
-      </c>
-      <c r="K36" s="86">
-        <v>0</v>
-      </c>
-      <c r="L36" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A37" s="87"/>
-      <c r="B37" s="88">
-        <v>3</v>
-      </c>
-      <c r="C37" s="90" t="s">
-        <v>177</v>
-      </c>
-      <c r="D37" s="89" t="s">
-        <v>202</v>
-      </c>
-      <c r="E37" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="G37" s="86" t="s">
-        <v>78</v>
-      </c>
-      <c r="H37" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" s="86">
-        <v>4</v>
-      </c>
-      <c r="J37" s="86">
-        <v>0</v>
-      </c>
-      <c r="K37" s="86">
-        <v>0</v>
-      </c>
-      <c r="L37" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A38" s="87"/>
-      <c r="B38" s="88">
-        <v>3</v>
-      </c>
-      <c r="C38" s="86" t="s">
-        <v>180</v>
-      </c>
-      <c r="D38" s="89" t="s">
-        <v>203</v>
-      </c>
-      <c r="E38" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F38" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="H38" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I38" s="86">
-        <v>4</v>
-      </c>
-      <c r="J38" s="86">
-        <v>0</v>
-      </c>
-      <c r="K38" s="86">
-        <v>0</v>
-      </c>
-      <c r="L38" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A39" s="87" t="s">
-        <v>212</v>
-      </c>
-      <c r="B39" s="88">
-        <v>3</v>
-      </c>
-      <c r="C39" s="86" t="s">
-        <v>195</v>
-      </c>
-      <c r="D39" s="89" t="s">
-        <v>204</v>
-      </c>
-      <c r="E39" s="90" t="s">
-        <v>86</v>
-      </c>
-      <c r="F39" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="H39" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I39" s="86">
-        <v>2</v>
-      </c>
-      <c r="J39" s="86">
-        <v>0</v>
-      </c>
-      <c r="K39" s="86">
-        <v>0</v>
-      </c>
-      <c r="L39" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A40" s="87" t="s">
-        <v>213</v>
-      </c>
-      <c r="B40" s="88">
-        <v>3</v>
-      </c>
-      <c r="C40" s="86" t="s">
-        <v>181</v>
-      </c>
-      <c r="D40" s="89" t="s">
-        <v>205</v>
-      </c>
-      <c r="E40" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="86" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="I40" s="86">
-        <v>4</v>
-      </c>
-      <c r="J40" s="86">
-        <v>0</v>
-      </c>
-      <c r="K40" s="86">
-        <v>0</v>
-      </c>
-      <c r="L40" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A41" s="87" t="s">
-        <v>214</v>
-      </c>
-      <c r="B41" s="88">
-        <v>3</v>
-      </c>
-      <c r="C41" s="86" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="89" t="s">
-        <v>206</v>
-      </c>
-      <c r="E41" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="86" t="s">
-        <v>28</v>
-      </c>
-      <c r="G41" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="H41" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="I41" s="86">
-        <v>3</v>
-      </c>
-      <c r="J41" s="86">
-        <v>0</v>
-      </c>
-      <c r="K41" s="86">
-        <v>0</v>
-      </c>
-      <c r="L41" s="86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A42" s="87" t="s">
-        <v>215</v>
-      </c>
-      <c r="B42" s="88">
-        <v>3</v>
-      </c>
-      <c r="C42" s="86" t="s">
-        <v>182</v>
-      </c>
-      <c r="D42" s="89" t="s">
-        <v>207</v>
-      </c>
-      <c r="E42" s="90" t="s">
-        <v>92</v>
-      </c>
-      <c r="H42" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="I42" s="86">
-        <v>4</v>
-      </c>
-      <c r="J42" s="86">
-        <v>0</v>
-      </c>
-      <c r="K42" s="86">
-        <v>0</v>
-      </c>
-      <c r="L42" s="86" t="s">
+      <c r="L42" s="78" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3557,191 +3557,191 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A47" s="87" t="s">
+    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="B47" s="88">
+      <c r="B47" s="80">
         <v>3</v>
       </c>
-      <c r="C47" s="86" t="s">
+      <c r="C47" s="78" t="s">
         <v>183</v>
       </c>
-      <c r="D47" s="89" t="s">
+      <c r="D47" s="81" t="s">
         <v>208</v>
       </c>
-      <c r="E47" s="90" t="s">
+      <c r="E47" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="F47" s="86" t="s">
+      <c r="F47" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G47" s="86" t="s">
+      <c r="G47" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="H47" s="86" t="s">
+      <c r="H47" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I47" s="86">
+      <c r="I47" s="78">
         <v>4</v>
       </c>
-      <c r="J47" s="86">
+      <c r="J47" s="78">
         <v>0</v>
       </c>
-      <c r="K47" s="86">
+      <c r="K47" s="78">
         <v>0</v>
       </c>
-      <c r="L47" s="86" t="s">
+      <c r="L47" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="86" customFormat="1" ht="30" x14ac:dyDescent="0.2">
-      <c r="A48" s="87" t="s">
+    <row r="48" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+      <c r="A48" s="79" t="s">
         <v>218</v>
       </c>
-      <c r="B48" s="88">
+      <c r="B48" s="80">
         <v>3</v>
       </c>
-      <c r="C48" s="86" t="s">
+      <c r="C48" s="78" t="s">
         <v>183</v>
       </c>
-      <c r="D48" s="89" t="s">
+      <c r="D48" s="81" t="s">
         <v>208</v>
       </c>
-      <c r="E48" s="90" t="s">
+      <c r="E48" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="F48" s="86" t="s">
+      <c r="F48" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="G48" s="86" t="s">
+      <c r="G48" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="H48" s="86" t="s">
+      <c r="H48" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I48" s="86">
+      <c r="I48" s="78">
         <v>4</v>
       </c>
-      <c r="J48" s="86">
+      <c r="J48" s="78">
         <v>0</v>
       </c>
-      <c r="K48" s="86">
+      <c r="K48" s="78">
         <v>0</v>
       </c>
-      <c r="L48" s="86" t="s">
+      <c r="L48" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A49" s="87" t="s">
+    <row r="49" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A49" s="79" t="s">
         <v>217</v>
       </c>
-      <c r="B49" s="88">
+      <c r="B49" s="80">
         <v>3</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C49" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="D49" s="89" t="s">
+      <c r="D49" s="81" t="s">
         <v>209</v>
       </c>
-      <c r="E49" s="90" t="s">
+      <c r="E49" s="82" t="s">
         <v>187</v>
       </c>
-      <c r="F49" s="86" t="s">
+      <c r="F49" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G49" s="86" t="s">
+      <c r="G49" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="H49" s="86" t="s">
+      <c r="H49" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="I49" s="86">
+      <c r="I49" s="78">
         <v>2</v>
       </c>
-      <c r="J49" s="86">
+      <c r="J49" s="78">
         <v>0</v>
       </c>
-      <c r="K49" s="86">
+      <c r="K49" s="78">
         <v>0</v>
       </c>
-      <c r="L49" s="86" t="s">
+      <c r="L49" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="86" customFormat="1" ht="45" x14ac:dyDescent="0.2">
-      <c r="A50" s="91" t="s">
+    <row r="50" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+      <c r="A50" s="83" t="s">
         <v>216</v>
       </c>
-      <c r="B50" s="92">
+      <c r="B50" s="84">
         <v>3</v>
       </c>
-      <c r="C50" s="90" t="s">
+      <c r="C50" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="D50" s="93" t="s">
+      <c r="D50" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="90" t="s">
+      <c r="E50" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="F50" s="90" t="s">
+      <c r="F50" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="G50" s="90" t="s">
+      <c r="G50" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="H50" s="90" t="s">
+      <c r="H50" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="I50" s="90">
+      <c r="I50" s="82">
         <v>5</v>
       </c>
-      <c r="J50" s="86">
+      <c r="J50" s="78">
         <v>0</v>
       </c>
-      <c r="K50" s="86">
+      <c r="K50" s="78">
         <v>0</v>
       </c>
-      <c r="L50" s="90" t="s">
+      <c r="L50" s="82" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="96" customFormat="1" ht="75" x14ac:dyDescent="0.2">
-      <c r="A51" s="94"/>
-      <c r="B51" s="95">
+    <row r="51" spans="1:17" s="88" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+      <c r="A51" s="86"/>
+      <c r="B51" s="87">
         <v>3</v>
       </c>
-      <c r="C51" s="96" t="s">
+      <c r="C51" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="D51" s="97" t="s">
+      <c r="D51" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="E51" s="96" t="s">
+      <c r="E51" s="88" t="s">
         <v>192</v>
       </c>
-      <c r="F51" s="96" t="s">
+      <c r="F51" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="G51" s="96" t="s">
+      <c r="G51" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="H51" s="96" t="s">
+      <c r="H51" s="88" t="s">
         <v>5</v>
       </c>
-      <c r="I51" s="96">
+      <c r="I51" s="88">
         <v>3</v>
       </c>
-      <c r="J51" s="96">
+      <c r="J51" s="88">
         <v>0</v>
       </c>
-      <c r="K51" s="96">
+      <c r="K51" s="88">
         <v>0</v>
       </c>
-      <c r="L51" s="90" t="s">
+      <c r="L51" s="82" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3802,12 +3802,12 @@
       <c r="B54" s="17"/>
       <c r="C54" s="18"/>
       <c r="D54" s="19"/>
-      <c r="L54" s="77"/>
-      <c r="M54" s="77"/>
-      <c r="N54" s="77"/>
-      <c r="O54" s="77"/>
-      <c r="P54" s="77"/>
-      <c r="Q54" s="77"/>
+      <c r="L54" s="94"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="94"/>
+      <c r="O54" s="94"/>
+      <c r="P54" s="94"/>
+      <c r="Q54" s="94"/>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E55" s="18"/>
@@ -3829,10 +3829,10 @@
       <c r="E56" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="G56" s="77" t="s">
+      <c r="G56" s="94" t="s">
         <v>148</v>
       </c>
-      <c r="H56" s="77"/>
+      <c r="H56" s="94"/>
       <c r="I56" s="1">
         <f>SUMIF(B2:B52,1,I2:I52)</f>
         <v>54</v>
@@ -3850,10 +3850,10 @@
       <c r="E57" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="G57" s="77" t="s">
+      <c r="G57" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="H57" s="77"/>
+      <c r="H57" s="94"/>
       <c r="I57" s="1">
         <f>SUMIF(B2:B52,2,I2:I52)</f>
         <v>81</v>
@@ -3871,35 +3871,35 @@
       <c r="E58" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="G58" s="77" t="s">
+      <c r="G58" s="94" t="s">
         <v>150</v>
       </c>
-      <c r="H58" s="77"/>
+      <c r="H58" s="94"/>
       <c r="I58" s="1">
         <f>SUMIF(B2:B52,3,I2:I52)</f>
         <v>62</v>
       </c>
       <c r="J58" s="1">
         <f>SUMIF(B2:B52,3,J2:J52)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K58" s="1">
         <f>SUMIF(B2:B52,3,K2:K52)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G62" s="70" t="s">
+      <c r="G62" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="H62" s="71"/>
-      <c r="I62" s="71"/>
-      <c r="J62" s="71"/>
-      <c r="K62" s="71"/>
-      <c r="L62" s="71"/>
-      <c r="M62" s="71"/>
-      <c r="N62" s="72"/>
+      <c r="H62" s="100"/>
+      <c r="I62" s="100"/>
+      <c r="J62" s="100"/>
+      <c r="K62" s="100"/>
+      <c r="L62" s="100"/>
+      <c r="M62" s="100"/>
+      <c r="N62" s="101"/>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="G63" s="66"/>
@@ -3924,10 +3924,10 @@
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="G64" s="73" t="s">
+      <c r="G64" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="H64" s="74"/>
+      <c r="H64" s="96"/>
       <c r="I64" s="18">
         <f>SUMIFS(I$2:I$52,$B$2:$B$52,1,$F$2:$F$52,"gfels6")</f>
         <v>9</v>
@@ -3954,10 +3954,10 @@
       </c>
     </row>
     <row r="65" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G65" s="73" t="s">
+      <c r="G65" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="H65" s="74"/>
+      <c r="H65" s="96"/>
       <c r="I65" s="18">
         <f>SUMIFS(I$2:I$52,$B$2:$B$52,2,$F$2:$F$52,"gfels6")</f>
         <v>17</v>
@@ -3984,10 +3984,10 @@
       </c>
     </row>
     <row r="66" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G66" s="75" t="s">
+      <c r="G66" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="H66" s="76"/>
+      <c r="H66" s="98"/>
       <c r="I66" s="68">
         <f>SUMIFS(I$2:I$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
         <v>14</v>
@@ -4015,16 +4015,16 @@
     </row>
     <row r="67" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G68" s="70" t="s">
+      <c r="G68" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="H68" s="71"/>
-      <c r="I68" s="71"/>
-      <c r="J68" s="71"/>
-      <c r="K68" s="71"/>
-      <c r="L68" s="71"/>
-      <c r="M68" s="71"/>
-      <c r="N68" s="72"/>
+      <c r="H68" s="100"/>
+      <c r="I68" s="100"/>
+      <c r="J68" s="100"/>
+      <c r="K68" s="100"/>
+      <c r="L68" s="100"/>
+      <c r="M68" s="100"/>
+      <c r="N68" s="101"/>
     </row>
     <row r="69" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G69" s="66"/>
@@ -4049,10 +4049,10 @@
       </c>
     </row>
     <row r="70" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G70" s="73" t="s">
+      <c r="G70" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="H70" s="74"/>
+      <c r="H70" s="96"/>
       <c r="I70" s="18">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,1,$F$2:$F$52,"gfels6")</f>
         <v>11</v>
@@ -4079,10 +4079,10 @@
       </c>
     </row>
     <row r="71" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G71" s="73" t="s">
+      <c r="G71" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="H71" s="74"/>
+      <c r="H71" s="96"/>
       <c r="I71" s="18">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,2,$F$2:$F$52,"gfels6")</f>
         <v>16</v>
@@ -4109,10 +4109,10 @@
       </c>
     </row>
     <row r="72" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G72" s="75" t="s">
+      <c r="G72" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="H72" s="76"/>
+      <c r="H72" s="98"/>
       <c r="I72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
         <v>0</v>
@@ -4123,7 +4123,7 @@
       </c>
       <c r="K72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"jntme")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"kybup1")</f>
@@ -4140,16 +4140,16 @@
     </row>
     <row r="73" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G74" s="70" t="s">
+      <c r="G74" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="H74" s="71"/>
-      <c r="I74" s="71"/>
-      <c r="J74" s="71"/>
-      <c r="K74" s="71"/>
-      <c r="L74" s="71"/>
-      <c r="M74" s="71"/>
-      <c r="N74" s="72"/>
+      <c r="H74" s="100"/>
+      <c r="I74" s="100"/>
+      <c r="J74" s="100"/>
+      <c r="K74" s="100"/>
+      <c r="L74" s="100"/>
+      <c r="M74" s="100"/>
+      <c r="N74" s="101"/>
     </row>
     <row r="75" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G75" s="66"/>
@@ -4174,10 +4174,10 @@
       </c>
     </row>
     <row r="76" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G76" s="73" t="s">
+      <c r="G76" s="95" t="s">
         <v>148</v>
       </c>
-      <c r="H76" s="74"/>
+      <c r="H76" s="96"/>
       <c r="I76" s="18">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,1,$F$2:$F$52,"gfels6")</f>
         <v>12</v>
@@ -4204,10 +4204,10 @@
       </c>
     </row>
     <row r="77" spans="7:14" x14ac:dyDescent="0.2">
-      <c r="G77" s="73" t="s">
+      <c r="G77" s="95" t="s">
         <v>149</v>
       </c>
-      <c r="H77" s="74"/>
+      <c r="H77" s="96"/>
       <c r="I77" s="18">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,2,$F$2:$F$52,"gfels6")</f>
         <v>12</v>
@@ -4234,10 +4234,10 @@
       </c>
     </row>
     <row r="78" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G78" s="75" t="s">
+      <c r="G78" s="97" t="s">
         <v>150</v>
       </c>
-      <c r="H78" s="76"/>
+      <c r="H78" s="98"/>
       <c r="I78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
         <v>0</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="K78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"jntme")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"kybup1")</f>

</xml_diff>

<commit_message>
Analyzed some FindBugs hits. Fixed some, from over 40 to 31. We have to discuss a lot of them together :D
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester/bfh_software-engineering/Project/sohpboia_git/doc/04-ScrumSetup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40000" yWindow="-9680" windowWidth="28800" windowHeight="17540" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="40005" yWindow="-9675" windowWidth="28800" windowHeight="17535" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$52</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -721,7 +721,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1232,8 +1232,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1534,21 +1534,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1627,12 +1627,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1640,26 +1640,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1931,35 +1931,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="32.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="8.1640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="8.140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="43" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="43" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41">
         <v>0.1</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="70" t="s">
         <v>66</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="79" t="s">
         <v>67</v>
       </c>
@@ -2078,6 +2078,9 @@
       <c r="H4" s="78" t="s">
         <v>7</v>
       </c>
+      <c r="I4" s="78">
+        <v>0</v>
+      </c>
       <c r="J4" s="78">
         <v>0</v>
       </c>
@@ -2088,7 +2091,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>164</v>
       </c>
@@ -2126,7 +2129,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="79" t="s">
         <v>219</v>
       </c>
@@ -2164,7 +2167,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="75">
         <v>1.1000000000000001</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="75">
         <v>1.2</v>
       </c>
@@ -2202,7 +2205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
         <v>1.3</v>
       </c>
@@ -2226,7 +2229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>63</v>
       </c>
@@ -2241,7 +2244,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>41</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2317,7 +2320,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="59">
         <v>2.2000000000000002</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="92" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="92" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="90">
         <v>2.2999999999999998</v>
       </c>
@@ -2374,7 +2377,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32">
         <v>3.1</v>
       </c>
@@ -2412,7 +2415,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32">
         <v>3.2</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="28" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
         <v>39</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
         <v>40</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="28" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>72</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="59" t="s">
         <v>118</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
         <v>118</v>
       </c>
@@ -2617,7 +2620,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
         <v>122</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32">
         <v>3.3</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32">
         <v>3.4</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="58" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="58" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="59" t="s">
         <v>137</v>
       </c>
@@ -2769,7 +2772,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
         <v>141</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32">
         <v>3.5</v>
       </c>
@@ -2845,7 +2848,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26">
         <v>3.6</v>
       </c>
@@ -2883,7 +2886,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="56" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="56" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="54" t="s">
         <v>160</v>
       </c>
@@ -2921,7 +2924,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="52" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="52" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="50">
         <v>4.0999999999999996</v>
       </c>
@@ -2959,7 +2962,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="79" t="s">
         <v>221</v>
       </c>
@@ -2997,7 +3000,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="79" t="s">
         <v>220</v>
       </c>
@@ -3035,7 +3038,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
         <v>222</v>
       </c>
@@ -3073,7 +3076,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
         <v>223</v>
       </c>
@@ -3111,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
         <v>224</v>
       </c>
@@ -3149,7 +3152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
         <v>225</v>
       </c>
@@ -3187,7 +3190,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="79"/>
       <c r="B37" s="80">
         <v>3</v>
@@ -3223,7 +3226,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="79"/>
       <c r="B38" s="80">
         <v>3</v>
@@ -3259,7 +3262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
         <v>212</v>
       </c>
@@ -3297,7 +3300,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
         <v>213</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
         <v>214</v>
       </c>
@@ -3373,7 +3376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
         <v>215</v>
       </c>
@@ -3405,7 +3408,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="52" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" s="52" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>116</v>
       </c>
@@ -3443,7 +3446,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="52" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>131</v>
       </c>
@@ -3481,7 +3484,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>133</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>146</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
@@ -3595,7 +3598,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="79" t="s">
         <v>218</v>
       </c>
@@ -3633,7 +3636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="79" t="s">
         <v>217</v>
       </c>
@@ -3671,7 +3674,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="83" t="s">
         <v>216</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="88" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" s="88" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" s="86"/>
       <c r="B51" s="87">
         <v>3</v>
@@ -3745,7 +3748,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="64" t="s">
         <v>158</v>
       </c>
@@ -3783,7 +3786,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="16"/>
       <c r="B53" s="17"/>
       <c r="C53" s="18"/>
@@ -3797,7 +3800,7 @@
       <c r="K53" s="18"/>
       <c r="L53" s="18"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="16"/>
       <c r="B54" s="17"/>
       <c r="C54" s="18"/>
@@ -3809,7 +3812,7 @@
       <c r="P54" s="94"/>
       <c r="Q54" s="94"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E55" s="18"/>
       <c r="F55" s="22"/>
       <c r="G55" s="18"/>
@@ -3825,7 +3828,7 @@
       </c>
       <c r="L55" s="18"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E56" s="1" t="s">
         <v>152</v>
       </c>
@@ -3846,7 +3849,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E57" s="1" t="s">
         <v>153</v>
       </c>
@@ -3867,7 +3870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E58" s="1" t="s">
         <v>154</v>
       </c>
@@ -3888,8 +3891,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G62" s="99" t="s">
         <v>54</v>
       </c>
@@ -3901,7 +3904,7 @@
       <c r="M62" s="100"/>
       <c r="N62" s="101"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G63" s="66"/>
       <c r="H63" s="18"/>
       <c r="I63" s="18" t="s">
@@ -3923,7 +3926,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G64" s="95" t="s">
         <v>148</v>
       </c>
@@ -3953,7 +3956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G65" s="95" t="s">
         <v>149</v>
       </c>
@@ -3983,7 +3986,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G66" s="97" t="s">
         <v>150</v>
       </c>
@@ -4013,8 +4016,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="68" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G68" s="99" t="s">
         <v>55</v>
       </c>
@@ -4026,7 +4029,7 @@
       <c r="M68" s="100"/>
       <c r="N68" s="101"/>
     </row>
-    <row r="69" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G69" s="66"/>
       <c r="H69" s="18"/>
       <c r="I69" s="18" t="s">
@@ -4048,7 +4051,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G70" s="95" t="s">
         <v>148</v>
       </c>
@@ -4078,7 +4081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G71" s="95" t="s">
         <v>149</v>
       </c>
@@ -4108,7 +4111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G72" s="97" t="s">
         <v>150</v>
       </c>
@@ -4138,8 +4141,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G74" s="99" t="s">
         <v>56</v>
       </c>
@@ -4151,7 +4154,7 @@
       <c r="M74" s="100"/>
       <c r="N74" s="101"/>
     </row>
-    <row r="75" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G75" s="66"/>
       <c r="H75" s="18"/>
       <c r="I75" s="18" t="s">
@@ -4173,7 +4176,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G76" s="95" t="s">
         <v>148</v>
       </c>
@@ -4203,7 +4206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="77" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G77" s="95" t="s">
         <v>149</v>
       </c>
@@ -4233,7 +4236,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G78" s="97" t="s">
         <v>150</v>
       </c>
@@ -4264,7 +4267,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:L52">
+  <autoFilter ref="B1:L52" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="0">
       <filters>
         <filter val="3"/>
@@ -4298,21 +4301,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -4326,10 +4329,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -4339,24 +4342,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O346"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
@@ -4367,7 +4370,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="39">
         <v>1</v>
       </c>
@@ -4390,7 +4393,7 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -4413,7 +4416,7 @@
       <c r="N9" s="39"/>
       <c r="O9" s="39"/>
     </row>
-    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="40">
         <v>1</v>
       </c>
@@ -4436,7 +4439,7 @@
       <c r="N10" s="39"/>
       <c r="O10" s="39"/>
     </row>
-    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="40"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39" t="s">
@@ -4455,7 +4458,7 @@
       <c r="N11" s="39"/>
       <c r="O11" s="39"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39" t="s">
@@ -4474,7 +4477,7 @@
       <c r="N12" s="39"/>
       <c r="O12" s="39"/>
     </row>
-    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="40">
         <v>1</v>
       </c>
@@ -4497,7 +4500,7 @@
       <c r="N13" s="39"/>
       <c r="O13" s="39"/>
     </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="40">
         <v>2</v>
       </c>
@@ -4520,7 +4523,7 @@
       <c r="N14" s="39"/>
       <c r="O14" s="39"/>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="40"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -4537,7 +4540,7 @@
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
     </row>
-    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="40"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -4554,7 +4557,7 @@
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
     </row>
-    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="40"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -4571,7 +4574,7 @@
       <c r="N17" s="39"/>
       <c r="O17" s="39"/>
     </row>
-    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="40"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -4588,7 +4591,7 @@
       <c r="N18" s="39"/>
       <c r="O18" s="39"/>
     </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="40"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -4605,7 +4608,7 @@
       <c r="N19" s="39"/>
       <c r="O19" s="39"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A20" s="40"/>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
@@ -4622,7 +4625,7 @@
       <c r="N20" s="39"/>
       <c r="O20" s="39"/>
     </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A21" s="40"/>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
@@ -4639,7 +4642,7 @@
       <c r="N21" s="39"/>
       <c r="O21" s="39"/>
     </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
@@ -4656,7 +4659,7 @@
       <c r="N22" s="39"/>
       <c r="O22" s="39"/>
     </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="40"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -4673,7 +4676,7 @@
       <c r="N23" s="39"/>
       <c r="O23" s="39"/>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A24" s="40"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -4690,7 +4693,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="40"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -4707,7 +4710,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="40"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -4724,7 +4727,7 @@
       <c r="N26" s="39"/>
       <c r="O26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="40"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
@@ -4741,7 +4744,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="40"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -4758,7 +4761,7 @@
       <c r="N28" s="39"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="40"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -4775,7 +4778,7 @@
       <c r="N29" s="39"/>
       <c r="O29" s="39"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="40"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -4792,7 +4795,7 @@
       <c r="N30" s="39"/>
       <c r="O30" s="39"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="40"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -4809,7 +4812,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="39"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="40"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -4826,7 +4829,7 @@
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -4843,7 +4846,7 @@
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="40"/>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -4860,7 +4863,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="40"/>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -4877,7 +4880,7 @@
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="40"/>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
@@ -4894,7 +4897,7 @@
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="40"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -4911,7 +4914,7 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="40"/>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
@@ -4928,7 +4931,7 @@
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="40"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -4945,7 +4948,7 @@
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="40"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -4962,7 +4965,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="40"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -4979,7 +4982,7 @@
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="40"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
@@ -4996,7 +4999,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="40"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -5013,7 +5016,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="40"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -5030,7 +5033,7 @@
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="40"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -5047,7 +5050,7 @@
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="40"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -5064,7 +5067,7 @@
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="40"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -5081,7 +5084,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="40"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -5098,7 +5101,7 @@
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="40"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -5115,7 +5118,7 @@
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="40"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -5132,7 +5135,7 @@
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="40"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -5149,7 +5152,7 @@
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="40"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -5166,7 +5169,7 @@
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="40"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -5183,7 +5186,7 @@
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="40"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -5200,7 +5203,7 @@
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="40"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -5217,7 +5220,7 @@
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="40"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -5234,7 +5237,7 @@
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="40"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -5251,7 +5254,7 @@
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -5268,7 +5271,7 @@
       <c r="N58" s="39"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -5285,7 +5288,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="39"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -5302,7 +5305,7 @@
       <c r="N60" s="39"/>
       <c r="O60" s="39"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -5319,7 +5322,7 @@
       <c r="N61" s="39"/>
       <c r="O61" s="39"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -5336,7 +5339,7 @@
       <c r="N62" s="39"/>
       <c r="O62" s="39"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -5353,7 +5356,7 @@
       <c r="N63" s="39"/>
       <c r="O63" s="39"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -5370,7 +5373,7 @@
       <c r="N64" s="39"/>
       <c r="O64" s="39"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -5387,7 +5390,7 @@
       <c r="N65" s="39"/>
       <c r="O65" s="39"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -5404,7 +5407,7 @@
       <c r="N66" s="39"/>
       <c r="O66" s="39"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -5421,7 +5424,7 @@
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -5438,7 +5441,7 @@
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -5455,7 +5458,7 @@
       <c r="N69" s="39"/>
       <c r="O69" s="39"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -5472,7 +5475,7 @@
       <c r="N70" s="39"/>
       <c r="O70" s="39"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -5489,7 +5492,7 @@
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -5506,7 +5509,7 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -5523,7 +5526,7 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -5540,7 +5543,7 @@
       <c r="N74" s="39"/>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -5557,7 +5560,7 @@
       <c r="N75" s="39"/>
       <c r="O75" s="39"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -5574,7 +5577,7 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -5591,7 +5594,7 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -5608,7 +5611,7 @@
       <c r="N78" s="39"/>
       <c r="O78" s="39"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -5625,7 +5628,7 @@
       <c r="N79" s="39"/>
       <c r="O79" s="39"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -5642,7 +5645,7 @@
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -5659,7 +5662,7 @@
       <c r="N81" s="39"/>
       <c r="O81" s="39"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -5676,7 +5679,7 @@
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -5693,7 +5696,7 @@
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -5710,7 +5713,7 @@
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -5727,7 +5730,7 @@
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -5744,7 +5747,7 @@
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -5761,7 +5764,7 @@
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -5778,7 +5781,7 @@
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -5795,7 +5798,7 @@
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -5812,7 +5815,7 @@
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -5829,7 +5832,7 @@
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -5846,7 +5849,7 @@
       <c r="N92" s="39"/>
       <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -5863,7 +5866,7 @@
       <c r="N93" s="39"/>
       <c r="O93" s="39"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -5880,7 +5883,7 @@
       <c r="N94" s="39"/>
       <c r="O94" s="39"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -5897,7 +5900,7 @@
       <c r="N95" s="39"/>
       <c r="O95" s="39"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -5914,7 +5917,7 @@
       <c r="N96" s="39"/>
       <c r="O96" s="39"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -5931,7 +5934,7 @@
       <c r="N97" s="39"/>
       <c r="O97" s="39"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -5948,7 +5951,7 @@
       <c r="N98" s="39"/>
       <c r="O98" s="39"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -5965,7 +5968,7 @@
       <c r="N99" s="39"/>
       <c r="O99" s="39"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="39"/>
       <c r="B100" s="39"/>
       <c r="C100" s="39"/>
@@ -5982,7 +5985,7 @@
       <c r="N100" s="39"/>
       <c r="O100" s="39"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A101" s="39"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -5999,7 +6002,7 @@
       <c r="N101" s="39"/>
       <c r="O101" s="39"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A102" s="39"/>
       <c r="B102" s="39"/>
       <c r="C102" s="39"/>
@@ -6016,7 +6019,7 @@
       <c r="N102" s="39"/>
       <c r="O102" s="39"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A103" s="39"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -6033,7 +6036,7 @@
       <c r="N103" s="39"/>
       <c r="O103" s="39"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -6050,7 +6053,7 @@
       <c r="N104" s="39"/>
       <c r="O104" s="39"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A105" s="39"/>
       <c r="B105" s="39"/>
       <c r="C105" s="39"/>
@@ -6067,7 +6070,7 @@
       <c r="N105" s="39"/>
       <c r="O105" s="39"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A106" s="39"/>
       <c r="B106" s="39"/>
       <c r="C106" s="39"/>
@@ -6084,7 +6087,7 @@
       <c r="N106" s="39"/>
       <c r="O106" s="39"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A107" s="39"/>
       <c r="B107" s="39"/>
       <c r="C107" s="39"/>
@@ -6101,7 +6104,7 @@
       <c r="N107" s="39"/>
       <c r="O107" s="39"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A108" s="39"/>
       <c r="B108" s="39"/>
       <c r="C108" s="39"/>
@@ -6118,7 +6121,7 @@
       <c r="N108" s="39"/>
       <c r="O108" s="39"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A109" s="39"/>
       <c r="B109" s="39"/>
       <c r="C109" s="39"/>
@@ -6135,7 +6138,7 @@
       <c r="N109" s="39"/>
       <c r="O109" s="39"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A110" s="39"/>
       <c r="B110" s="39"/>
       <c r="C110" s="39"/>
@@ -6152,7 +6155,7 @@
       <c r="N110" s="39"/>
       <c r="O110" s="39"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A111" s="39"/>
       <c r="B111" s="39"/>
       <c r="C111" s="39"/>
@@ -6169,7 +6172,7 @@
       <c r="N111" s="39"/>
       <c r="O111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A112" s="39"/>
       <c r="B112" s="39"/>
       <c r="C112" s="39"/>
@@ -6186,7 +6189,7 @@
       <c r="N112" s="39"/>
       <c r="O112" s="39"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="39"/>
       <c r="B113" s="39"/>
       <c r="C113" s="39"/>
@@ -6203,7 +6206,7 @@
       <c r="N113" s="39"/>
       <c r="O113" s="39"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A114" s="39"/>
       <c r="B114" s="39"/>
       <c r="C114" s="39"/>
@@ -6220,7 +6223,7 @@
       <c r="N114" s="39"/>
       <c r="O114" s="39"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A115" s="39"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
@@ -6237,7 +6240,7 @@
       <c r="N115" s="39"/>
       <c r="O115" s="39"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A116" s="39"/>
       <c r="B116" s="39"/>
       <c r="C116" s="39"/>
@@ -6254,7 +6257,7 @@
       <c r="N116" s="39"/>
       <c r="O116" s="39"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A117" s="39"/>
       <c r="B117" s="39"/>
       <c r="C117" s="39"/>
@@ -6271,7 +6274,7 @@
       <c r="N117" s="39"/>
       <c r="O117" s="39"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A118" s="39"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
@@ -6288,7 +6291,7 @@
       <c r="N118" s="39"/>
       <c r="O118" s="39"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A119" s="39"/>
       <c r="B119" s="39"/>
       <c r="C119" s="39"/>
@@ -6305,7 +6308,7 @@
       <c r="N119" s="39"/>
       <c r="O119" s="39"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -6322,7 +6325,7 @@
       <c r="N120" s="39"/>
       <c r="O120" s="39"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A121" s="39"/>
       <c r="B121" s="39"/>
       <c r="C121" s="39"/>
@@ -6339,7 +6342,7 @@
       <c r="N121" s="39"/>
       <c r="O121" s="39"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A122" s="39"/>
       <c r="B122" s="39"/>
       <c r="C122" s="39"/>
@@ -6356,7 +6359,7 @@
       <c r="N122" s="39"/>
       <c r="O122" s="39"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A123" s="39"/>
       <c r="B123" s="39"/>
       <c r="C123" s="39"/>
@@ -6373,7 +6376,7 @@
       <c r="N123" s="39"/>
       <c r="O123" s="39"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A124" s="39"/>
       <c r="B124" s="39"/>
       <c r="C124" s="39"/>
@@ -6390,7 +6393,7 @@
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A125" s="39"/>
       <c r="B125" s="39"/>
       <c r="C125" s="39"/>
@@ -6407,7 +6410,7 @@
       <c r="N125" s="39"/>
       <c r="O125" s="39"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A126" s="39"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -6424,7 +6427,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="39"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A127" s="39"/>
       <c r="B127" s="39"/>
       <c r="C127" s="39"/>
@@ -6441,7 +6444,7 @@
       <c r="N127" s="39"/>
       <c r="O127" s="39"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39"/>
@@ -6458,7 +6461,7 @@
       <c r="N128" s="39"/>
       <c r="O128" s="39"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39"/>
@@ -6475,7 +6478,7 @@
       <c r="N129" s="39"/>
       <c r="O129" s="39"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39"/>
@@ -6492,7 +6495,7 @@
       <c r="N130" s="39"/>
       <c r="O130" s="39"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -6509,7 +6512,7 @@
       <c r="N131" s="39"/>
       <c r="O131" s="39"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -6526,7 +6529,7 @@
       <c r="N132" s="39"/>
       <c r="O132" s="39"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A133" s="39"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
@@ -6543,7 +6546,7 @@
       <c r="N133" s="39"/>
       <c r="O133" s="39"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A134" s="39"/>
       <c r="B134" s="39"/>
       <c r="C134" s="39"/>
@@ -6560,7 +6563,7 @@
       <c r="N134" s="39"/>
       <c r="O134" s="39"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -6577,7 +6580,7 @@
       <c r="N135" s="39"/>
       <c r="O135" s="39"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A136" s="39"/>
       <c r="B136" s="39"/>
       <c r="C136" s="39"/>
@@ -6594,7 +6597,7 @@
       <c r="N136" s="39"/>
       <c r="O136" s="39"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A137" s="39"/>
       <c r="B137" s="39"/>
       <c r="C137" s="39"/>
@@ -6611,7 +6614,7 @@
       <c r="N137" s="39"/>
       <c r="O137" s="39"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A138" s="39"/>
       <c r="B138" s="39"/>
       <c r="C138" s="39"/>
@@ -6628,7 +6631,7 @@
       <c r="N138" s="39"/>
       <c r="O138" s="39"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A139" s="39"/>
       <c r="B139" s="39"/>
       <c r="C139" s="39"/>
@@ -6645,7 +6648,7 @@
       <c r="N139" s="39"/>
       <c r="O139" s="39"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A140" s="39"/>
       <c r="B140" s="39"/>
       <c r="C140" s="39"/>
@@ -6662,7 +6665,7 @@
       <c r="N140" s="39"/>
       <c r="O140" s="39"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A141" s="39"/>
       <c r="B141" s="39"/>
       <c r="C141" s="39"/>
@@ -6679,7 +6682,7 @@
       <c r="N141" s="39"/>
       <c r="O141" s="39"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A142" s="39"/>
       <c r="B142" s="39"/>
       <c r="C142" s="39"/>
@@ -6696,7 +6699,7 @@
       <c r="N142" s="39"/>
       <c r="O142" s="39"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A143" s="39"/>
       <c r="B143" s="39"/>
       <c r="C143" s="39"/>
@@ -6713,7 +6716,7 @@
       <c r="N143" s="39"/>
       <c r="O143" s="39"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A144" s="39"/>
       <c r="B144" s="39"/>
       <c r="C144" s="39"/>
@@ -6730,7 +6733,7 @@
       <c r="N144" s="39"/>
       <c r="O144" s="39"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A145" s="39"/>
       <c r="B145" s="39"/>
       <c r="C145" s="39"/>
@@ -6747,7 +6750,7 @@
       <c r="N145" s="39"/>
       <c r="O145" s="39"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A146" s="39"/>
       <c r="B146" s="39"/>
       <c r="C146" s="39"/>
@@ -6764,7 +6767,7 @@
       <c r="N146" s="39"/>
       <c r="O146" s="39"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A147" s="39"/>
       <c r="B147" s="39"/>
       <c r="C147" s="39"/>
@@ -6781,7 +6784,7 @@
       <c r="N147" s="39"/>
       <c r="O147" s="39"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A148" s="39"/>
       <c r="B148" s="39"/>
       <c r="C148" s="39"/>
@@ -6798,7 +6801,7 @@
       <c r="N148" s="39"/>
       <c r="O148" s="39"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A149" s="39"/>
       <c r="B149" s="39"/>
       <c r="C149" s="39"/>
@@ -6815,7 +6818,7 @@
       <c r="N149" s="39"/>
       <c r="O149" s="39"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A150" s="39"/>
       <c r="B150" s="39"/>
       <c r="C150" s="39"/>
@@ -6832,7 +6835,7 @@
       <c r="N150" s="39"/>
       <c r="O150" s="39"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A151" s="39"/>
       <c r="B151" s="39"/>
       <c r="C151" s="39"/>
@@ -6849,7 +6852,7 @@
       <c r="N151" s="39"/>
       <c r="O151" s="39"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A152" s="39"/>
       <c r="B152" s="39"/>
       <c r="C152" s="39"/>
@@ -6866,7 +6869,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A153" s="39"/>
       <c r="B153" s="39"/>
       <c r="C153" s="39"/>
@@ -6883,7 +6886,7 @@
       <c r="N153" s="39"/>
       <c r="O153" s="39"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A154" s="39"/>
       <c r="B154" s="39"/>
       <c r="C154" s="39"/>
@@ -6900,7 +6903,7 @@
       <c r="N154" s="39"/>
       <c r="O154" s="39"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A155" s="39"/>
       <c r="B155" s="39"/>
       <c r="C155" s="39"/>
@@ -6917,7 +6920,7 @@
       <c r="N155" s="39"/>
       <c r="O155" s="39"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A156" s="39"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
@@ -6934,7 +6937,7 @@
       <c r="N156" s="39"/>
       <c r="O156" s="39"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A157" s="39"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
@@ -6951,7 +6954,7 @@
       <c r="N157" s="39"/>
       <c r="O157" s="39"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A158" s="39"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -6968,7 +6971,7 @@
       <c r="N158" s="39"/>
       <c r="O158" s="39"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A159" s="39"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -6985,7 +6988,7 @@
       <c r="N159" s="39"/>
       <c r="O159" s="39"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A160" s="39"/>
       <c r="B160" s="39"/>
       <c r="C160" s="39"/>
@@ -7002,7 +7005,7 @@
       <c r="N160" s="39"/>
       <c r="O160" s="39"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A161" s="39"/>
       <c r="B161" s="39"/>
       <c r="C161" s="39"/>
@@ -7019,7 +7022,7 @@
       <c r="N161" s="39"/>
       <c r="O161" s="39"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A162" s="39"/>
       <c r="B162" s="39"/>
       <c r="C162" s="39"/>
@@ -7036,7 +7039,7 @@
       <c r="N162" s="39"/>
       <c r="O162" s="39"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A163" s="39"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
@@ -7053,7 +7056,7 @@
       <c r="N163" s="39"/>
       <c r="O163" s="39"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A164" s="39"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
@@ -7070,7 +7073,7 @@
       <c r="N164" s="39"/>
       <c r="O164" s="39"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A165" s="39"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
@@ -7087,7 +7090,7 @@
       <c r="N165" s="39"/>
       <c r="O165" s="39"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A166" s="39"/>
       <c r="B166" s="39"/>
       <c r="C166" s="39"/>
@@ -7104,7 +7107,7 @@
       <c r="N166" s="39"/>
       <c r="O166" s="39"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A167" s="39"/>
       <c r="B167" s="39"/>
       <c r="C167" s="39"/>
@@ -7121,7 +7124,7 @@
       <c r="N167" s="39"/>
       <c r="O167" s="39"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A168" s="39"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -7138,7 +7141,7 @@
       <c r="N168" s="39"/>
       <c r="O168" s="39"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A169" s="39"/>
       <c r="B169" s="39"/>
       <c r="C169" s="39"/>
@@ -7155,7 +7158,7 @@
       <c r="N169" s="39"/>
       <c r="O169" s="39"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A170" s="39"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
@@ -7172,7 +7175,7 @@
       <c r="N170" s="39"/>
       <c r="O170" s="39"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A171" s="39"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -7189,7 +7192,7 @@
       <c r="N171" s="39"/>
       <c r="O171" s="39"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A172" s="39"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
@@ -7206,7 +7209,7 @@
       <c r="N172" s="39"/>
       <c r="O172" s="39"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A173" s="39"/>
       <c r="B173" s="39"/>
       <c r="C173" s="39"/>
@@ -7223,7 +7226,7 @@
       <c r="N173" s="39"/>
       <c r="O173" s="39"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A174" s="39"/>
       <c r="B174" s="39"/>
       <c r="C174" s="39"/>
@@ -7240,7 +7243,7 @@
       <c r="N174" s="39"/>
       <c r="O174" s="39"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A175" s="39"/>
       <c r="B175" s="39"/>
       <c r="C175" s="39"/>
@@ -7257,7 +7260,7 @@
       <c r="N175" s="39"/>
       <c r="O175" s="39"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A176" s="39"/>
       <c r="B176" s="39"/>
       <c r="C176" s="39"/>
@@ -7274,7 +7277,7 @@
       <c r="N176" s="39"/>
       <c r="O176" s="39"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A177" s="39"/>
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
@@ -7291,7 +7294,7 @@
       <c r="N177" s="39"/>
       <c r="O177" s="39"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A178" s="39"/>
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
@@ -7308,7 +7311,7 @@
       <c r="N178" s="39"/>
       <c r="O178" s="39"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A179" s="39"/>
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
@@ -7325,7 +7328,7 @@
       <c r="N179" s="39"/>
       <c r="O179" s="39"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A180" s="39"/>
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
@@ -7342,7 +7345,7 @@
       <c r="N180" s="39"/>
       <c r="O180" s="39"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A181" s="39"/>
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
@@ -7359,7 +7362,7 @@
       <c r="N181" s="39"/>
       <c r="O181" s="39"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A182" s="39"/>
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
@@ -7376,7 +7379,7 @@
       <c r="N182" s="39"/>
       <c r="O182" s="39"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A183" s="39"/>
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
@@ -7393,7 +7396,7 @@
       <c r="N183" s="39"/>
       <c r="O183" s="39"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A184" s="39"/>
       <c r="B184" s="39"/>
       <c r="C184" s="39"/>
@@ -7410,7 +7413,7 @@
       <c r="N184" s="39"/>
       <c r="O184" s="39"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
       <c r="C185" s="39"/>
@@ -7427,7 +7430,7 @@
       <c r="N185" s="39"/>
       <c r="O185" s="39"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
       <c r="C186" s="39"/>
@@ -7444,7 +7447,7 @@
       <c r="N186" s="39"/>
       <c r="O186" s="39"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A187" s="39"/>
       <c r="B187" s="39"/>
       <c r="C187" s="39"/>
@@ -7461,7 +7464,7 @@
       <c r="N187" s="39"/>
       <c r="O187" s="39"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A188" s="39"/>
       <c r="B188" s="39"/>
       <c r="C188" s="39"/>
@@ -7478,7 +7481,7 @@
       <c r="N188" s="39"/>
       <c r="O188" s="39"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A189" s="39"/>
       <c r="B189" s="39"/>
       <c r="C189" s="39"/>
@@ -7495,7 +7498,7 @@
       <c r="N189" s="39"/>
       <c r="O189" s="39"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A190" s="39"/>
       <c r="B190" s="39"/>
       <c r="C190" s="39"/>
@@ -7512,7 +7515,7 @@
       <c r="N190" s="39"/>
       <c r="O190" s="39"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A191" s="39"/>
       <c r="B191" s="39"/>
       <c r="C191" s="39"/>
@@ -7529,7 +7532,7 @@
       <c r="N191" s="39"/>
       <c r="O191" s="39"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A192" s="39"/>
       <c r="B192" s="39"/>
       <c r="C192" s="39"/>
@@ -7546,7 +7549,7 @@
       <c r="N192" s="39"/>
       <c r="O192" s="39"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A193" s="39"/>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -7563,7 +7566,7 @@
       <c r="N193" s="39"/>
       <c r="O193" s="39"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A194" s="39"/>
       <c r="B194" s="39"/>
       <c r="C194" s="39"/>
@@ -7580,7 +7583,7 @@
       <c r="N194" s="39"/>
       <c r="O194" s="39"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A195" s="39"/>
       <c r="B195" s="39"/>
       <c r="C195" s="39"/>
@@ -7597,7 +7600,7 @@
       <c r="N195" s="39"/>
       <c r="O195" s="39"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A196" s="39"/>
       <c r="B196" s="39"/>
       <c r="C196" s="39"/>
@@ -7614,7 +7617,7 @@
       <c r="N196" s="39"/>
       <c r="O196" s="39"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A197" s="39"/>
       <c r="B197" s="39"/>
       <c r="C197" s="39"/>
@@ -7631,7 +7634,7 @@
       <c r="N197" s="39"/>
       <c r="O197" s="39"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A198" s="39"/>
       <c r="B198" s="39"/>
       <c r="C198" s="39"/>
@@ -7648,7 +7651,7 @@
       <c r="N198" s="39"/>
       <c r="O198" s="39"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A199" s="39"/>
       <c r="B199" s="39"/>
       <c r="C199" s="39"/>
@@ -7665,7 +7668,7 @@
       <c r="N199" s="39"/>
       <c r="O199" s="39"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A200" s="39"/>
       <c r="B200" s="39"/>
       <c r="C200" s="39"/>
@@ -7682,7 +7685,7 @@
       <c r="N200" s="39"/>
       <c r="O200" s="39"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A201" s="39"/>
       <c r="B201" s="39"/>
       <c r="C201" s="39"/>
@@ -7699,7 +7702,7 @@
       <c r="N201" s="39"/>
       <c r="O201" s="39"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A202" s="39"/>
       <c r="B202" s="39"/>
       <c r="C202" s="39"/>
@@ -7716,7 +7719,7 @@
       <c r="N202" s="39"/>
       <c r="O202" s="39"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A203" s="39"/>
       <c r="B203" s="39"/>
       <c r="C203" s="39"/>
@@ -7733,7 +7736,7 @@
       <c r="N203" s="39"/>
       <c r="O203" s="39"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A204" s="39"/>
       <c r="B204" s="39"/>
       <c r="C204" s="39"/>
@@ -7750,7 +7753,7 @@
       <c r="N204" s="39"/>
       <c r="O204" s="39"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A205" s="39"/>
       <c r="B205" s="39"/>
       <c r="C205" s="39"/>
@@ -7767,7 +7770,7 @@
       <c r="N205" s="39"/>
       <c r="O205" s="39"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A206" s="39"/>
       <c r="B206" s="39"/>
       <c r="C206" s="39"/>
@@ -7784,7 +7787,7 @@
       <c r="N206" s="39"/>
       <c r="O206" s="39"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A207" s="39"/>
       <c r="B207" s="39"/>
       <c r="C207" s="39"/>
@@ -7801,7 +7804,7 @@
       <c r="N207" s="39"/>
       <c r="O207" s="39"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A208" s="39"/>
       <c r="B208" s="39"/>
       <c r="C208" s="39"/>
@@ -7818,7 +7821,7 @@
       <c r="N208" s="39"/>
       <c r="O208" s="39"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A209" s="39"/>
       <c r="B209" s="39"/>
       <c r="C209" s="39"/>
@@ -7835,7 +7838,7 @@
       <c r="N209" s="39"/>
       <c r="O209" s="39"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A210" s="39"/>
       <c r="B210" s="39"/>
       <c r="C210" s="39"/>
@@ -7852,7 +7855,7 @@
       <c r="N210" s="39"/>
       <c r="O210" s="39"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A211" s="39"/>
       <c r="B211" s="39"/>
       <c r="C211" s="39"/>
@@ -7869,7 +7872,7 @@
       <c r="N211" s="39"/>
       <c r="O211" s="39"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A212" s="39"/>
       <c r="B212" s="39"/>
       <c r="C212" s="39"/>
@@ -7886,7 +7889,7 @@
       <c r="N212" s="39"/>
       <c r="O212" s="39"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A213" s="39"/>
       <c r="B213" s="39"/>
       <c r="C213" s="39"/>
@@ -7903,7 +7906,7 @@
       <c r="N213" s="39"/>
       <c r="O213" s="39"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A214" s="39"/>
       <c r="B214" s="39"/>
       <c r="C214" s="39"/>
@@ -7920,7 +7923,7 @@
       <c r="N214" s="39"/>
       <c r="O214" s="39"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A215" s="39"/>
       <c r="B215" s="39"/>
       <c r="C215" s="39"/>
@@ -7937,7 +7940,7 @@
       <c r="N215" s="39"/>
       <c r="O215" s="39"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A216" s="39"/>
       <c r="B216" s="39"/>
       <c r="C216" s="39"/>
@@ -7954,7 +7957,7 @@
       <c r="N216" s="39"/>
       <c r="O216" s="39"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A217" s="39"/>
       <c r="B217" s="39"/>
       <c r="C217" s="39"/>
@@ -7971,7 +7974,7 @@
       <c r="N217" s="39"/>
       <c r="O217" s="39"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A218" s="39"/>
       <c r="B218" s="39"/>
       <c r="C218" s="39"/>
@@ -7988,7 +7991,7 @@
       <c r="N218" s="39"/>
       <c r="O218" s="39"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A219" s="39"/>
       <c r="B219" s="39"/>
       <c r="C219" s="39"/>
@@ -8005,7 +8008,7 @@
       <c r="N219" s="39"/>
       <c r="O219" s="39"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A220" s="39"/>
       <c r="B220" s="39"/>
       <c r="C220" s="39"/>
@@ -8022,7 +8025,7 @@
       <c r="N220" s="39"/>
       <c r="O220" s="39"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="39"/>
       <c r="B221" s="39"/>
       <c r="C221" s="39"/>
@@ -8039,7 +8042,7 @@
       <c r="N221" s="39"/>
       <c r="O221" s="39"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A222" s="39"/>
       <c r="B222" s="39"/>
       <c r="C222" s="39"/>
@@ -8056,7 +8059,7 @@
       <c r="N222" s="39"/>
       <c r="O222" s="39"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A223" s="39"/>
       <c r="B223" s="39"/>
       <c r="C223" s="39"/>
@@ -8073,7 +8076,7 @@
       <c r="N223" s="39"/>
       <c r="O223" s="39"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A224" s="39"/>
       <c r="B224" s="39"/>
       <c r="C224" s="39"/>
@@ -8090,7 +8093,7 @@
       <c r="N224" s="39"/>
       <c r="O224" s="39"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A225" s="39"/>
       <c r="B225" s="39"/>
       <c r="C225" s="39"/>
@@ -8107,7 +8110,7 @@
       <c r="N225" s="39"/>
       <c r="O225" s="39"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A226" s="39"/>
       <c r="B226" s="39"/>
       <c r="C226" s="39"/>
@@ -8124,7 +8127,7 @@
       <c r="N226" s="39"/>
       <c r="O226" s="39"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A227" s="39"/>
       <c r="B227" s="39"/>
       <c r="C227" s="39"/>
@@ -8141,7 +8144,7 @@
       <c r="N227" s="39"/>
       <c r="O227" s="39"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A228" s="39"/>
       <c r="B228" s="39"/>
       <c r="C228" s="39"/>
@@ -8158,7 +8161,7 @@
       <c r="N228" s="39"/>
       <c r="O228" s="39"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A229" s="39"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
@@ -8175,7 +8178,7 @@
       <c r="N229" s="39"/>
       <c r="O229" s="39"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A230" s="39"/>
       <c r="B230" s="39"/>
       <c r="C230" s="39"/>
@@ -8192,7 +8195,7 @@
       <c r="N230" s="39"/>
       <c r="O230" s="39"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A231" s="39"/>
       <c r="B231" s="39"/>
       <c r="C231" s="39"/>
@@ -8209,7 +8212,7 @@
       <c r="N231" s="39"/>
       <c r="O231" s="39"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A232" s="39"/>
       <c r="B232" s="39"/>
       <c r="C232" s="39"/>
@@ -8226,7 +8229,7 @@
       <c r="N232" s="39"/>
       <c r="O232" s="39"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A233" s="39"/>
       <c r="B233" s="39"/>
       <c r="C233" s="39"/>
@@ -8243,7 +8246,7 @@
       <c r="N233" s="39"/>
       <c r="O233" s="39"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A234" s="39"/>
       <c r="B234" s="39"/>
       <c r="C234" s="39"/>
@@ -8260,7 +8263,7 @@
       <c r="N234" s="39"/>
       <c r="O234" s="39"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A235" s="39"/>
       <c r="B235" s="39"/>
       <c r="C235" s="39"/>
@@ -8277,7 +8280,7 @@
       <c r="N235" s="39"/>
       <c r="O235" s="39"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A236" s="39"/>
       <c r="B236" s="39"/>
       <c r="C236" s="39"/>
@@ -8294,7 +8297,7 @@
       <c r="N236" s="39"/>
       <c r="O236" s="39"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A237" s="39"/>
       <c r="B237" s="39"/>
       <c r="C237" s="39"/>
@@ -8311,7 +8314,7 @@
       <c r="N237" s="39"/>
       <c r="O237" s="39"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A238" s="39"/>
       <c r="B238" s="39"/>
       <c r="C238" s="39"/>
@@ -8328,7 +8331,7 @@
       <c r="N238" s="39"/>
       <c r="O238" s="39"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A239" s="39"/>
       <c r="B239" s="39"/>
       <c r="C239" s="39"/>
@@ -8345,7 +8348,7 @@
       <c r="N239" s="39"/>
       <c r="O239" s="39"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A240" s="39"/>
       <c r="B240" s="39"/>
       <c r="C240" s="39"/>
@@ -8362,7 +8365,7 @@
       <c r="N240" s="39"/>
       <c r="O240" s="39"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A241" s="39"/>
       <c r="B241" s="39"/>
       <c r="C241" s="39"/>
@@ -8379,7 +8382,7 @@
       <c r="N241" s="39"/>
       <c r="O241" s="39"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A242" s="39"/>
       <c r="B242" s="39"/>
       <c r="C242" s="39"/>
@@ -8396,7 +8399,7 @@
       <c r="N242" s="39"/>
       <c r="O242" s="39"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A243" s="39"/>
       <c r="B243" s="39"/>
       <c r="C243" s="39"/>
@@ -8413,7 +8416,7 @@
       <c r="N243" s="39"/>
       <c r="O243" s="39"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A244" s="39"/>
       <c r="B244" s="39"/>
       <c r="C244" s="39"/>
@@ -8430,7 +8433,7 @@
       <c r="N244" s="39"/>
       <c r="O244" s="39"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A245" s="39"/>
       <c r="B245" s="39"/>
       <c r="C245" s="39"/>
@@ -8447,7 +8450,7 @@
       <c r="N245" s="39"/>
       <c r="O245" s="39"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A246" s="39"/>
       <c r="B246" s="39"/>
       <c r="C246" s="39"/>
@@ -8464,7 +8467,7 @@
       <c r="N246" s="39"/>
       <c r="O246" s="39"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A247" s="39"/>
       <c r="B247" s="39"/>
       <c r="C247" s="39"/>
@@ -8481,7 +8484,7 @@
       <c r="N247" s="39"/>
       <c r="O247" s="39"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A248" s="39"/>
       <c r="B248" s="39"/>
       <c r="C248" s="39"/>
@@ -8498,7 +8501,7 @@
       <c r="N248" s="39"/>
       <c r="O248" s="39"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A249" s="39"/>
       <c r="B249" s="39"/>
       <c r="C249" s="39"/>
@@ -8515,7 +8518,7 @@
       <c r="N249" s="39"/>
       <c r="O249" s="39"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A250" s="39"/>
       <c r="B250" s="39"/>
       <c r="C250" s="39"/>
@@ -8532,7 +8535,7 @@
       <c r="N250" s="39"/>
       <c r="O250" s="39"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A251" s="39"/>
       <c r="B251" s="39"/>
       <c r="C251" s="39"/>
@@ -8549,7 +8552,7 @@
       <c r="N251" s="39"/>
       <c r="O251" s="39"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A252" s="39"/>
       <c r="B252" s="39"/>
       <c r="C252" s="39"/>
@@ -8566,7 +8569,7 @@
       <c r="N252" s="39"/>
       <c r="O252" s="39"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A253" s="39"/>
       <c r="B253" s="39"/>
       <c r="C253" s="39"/>
@@ -8583,7 +8586,7 @@
       <c r="N253" s="39"/>
       <c r="O253" s="39"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A254" s="39"/>
       <c r="B254" s="39"/>
       <c r="C254" s="39"/>
@@ -8600,7 +8603,7 @@
       <c r="N254" s="39"/>
       <c r="O254" s="39"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A255" s="39"/>
       <c r="B255" s="39"/>
       <c r="C255" s="39"/>
@@ -8617,7 +8620,7 @@
       <c r="N255" s="39"/>
       <c r="O255" s="39"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A256" s="39"/>
       <c r="B256" s="39"/>
       <c r="C256" s="39"/>
@@ -8634,7 +8637,7 @@
       <c r="N256" s="39"/>
       <c r="O256" s="39"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A257" s="39"/>
       <c r="B257" s="39"/>
       <c r="C257" s="39"/>
@@ -8651,7 +8654,7 @@
       <c r="N257" s="39"/>
       <c r="O257" s="39"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A258" s="39"/>
       <c r="B258" s="39"/>
       <c r="C258" s="39"/>
@@ -8668,7 +8671,7 @@
       <c r="N258" s="39"/>
       <c r="O258" s="39"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A259" s="39"/>
       <c r="B259" s="39"/>
       <c r="C259" s="39"/>
@@ -8685,7 +8688,7 @@
       <c r="N259" s="39"/>
       <c r="O259" s="39"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A260" s="39"/>
       <c r="B260" s="39"/>
       <c r="C260" s="39"/>
@@ -8702,7 +8705,7 @@
       <c r="N260" s="39"/>
       <c r="O260" s="39"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A261" s="39"/>
       <c r="B261" s="39"/>
       <c r="C261" s="39"/>
@@ -8719,7 +8722,7 @@
       <c r="N261" s="39"/>
       <c r="O261" s="39"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A262" s="39"/>
       <c r="B262" s="39"/>
       <c r="C262" s="39"/>
@@ -8736,7 +8739,7 @@
       <c r="N262" s="39"/>
       <c r="O262" s="39"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A263" s="39"/>
       <c r="B263" s="39"/>
       <c r="C263" s="39"/>
@@ -8753,7 +8756,7 @@
       <c r="N263" s="39"/>
       <c r="O263" s="39"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A264" s="39"/>
       <c r="B264" s="39"/>
       <c r="C264" s="39"/>
@@ -8770,7 +8773,7 @@
       <c r="N264" s="39"/>
       <c r="O264" s="39"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A265" s="39"/>
       <c r="B265" s="39"/>
       <c r="C265" s="39"/>
@@ -8787,7 +8790,7 @@
       <c r="N265" s="39"/>
       <c r="O265" s="39"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A266" s="39"/>
       <c r="B266" s="39"/>
       <c r="C266" s="39"/>
@@ -8804,7 +8807,7 @@
       <c r="N266" s="39"/>
       <c r="O266" s="39"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A267" s="39"/>
       <c r="B267" s="39"/>
       <c r="C267" s="39"/>
@@ -8821,7 +8824,7 @@
       <c r="N267" s="39"/>
       <c r="O267" s="39"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A268" s="39"/>
       <c r="B268" s="39"/>
       <c r="C268" s="39"/>
@@ -8838,7 +8841,7 @@
       <c r="N268" s="39"/>
       <c r="O268" s="39"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
@@ -8855,7 +8858,7 @@
       <c r="N269" s="39"/>
       <c r="O269" s="39"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A270" s="39"/>
       <c r="B270" s="39"/>
       <c r="C270" s="39"/>
@@ -8872,7 +8875,7 @@
       <c r="N270" s="39"/>
       <c r="O270" s="39"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A271" s="39"/>
       <c r="B271" s="39"/>
       <c r="C271" s="39"/>
@@ -8889,7 +8892,7 @@
       <c r="N271" s="39"/>
       <c r="O271" s="39"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A272" s="39"/>
       <c r="B272" s="39"/>
       <c r="C272" s="39"/>
@@ -8906,7 +8909,7 @@
       <c r="N272" s="39"/>
       <c r="O272" s="39"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A273" s="39"/>
       <c r="B273" s="39"/>
       <c r="C273" s="39"/>
@@ -8923,7 +8926,7 @@
       <c r="N273" s="39"/>
       <c r="O273" s="39"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A274" s="39"/>
       <c r="B274" s="39"/>
       <c r="C274" s="39"/>
@@ -8940,7 +8943,7 @@
       <c r="N274" s="39"/>
       <c r="O274" s="39"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A275" s="39"/>
       <c r="B275" s="39"/>
       <c r="C275" s="39"/>
@@ -8957,7 +8960,7 @@
       <c r="N275" s="39"/>
       <c r="O275" s="39"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A276" s="39"/>
       <c r="B276" s="39"/>
       <c r="C276" s="39"/>
@@ -8974,7 +8977,7 @@
       <c r="N276" s="39"/>
       <c r="O276" s="39"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A277" s="39"/>
       <c r="B277" s="39"/>
       <c r="C277" s="39"/>
@@ -8991,7 +8994,7 @@
       <c r="N277" s="39"/>
       <c r="O277" s="39"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A278" s="39"/>
       <c r="B278" s="39"/>
       <c r="C278" s="39"/>
@@ -9008,7 +9011,7 @@
       <c r="N278" s="39"/>
       <c r="O278" s="39"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A279" s="39"/>
       <c r="B279" s="39"/>
       <c r="C279" s="39"/>
@@ -9025,7 +9028,7 @@
       <c r="N279" s="39"/>
       <c r="O279" s="39"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A280" s="39"/>
       <c r="B280" s="39"/>
       <c r="C280" s="39"/>
@@ -9042,7 +9045,7 @@
       <c r="N280" s="39"/>
       <c r="O280" s="39"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A281" s="39"/>
       <c r="B281" s="39"/>
       <c r="C281" s="39"/>
@@ -9059,7 +9062,7 @@
       <c r="N281" s="39"/>
       <c r="O281" s="39"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A282" s="39"/>
       <c r="B282" s="39"/>
       <c r="C282" s="39"/>
@@ -9076,7 +9079,7 @@
       <c r="N282" s="39"/>
       <c r="O282" s="39"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A283" s="39"/>
       <c r="B283" s="39"/>
       <c r="C283" s="39"/>
@@ -9093,7 +9096,7 @@
       <c r="N283" s="39"/>
       <c r="O283" s="39"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A284" s="39"/>
       <c r="B284" s="39"/>
       <c r="C284" s="39"/>
@@ -9110,7 +9113,7 @@
       <c r="N284" s="39"/>
       <c r="O284" s="39"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A285" s="39"/>
       <c r="B285" s="39"/>
       <c r="C285" s="39"/>
@@ -9127,7 +9130,7 @@
       <c r="N285" s="39"/>
       <c r="O285" s="39"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A286" s="39"/>
       <c r="B286" s="39"/>
       <c r="C286" s="39"/>
@@ -9144,7 +9147,7 @@
       <c r="N286" s="39"/>
       <c r="O286" s="39"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A287" s="39"/>
       <c r="B287" s="39"/>
       <c r="C287" s="39"/>
@@ -9161,7 +9164,7 @@
       <c r="N287" s="39"/>
       <c r="O287" s="39"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A288" s="39"/>
       <c r="B288" s="39"/>
       <c r="C288" s="39"/>
@@ -9178,7 +9181,7 @@
       <c r="N288" s="39"/>
       <c r="O288" s="39"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A289" s="39"/>
       <c r="B289" s="39"/>
       <c r="C289" s="39"/>
@@ -9195,7 +9198,7 @@
       <c r="N289" s="39"/>
       <c r="O289" s="39"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A290" s="39"/>
       <c r="B290" s="39"/>
       <c r="C290" s="39"/>
@@ -9212,7 +9215,7 @@
       <c r="N290" s="39"/>
       <c r="O290" s="39"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A291" s="39"/>
       <c r="B291" s="39"/>
       <c r="C291" s="39"/>
@@ -9229,7 +9232,7 @@
       <c r="N291" s="39"/>
       <c r="O291" s="39"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A292" s="39"/>
       <c r="B292" s="39"/>
       <c r="C292" s="39"/>
@@ -9246,7 +9249,7 @@
       <c r="N292" s="39"/>
       <c r="O292" s="39"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A293" s="39"/>
       <c r="B293" s="39"/>
       <c r="C293" s="39"/>
@@ -9263,7 +9266,7 @@
       <c r="N293" s="39"/>
       <c r="O293" s="39"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A294" s="39"/>
       <c r="B294" s="39"/>
       <c r="C294" s="39"/>
@@ -9280,7 +9283,7 @@
       <c r="N294" s="39"/>
       <c r="O294" s="39"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A295" s="39"/>
       <c r="B295" s="39"/>
       <c r="C295" s="39"/>
@@ -9297,7 +9300,7 @@
       <c r="N295" s="39"/>
       <c r="O295" s="39"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A296" s="39"/>
       <c r="B296" s="39"/>
       <c r="C296" s="39"/>
@@ -9314,7 +9317,7 @@
       <c r="N296" s="39"/>
       <c r="O296" s="39"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A297" s="39"/>
       <c r="B297" s="39"/>
       <c r="C297" s="39"/>
@@ -9331,7 +9334,7 @@
       <c r="N297" s="39"/>
       <c r="O297" s="39"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A298" s="39"/>
       <c r="B298" s="39"/>
       <c r="C298" s="39"/>
@@ -9348,7 +9351,7 @@
       <c r="N298" s="39"/>
       <c r="O298" s="39"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A299" s="39"/>
       <c r="B299" s="39"/>
       <c r="C299" s="39"/>
@@ -9365,7 +9368,7 @@
       <c r="N299" s="39"/>
       <c r="O299" s="39"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A300" s="39"/>
       <c r="B300" s="39"/>
       <c r="C300" s="39"/>
@@ -9382,7 +9385,7 @@
       <c r="N300" s="39"/>
       <c r="O300" s="39"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A301" s="39"/>
       <c r="B301" s="39"/>
       <c r="C301" s="39"/>
@@ -9399,7 +9402,7 @@
       <c r="N301" s="39"/>
       <c r="O301" s="39"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A302" s="39"/>
       <c r="B302" s="39"/>
       <c r="C302" s="39"/>
@@ -9416,7 +9419,7 @@
       <c r="N302" s="39"/>
       <c r="O302" s="39"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A303" s="39"/>
       <c r="B303" s="39"/>
       <c r="C303" s="39"/>
@@ -9433,7 +9436,7 @@
       <c r="N303" s="39"/>
       <c r="O303" s="39"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A304" s="39"/>
       <c r="B304" s="39"/>
       <c r="C304" s="39"/>
@@ -9450,7 +9453,7 @@
       <c r="N304" s="39"/>
       <c r="O304" s="39"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A305" s="39"/>
       <c r="B305" s="39"/>
       <c r="C305" s="39"/>
@@ -9467,7 +9470,7 @@
       <c r="N305" s="39"/>
       <c r="O305" s="39"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A306" s="39"/>
       <c r="B306" s="39"/>
       <c r="C306" s="39"/>
@@ -9484,7 +9487,7 @@
       <c r="N306" s="39"/>
       <c r="O306" s="39"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A307" s="39"/>
       <c r="B307" s="39"/>
       <c r="C307" s="39"/>
@@ -9501,7 +9504,7 @@
       <c r="N307" s="39"/>
       <c r="O307" s="39"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A308" s="39"/>
       <c r="B308" s="39"/>
       <c r="C308" s="39"/>
@@ -9518,7 +9521,7 @@
       <c r="N308" s="39"/>
       <c r="O308" s="39"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A309" s="39"/>
       <c r="B309" s="39"/>
       <c r="C309" s="39"/>
@@ -9535,7 +9538,7 @@
       <c r="N309" s="39"/>
       <c r="O309" s="39"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A310" s="39"/>
       <c r="B310" s="39"/>
       <c r="C310" s="39"/>
@@ -9552,7 +9555,7 @@
       <c r="N310" s="39"/>
       <c r="O310" s="39"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A311" s="39"/>
       <c r="B311" s="39"/>
       <c r="C311" s="39"/>
@@ -9569,7 +9572,7 @@
       <c r="N311" s="39"/>
       <c r="O311" s="39"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A312" s="39"/>
       <c r="B312" s="39"/>
       <c r="C312" s="39"/>
@@ -9586,7 +9589,7 @@
       <c r="N312" s="39"/>
       <c r="O312" s="39"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A313" s="39"/>
       <c r="B313" s="39"/>
       <c r="C313" s="39"/>
@@ -9603,7 +9606,7 @@
       <c r="N313" s="39"/>
       <c r="O313" s="39"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A314" s="39"/>
       <c r="B314" s="39"/>
       <c r="C314" s="39"/>
@@ -9620,7 +9623,7 @@
       <c r="N314" s="39"/>
       <c r="O314" s="39"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A315" s="39"/>
       <c r="B315" s="39"/>
       <c r="C315" s="39"/>
@@ -9637,7 +9640,7 @@
       <c r="N315" s="39"/>
       <c r="O315" s="39"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A316" s="39"/>
       <c r="B316" s="39"/>
       <c r="C316" s="39"/>
@@ -9654,7 +9657,7 @@
       <c r="N316" s="39"/>
       <c r="O316" s="39"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A317" s="39"/>
       <c r="B317" s="39"/>
       <c r="C317" s="39"/>
@@ -9671,7 +9674,7 @@
       <c r="N317" s="39"/>
       <c r="O317" s="39"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A318" s="39"/>
       <c r="B318" s="39"/>
       <c r="C318" s="39"/>
@@ -9688,7 +9691,7 @@
       <c r="N318" s="39"/>
       <c r="O318" s="39"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A319" s="39"/>
       <c r="B319" s="39"/>
       <c r="C319" s="39"/>
@@ -9705,7 +9708,7 @@
       <c r="N319" s="39"/>
       <c r="O319" s="39"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A320" s="39"/>
       <c r="B320" s="39"/>
       <c r="C320" s="39"/>
@@ -9722,7 +9725,7 @@
       <c r="N320" s="39"/>
       <c r="O320" s="39"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A321" s="39"/>
       <c r="B321" s="39"/>
       <c r="C321" s="39"/>
@@ -9739,7 +9742,7 @@
       <c r="N321" s="39"/>
       <c r="O321" s="39"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A322" s="39"/>
       <c r="B322" s="39"/>
       <c r="C322" s="39"/>
@@ -9756,7 +9759,7 @@
       <c r="N322" s="39"/>
       <c r="O322" s="39"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A323" s="39"/>
       <c r="B323" s="39"/>
       <c r="C323" s="39"/>
@@ -9773,7 +9776,7 @@
       <c r="N323" s="39"/>
       <c r="O323" s="39"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A324" s="39"/>
       <c r="B324" s="39"/>
       <c r="C324" s="39"/>
@@ -9790,7 +9793,7 @@
       <c r="N324" s="39"/>
       <c r="O324" s="39"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A325" s="39"/>
       <c r="B325" s="39"/>
       <c r="C325" s="39"/>
@@ -9807,7 +9810,7 @@
       <c r="N325" s="39"/>
       <c r="O325" s="39"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A326" s="39"/>
       <c r="B326" s="39"/>
       <c r="C326" s="39"/>
@@ -9824,7 +9827,7 @@
       <c r="N326" s="39"/>
       <c r="O326" s="39"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
       <c r="C327" s="39"/>
@@ -9841,7 +9844,7 @@
       <c r="N327" s="39"/>
       <c r="O327" s="39"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A328" s="39"/>
       <c r="B328" s="39"/>
       <c r="C328" s="39"/>
@@ -9858,7 +9861,7 @@
       <c r="N328" s="39"/>
       <c r="O328" s="39"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A329" s="39"/>
       <c r="B329" s="39"/>
       <c r="C329" s="39"/>
@@ -9875,7 +9878,7 @@
       <c r="N329" s="39"/>
       <c r="O329" s="39"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A330" s="39"/>
       <c r="B330" s="39"/>
       <c r="C330" s="39"/>
@@ -9892,7 +9895,7 @@
       <c r="N330" s="39"/>
       <c r="O330" s="39"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A331" s="39"/>
       <c r="B331" s="39"/>
       <c r="C331" s="39"/>
@@ -9909,7 +9912,7 @@
       <c r="N331" s="39"/>
       <c r="O331" s="39"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A332" s="39"/>
       <c r="B332" s="39"/>
       <c r="C332" s="39"/>
@@ -9926,7 +9929,7 @@
       <c r="N332" s="39"/>
       <c r="O332" s="39"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A333" s="39"/>
       <c r="B333" s="39"/>
       <c r="C333" s="39"/>
@@ -9943,7 +9946,7 @@
       <c r="N333" s="39"/>
       <c r="O333" s="39"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A334" s="39"/>
       <c r="B334" s="39"/>
       <c r="C334" s="39"/>
@@ -9960,7 +9963,7 @@
       <c r="N334" s="39"/>
       <c r="O334" s="39"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A335" s="39"/>
       <c r="B335" s="39"/>
       <c r="C335" s="39"/>
@@ -9977,7 +9980,7 @@
       <c r="N335" s="39"/>
       <c r="O335" s="39"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A336" s="39"/>
       <c r="B336" s="39"/>
       <c r="C336" s="39"/>
@@ -9994,7 +9997,7 @@
       <c r="N336" s="39"/>
       <c r="O336" s="39"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A337" s="39"/>
       <c r="B337" s="39"/>
       <c r="C337" s="39"/>
@@ -10011,7 +10014,7 @@
       <c r="N337" s="39"/>
       <c r="O337" s="39"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A338" s="39"/>
       <c r="B338" s="39"/>
       <c r="C338" s="39"/>
@@ -10028,7 +10031,7 @@
       <c r="N338" s="39"/>
       <c r="O338" s="39"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A339" s="39"/>
       <c r="B339" s="39"/>
       <c r="C339" s="39"/>
@@ -10045,7 +10048,7 @@
       <c r="N339" s="39"/>
       <c r="O339" s="39"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A340" s="39"/>
       <c r="B340" s="39"/>
       <c r="C340" s="39"/>
@@ -10062,7 +10065,7 @@
       <c r="N340" s="39"/>
       <c r="O340" s="39"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A341" s="39"/>
       <c r="B341" s="39"/>
       <c r="C341" s="39"/>
@@ -10079,7 +10082,7 @@
       <c r="N341" s="39"/>
       <c r="O341" s="39"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A342" s="39"/>
       <c r="B342" s="39"/>
       <c r="C342" s="39"/>
@@ -10096,7 +10099,7 @@
       <c r="N342" s="39"/>
       <c r="O342" s="39"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A343" s="39"/>
       <c r="B343" s="39"/>
       <c r="C343" s="39"/>
@@ -10113,7 +10116,7 @@
       <c r="N343" s="39"/>
       <c r="O343" s="39"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A344" s="39"/>
       <c r="B344" s="39"/>
       <c r="C344" s="39"/>
@@ -10130,7 +10133,7 @@
       <c r="N344" s="39"/>
       <c r="O344" s="39"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A345" s="39"/>
       <c r="B345" s="39"/>
       <c r="C345" s="39"/>
@@ -10147,7 +10150,7 @@
       <c r="N345" s="39"/>
       <c r="O345" s="39"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="39"/>
@@ -10170,24 +10173,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
         <v>126</v>
       </c>
@@ -10204,7 +10207,7 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A5" s="24">
         <v>43070</v>
       </c>
@@ -10221,7 +10224,7 @@
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
     </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A6" s="39"/>
       <c r="B6" s="39" t="s">
         <v>112</v>
@@ -10236,7 +10239,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A7" s="39"/>
       <c r="B7" s="39" t="s">
         <v>113</v>
@@ -10251,7 +10254,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -10264,7 +10267,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="39"/>
       <c r="B9" s="39"/>
       <c r="C9" s="39"/>
@@ -10277,7 +10280,7 @@
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="39"/>
       <c r="B10" s="39"/>
       <c r="C10" s="39"/>
@@ -10290,7 +10293,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -10303,7 +10306,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -10316,7 +10319,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -10329,7 +10332,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -10342,7 +10345,7 @@
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -10355,7 +10358,7 @@
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
     </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -10368,7 +10371,7 @@
       <c r="J16" s="39"/>
       <c r="K16" s="39"/>
     </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -10381,7 +10384,7 @@
       <c r="J17" s="39"/>
       <c r="K17" s="39"/>
     </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -10394,7 +10397,7 @@
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
     </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>

</xml_diff>

<commit_message>
added container and content layout to implement a home button. home button is temporary, breadcrumb would be nice. switched css stuff on the different containers. modified scrum file
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="229">
   <si>
     <t>ID</t>
   </si>
@@ -716,6 +716,12 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>Model muss persistieren nicht der Presenter</t>
+  </si>
+  <si>
+    <t>Design ist nicht gerade der Bringer.</t>
   </si>
 </sst>
 </file>
@@ -1936,7 +1942,7 @@
   <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,10 +2164,10 @@
         <v>4</v>
       </c>
       <c r="J6" s="78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K6" s="78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L6" s="78" t="s">
         <v>8</v>
@@ -3105,7 +3111,7 @@
         <v>4</v>
       </c>
       <c r="J34" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K34" s="78">
         <v>0</v>
@@ -3143,7 +3149,7 @@
         <v>4</v>
       </c>
       <c r="J35" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K35" s="78">
         <v>0</v>
@@ -3181,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="J36" s="78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K36" s="78">
         <v>0</v>
@@ -3217,7 +3223,7 @@
         <v>4</v>
       </c>
       <c r="J37" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K37" s="78">
         <v>0</v>
@@ -3253,7 +3259,7 @@
         <v>4</v>
       </c>
       <c r="J38" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K38" s="78">
         <v>0</v>
@@ -3291,7 +3297,7 @@
         <v>2</v>
       </c>
       <c r="J39" s="78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K39" s="78">
         <v>0</v>
@@ -3329,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="J40" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40" s="78">
         <v>0</v>
@@ -3367,7 +3373,7 @@
         <v>3</v>
       </c>
       <c r="J41" s="78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K41" s="78">
         <v>0</v>
@@ -3399,7 +3405,7 @@
         <v>4</v>
       </c>
       <c r="J42" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K42" s="78">
         <v>0</v>
@@ -3589,7 +3595,7 @@
         <v>4</v>
       </c>
       <c r="J47" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K47" s="78">
         <v>0</v>
@@ -3627,7 +3633,7 @@
         <v>4</v>
       </c>
       <c r="J48" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K48" s="78">
         <v>0</v>
@@ -3665,7 +3671,7 @@
         <v>2</v>
       </c>
       <c r="J49" s="78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K49" s="78">
         <v>0</v>
@@ -3703,7 +3709,7 @@
         <v>5</v>
       </c>
       <c r="J50" s="78">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K50" s="78">
         <v>0</v>
@@ -3739,10 +3745,10 @@
         <v>3</v>
       </c>
       <c r="J51" s="88">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K51" s="88">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="L51" s="82" t="s">
         <v>8</v>
@@ -3884,11 +3890,11 @@
       </c>
       <c r="J58" s="1">
         <f>SUMIF(B2:B52,3,J2:J52)</f>
-        <v>10</v>
+        <v>63</v>
       </c>
       <c r="K58" s="1">
         <f>SUMIF(B2:B52,3,K2:K52)</f>
-        <v>10</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4118,27 +4124,27 @@
       <c r="H72" s="98"/>
       <c r="I72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"ziegm")</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="K72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"jntme")</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="L72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"kybup1")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M72" s="68">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"petim1")</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="N72" s="69">
         <f>SUMIFS(J$2:J$52,$B$2:$B$52,3,$F$2:$F$52,"odaoj1")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4243,7 +4249,7 @@
       <c r="H78" s="98"/>
       <c r="I78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="J78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"ziegm")</f>
@@ -10177,7 +10183,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10268,8 +10274,12 @@
       <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
+      <c r="A9" s="24">
+        <v>43091</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>227</v>
+      </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -10282,7 +10292,9 @@
     </row>
     <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
       <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
+      <c r="B10" s="39" t="s">
+        <v>228</v>
+      </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>

</xml_diff>

<commit_message>
added a new topview "activityView", implemented the url navigation
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="230">
   <si>
     <t>ID</t>
   </si>
@@ -722,6 +722,9 @@
   </si>
   <si>
     <t>Design ist nicht gerade der Bringer.</t>
+  </si>
+  <si>
+    <t>to define ob no öppis mues gmacht wärde, süsch erledigt dür säschu</t>
   </si>
 </sst>
 </file>
@@ -1942,7 +1945,7 @@
   <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3044,7 +3047,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="79" t="s">
         <v>222</v>
       </c>
@@ -3082,7 +3085,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="79" t="s">
         <v>223</v>
       </c>
@@ -3119,8 +3122,11 @@
       <c r="L34" s="78" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="M34" s="78" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="79" t="s">
         <v>224</v>
       </c>
@@ -3158,7 +3164,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="79" t="s">
         <v>225</v>
       </c>
@@ -3190,13 +3196,13 @@
         <v>3</v>
       </c>
       <c r="K36" s="78">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="L36" s="78" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="79"/>
       <c r="B37" s="80">
         <v>3</v>
@@ -3232,7 +3238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="79"/>
       <c r="B38" s="80">
         <v>3</v>
@@ -3268,7 +3274,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="79" t="s">
         <v>212</v>
       </c>
@@ -3306,7 +3312,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="79" t="s">
         <v>213</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="79" t="s">
         <v>214</v>
       </c>
@@ -3382,7 +3388,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="79" t="s">
         <v>215</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="52" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" s="52" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="64" t="s">
         <v>116</v>
       </c>
@@ -3452,7 +3458,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="64" t="s">
         <v>131</v>
       </c>
@@ -3490,7 +3496,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="64" t="s">
         <v>133</v>
       </c>
@@ -3528,7 +3534,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="64" t="s">
         <v>146</v>
       </c>
@@ -3566,7 +3572,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="79" t="s">
         <v>218</v>
       </c>
@@ -3894,7 +3900,7 @@
       </c>
       <c r="K58" s="1">
         <f>SUMIF(B2:B52,3,K2:K52)</f>
-        <v>14.5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="61" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4249,7 +4255,7 @@
       <c r="H78" s="98"/>
       <c r="I78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"gfels6")</f>
-        <v>4.5</v>
+        <v>9</v>
       </c>
       <c r="J78" s="68">
         <f>SUMIFS(K$2:K$52,$B$2:$B$52,3,$F$2:$F$52,"ziegm")</f>

</xml_diff>

<commit_message>
delete captions from buttons // update scrum
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michi\workspace\ch.bfh.btx8081.w2017.blue\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\03_Sem_HS\BTX8081_SoftwareEngineeringAndDesign\Eclipse\ch.bfh.btx8081.w2017.blue.git\doc\04-ScrumSetup\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8592" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -1559,14 +1559,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1665,19 +1665,19 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1954,30 +1954,30 @@
   <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L52" sqref="L52"/>
+      <selection activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="25" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.140625" style="1"/>
-    <col min="16" max="16" width="8.140625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.33203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.109375" style="1"/>
+    <col min="16" max="16" width="8.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="43" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="43" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41">
         <v>0.1</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
         <v>66</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>67</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="50" t="s">
         <v>164</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="79" t="s">
         <v>219</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="75">
         <v>1.1000000000000001</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="75">
         <v>1.2</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="70">
         <v>1.3</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>63</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>41</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="59">
         <v>2.2000000000000002</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="87">
         <v>2.2999999999999998</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
         <v>3.1</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="32">
         <v>3.2</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="28" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>39</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" s="28" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
         <v>40</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="28" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="28" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>72</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="59" t="s">
         <v>118</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="59" t="s">
         <v>118</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="58" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" s="58" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="59" t="s">
         <v>122</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="32">
         <v>3.3</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="32">
         <v>3.4</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="58" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="58" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="59" t="s">
         <v>137</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="59" t="s">
         <v>141</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32">
         <v>3.5</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26">
         <v>3.6</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="56" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" s="56" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
         <v>160</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="52" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" s="52" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="50">
         <v>4.0999999999999996</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="79" t="s">
         <v>221</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="79" t="s">
         <v>220</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="79" t="s">
         <v>222</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="79" t="s">
         <v>223</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="79" t="s">
         <v>224</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="79" t="s">
         <v>225</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="79"/>
       <c r="B37" s="80">
         <v>3</v>
@@ -3250,7 +3250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="79"/>
       <c r="B38" s="80">
         <v>3</v>
@@ -3286,7 +3286,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="79" t="s">
         <v>212</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="79" t="s">
         <v>213</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="78" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" s="78" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="79" t="s">
         <v>214</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" s="78" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A42" s="79" t="s">
         <v>215</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="52" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" s="52" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="64" t="s">
         <v>116</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="64" t="s">
         <v>131</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="64" t="s">
         <v>133</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="64" t="s">
         <v>146</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="79" t="s">
         <v>233</v>
       </c>
@@ -3660,13 +3660,13 @@
         <v>4</v>
       </c>
       <c r="K48" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L48" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="79" t="s">
         <v>217</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:17" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="79" t="s">
         <v>229</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:17" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="83" t="s">
         <v>216</v>
       </c>
@@ -3780,7 +3780,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:17" s="82" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" s="82" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="83" t="s">
         <v>234</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="84">
         <v>7.11</v>
       </c>
@@ -3847,16 +3847,16 @@
         <v>2</v>
       </c>
       <c r="J53" s="84">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K53" s="84">
-        <v>0</v>
+        <v>2.75</v>
       </c>
       <c r="L53" s="84" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="86">
         <v>7.12</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" s="52" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="64" t="s">
         <v>158</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A56" s="16"/>
       <c r="B56" s="17"/>
       <c r="C56" s="18"/>
@@ -3937,7 +3937,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A57" s="16"/>
       <c r="B57" s="17"/>
       <c r="C57" s="18"/>
@@ -3949,7 +3949,7 @@
       <c r="P57" s="91"/>
       <c r="Q57" s="91"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E58" s="18"/>
       <c r="F58" s="22"/>
       <c r="G58" s="18"/>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E59" s="1" t="s">
         <v>152</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E60" s="1" t="s">
         <v>153</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E61" s="1" t="s">
         <v>154</v>
       </c>
@@ -4021,15 +4021,15 @@
       </c>
       <c r="J61" s="1">
         <f>SUMIF(B2:B55,3,J2:J55)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K61" s="1">
         <f>SUMIF(B2:B55,3,K2:K55)</f>
-        <v>35.5</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="7:14" x14ac:dyDescent="0.25">
+        <v>42.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G65" s="96" t="s">
         <v>54</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="M65" s="97"/>
       <c r="N65" s="98"/>
     </row>
-    <row r="66" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G66" s="66"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
@@ -4063,7 +4063,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G67" s="92" t="s">
         <v>148</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G68" s="92" t="s">
         <v>149</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G69" s="94" t="s">
         <v>150</v>
       </c>
@@ -4153,8 +4153,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G71" s="96" t="s">
         <v>55</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="M71" s="97"/>
       <c r="N71" s="98"/>
     </row>
-    <row r="72" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G72" s="66"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18" t="s">
@@ -4188,7 +4188,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G73" s="92" t="s">
         <v>148</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G74" s="92" t="s">
         <v>149</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G75" s="94" t="s">
         <v>150</v>
       </c>
@@ -4271,15 +4271,15 @@
       </c>
       <c r="M75" s="68">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"petim1")</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N75" s="69">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"odaoj1")</f>
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G77" s="96" t="s">
         <v>56</v>
       </c>
@@ -4291,7 +4291,7 @@
       <c r="M77" s="97"/>
       <c r="N77" s="98"/>
     </row>
-    <row r="78" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G78" s="66"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18" t="s">
@@ -4313,7 +4313,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G79" s="92" t="s">
         <v>148</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G80" s="92" t="s">
         <v>149</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G81" s="94" t="s">
         <v>150</v>
       </c>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="M81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"petim1")</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
       <c r="N81" s="69">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"odaoj1")</f>
@@ -4448,14 +4448,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -4469,10 +4469,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -4489,17 +4489,17 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="39">
         <v>1</v>
       </c>
@@ -4533,7 +4533,7 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -4556,7 +4556,7 @@
       <c r="N9" s="39"/>
       <c r="O9" s="39"/>
     </row>
-    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="40">
         <v>1</v>
       </c>
@@ -4579,7 +4579,7 @@
       <c r="N10" s="39"/>
       <c r="O10" s="39"/>
     </row>
-    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="40"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39" t="s">
@@ -4598,7 +4598,7 @@
       <c r="N11" s="39"/>
       <c r="O11" s="39"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39" t="s">
@@ -4617,7 +4617,7 @@
       <c r="N12" s="39"/>
       <c r="O12" s="39"/>
     </row>
-    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="40">
         <v>1</v>
       </c>
@@ -4640,7 +4640,7 @@
       <c r="N13" s="39"/>
       <c r="O13" s="39"/>
     </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="40">
         <v>2</v>
       </c>
@@ -4663,7 +4663,7 @@
       <c r="N14" s="39"/>
       <c r="O14" s="39"/>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="40"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -4680,7 +4680,7 @@
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
     </row>
-    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="40"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -4697,7 +4697,7 @@
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
     </row>
-    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="40"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -4714,7 +4714,7 @@
       <c r="N17" s="39"/>
       <c r="O17" s="39"/>
     </row>
-    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="40"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -4731,7 +4731,7 @@
       <c r="N18" s="39"/>
       <c r="O18" s="39"/>
     </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="40"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -4748,7 +4748,7 @@
       <c r="N19" s="39"/>
       <c r="O19" s="39"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A20" s="40"/>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
@@ -4765,7 +4765,7 @@
       <c r="N20" s="39"/>
       <c r="O20" s="39"/>
     </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A21" s="40"/>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
@@ -4782,7 +4782,7 @@
       <c r="N21" s="39"/>
       <c r="O21" s="39"/>
     </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A22" s="40"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
@@ -4799,7 +4799,7 @@
       <c r="N22" s="39"/>
       <c r="O22" s="39"/>
     </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A23" s="40"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -4816,7 +4816,7 @@
       <c r="N23" s="39"/>
       <c r="O23" s="39"/>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A24" s="40"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -4833,7 +4833,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="40"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -4850,7 +4850,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A26" s="40"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -4867,7 +4867,7 @@
       <c r="N26" s="39"/>
       <c r="O26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A27" s="40"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
@@ -4884,7 +4884,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A28" s="40"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -4901,7 +4901,7 @@
       <c r="N28" s="39"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A29" s="40"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -4918,7 +4918,7 @@
       <c r="N29" s="39"/>
       <c r="O29" s="39"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="40"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -4935,7 +4935,7 @@
       <c r="N30" s="39"/>
       <c r="O30" s="39"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A31" s="40"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -4952,7 +4952,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="39"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A32" s="40"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -4969,7 +4969,7 @@
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A33" s="40"/>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -4986,7 +4986,7 @@
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A34" s="40"/>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -5003,7 +5003,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A35" s="40"/>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -5020,7 +5020,7 @@
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A36" s="40"/>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
@@ -5037,7 +5037,7 @@
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A37" s="40"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -5054,7 +5054,7 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A38" s="40"/>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
@@ -5071,7 +5071,7 @@
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A39" s="40"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -5088,7 +5088,7 @@
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A40" s="40"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -5105,7 +5105,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A41" s="40"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -5122,7 +5122,7 @@
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A42" s="40"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
@@ -5139,7 +5139,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A43" s="40"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -5156,7 +5156,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A44" s="40"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -5173,7 +5173,7 @@
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A45" s="40"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -5190,7 +5190,7 @@
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A46" s="40"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -5207,7 +5207,7 @@
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A47" s="40"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -5224,7 +5224,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A48" s="40"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -5241,7 +5241,7 @@
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A49" s="40"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -5258,7 +5258,7 @@
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A50" s="40"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -5275,7 +5275,7 @@
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A51" s="40"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -5292,7 +5292,7 @@
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A52" s="40"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -5309,7 +5309,7 @@
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A53" s="40"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -5326,7 +5326,7 @@
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A54" s="40"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -5343,7 +5343,7 @@
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A55" s="40"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -5360,7 +5360,7 @@
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A56" s="40"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -5377,7 +5377,7 @@
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A57" s="40"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -5394,7 +5394,7 @@
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -5411,7 +5411,7 @@
       <c r="N58" s="39"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -5428,7 +5428,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="39"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -5445,7 +5445,7 @@
       <c r="N60" s="39"/>
       <c r="O60" s="39"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -5462,7 +5462,7 @@
       <c r="N61" s="39"/>
       <c r="O61" s="39"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -5479,7 +5479,7 @@
       <c r="N62" s="39"/>
       <c r="O62" s="39"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -5496,7 +5496,7 @@
       <c r="N63" s="39"/>
       <c r="O63" s="39"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -5513,7 +5513,7 @@
       <c r="N64" s="39"/>
       <c r="O64" s="39"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -5530,7 +5530,7 @@
       <c r="N65" s="39"/>
       <c r="O65" s="39"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -5547,7 +5547,7 @@
       <c r="N66" s="39"/>
       <c r="O66" s="39"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -5564,7 +5564,7 @@
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -5581,7 +5581,7 @@
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -5598,7 +5598,7 @@
       <c r="N69" s="39"/>
       <c r="O69" s="39"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -5615,7 +5615,7 @@
       <c r="N70" s="39"/>
       <c r="O70" s="39"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -5632,7 +5632,7 @@
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -5649,7 +5649,7 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -5666,7 +5666,7 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -5683,7 +5683,7 @@
       <c r="N74" s="39"/>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -5700,7 +5700,7 @@
       <c r="N75" s="39"/>
       <c r="O75" s="39"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -5717,7 +5717,7 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -5734,7 +5734,7 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -5751,7 +5751,7 @@
       <c r="N78" s="39"/>
       <c r="O78" s="39"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -5768,7 +5768,7 @@
       <c r="N79" s="39"/>
       <c r="O79" s="39"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -5785,7 +5785,7 @@
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -5802,7 +5802,7 @@
       <c r="N81" s="39"/>
       <c r="O81" s="39"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -5819,7 +5819,7 @@
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -5836,7 +5836,7 @@
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -5853,7 +5853,7 @@
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -5870,7 +5870,7 @@
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -5887,7 +5887,7 @@
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -5904,7 +5904,7 @@
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -5921,7 +5921,7 @@
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -5938,7 +5938,7 @@
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -5955,7 +5955,7 @@
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -5972,7 +5972,7 @@
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -5989,7 +5989,7 @@
       <c r="N92" s="39"/>
       <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -6006,7 +6006,7 @@
       <c r="N93" s="39"/>
       <c r="O93" s="39"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -6023,7 +6023,7 @@
       <c r="N94" s="39"/>
       <c r="O94" s="39"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -6040,7 +6040,7 @@
       <c r="N95" s="39"/>
       <c r="O95" s="39"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -6057,7 +6057,7 @@
       <c r="N96" s="39"/>
       <c r="O96" s="39"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -6074,7 +6074,7 @@
       <c r="N97" s="39"/>
       <c r="O97" s="39"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -6091,7 +6091,7 @@
       <c r="N98" s="39"/>
       <c r="O98" s="39"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -6108,7 +6108,7 @@
       <c r="N99" s="39"/>
       <c r="O99" s="39"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A100" s="39"/>
       <c r="B100" s="39"/>
       <c r="C100" s="39"/>
@@ -6125,7 +6125,7 @@
       <c r="N100" s="39"/>
       <c r="O100" s="39"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A101" s="39"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -6142,7 +6142,7 @@
       <c r="N101" s="39"/>
       <c r="O101" s="39"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A102" s="39"/>
       <c r="B102" s="39"/>
       <c r="C102" s="39"/>
@@ -6159,7 +6159,7 @@
       <c r="N102" s="39"/>
       <c r="O102" s="39"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A103" s="39"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -6176,7 +6176,7 @@
       <c r="N103" s="39"/>
       <c r="O103" s="39"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -6193,7 +6193,7 @@
       <c r="N104" s="39"/>
       <c r="O104" s="39"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A105" s="39"/>
       <c r="B105" s="39"/>
       <c r="C105" s="39"/>
@@ -6210,7 +6210,7 @@
       <c r="N105" s="39"/>
       <c r="O105" s="39"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A106" s="39"/>
       <c r="B106" s="39"/>
       <c r="C106" s="39"/>
@@ -6227,7 +6227,7 @@
       <c r="N106" s="39"/>
       <c r="O106" s="39"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A107" s="39"/>
       <c r="B107" s="39"/>
       <c r="C107" s="39"/>
@@ -6244,7 +6244,7 @@
       <c r="N107" s="39"/>
       <c r="O107" s="39"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A108" s="39"/>
       <c r="B108" s="39"/>
       <c r="C108" s="39"/>
@@ -6261,7 +6261,7 @@
       <c r="N108" s="39"/>
       <c r="O108" s="39"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A109" s="39"/>
       <c r="B109" s="39"/>
       <c r="C109" s="39"/>
@@ -6278,7 +6278,7 @@
       <c r="N109" s="39"/>
       <c r="O109" s="39"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A110" s="39"/>
       <c r="B110" s="39"/>
       <c r="C110" s="39"/>
@@ -6295,7 +6295,7 @@
       <c r="N110" s="39"/>
       <c r="O110" s="39"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A111" s="39"/>
       <c r="B111" s="39"/>
       <c r="C111" s="39"/>
@@ -6312,7 +6312,7 @@
       <c r="N111" s="39"/>
       <c r="O111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A112" s="39"/>
       <c r="B112" s="39"/>
       <c r="C112" s="39"/>
@@ -6329,7 +6329,7 @@
       <c r="N112" s="39"/>
       <c r="O112" s="39"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A113" s="39"/>
       <c r="B113" s="39"/>
       <c r="C113" s="39"/>
@@ -6346,7 +6346,7 @@
       <c r="N113" s="39"/>
       <c r="O113" s="39"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A114" s="39"/>
       <c r="B114" s="39"/>
       <c r="C114" s="39"/>
@@ -6363,7 +6363,7 @@
       <c r="N114" s="39"/>
       <c r="O114" s="39"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A115" s="39"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
@@ -6380,7 +6380,7 @@
       <c r="N115" s="39"/>
       <c r="O115" s="39"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A116" s="39"/>
       <c r="B116" s="39"/>
       <c r="C116" s="39"/>
@@ -6397,7 +6397,7 @@
       <c r="N116" s="39"/>
       <c r="O116" s="39"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A117" s="39"/>
       <c r="B117" s="39"/>
       <c r="C117" s="39"/>
@@ -6414,7 +6414,7 @@
       <c r="N117" s="39"/>
       <c r="O117" s="39"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A118" s="39"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
@@ -6431,7 +6431,7 @@
       <c r="N118" s="39"/>
       <c r="O118" s="39"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A119" s="39"/>
       <c r="B119" s="39"/>
       <c r="C119" s="39"/>
@@ -6448,7 +6448,7 @@
       <c r="N119" s="39"/>
       <c r="O119" s="39"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -6465,7 +6465,7 @@
       <c r="N120" s="39"/>
       <c r="O120" s="39"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A121" s="39"/>
       <c r="B121" s="39"/>
       <c r="C121" s="39"/>
@@ -6482,7 +6482,7 @@
       <c r="N121" s="39"/>
       <c r="O121" s="39"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A122" s="39"/>
       <c r="B122" s="39"/>
       <c r="C122" s="39"/>
@@ -6499,7 +6499,7 @@
       <c r="N122" s="39"/>
       <c r="O122" s="39"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A123" s="39"/>
       <c r="B123" s="39"/>
       <c r="C123" s="39"/>
@@ -6516,7 +6516,7 @@
       <c r="N123" s="39"/>
       <c r="O123" s="39"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A124" s="39"/>
       <c r="B124" s="39"/>
       <c r="C124" s="39"/>
@@ -6533,7 +6533,7 @@
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A125" s="39"/>
       <c r="B125" s="39"/>
       <c r="C125" s="39"/>
@@ -6550,7 +6550,7 @@
       <c r="N125" s="39"/>
       <c r="O125" s="39"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A126" s="39"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -6567,7 +6567,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="39"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A127" s="39"/>
       <c r="B127" s="39"/>
       <c r="C127" s="39"/>
@@ -6584,7 +6584,7 @@
       <c r="N127" s="39"/>
       <c r="O127" s="39"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39"/>
@@ -6601,7 +6601,7 @@
       <c r="N128" s="39"/>
       <c r="O128" s="39"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39"/>
@@ -6618,7 +6618,7 @@
       <c r="N129" s="39"/>
       <c r="O129" s="39"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39"/>
@@ -6635,7 +6635,7 @@
       <c r="N130" s="39"/>
       <c r="O130" s="39"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -6652,7 +6652,7 @@
       <c r="N131" s="39"/>
       <c r="O131" s="39"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -6669,7 +6669,7 @@
       <c r="N132" s="39"/>
       <c r="O132" s="39"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A133" s="39"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
@@ -6686,7 +6686,7 @@
       <c r="N133" s="39"/>
       <c r="O133" s="39"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A134" s="39"/>
       <c r="B134" s="39"/>
       <c r="C134" s="39"/>
@@ -6703,7 +6703,7 @@
       <c r="N134" s="39"/>
       <c r="O134" s="39"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -6720,7 +6720,7 @@
       <c r="N135" s="39"/>
       <c r="O135" s="39"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A136" s="39"/>
       <c r="B136" s="39"/>
       <c r="C136" s="39"/>
@@ -6737,7 +6737,7 @@
       <c r="N136" s="39"/>
       <c r="O136" s="39"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A137" s="39"/>
       <c r="B137" s="39"/>
       <c r="C137" s="39"/>
@@ -6754,7 +6754,7 @@
       <c r="N137" s="39"/>
       <c r="O137" s="39"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A138" s="39"/>
       <c r="B138" s="39"/>
       <c r="C138" s="39"/>
@@ -6771,7 +6771,7 @@
       <c r="N138" s="39"/>
       <c r="O138" s="39"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A139" s="39"/>
       <c r="B139" s="39"/>
       <c r="C139" s="39"/>
@@ -6788,7 +6788,7 @@
       <c r="N139" s="39"/>
       <c r="O139" s="39"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A140" s="39"/>
       <c r="B140" s="39"/>
       <c r="C140" s="39"/>
@@ -6805,7 +6805,7 @@
       <c r="N140" s="39"/>
       <c r="O140" s="39"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A141" s="39"/>
       <c r="B141" s="39"/>
       <c r="C141" s="39"/>
@@ -6822,7 +6822,7 @@
       <c r="N141" s="39"/>
       <c r="O141" s="39"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A142" s="39"/>
       <c r="B142" s="39"/>
       <c r="C142" s="39"/>
@@ -6839,7 +6839,7 @@
       <c r="N142" s="39"/>
       <c r="O142" s="39"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A143" s="39"/>
       <c r="B143" s="39"/>
       <c r="C143" s="39"/>
@@ -6856,7 +6856,7 @@
       <c r="N143" s="39"/>
       <c r="O143" s="39"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A144" s="39"/>
       <c r="B144" s="39"/>
       <c r="C144" s="39"/>
@@ -6873,7 +6873,7 @@
       <c r="N144" s="39"/>
       <c r="O144" s="39"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A145" s="39"/>
       <c r="B145" s="39"/>
       <c r="C145" s="39"/>
@@ -6890,7 +6890,7 @@
       <c r="N145" s="39"/>
       <c r="O145" s="39"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A146" s="39"/>
       <c r="B146" s="39"/>
       <c r="C146" s="39"/>
@@ -6907,7 +6907,7 @@
       <c r="N146" s="39"/>
       <c r="O146" s="39"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A147" s="39"/>
       <c r="B147" s="39"/>
       <c r="C147" s="39"/>
@@ -6924,7 +6924,7 @@
       <c r="N147" s="39"/>
       <c r="O147" s="39"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A148" s="39"/>
       <c r="B148" s="39"/>
       <c r="C148" s="39"/>
@@ -6941,7 +6941,7 @@
       <c r="N148" s="39"/>
       <c r="O148" s="39"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A149" s="39"/>
       <c r="B149" s="39"/>
       <c r="C149" s="39"/>
@@ -6958,7 +6958,7 @@
       <c r="N149" s="39"/>
       <c r="O149" s="39"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A150" s="39"/>
       <c r="B150" s="39"/>
       <c r="C150" s="39"/>
@@ -6975,7 +6975,7 @@
       <c r="N150" s="39"/>
       <c r="O150" s="39"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A151" s="39"/>
       <c r="B151" s="39"/>
       <c r="C151" s="39"/>
@@ -6992,7 +6992,7 @@
       <c r="N151" s="39"/>
       <c r="O151" s="39"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A152" s="39"/>
       <c r="B152" s="39"/>
       <c r="C152" s="39"/>
@@ -7009,7 +7009,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A153" s="39"/>
       <c r="B153" s="39"/>
       <c r="C153" s="39"/>
@@ -7026,7 +7026,7 @@
       <c r="N153" s="39"/>
       <c r="O153" s="39"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A154" s="39"/>
       <c r="B154" s="39"/>
       <c r="C154" s="39"/>
@@ -7043,7 +7043,7 @@
       <c r="N154" s="39"/>
       <c r="O154" s="39"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A155" s="39"/>
       <c r="B155" s="39"/>
       <c r="C155" s="39"/>
@@ -7060,7 +7060,7 @@
       <c r="N155" s="39"/>
       <c r="O155" s="39"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A156" s="39"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
@@ -7077,7 +7077,7 @@
       <c r="N156" s="39"/>
       <c r="O156" s="39"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A157" s="39"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
@@ -7094,7 +7094,7 @@
       <c r="N157" s="39"/>
       <c r="O157" s="39"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A158" s="39"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -7111,7 +7111,7 @@
       <c r="N158" s="39"/>
       <c r="O158" s="39"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A159" s="39"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -7128,7 +7128,7 @@
       <c r="N159" s="39"/>
       <c r="O159" s="39"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A160" s="39"/>
       <c r="B160" s="39"/>
       <c r="C160" s="39"/>
@@ -7145,7 +7145,7 @@
       <c r="N160" s="39"/>
       <c r="O160" s="39"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A161" s="39"/>
       <c r="B161" s="39"/>
       <c r="C161" s="39"/>
@@ -7162,7 +7162,7 @@
       <c r="N161" s="39"/>
       <c r="O161" s="39"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A162" s="39"/>
       <c r="B162" s="39"/>
       <c r="C162" s="39"/>
@@ -7179,7 +7179,7 @@
       <c r="N162" s="39"/>
       <c r="O162" s="39"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A163" s="39"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
@@ -7196,7 +7196,7 @@
       <c r="N163" s="39"/>
       <c r="O163" s="39"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A164" s="39"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
@@ -7213,7 +7213,7 @@
       <c r="N164" s="39"/>
       <c r="O164" s="39"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A165" s="39"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
@@ -7230,7 +7230,7 @@
       <c r="N165" s="39"/>
       <c r="O165" s="39"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A166" s="39"/>
       <c r="B166" s="39"/>
       <c r="C166" s="39"/>
@@ -7247,7 +7247,7 @@
       <c r="N166" s="39"/>
       <c r="O166" s="39"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A167" s="39"/>
       <c r="B167" s="39"/>
       <c r="C167" s="39"/>
@@ -7264,7 +7264,7 @@
       <c r="N167" s="39"/>
       <c r="O167" s="39"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A168" s="39"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -7281,7 +7281,7 @@
       <c r="N168" s="39"/>
       <c r="O168" s="39"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A169" s="39"/>
       <c r="B169" s="39"/>
       <c r="C169" s="39"/>
@@ -7298,7 +7298,7 @@
       <c r="N169" s="39"/>
       <c r="O169" s="39"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A170" s="39"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
@@ -7315,7 +7315,7 @@
       <c r="N170" s="39"/>
       <c r="O170" s="39"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A171" s="39"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -7332,7 +7332,7 @@
       <c r="N171" s="39"/>
       <c r="O171" s="39"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A172" s="39"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
@@ -7349,7 +7349,7 @@
       <c r="N172" s="39"/>
       <c r="O172" s="39"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A173" s="39"/>
       <c r="B173" s="39"/>
       <c r="C173" s="39"/>
@@ -7366,7 +7366,7 @@
       <c r="N173" s="39"/>
       <c r="O173" s="39"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A174" s="39"/>
       <c r="B174" s="39"/>
       <c r="C174" s="39"/>
@@ -7383,7 +7383,7 @@
       <c r="N174" s="39"/>
       <c r="O174" s="39"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A175" s="39"/>
       <c r="B175" s="39"/>
       <c r="C175" s="39"/>
@@ -7400,7 +7400,7 @@
       <c r="N175" s="39"/>
       <c r="O175" s="39"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A176" s="39"/>
       <c r="B176" s="39"/>
       <c r="C176" s="39"/>
@@ -7417,7 +7417,7 @@
       <c r="N176" s="39"/>
       <c r="O176" s="39"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A177" s="39"/>
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
@@ -7434,7 +7434,7 @@
       <c r="N177" s="39"/>
       <c r="O177" s="39"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A178" s="39"/>
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
@@ -7451,7 +7451,7 @@
       <c r="N178" s="39"/>
       <c r="O178" s="39"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A179" s="39"/>
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
@@ -7468,7 +7468,7 @@
       <c r="N179" s="39"/>
       <c r="O179" s="39"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A180" s="39"/>
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
@@ -7485,7 +7485,7 @@
       <c r="N180" s="39"/>
       <c r="O180" s="39"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A181" s="39"/>
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
@@ -7502,7 +7502,7 @@
       <c r="N181" s="39"/>
       <c r="O181" s="39"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A182" s="39"/>
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
@@ -7519,7 +7519,7 @@
       <c r="N182" s="39"/>
       <c r="O182" s="39"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A183" s="39"/>
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
@@ -7536,7 +7536,7 @@
       <c r="N183" s="39"/>
       <c r="O183" s="39"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A184" s="39"/>
       <c r="B184" s="39"/>
       <c r="C184" s="39"/>
@@ -7553,7 +7553,7 @@
       <c r="N184" s="39"/>
       <c r="O184" s="39"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
       <c r="C185" s="39"/>
@@ -7570,7 +7570,7 @@
       <c r="N185" s="39"/>
       <c r="O185" s="39"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
       <c r="C186" s="39"/>
@@ -7587,7 +7587,7 @@
       <c r="N186" s="39"/>
       <c r="O186" s="39"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A187" s="39"/>
       <c r="B187" s="39"/>
       <c r="C187" s="39"/>
@@ -7604,7 +7604,7 @@
       <c r="N187" s="39"/>
       <c r="O187" s="39"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A188" s="39"/>
       <c r="B188" s="39"/>
       <c r="C188" s="39"/>
@@ -7621,7 +7621,7 @@
       <c r="N188" s="39"/>
       <c r="O188" s="39"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A189" s="39"/>
       <c r="B189" s="39"/>
       <c r="C189" s="39"/>
@@ -7638,7 +7638,7 @@
       <c r="N189" s="39"/>
       <c r="O189" s="39"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A190" s="39"/>
       <c r="B190" s="39"/>
       <c r="C190" s="39"/>
@@ -7655,7 +7655,7 @@
       <c r="N190" s="39"/>
       <c r="O190" s="39"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A191" s="39"/>
       <c r="B191" s="39"/>
       <c r="C191" s="39"/>
@@ -7672,7 +7672,7 @@
       <c r="N191" s="39"/>
       <c r="O191" s="39"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A192" s="39"/>
       <c r="B192" s="39"/>
       <c r="C192" s="39"/>
@@ -7689,7 +7689,7 @@
       <c r="N192" s="39"/>
       <c r="O192" s="39"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A193" s="39"/>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -7706,7 +7706,7 @@
       <c r="N193" s="39"/>
       <c r="O193" s="39"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A194" s="39"/>
       <c r="B194" s="39"/>
       <c r="C194" s="39"/>
@@ -7723,7 +7723,7 @@
       <c r="N194" s="39"/>
       <c r="O194" s="39"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A195" s="39"/>
       <c r="B195" s="39"/>
       <c r="C195" s="39"/>
@@ -7740,7 +7740,7 @@
       <c r="N195" s="39"/>
       <c r="O195" s="39"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A196" s="39"/>
       <c r="B196" s="39"/>
       <c r="C196" s="39"/>
@@ -7757,7 +7757,7 @@
       <c r="N196" s="39"/>
       <c r="O196" s="39"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A197" s="39"/>
       <c r="B197" s="39"/>
       <c r="C197" s="39"/>
@@ -7774,7 +7774,7 @@
       <c r="N197" s="39"/>
       <c r="O197" s="39"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A198" s="39"/>
       <c r="B198" s="39"/>
       <c r="C198" s="39"/>
@@ -7791,7 +7791,7 @@
       <c r="N198" s="39"/>
       <c r="O198" s="39"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A199" s="39"/>
       <c r="B199" s="39"/>
       <c r="C199" s="39"/>
@@ -7808,7 +7808,7 @@
       <c r="N199" s="39"/>
       <c r="O199" s="39"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A200" s="39"/>
       <c r="B200" s="39"/>
       <c r="C200" s="39"/>
@@ -7825,7 +7825,7 @@
       <c r="N200" s="39"/>
       <c r="O200" s="39"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A201" s="39"/>
       <c r="B201" s="39"/>
       <c r="C201" s="39"/>
@@ -7842,7 +7842,7 @@
       <c r="N201" s="39"/>
       <c r="O201" s="39"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A202" s="39"/>
       <c r="B202" s="39"/>
       <c r="C202" s="39"/>
@@ -7859,7 +7859,7 @@
       <c r="N202" s="39"/>
       <c r="O202" s="39"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A203" s="39"/>
       <c r="B203" s="39"/>
       <c r="C203" s="39"/>
@@ -7876,7 +7876,7 @@
       <c r="N203" s="39"/>
       <c r="O203" s="39"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A204" s="39"/>
       <c r="B204" s="39"/>
       <c r="C204" s="39"/>
@@ -7893,7 +7893,7 @@
       <c r="N204" s="39"/>
       <c r="O204" s="39"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A205" s="39"/>
       <c r="B205" s="39"/>
       <c r="C205" s="39"/>
@@ -7910,7 +7910,7 @@
       <c r="N205" s="39"/>
       <c r="O205" s="39"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A206" s="39"/>
       <c r="B206" s="39"/>
       <c r="C206" s="39"/>
@@ -7927,7 +7927,7 @@
       <c r="N206" s="39"/>
       <c r="O206" s="39"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A207" s="39"/>
       <c r="B207" s="39"/>
       <c r="C207" s="39"/>
@@ -7944,7 +7944,7 @@
       <c r="N207" s="39"/>
       <c r="O207" s="39"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A208" s="39"/>
       <c r="B208" s="39"/>
       <c r="C208" s="39"/>
@@ -7961,7 +7961,7 @@
       <c r="N208" s="39"/>
       <c r="O208" s="39"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A209" s="39"/>
       <c r="B209" s="39"/>
       <c r="C209" s="39"/>
@@ -7978,7 +7978,7 @@
       <c r="N209" s="39"/>
       <c r="O209" s="39"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A210" s="39"/>
       <c r="B210" s="39"/>
       <c r="C210" s="39"/>
@@ -7995,7 +7995,7 @@
       <c r="N210" s="39"/>
       <c r="O210" s="39"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A211" s="39"/>
       <c r="B211" s="39"/>
       <c r="C211" s="39"/>
@@ -8012,7 +8012,7 @@
       <c r="N211" s="39"/>
       <c r="O211" s="39"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A212" s="39"/>
       <c r="B212" s="39"/>
       <c r="C212" s="39"/>
@@ -8029,7 +8029,7 @@
       <c r="N212" s="39"/>
       <c r="O212" s="39"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A213" s="39"/>
       <c r="B213" s="39"/>
       <c r="C213" s="39"/>
@@ -8046,7 +8046,7 @@
       <c r="N213" s="39"/>
       <c r="O213" s="39"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A214" s="39"/>
       <c r="B214" s="39"/>
       <c r="C214" s="39"/>
@@ -8063,7 +8063,7 @@
       <c r="N214" s="39"/>
       <c r="O214" s="39"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A215" s="39"/>
       <c r="B215" s="39"/>
       <c r="C215" s="39"/>
@@ -8080,7 +8080,7 @@
       <c r="N215" s="39"/>
       <c r="O215" s="39"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A216" s="39"/>
       <c r="B216" s="39"/>
       <c r="C216" s="39"/>
@@ -8097,7 +8097,7 @@
       <c r="N216" s="39"/>
       <c r="O216" s="39"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A217" s="39"/>
       <c r="B217" s="39"/>
       <c r="C217" s="39"/>
@@ -8114,7 +8114,7 @@
       <c r="N217" s="39"/>
       <c r="O217" s="39"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A218" s="39"/>
       <c r="B218" s="39"/>
       <c r="C218" s="39"/>
@@ -8131,7 +8131,7 @@
       <c r="N218" s="39"/>
       <c r="O218" s="39"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A219" s="39"/>
       <c r="B219" s="39"/>
       <c r="C219" s="39"/>
@@ -8148,7 +8148,7 @@
       <c r="N219" s="39"/>
       <c r="O219" s="39"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A220" s="39"/>
       <c r="B220" s="39"/>
       <c r="C220" s="39"/>
@@ -8165,7 +8165,7 @@
       <c r="N220" s="39"/>
       <c r="O220" s="39"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A221" s="39"/>
       <c r="B221" s="39"/>
       <c r="C221" s="39"/>
@@ -8182,7 +8182,7 @@
       <c r="N221" s="39"/>
       <c r="O221" s="39"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A222" s="39"/>
       <c r="B222" s="39"/>
       <c r="C222" s="39"/>
@@ -8199,7 +8199,7 @@
       <c r="N222" s="39"/>
       <c r="O222" s="39"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A223" s="39"/>
       <c r="B223" s="39"/>
       <c r="C223" s="39"/>
@@ -8216,7 +8216,7 @@
       <c r="N223" s="39"/>
       <c r="O223" s="39"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A224" s="39"/>
       <c r="B224" s="39"/>
       <c r="C224" s="39"/>
@@ -8233,7 +8233,7 @@
       <c r="N224" s="39"/>
       <c r="O224" s="39"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A225" s="39"/>
       <c r="B225" s="39"/>
       <c r="C225" s="39"/>
@@ -8250,7 +8250,7 @@
       <c r="N225" s="39"/>
       <c r="O225" s="39"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A226" s="39"/>
       <c r="B226" s="39"/>
       <c r="C226" s="39"/>
@@ -8267,7 +8267,7 @@
       <c r="N226" s="39"/>
       <c r="O226" s="39"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A227" s="39"/>
       <c r="B227" s="39"/>
       <c r="C227" s="39"/>
@@ -8284,7 +8284,7 @@
       <c r="N227" s="39"/>
       <c r="O227" s="39"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A228" s="39"/>
       <c r="B228" s="39"/>
       <c r="C228" s="39"/>
@@ -8301,7 +8301,7 @@
       <c r="N228" s="39"/>
       <c r="O228" s="39"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A229" s="39"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
@@ -8318,7 +8318,7 @@
       <c r="N229" s="39"/>
       <c r="O229" s="39"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A230" s="39"/>
       <c r="B230" s="39"/>
       <c r="C230" s="39"/>
@@ -8335,7 +8335,7 @@
       <c r="N230" s="39"/>
       <c r="O230" s="39"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A231" s="39"/>
       <c r="B231" s="39"/>
       <c r="C231" s="39"/>
@@ -8352,7 +8352,7 @@
       <c r="N231" s="39"/>
       <c r="O231" s="39"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A232" s="39"/>
       <c r="B232" s="39"/>
       <c r="C232" s="39"/>
@@ -8369,7 +8369,7 @@
       <c r="N232" s="39"/>
       <c r="O232" s="39"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A233" s="39"/>
       <c r="B233" s="39"/>
       <c r="C233" s="39"/>
@@ -8386,7 +8386,7 @@
       <c r="N233" s="39"/>
       <c r="O233" s="39"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A234" s="39"/>
       <c r="B234" s="39"/>
       <c r="C234" s="39"/>
@@ -8403,7 +8403,7 @@
       <c r="N234" s="39"/>
       <c r="O234" s="39"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A235" s="39"/>
       <c r="B235" s="39"/>
       <c r="C235" s="39"/>
@@ -8420,7 +8420,7 @@
       <c r="N235" s="39"/>
       <c r="O235" s="39"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A236" s="39"/>
       <c r="B236" s="39"/>
       <c r="C236" s="39"/>
@@ -8437,7 +8437,7 @@
       <c r="N236" s="39"/>
       <c r="O236" s="39"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A237" s="39"/>
       <c r="B237" s="39"/>
       <c r="C237" s="39"/>
@@ -8454,7 +8454,7 @@
       <c r="N237" s="39"/>
       <c r="O237" s="39"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A238" s="39"/>
       <c r="B238" s="39"/>
       <c r="C238" s="39"/>
@@ -8471,7 +8471,7 @@
       <c r="N238" s="39"/>
       <c r="O238" s="39"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A239" s="39"/>
       <c r="B239" s="39"/>
       <c r="C239" s="39"/>
@@ -8488,7 +8488,7 @@
       <c r="N239" s="39"/>
       <c r="O239" s="39"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A240" s="39"/>
       <c r="B240" s="39"/>
       <c r="C240" s="39"/>
@@ -8505,7 +8505,7 @@
       <c r="N240" s="39"/>
       <c r="O240" s="39"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A241" s="39"/>
       <c r="B241" s="39"/>
       <c r="C241" s="39"/>
@@ -8522,7 +8522,7 @@
       <c r="N241" s="39"/>
       <c r="O241" s="39"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A242" s="39"/>
       <c r="B242" s="39"/>
       <c r="C242" s="39"/>
@@ -8539,7 +8539,7 @@
       <c r="N242" s="39"/>
       <c r="O242" s="39"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A243" s="39"/>
       <c r="B243" s="39"/>
       <c r="C243" s="39"/>
@@ -8556,7 +8556,7 @@
       <c r="N243" s="39"/>
       <c r="O243" s="39"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A244" s="39"/>
       <c r="B244" s="39"/>
       <c r="C244" s="39"/>
@@ -8573,7 +8573,7 @@
       <c r="N244" s="39"/>
       <c r="O244" s="39"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A245" s="39"/>
       <c r="B245" s="39"/>
       <c r="C245" s="39"/>
@@ -8590,7 +8590,7 @@
       <c r="N245" s="39"/>
       <c r="O245" s="39"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A246" s="39"/>
       <c r="B246" s="39"/>
       <c r="C246" s="39"/>
@@ -8607,7 +8607,7 @@
       <c r="N246" s="39"/>
       <c r="O246" s="39"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A247" s="39"/>
       <c r="B247" s="39"/>
       <c r="C247" s="39"/>
@@ -8624,7 +8624,7 @@
       <c r="N247" s="39"/>
       <c r="O247" s="39"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A248" s="39"/>
       <c r="B248" s="39"/>
       <c r="C248" s="39"/>
@@ -8641,7 +8641,7 @@
       <c r="N248" s="39"/>
       <c r="O248" s="39"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A249" s="39"/>
       <c r="B249" s="39"/>
       <c r="C249" s="39"/>
@@ -8658,7 +8658,7 @@
       <c r="N249" s="39"/>
       <c r="O249" s="39"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A250" s="39"/>
       <c r="B250" s="39"/>
       <c r="C250" s="39"/>
@@ -8675,7 +8675,7 @@
       <c r="N250" s="39"/>
       <c r="O250" s="39"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A251" s="39"/>
       <c r="B251" s="39"/>
       <c r="C251" s="39"/>
@@ -8692,7 +8692,7 @@
       <c r="N251" s="39"/>
       <c r="O251" s="39"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A252" s="39"/>
       <c r="B252" s="39"/>
       <c r="C252" s="39"/>
@@ -8709,7 +8709,7 @@
       <c r="N252" s="39"/>
       <c r="O252" s="39"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A253" s="39"/>
       <c r="B253" s="39"/>
       <c r="C253" s="39"/>
@@ -8726,7 +8726,7 @@
       <c r="N253" s="39"/>
       <c r="O253" s="39"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A254" s="39"/>
       <c r="B254" s="39"/>
       <c r="C254" s="39"/>
@@ -8743,7 +8743,7 @@
       <c r="N254" s="39"/>
       <c r="O254" s="39"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A255" s="39"/>
       <c r="B255" s="39"/>
       <c r="C255" s="39"/>
@@ -8760,7 +8760,7 @@
       <c r="N255" s="39"/>
       <c r="O255" s="39"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A256" s="39"/>
       <c r="B256" s="39"/>
       <c r="C256" s="39"/>
@@ -8777,7 +8777,7 @@
       <c r="N256" s="39"/>
       <c r="O256" s="39"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A257" s="39"/>
       <c r="B257" s="39"/>
       <c r="C257" s="39"/>
@@ -8794,7 +8794,7 @@
       <c r="N257" s="39"/>
       <c r="O257" s="39"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A258" s="39"/>
       <c r="B258" s="39"/>
       <c r="C258" s="39"/>
@@ -8811,7 +8811,7 @@
       <c r="N258" s="39"/>
       <c r="O258" s="39"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A259" s="39"/>
       <c r="B259" s="39"/>
       <c r="C259" s="39"/>
@@ -8828,7 +8828,7 @@
       <c r="N259" s="39"/>
       <c r="O259" s="39"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A260" s="39"/>
       <c r="B260" s="39"/>
       <c r="C260" s="39"/>
@@ -8845,7 +8845,7 @@
       <c r="N260" s="39"/>
       <c r="O260" s="39"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A261" s="39"/>
       <c r="B261" s="39"/>
       <c r="C261" s="39"/>
@@ -8862,7 +8862,7 @@
       <c r="N261" s="39"/>
       <c r="O261" s="39"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A262" s="39"/>
       <c r="B262" s="39"/>
       <c r="C262" s="39"/>
@@ -8879,7 +8879,7 @@
       <c r="N262" s="39"/>
       <c r="O262" s="39"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A263" s="39"/>
       <c r="B263" s="39"/>
       <c r="C263" s="39"/>
@@ -8896,7 +8896,7 @@
       <c r="N263" s="39"/>
       <c r="O263" s="39"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A264" s="39"/>
       <c r="B264" s="39"/>
       <c r="C264" s="39"/>
@@ -8913,7 +8913,7 @@
       <c r="N264" s="39"/>
       <c r="O264" s="39"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A265" s="39"/>
       <c r="B265" s="39"/>
       <c r="C265" s="39"/>
@@ -8930,7 +8930,7 @@
       <c r="N265" s="39"/>
       <c r="O265" s="39"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A266" s="39"/>
       <c r="B266" s="39"/>
       <c r="C266" s="39"/>
@@ -8947,7 +8947,7 @@
       <c r="N266" s="39"/>
       <c r="O266" s="39"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A267" s="39"/>
       <c r="B267" s="39"/>
       <c r="C267" s="39"/>
@@ -8964,7 +8964,7 @@
       <c r="N267" s="39"/>
       <c r="O267" s="39"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A268" s="39"/>
       <c r="B268" s="39"/>
       <c r="C268" s="39"/>
@@ -8981,7 +8981,7 @@
       <c r="N268" s="39"/>
       <c r="O268" s="39"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
@@ -8998,7 +8998,7 @@
       <c r="N269" s="39"/>
       <c r="O269" s="39"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A270" s="39"/>
       <c r="B270" s="39"/>
       <c r="C270" s="39"/>
@@ -9015,7 +9015,7 @@
       <c r="N270" s="39"/>
       <c r="O270" s="39"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A271" s="39"/>
       <c r="B271" s="39"/>
       <c r="C271" s="39"/>
@@ -9032,7 +9032,7 @@
       <c r="N271" s="39"/>
       <c r="O271" s="39"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A272" s="39"/>
       <c r="B272" s="39"/>
       <c r="C272" s="39"/>
@@ -9049,7 +9049,7 @@
       <c r="N272" s="39"/>
       <c r="O272" s="39"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A273" s="39"/>
       <c r="B273" s="39"/>
       <c r="C273" s="39"/>
@@ -9066,7 +9066,7 @@
       <c r="N273" s="39"/>
       <c r="O273" s="39"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A274" s="39"/>
       <c r="B274" s="39"/>
       <c r="C274" s="39"/>
@@ -9083,7 +9083,7 @@
       <c r="N274" s="39"/>
       <c r="O274" s="39"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A275" s="39"/>
       <c r="B275" s="39"/>
       <c r="C275" s="39"/>
@@ -9100,7 +9100,7 @@
       <c r="N275" s="39"/>
       <c r="O275" s="39"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A276" s="39"/>
       <c r="B276" s="39"/>
       <c r="C276" s="39"/>
@@ -9117,7 +9117,7 @@
       <c r="N276" s="39"/>
       <c r="O276" s="39"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A277" s="39"/>
       <c r="B277" s="39"/>
       <c r="C277" s="39"/>
@@ -9134,7 +9134,7 @@
       <c r="N277" s="39"/>
       <c r="O277" s="39"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A278" s="39"/>
       <c r="B278" s="39"/>
       <c r="C278" s="39"/>
@@ -9151,7 +9151,7 @@
       <c r="N278" s="39"/>
       <c r="O278" s="39"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A279" s="39"/>
       <c r="B279" s="39"/>
       <c r="C279" s="39"/>
@@ -9168,7 +9168,7 @@
       <c r="N279" s="39"/>
       <c r="O279" s="39"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A280" s="39"/>
       <c r="B280" s="39"/>
       <c r="C280" s="39"/>
@@ -9185,7 +9185,7 @@
       <c r="N280" s="39"/>
       <c r="O280" s="39"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A281" s="39"/>
       <c r="B281" s="39"/>
       <c r="C281" s="39"/>
@@ -9202,7 +9202,7 @@
       <c r="N281" s="39"/>
       <c r="O281" s="39"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A282" s="39"/>
       <c r="B282" s="39"/>
       <c r="C282" s="39"/>
@@ -9219,7 +9219,7 @@
       <c r="N282" s="39"/>
       <c r="O282" s="39"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A283" s="39"/>
       <c r="B283" s="39"/>
       <c r="C283" s="39"/>
@@ -9236,7 +9236,7 @@
       <c r="N283" s="39"/>
       <c r="O283" s="39"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A284" s="39"/>
       <c r="B284" s="39"/>
       <c r="C284" s="39"/>
@@ -9253,7 +9253,7 @@
       <c r="N284" s="39"/>
       <c r="O284" s="39"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A285" s="39"/>
       <c r="B285" s="39"/>
       <c r="C285" s="39"/>
@@ -9270,7 +9270,7 @@
       <c r="N285" s="39"/>
       <c r="O285" s="39"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A286" s="39"/>
       <c r="B286" s="39"/>
       <c r="C286" s="39"/>
@@ -9287,7 +9287,7 @@
       <c r="N286" s="39"/>
       <c r="O286" s="39"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A287" s="39"/>
       <c r="B287" s="39"/>
       <c r="C287" s="39"/>
@@ -9304,7 +9304,7 @@
       <c r="N287" s="39"/>
       <c r="O287" s="39"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A288" s="39"/>
       <c r="B288" s="39"/>
       <c r="C288" s="39"/>
@@ -9321,7 +9321,7 @@
       <c r="N288" s="39"/>
       <c r="O288" s="39"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A289" s="39"/>
       <c r="B289" s="39"/>
       <c r="C289" s="39"/>
@@ -9338,7 +9338,7 @@
       <c r="N289" s="39"/>
       <c r="O289" s="39"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A290" s="39"/>
       <c r="B290" s="39"/>
       <c r="C290" s="39"/>
@@ -9355,7 +9355,7 @@
       <c r="N290" s="39"/>
       <c r="O290" s="39"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A291" s="39"/>
       <c r="B291" s="39"/>
       <c r="C291" s="39"/>
@@ -9372,7 +9372,7 @@
       <c r="N291" s="39"/>
       <c r="O291" s="39"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A292" s="39"/>
       <c r="B292" s="39"/>
       <c r="C292" s="39"/>
@@ -9389,7 +9389,7 @@
       <c r="N292" s="39"/>
       <c r="O292" s="39"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A293" s="39"/>
       <c r="B293" s="39"/>
       <c r="C293" s="39"/>
@@ -9406,7 +9406,7 @@
       <c r="N293" s="39"/>
       <c r="O293" s="39"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A294" s="39"/>
       <c r="B294" s="39"/>
       <c r="C294" s="39"/>
@@ -9423,7 +9423,7 @@
       <c r="N294" s="39"/>
       <c r="O294" s="39"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A295" s="39"/>
       <c r="B295" s="39"/>
       <c r="C295" s="39"/>
@@ -9440,7 +9440,7 @@
       <c r="N295" s="39"/>
       <c r="O295" s="39"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A296" s="39"/>
       <c r="B296" s="39"/>
       <c r="C296" s="39"/>
@@ -9457,7 +9457,7 @@
       <c r="N296" s="39"/>
       <c r="O296" s="39"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A297" s="39"/>
       <c r="B297" s="39"/>
       <c r="C297" s="39"/>
@@ -9474,7 +9474,7 @@
       <c r="N297" s="39"/>
       <c r="O297" s="39"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A298" s="39"/>
       <c r="B298" s="39"/>
       <c r="C298" s="39"/>
@@ -9491,7 +9491,7 @@
       <c r="N298" s="39"/>
       <c r="O298" s="39"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A299" s="39"/>
       <c r="B299" s="39"/>
       <c r="C299" s="39"/>
@@ -9508,7 +9508,7 @@
       <c r="N299" s="39"/>
       <c r="O299" s="39"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A300" s="39"/>
       <c r="B300" s="39"/>
       <c r="C300" s="39"/>
@@ -9525,7 +9525,7 @@
       <c r="N300" s="39"/>
       <c r="O300" s="39"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A301" s="39"/>
       <c r="B301" s="39"/>
       <c r="C301" s="39"/>
@@ -9542,7 +9542,7 @@
       <c r="N301" s="39"/>
       <c r="O301" s="39"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A302" s="39"/>
       <c r="B302" s="39"/>
       <c r="C302" s="39"/>
@@ -9559,7 +9559,7 @@
       <c r="N302" s="39"/>
       <c r="O302" s="39"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A303" s="39"/>
       <c r="B303" s="39"/>
       <c r="C303" s="39"/>
@@ -9576,7 +9576,7 @@
       <c r="N303" s="39"/>
       <c r="O303" s="39"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A304" s="39"/>
       <c r="B304" s="39"/>
       <c r="C304" s="39"/>
@@ -9593,7 +9593,7 @@
       <c r="N304" s="39"/>
       <c r="O304" s="39"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A305" s="39"/>
       <c r="B305" s="39"/>
       <c r="C305" s="39"/>
@@ -9610,7 +9610,7 @@
       <c r="N305" s="39"/>
       <c r="O305" s="39"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A306" s="39"/>
       <c r="B306" s="39"/>
       <c r="C306" s="39"/>
@@ -9627,7 +9627,7 @@
       <c r="N306" s="39"/>
       <c r="O306" s="39"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A307" s="39"/>
       <c r="B307" s="39"/>
       <c r="C307" s="39"/>
@@ -9644,7 +9644,7 @@
       <c r="N307" s="39"/>
       <c r="O307" s="39"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A308" s="39"/>
       <c r="B308" s="39"/>
       <c r="C308" s="39"/>
@@ -9661,7 +9661,7 @@
       <c r="N308" s="39"/>
       <c r="O308" s="39"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A309" s="39"/>
       <c r="B309" s="39"/>
       <c r="C309" s="39"/>
@@ -9678,7 +9678,7 @@
       <c r="N309" s="39"/>
       <c r="O309" s="39"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A310" s="39"/>
       <c r="B310" s="39"/>
       <c r="C310" s="39"/>
@@ -9695,7 +9695,7 @@
       <c r="N310" s="39"/>
       <c r="O310" s="39"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A311" s="39"/>
       <c r="B311" s="39"/>
       <c r="C311" s="39"/>
@@ -9712,7 +9712,7 @@
       <c r="N311" s="39"/>
       <c r="O311" s="39"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A312" s="39"/>
       <c r="B312" s="39"/>
       <c r="C312" s="39"/>
@@ -9729,7 +9729,7 @@
       <c r="N312" s="39"/>
       <c r="O312" s="39"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A313" s="39"/>
       <c r="B313" s="39"/>
       <c r="C313" s="39"/>
@@ -9746,7 +9746,7 @@
       <c r="N313" s="39"/>
       <c r="O313" s="39"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A314" s="39"/>
       <c r="B314" s="39"/>
       <c r="C314" s="39"/>
@@ -9763,7 +9763,7 @@
       <c r="N314" s="39"/>
       <c r="O314" s="39"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A315" s="39"/>
       <c r="B315" s="39"/>
       <c r="C315" s="39"/>
@@ -9780,7 +9780,7 @@
       <c r="N315" s="39"/>
       <c r="O315" s="39"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A316" s="39"/>
       <c r="B316" s="39"/>
       <c r="C316" s="39"/>
@@ -9797,7 +9797,7 @@
       <c r="N316" s="39"/>
       <c r="O316" s="39"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A317" s="39"/>
       <c r="B317" s="39"/>
       <c r="C317" s="39"/>
@@ -9814,7 +9814,7 @@
       <c r="N317" s="39"/>
       <c r="O317" s="39"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A318" s="39"/>
       <c r="B318" s="39"/>
       <c r="C318" s="39"/>
@@ -9831,7 +9831,7 @@
       <c r="N318" s="39"/>
       <c r="O318" s="39"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A319" s="39"/>
       <c r="B319" s="39"/>
       <c r="C319" s="39"/>
@@ -9848,7 +9848,7 @@
       <c r="N319" s="39"/>
       <c r="O319" s="39"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A320" s="39"/>
       <c r="B320" s="39"/>
       <c r="C320" s="39"/>
@@ -9865,7 +9865,7 @@
       <c r="N320" s="39"/>
       <c r="O320" s="39"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A321" s="39"/>
       <c r="B321" s="39"/>
       <c r="C321" s="39"/>
@@ -9882,7 +9882,7 @@
       <c r="N321" s="39"/>
       <c r="O321" s="39"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A322" s="39"/>
       <c r="B322" s="39"/>
       <c r="C322" s="39"/>
@@ -9899,7 +9899,7 @@
       <c r="N322" s="39"/>
       <c r="O322" s="39"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A323" s="39"/>
       <c r="B323" s="39"/>
       <c r="C323" s="39"/>
@@ -9916,7 +9916,7 @@
       <c r="N323" s="39"/>
       <c r="O323" s="39"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A324" s="39"/>
       <c r="B324" s="39"/>
       <c r="C324" s="39"/>
@@ -9933,7 +9933,7 @@
       <c r="N324" s="39"/>
       <c r="O324" s="39"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A325" s="39"/>
       <c r="B325" s="39"/>
       <c r="C325" s="39"/>
@@ -9950,7 +9950,7 @@
       <c r="N325" s="39"/>
       <c r="O325" s="39"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A326" s="39"/>
       <c r="B326" s="39"/>
       <c r="C326" s="39"/>
@@ -9967,7 +9967,7 @@
       <c r="N326" s="39"/>
       <c r="O326" s="39"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
       <c r="C327" s="39"/>
@@ -9984,7 +9984,7 @@
       <c r="N327" s="39"/>
       <c r="O327" s="39"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A328" s="39"/>
       <c r="B328" s="39"/>
       <c r="C328" s="39"/>
@@ -10001,7 +10001,7 @@
       <c r="N328" s="39"/>
       <c r="O328" s="39"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A329" s="39"/>
       <c r="B329" s="39"/>
       <c r="C329" s="39"/>
@@ -10018,7 +10018,7 @@
       <c r="N329" s="39"/>
       <c r="O329" s="39"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A330" s="39"/>
       <c r="B330" s="39"/>
       <c r="C330" s="39"/>
@@ -10035,7 +10035,7 @@
       <c r="N330" s="39"/>
       <c r="O330" s="39"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A331" s="39"/>
       <c r="B331" s="39"/>
       <c r="C331" s="39"/>
@@ -10052,7 +10052,7 @@
       <c r="N331" s="39"/>
       <c r="O331" s="39"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A332" s="39"/>
       <c r="B332" s="39"/>
       <c r="C332" s="39"/>
@@ -10069,7 +10069,7 @@
       <c r="N332" s="39"/>
       <c r="O332" s="39"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A333" s="39"/>
       <c r="B333" s="39"/>
       <c r="C333" s="39"/>
@@ -10086,7 +10086,7 @@
       <c r="N333" s="39"/>
       <c r="O333" s="39"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A334" s="39"/>
       <c r="B334" s="39"/>
       <c r="C334" s="39"/>
@@ -10103,7 +10103,7 @@
       <c r="N334" s="39"/>
       <c r="O334" s="39"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A335" s="39"/>
       <c r="B335" s="39"/>
       <c r="C335" s="39"/>
@@ -10120,7 +10120,7 @@
       <c r="N335" s="39"/>
       <c r="O335" s="39"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A336" s="39"/>
       <c r="B336" s="39"/>
       <c r="C336" s="39"/>
@@ -10137,7 +10137,7 @@
       <c r="N336" s="39"/>
       <c r="O336" s="39"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A337" s="39"/>
       <c r="B337" s="39"/>
       <c r="C337" s="39"/>
@@ -10154,7 +10154,7 @@
       <c r="N337" s="39"/>
       <c r="O337" s="39"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A338" s="39"/>
       <c r="B338" s="39"/>
       <c r="C338" s="39"/>
@@ -10171,7 +10171,7 @@
       <c r="N338" s="39"/>
       <c r="O338" s="39"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A339" s="39"/>
       <c r="B339" s="39"/>
       <c r="C339" s="39"/>
@@ -10188,7 +10188,7 @@
       <c r="N339" s="39"/>
       <c r="O339" s="39"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A340" s="39"/>
       <c r="B340" s="39"/>
       <c r="C340" s="39"/>
@@ -10205,7 +10205,7 @@
       <c r="N340" s="39"/>
       <c r="O340" s="39"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A341" s="39"/>
       <c r="B341" s="39"/>
       <c r="C341" s="39"/>
@@ -10222,7 +10222,7 @@
       <c r="N341" s="39"/>
       <c r="O341" s="39"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A342" s="39"/>
       <c r="B342" s="39"/>
       <c r="C342" s="39"/>
@@ -10239,7 +10239,7 @@
       <c r="N342" s="39"/>
       <c r="O342" s="39"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A343" s="39"/>
       <c r="B343" s="39"/>
       <c r="C343" s="39"/>
@@ -10256,7 +10256,7 @@
       <c r="N343" s="39"/>
       <c r="O343" s="39"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A344" s="39"/>
       <c r="B344" s="39"/>
       <c r="C344" s="39"/>
@@ -10273,7 +10273,7 @@
       <c r="N344" s="39"/>
       <c r="O344" s="39"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A345" s="39"/>
       <c r="B345" s="39"/>
       <c r="C345" s="39"/>
@@ -10290,7 +10290,7 @@
       <c r="N345" s="39"/>
       <c r="O345" s="39"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="39"/>
@@ -10320,17 +10320,17 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="36" t="s">
         <v>126</v>
       </c>
@@ -10347,7 +10347,7 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="24">
         <v>43070</v>
       </c>
@@ -10364,7 +10364,7 @@
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
     </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="39"/>
       <c r="B6" s="39" t="s">
         <v>112</v>
@@ -10379,7 +10379,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="39"/>
       <c r="B7" s="39" t="s">
         <v>113</v>
@@ -10394,7 +10394,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -10407,7 +10407,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="24">
         <v>43091</v>
       </c>
@@ -10424,7 +10424,7 @@
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A10" s="39"/>
       <c r="B10" s="39" t="s">
         <v>227</v>
@@ -10439,7 +10439,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -10452,7 +10452,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -10465,7 +10465,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -10478,7 +10478,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -10491,7 +10491,7 @@
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -10504,7 +10504,7 @@
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
     </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -10517,7 +10517,7 @@
       <c r="J16" s="39"/>
       <c r="K16" s="39"/>
     </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -10530,7 +10530,7 @@
       <c r="J17" s="39"/>
       <c r="K17" s="39"/>
     </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -10543,7 +10543,7 @@
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
     </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>

</xml_diff>

<commit_message>
update authors on group meeting
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\03_Sem_HS\BTX8081_SoftwareEngineeringAndDesign\Eclipse\ch.bfh.btx8081.w2017.blue.git\doc\04-ScrumSetup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester 2017/bfh_software-engineering/Project/sohpboia_git/doc/04-ScrumSetup/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8592" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$55</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -748,7 +748,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1250,8 +1250,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1552,21 +1552,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1645,12 +1645,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/jntme"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://github.com/gfels6"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://github.com/kybup1"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://github.com/ziegm"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://github.com/Odaoj1"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://github.com/petim1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
@@ -1658,26 +1658,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="13">
         <v>0</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="13">
         <v>2</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="13">
         <v>3</v>
       </c>
@@ -1811,7 +1811,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="90" x14ac:dyDescent="0.2">
       <c r="A6" s="13">
         <v>4</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="13">
         <v>5</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="135" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="13">
         <v>6</v>
       </c>
@@ -1883,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1949,35 +1949,35 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="21" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="25" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.109375" style="1"/>
-    <col min="16" max="16" width="8.109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.1640625" style="1"/>
+    <col min="16" max="16" width="8.1640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="43" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" s="43" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="41">
         <v>0.1</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>66</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="79" t="s">
         <v>67</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="50" t="s">
         <v>164</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="79" t="s">
         <v>219</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="75">
         <v>1.1000000000000001</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="75">
         <v>1.2</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="70">
         <v>1.3</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>63</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>41</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:12" s="28" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>62</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="59">
         <v>2.2000000000000002</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="87">
         <v>2.2999999999999998</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" s="28" customFormat="1" ht="62.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32">
         <v>3.1</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32">
         <v>3.2</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>39</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="28" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>40</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:12" s="28" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" s="28" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>72</v>
       </c>
@@ -2568,7 +2568,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="s">
         <v>118</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="s">
         <v>118</v>
       </c>
@@ -2644,7 +2644,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:12" s="58" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="59" t="s">
         <v>122</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="28" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" s="28" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32">
         <v>3.3</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="28" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" s="28" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32">
         <v>3.4</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="58" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" s="58" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="59" t="s">
         <v>137</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="58" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" s="58" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="59" t="s">
         <v>141</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="28" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="32">
         <v>3.5</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="28" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" s="28" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26">
         <v>3.6</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="56" customFormat="1" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" s="56" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="54" t="s">
         <v>160</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="52" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" s="52" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="50">
         <v>4.0999999999999996</v>
       </c>
@@ -2986,7 +2986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="79" t="s">
         <v>221</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="79" t="s">
         <v>220</v>
       </c>
@@ -3062,7 +3062,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="79" t="s">
         <v>222</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" s="78" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="79" t="s">
         <v>223</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" s="79" t="s">
         <v>224</v>
       </c>
@@ -3173,10 +3173,10 @@
         <v>0</v>
       </c>
       <c r="L35" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" s="79" t="s">
         <v>225</v>
       </c>
@@ -3211,10 +3211,10 @@
         <v>0</v>
       </c>
       <c r="L36" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" s="79"/>
       <c r="B37" s="80">
         <v>3</v>
@@ -3247,10 +3247,10 @@
         <v>0</v>
       </c>
       <c r="L37" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="79"/>
       <c r="B38" s="80">
         <v>3</v>
@@ -3286,7 +3286,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="79" t="s">
         <v>212</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="78" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="79" t="s">
         <v>213</v>
       </c>
@@ -3362,7 +3362,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:12" s="78" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" s="78" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A41" s="79" t="s">
         <v>214</v>
       </c>
@@ -3397,10 +3397,10 @@
         <v>1.5</v>
       </c>
       <c r="L41" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="78" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A42" s="79" t="s">
         <v>215</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:12" s="52" customFormat="1" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" s="52" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="64" t="s">
         <v>116</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" s="52" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="64" t="s">
         <v>131</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
         <v>133</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="52" customFormat="1" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" s="52" customFormat="1" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="64" t="s">
         <v>146</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" s="78" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="79" t="s">
         <v>233</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A49" s="79" t="s">
         <v>217</v>
       </c>
@@ -3701,10 +3701,10 @@
         <v>0</v>
       </c>
       <c r="L49" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="79" t="s">
         <v>229</v>
       </c>
@@ -3739,10 +3739,10 @@
         <v>0</v>
       </c>
       <c r="L50" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" s="78" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A51" s="83" t="s">
         <v>216</v>
       </c>
@@ -3777,10 +3777,10 @@
         <v>0</v>
       </c>
       <c r="L51" s="78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" s="82" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="82" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="83" t="s">
         <v>234</v>
       </c>
@@ -3815,10 +3815,10 @@
         <v>0</v>
       </c>
       <c r="L52" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="84">
         <v>7.11</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" s="86" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="86">
         <v>7.12</v>
       </c>
@@ -3885,7 +3885,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="1:17" s="52" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" s="52" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="64" t="s">
         <v>158</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="17"/>
       <c r="C56" s="18"/>
@@ -3937,7 +3937,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="17"/>
       <c r="C57" s="18"/>
@@ -3949,7 +3949,7 @@
       <c r="P57" s="91"/>
       <c r="Q57" s="91"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E58" s="18"/>
       <c r="F58" s="22"/>
       <c r="G58" s="18"/>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E59" s="1" t="s">
         <v>152</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E60" s="1" t="s">
         <v>153</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E61" s="1" t="s">
         <v>154</v>
       </c>
@@ -4028,8 +4028,8 @@
         <v>42.25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="65" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G65" s="96" t="s">
         <v>54</v>
       </c>
@@ -4041,7 +4041,7 @@
       <c r="M65" s="97"/>
       <c r="N65" s="98"/>
     </row>
-    <row r="66" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G66" s="66"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
@@ -4063,7 +4063,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G67" s="92" t="s">
         <v>148</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G68" s="92" t="s">
         <v>149</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G69" s="94" t="s">
         <v>150</v>
       </c>
@@ -4153,8 +4153,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G71" s="96" t="s">
         <v>55</v>
       </c>
@@ -4166,7 +4166,7 @@
       <c r="M71" s="97"/>
       <c r="N71" s="98"/>
     </row>
-    <row r="72" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G72" s="66"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18" t="s">
@@ -4188,7 +4188,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G73" s="92" t="s">
         <v>148</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G74" s="92" t="s">
         <v>149</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G75" s="94" t="s">
         <v>150</v>
       </c>
@@ -4278,8 +4278,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="77" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G77" s="96" t="s">
         <v>56</v>
       </c>
@@ -4291,7 +4291,7 @@
       <c r="M77" s="97"/>
       <c r="N77" s="98"/>
     </row>
-    <row r="78" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G78" s="66"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18" t="s">
@@ -4313,7 +4313,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G79" s="92" t="s">
         <v>148</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="7:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G80" s="92" t="s">
         <v>149</v>
       </c>
@@ -4373,7 +4373,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G81" s="94" t="s">
         <v>150</v>
       </c>
@@ -4404,10 +4404,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:L55" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="B1:L55">
     <filterColumn colId="0">
-      <filters blank="1">
+      <filters>
         <filter val="3"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="10">
+      <filters>
+        <filter val="pending"/>
+        <filter val="waiting"/>
       </filters>
     </filterColumn>
     <sortState ref="B4:L54">
@@ -4441,21 +4447,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -4469,10 +4475,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -4482,24 +4488,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O346"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="37" t="s">
         <v>14</v>
       </c>
@@ -4510,7 +4516,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>1</v>
       </c>
@@ -4533,7 +4539,7 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -4556,7 +4562,7 @@
       <c r="N9" s="39"/>
       <c r="O9" s="39"/>
     </row>
-    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>1</v>
       </c>
@@ -4579,7 +4585,7 @@
       <c r="N10" s="39"/>
       <c r="O10" s="39"/>
     </row>
-    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39" t="s">
@@ -4598,7 +4604,7 @@
       <c r="N11" s="39"/>
       <c r="O11" s="39"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39" t="s">
@@ -4617,7 +4623,7 @@
       <c r="N12" s="39"/>
       <c r="O12" s="39"/>
     </row>
-    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="40">
         <v>1</v>
       </c>
@@ -4640,7 +4646,7 @@
       <c r="N13" s="39"/>
       <c r="O13" s="39"/>
     </row>
-    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="40">
         <v>2</v>
       </c>
@@ -4663,7 +4669,7 @@
       <c r="N14" s="39"/>
       <c r="O14" s="39"/>
     </row>
-    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -4680,7 +4686,7 @@
       <c r="N15" s="39"/>
       <c r="O15" s="39"/>
     </row>
-    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -4697,7 +4703,7 @@
       <c r="N16" s="39"/>
       <c r="O16" s="39"/>
     </row>
-    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -4714,7 +4720,7 @@
       <c r="N17" s="39"/>
       <c r="O17" s="39"/>
     </row>
-    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="40"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -4731,7 +4737,7 @@
       <c r="N18" s="39"/>
       <c r="O18" s="39"/>
     </row>
-    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="40"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
@@ -4748,7 +4754,7 @@
       <c r="N19" s="39"/>
       <c r="O19" s="39"/>
     </row>
-    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
@@ -4765,7 +4771,7 @@
       <c r="N20" s="39"/>
       <c r="O20" s="39"/>
     </row>
-    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
@@ -4782,7 +4788,7 @@
       <c r="N21" s="39"/>
       <c r="O21" s="39"/>
     </row>
-    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
@@ -4799,7 +4805,7 @@
       <c r="N22" s="39"/>
       <c r="O22" s="39"/>
     </row>
-    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
@@ -4816,7 +4822,7 @@
       <c r="N23" s="39"/>
       <c r="O23" s="39"/>
     </row>
-    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="40"/>
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
@@ -4833,7 +4839,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -4850,7 +4856,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -4867,7 +4873,7 @@
       <c r="N26" s="39"/>
       <c r="O26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
@@ -4884,7 +4890,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -4901,7 +4907,7 @@
       <c r="N28" s="39"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -4918,7 +4924,7 @@
       <c r="N29" s="39"/>
       <c r="O29" s="39"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -4935,7 +4941,7 @@
       <c r="N30" s="39"/>
       <c r="O30" s="39"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -4952,7 +4958,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="39"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -4969,7 +4975,7 @@
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -4986,7 +4992,7 @@
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -5003,7 +5009,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -5020,7 +5026,7 @@
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
@@ -5037,7 +5043,7 @@
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -5054,7 +5060,7 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
@@ -5071,7 +5077,7 @@
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -5088,7 +5094,7 @@
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -5105,7 +5111,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -5122,7 +5128,7 @@
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
@@ -5139,7 +5145,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -5156,7 +5162,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -5173,7 +5179,7 @@
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -5190,7 +5196,7 @@
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -5207,7 +5213,7 @@
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -5224,7 +5230,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -5241,7 +5247,7 @@
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -5258,7 +5264,7 @@
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -5275,7 +5281,7 @@
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -5292,7 +5298,7 @@
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -5309,7 +5315,7 @@
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -5326,7 +5332,7 @@
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -5343,7 +5349,7 @@
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -5360,7 +5366,7 @@
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -5377,7 +5383,7 @@
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -5394,7 +5400,7 @@
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -5411,7 +5417,7 @@
       <c r="N58" s="39"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -5428,7 +5434,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="39"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -5445,7 +5451,7 @@
       <c r="N60" s="39"/>
       <c r="O60" s="39"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -5462,7 +5468,7 @@
       <c r="N61" s="39"/>
       <c r="O61" s="39"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -5479,7 +5485,7 @@
       <c r="N62" s="39"/>
       <c r="O62" s="39"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -5496,7 +5502,7 @@
       <c r="N63" s="39"/>
       <c r="O63" s="39"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -5513,7 +5519,7 @@
       <c r="N64" s="39"/>
       <c r="O64" s="39"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -5530,7 +5536,7 @@
       <c r="N65" s="39"/>
       <c r="O65" s="39"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -5547,7 +5553,7 @@
       <c r="N66" s="39"/>
       <c r="O66" s="39"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -5564,7 +5570,7 @@
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -5581,7 +5587,7 @@
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -5598,7 +5604,7 @@
       <c r="N69" s="39"/>
       <c r="O69" s="39"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -5615,7 +5621,7 @@
       <c r="N70" s="39"/>
       <c r="O70" s="39"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -5632,7 +5638,7 @@
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -5649,7 +5655,7 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -5666,7 +5672,7 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -5683,7 +5689,7 @@
       <c r="N74" s="39"/>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -5700,7 +5706,7 @@
       <c r="N75" s="39"/>
       <c r="O75" s="39"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -5717,7 +5723,7 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -5734,7 +5740,7 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -5751,7 +5757,7 @@
       <c r="N78" s="39"/>
       <c r="O78" s="39"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -5768,7 +5774,7 @@
       <c r="N79" s="39"/>
       <c r="O79" s="39"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -5785,7 +5791,7 @@
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -5802,7 +5808,7 @@
       <c r="N81" s="39"/>
       <c r="O81" s="39"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -5819,7 +5825,7 @@
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -5836,7 +5842,7 @@
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -5853,7 +5859,7 @@
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -5870,7 +5876,7 @@
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -5887,7 +5893,7 @@
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -5904,7 +5910,7 @@
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -5921,7 +5927,7 @@
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -5938,7 +5944,7 @@
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -5955,7 +5961,7 @@
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -5972,7 +5978,7 @@
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -5989,7 +5995,7 @@
       <c r="N92" s="39"/>
       <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -6006,7 +6012,7 @@
       <c r="N93" s="39"/>
       <c r="O93" s="39"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -6023,7 +6029,7 @@
       <c r="N94" s="39"/>
       <c r="O94" s="39"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -6040,7 +6046,7 @@
       <c r="N95" s="39"/>
       <c r="O95" s="39"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -6057,7 +6063,7 @@
       <c r="N96" s="39"/>
       <c r="O96" s="39"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -6074,7 +6080,7 @@
       <c r="N97" s="39"/>
       <c r="O97" s="39"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -6091,7 +6097,7 @@
       <c r="N98" s="39"/>
       <c r="O98" s="39"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -6108,7 +6114,7 @@
       <c r="N99" s="39"/>
       <c r="O99" s="39"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="39"/>
       <c r="B100" s="39"/>
       <c r="C100" s="39"/>
@@ -6125,7 +6131,7 @@
       <c r="N100" s="39"/>
       <c r="O100" s="39"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="39"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -6142,7 +6148,7 @@
       <c r="N101" s="39"/>
       <c r="O101" s="39"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A102" s="39"/>
       <c r="B102" s="39"/>
       <c r="C102" s="39"/>
@@ -6159,7 +6165,7 @@
       <c r="N102" s="39"/>
       <c r="O102" s="39"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A103" s="39"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -6176,7 +6182,7 @@
       <c r="N103" s="39"/>
       <c r="O103" s="39"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -6193,7 +6199,7 @@
       <c r="N104" s="39"/>
       <c r="O104" s="39"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="39"/>
       <c r="B105" s="39"/>
       <c r="C105" s="39"/>
@@ -6210,7 +6216,7 @@
       <c r="N105" s="39"/>
       <c r="O105" s="39"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A106" s="39"/>
       <c r="B106" s="39"/>
       <c r="C106" s="39"/>
@@ -6227,7 +6233,7 @@
       <c r="N106" s="39"/>
       <c r="O106" s="39"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A107" s="39"/>
       <c r="B107" s="39"/>
       <c r="C107" s="39"/>
@@ -6244,7 +6250,7 @@
       <c r="N107" s="39"/>
       <c r="O107" s="39"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A108" s="39"/>
       <c r="B108" s="39"/>
       <c r="C108" s="39"/>
@@ -6261,7 +6267,7 @@
       <c r="N108" s="39"/>
       <c r="O108" s="39"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A109" s="39"/>
       <c r="B109" s="39"/>
       <c r="C109" s="39"/>
@@ -6278,7 +6284,7 @@
       <c r="N109" s="39"/>
       <c r="O109" s="39"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="39"/>
       <c r="B110" s="39"/>
       <c r="C110" s="39"/>
@@ -6295,7 +6301,7 @@
       <c r="N110" s="39"/>
       <c r="O110" s="39"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A111" s="39"/>
       <c r="B111" s="39"/>
       <c r="C111" s="39"/>
@@ -6312,7 +6318,7 @@
       <c r="N111" s="39"/>
       <c r="O111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A112" s="39"/>
       <c r="B112" s="39"/>
       <c r="C112" s="39"/>
@@ -6329,7 +6335,7 @@
       <c r="N112" s="39"/>
       <c r="O112" s="39"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A113" s="39"/>
       <c r="B113" s="39"/>
       <c r="C113" s="39"/>
@@ -6346,7 +6352,7 @@
       <c r="N113" s="39"/>
       <c r="O113" s="39"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A114" s="39"/>
       <c r="B114" s="39"/>
       <c r="C114" s="39"/>
@@ -6363,7 +6369,7 @@
       <c r="N114" s="39"/>
       <c r="O114" s="39"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A115" s="39"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
@@ -6380,7 +6386,7 @@
       <c r="N115" s="39"/>
       <c r="O115" s="39"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A116" s="39"/>
       <c r="B116" s="39"/>
       <c r="C116" s="39"/>
@@ -6397,7 +6403,7 @@
       <c r="N116" s="39"/>
       <c r="O116" s="39"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A117" s="39"/>
       <c r="B117" s="39"/>
       <c r="C117" s="39"/>
@@ -6414,7 +6420,7 @@
       <c r="N117" s="39"/>
       <c r="O117" s="39"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A118" s="39"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
@@ -6431,7 +6437,7 @@
       <c r="N118" s="39"/>
       <c r="O118" s="39"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A119" s="39"/>
       <c r="B119" s="39"/>
       <c r="C119" s="39"/>
@@ -6448,7 +6454,7 @@
       <c r="N119" s="39"/>
       <c r="O119" s="39"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -6465,7 +6471,7 @@
       <c r="N120" s="39"/>
       <c r="O120" s="39"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A121" s="39"/>
       <c r="B121" s="39"/>
       <c r="C121" s="39"/>
@@ -6482,7 +6488,7 @@
       <c r="N121" s="39"/>
       <c r="O121" s="39"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A122" s="39"/>
       <c r="B122" s="39"/>
       <c r="C122" s="39"/>
@@ -6499,7 +6505,7 @@
       <c r="N122" s="39"/>
       <c r="O122" s="39"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A123" s="39"/>
       <c r="B123" s="39"/>
       <c r="C123" s="39"/>
@@ -6516,7 +6522,7 @@
       <c r="N123" s="39"/>
       <c r="O123" s="39"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A124" s="39"/>
       <c r="B124" s="39"/>
       <c r="C124" s="39"/>
@@ -6533,7 +6539,7 @@
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A125" s="39"/>
       <c r="B125" s="39"/>
       <c r="C125" s="39"/>
@@ -6550,7 +6556,7 @@
       <c r="N125" s="39"/>
       <c r="O125" s="39"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A126" s="39"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -6567,7 +6573,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="39"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A127" s="39"/>
       <c r="B127" s="39"/>
       <c r="C127" s="39"/>
@@ -6584,7 +6590,7 @@
       <c r="N127" s="39"/>
       <c r="O127" s="39"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39"/>
@@ -6601,7 +6607,7 @@
       <c r="N128" s="39"/>
       <c r="O128" s="39"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39"/>
@@ -6618,7 +6624,7 @@
       <c r="N129" s="39"/>
       <c r="O129" s="39"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39"/>
@@ -6635,7 +6641,7 @@
       <c r="N130" s="39"/>
       <c r="O130" s="39"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -6652,7 +6658,7 @@
       <c r="N131" s="39"/>
       <c r="O131" s="39"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -6669,7 +6675,7 @@
       <c r="N132" s="39"/>
       <c r="O132" s="39"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A133" s="39"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
@@ -6686,7 +6692,7 @@
       <c r="N133" s="39"/>
       <c r="O133" s="39"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A134" s="39"/>
       <c r="B134" s="39"/>
       <c r="C134" s="39"/>
@@ -6703,7 +6709,7 @@
       <c r="N134" s="39"/>
       <c r="O134" s="39"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -6720,7 +6726,7 @@
       <c r="N135" s="39"/>
       <c r="O135" s="39"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A136" s="39"/>
       <c r="B136" s="39"/>
       <c r="C136" s="39"/>
@@ -6737,7 +6743,7 @@
       <c r="N136" s="39"/>
       <c r="O136" s="39"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A137" s="39"/>
       <c r="B137" s="39"/>
       <c r="C137" s="39"/>
@@ -6754,7 +6760,7 @@
       <c r="N137" s="39"/>
       <c r="O137" s="39"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A138" s="39"/>
       <c r="B138" s="39"/>
       <c r="C138" s="39"/>
@@ -6771,7 +6777,7 @@
       <c r="N138" s="39"/>
       <c r="O138" s="39"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A139" s="39"/>
       <c r="B139" s="39"/>
       <c r="C139" s="39"/>
@@ -6788,7 +6794,7 @@
       <c r="N139" s="39"/>
       <c r="O139" s="39"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A140" s="39"/>
       <c r="B140" s="39"/>
       <c r="C140" s="39"/>
@@ -6805,7 +6811,7 @@
       <c r="N140" s="39"/>
       <c r="O140" s="39"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="39"/>
       <c r="B141" s="39"/>
       <c r="C141" s="39"/>
@@ -6822,7 +6828,7 @@
       <c r="N141" s="39"/>
       <c r="O141" s="39"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A142" s="39"/>
       <c r="B142" s="39"/>
       <c r="C142" s="39"/>
@@ -6839,7 +6845,7 @@
       <c r="N142" s="39"/>
       <c r="O142" s="39"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A143" s="39"/>
       <c r="B143" s="39"/>
       <c r="C143" s="39"/>
@@ -6856,7 +6862,7 @@
       <c r="N143" s="39"/>
       <c r="O143" s="39"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A144" s="39"/>
       <c r="B144" s="39"/>
       <c r="C144" s="39"/>
@@ -6873,7 +6879,7 @@
       <c r="N144" s="39"/>
       <c r="O144" s="39"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A145" s="39"/>
       <c r="B145" s="39"/>
       <c r="C145" s="39"/>
@@ -6890,7 +6896,7 @@
       <c r="N145" s="39"/>
       <c r="O145" s="39"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A146" s="39"/>
       <c r="B146" s="39"/>
       <c r="C146" s="39"/>
@@ -6907,7 +6913,7 @@
       <c r="N146" s="39"/>
       <c r="O146" s="39"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A147" s="39"/>
       <c r="B147" s="39"/>
       <c r="C147" s="39"/>
@@ -6924,7 +6930,7 @@
       <c r="N147" s="39"/>
       <c r="O147" s="39"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A148" s="39"/>
       <c r="B148" s="39"/>
       <c r="C148" s="39"/>
@@ -6941,7 +6947,7 @@
       <c r="N148" s="39"/>
       <c r="O148" s="39"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A149" s="39"/>
       <c r="B149" s="39"/>
       <c r="C149" s="39"/>
@@ -6958,7 +6964,7 @@
       <c r="N149" s="39"/>
       <c r="O149" s="39"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A150" s="39"/>
       <c r="B150" s="39"/>
       <c r="C150" s="39"/>
@@ -6975,7 +6981,7 @@
       <c r="N150" s="39"/>
       <c r="O150" s="39"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A151" s="39"/>
       <c r="B151" s="39"/>
       <c r="C151" s="39"/>
@@ -6992,7 +6998,7 @@
       <c r="N151" s="39"/>
       <c r="O151" s="39"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A152" s="39"/>
       <c r="B152" s="39"/>
       <c r="C152" s="39"/>
@@ -7009,7 +7015,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A153" s="39"/>
       <c r="B153" s="39"/>
       <c r="C153" s="39"/>
@@ -7026,7 +7032,7 @@
       <c r="N153" s="39"/>
       <c r="O153" s="39"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A154" s="39"/>
       <c r="B154" s="39"/>
       <c r="C154" s="39"/>
@@ -7043,7 +7049,7 @@
       <c r="N154" s="39"/>
       <c r="O154" s="39"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A155" s="39"/>
       <c r="B155" s="39"/>
       <c r="C155" s="39"/>
@@ -7060,7 +7066,7 @@
       <c r="N155" s="39"/>
       <c r="O155" s="39"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A156" s="39"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
@@ -7077,7 +7083,7 @@
       <c r="N156" s="39"/>
       <c r="O156" s="39"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A157" s="39"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
@@ -7094,7 +7100,7 @@
       <c r="N157" s="39"/>
       <c r="O157" s="39"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A158" s="39"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -7111,7 +7117,7 @@
       <c r="N158" s="39"/>
       <c r="O158" s="39"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A159" s="39"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -7128,7 +7134,7 @@
       <c r="N159" s="39"/>
       <c r="O159" s="39"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A160" s="39"/>
       <c r="B160" s="39"/>
       <c r="C160" s="39"/>
@@ -7145,7 +7151,7 @@
       <c r="N160" s="39"/>
       <c r="O160" s="39"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A161" s="39"/>
       <c r="B161" s="39"/>
       <c r="C161" s="39"/>
@@ -7162,7 +7168,7 @@
       <c r="N161" s="39"/>
       <c r="O161" s="39"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A162" s="39"/>
       <c r="B162" s="39"/>
       <c r="C162" s="39"/>
@@ -7179,7 +7185,7 @@
       <c r="N162" s="39"/>
       <c r="O162" s="39"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A163" s="39"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
@@ -7196,7 +7202,7 @@
       <c r="N163" s="39"/>
       <c r="O163" s="39"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A164" s="39"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
@@ -7213,7 +7219,7 @@
       <c r="N164" s="39"/>
       <c r="O164" s="39"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A165" s="39"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
@@ -7230,7 +7236,7 @@
       <c r="N165" s="39"/>
       <c r="O165" s="39"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A166" s="39"/>
       <c r="B166" s="39"/>
       <c r="C166" s="39"/>
@@ -7247,7 +7253,7 @@
       <c r="N166" s="39"/>
       <c r="O166" s="39"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A167" s="39"/>
       <c r="B167" s="39"/>
       <c r="C167" s="39"/>
@@ -7264,7 +7270,7 @@
       <c r="N167" s="39"/>
       <c r="O167" s="39"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A168" s="39"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -7281,7 +7287,7 @@
       <c r="N168" s="39"/>
       <c r="O168" s="39"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A169" s="39"/>
       <c r="B169" s="39"/>
       <c r="C169" s="39"/>
@@ -7298,7 +7304,7 @@
       <c r="N169" s="39"/>
       <c r="O169" s="39"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A170" s="39"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
@@ -7315,7 +7321,7 @@
       <c r="N170" s="39"/>
       <c r="O170" s="39"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A171" s="39"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -7332,7 +7338,7 @@
       <c r="N171" s="39"/>
       <c r="O171" s="39"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A172" s="39"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
@@ -7349,7 +7355,7 @@
       <c r="N172" s="39"/>
       <c r="O172" s="39"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A173" s="39"/>
       <c r="B173" s="39"/>
       <c r="C173" s="39"/>
@@ -7366,7 +7372,7 @@
       <c r="N173" s="39"/>
       <c r="O173" s="39"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A174" s="39"/>
       <c r="B174" s="39"/>
       <c r="C174" s="39"/>
@@ -7383,7 +7389,7 @@
       <c r="N174" s="39"/>
       <c r="O174" s="39"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A175" s="39"/>
       <c r="B175" s="39"/>
       <c r="C175" s="39"/>
@@ -7400,7 +7406,7 @@
       <c r="N175" s="39"/>
       <c r="O175" s="39"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A176" s="39"/>
       <c r="B176" s="39"/>
       <c r="C176" s="39"/>
@@ -7417,7 +7423,7 @@
       <c r="N176" s="39"/>
       <c r="O176" s="39"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A177" s="39"/>
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
@@ -7434,7 +7440,7 @@
       <c r="N177" s="39"/>
       <c r="O177" s="39"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A178" s="39"/>
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
@@ -7451,7 +7457,7 @@
       <c r="N178" s="39"/>
       <c r="O178" s="39"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A179" s="39"/>
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
@@ -7468,7 +7474,7 @@
       <c r="N179" s="39"/>
       <c r="O179" s="39"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A180" s="39"/>
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
@@ -7485,7 +7491,7 @@
       <c r="N180" s="39"/>
       <c r="O180" s="39"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A181" s="39"/>
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
@@ -7502,7 +7508,7 @@
       <c r="N181" s="39"/>
       <c r="O181" s="39"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A182" s="39"/>
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
@@ -7519,7 +7525,7 @@
       <c r="N182" s="39"/>
       <c r="O182" s="39"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A183" s="39"/>
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
@@ -7536,7 +7542,7 @@
       <c r="N183" s="39"/>
       <c r="O183" s="39"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A184" s="39"/>
       <c r="B184" s="39"/>
       <c r="C184" s="39"/>
@@ -7553,7 +7559,7 @@
       <c r="N184" s="39"/>
       <c r="O184" s="39"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
       <c r="C185" s="39"/>
@@ -7570,7 +7576,7 @@
       <c r="N185" s="39"/>
       <c r="O185" s="39"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
       <c r="C186" s="39"/>
@@ -7587,7 +7593,7 @@
       <c r="N186" s="39"/>
       <c r="O186" s="39"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A187" s="39"/>
       <c r="B187" s="39"/>
       <c r="C187" s="39"/>
@@ -7604,7 +7610,7 @@
       <c r="N187" s="39"/>
       <c r="O187" s="39"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A188" s="39"/>
       <c r="B188" s="39"/>
       <c r="C188" s="39"/>
@@ -7621,7 +7627,7 @@
       <c r="N188" s="39"/>
       <c r="O188" s="39"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A189" s="39"/>
       <c r="B189" s="39"/>
       <c r="C189" s="39"/>
@@ -7638,7 +7644,7 @@
       <c r="N189" s="39"/>
       <c r="O189" s="39"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A190" s="39"/>
       <c r="B190" s="39"/>
       <c r="C190" s="39"/>
@@ -7655,7 +7661,7 @@
       <c r="N190" s="39"/>
       <c r="O190" s="39"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A191" s="39"/>
       <c r="B191" s="39"/>
       <c r="C191" s="39"/>
@@ -7672,7 +7678,7 @@
       <c r="N191" s="39"/>
       <c r="O191" s="39"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="39"/>
       <c r="B192" s="39"/>
       <c r="C192" s="39"/>
@@ -7689,7 +7695,7 @@
       <c r="N192" s="39"/>
       <c r="O192" s="39"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A193" s="39"/>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -7706,7 +7712,7 @@
       <c r="N193" s="39"/>
       <c r="O193" s="39"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="39"/>
       <c r="B194" s="39"/>
       <c r="C194" s="39"/>
@@ -7723,7 +7729,7 @@
       <c r="N194" s="39"/>
       <c r="O194" s="39"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A195" s="39"/>
       <c r="B195" s="39"/>
       <c r="C195" s="39"/>
@@ -7740,7 +7746,7 @@
       <c r="N195" s="39"/>
       <c r="O195" s="39"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A196" s="39"/>
       <c r="B196" s="39"/>
       <c r="C196" s="39"/>
@@ -7757,7 +7763,7 @@
       <c r="N196" s="39"/>
       <c r="O196" s="39"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A197" s="39"/>
       <c r="B197" s="39"/>
       <c r="C197" s="39"/>
@@ -7774,7 +7780,7 @@
       <c r="N197" s="39"/>
       <c r="O197" s="39"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A198" s="39"/>
       <c r="B198" s="39"/>
       <c r="C198" s="39"/>
@@ -7791,7 +7797,7 @@
       <c r="N198" s="39"/>
       <c r="O198" s="39"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A199" s="39"/>
       <c r="B199" s="39"/>
       <c r="C199" s="39"/>
@@ -7808,7 +7814,7 @@
       <c r="N199" s="39"/>
       <c r="O199" s="39"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A200" s="39"/>
       <c r="B200" s="39"/>
       <c r="C200" s="39"/>
@@ -7825,7 +7831,7 @@
       <c r="N200" s="39"/>
       <c r="O200" s="39"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A201" s="39"/>
       <c r="B201" s="39"/>
       <c r="C201" s="39"/>
@@ -7842,7 +7848,7 @@
       <c r="N201" s="39"/>
       <c r="O201" s="39"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A202" s="39"/>
       <c r="B202" s="39"/>
       <c r="C202" s="39"/>
@@ -7859,7 +7865,7 @@
       <c r="N202" s="39"/>
       <c r="O202" s="39"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A203" s="39"/>
       <c r="B203" s="39"/>
       <c r="C203" s="39"/>
@@ -7876,7 +7882,7 @@
       <c r="N203" s="39"/>
       <c r="O203" s="39"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A204" s="39"/>
       <c r="B204" s="39"/>
       <c r="C204" s="39"/>
@@ -7893,7 +7899,7 @@
       <c r="N204" s="39"/>
       <c r="O204" s="39"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A205" s="39"/>
       <c r="B205" s="39"/>
       <c r="C205" s="39"/>
@@ -7910,7 +7916,7 @@
       <c r="N205" s="39"/>
       <c r="O205" s="39"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A206" s="39"/>
       <c r="B206" s="39"/>
       <c r="C206" s="39"/>
@@ -7927,7 +7933,7 @@
       <c r="N206" s="39"/>
       <c r="O206" s="39"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A207" s="39"/>
       <c r="B207" s="39"/>
       <c r="C207" s="39"/>
@@ -7944,7 +7950,7 @@
       <c r="N207" s="39"/>
       <c r="O207" s="39"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A208" s="39"/>
       <c r="B208" s="39"/>
       <c r="C208" s="39"/>
@@ -7961,7 +7967,7 @@
       <c r="N208" s="39"/>
       <c r="O208" s="39"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A209" s="39"/>
       <c r="B209" s="39"/>
       <c r="C209" s="39"/>
@@ -7978,7 +7984,7 @@
       <c r="N209" s="39"/>
       <c r="O209" s="39"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A210" s="39"/>
       <c r="B210" s="39"/>
       <c r="C210" s="39"/>
@@ -7995,7 +8001,7 @@
       <c r="N210" s="39"/>
       <c r="O210" s="39"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A211" s="39"/>
       <c r="B211" s="39"/>
       <c r="C211" s="39"/>
@@ -8012,7 +8018,7 @@
       <c r="N211" s="39"/>
       <c r="O211" s="39"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A212" s="39"/>
       <c r="B212" s="39"/>
       <c r="C212" s="39"/>
@@ -8029,7 +8035,7 @@
       <c r="N212" s="39"/>
       <c r="O212" s="39"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A213" s="39"/>
       <c r="B213" s="39"/>
       <c r="C213" s="39"/>
@@ -8046,7 +8052,7 @@
       <c r="N213" s="39"/>
       <c r="O213" s="39"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A214" s="39"/>
       <c r="B214" s="39"/>
       <c r="C214" s="39"/>
@@ -8063,7 +8069,7 @@
       <c r="N214" s="39"/>
       <c r="O214" s="39"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A215" s="39"/>
       <c r="B215" s="39"/>
       <c r="C215" s="39"/>
@@ -8080,7 +8086,7 @@
       <c r="N215" s="39"/>
       <c r="O215" s="39"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A216" s="39"/>
       <c r="B216" s="39"/>
       <c r="C216" s="39"/>
@@ -8097,7 +8103,7 @@
       <c r="N216" s="39"/>
       <c r="O216" s="39"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A217" s="39"/>
       <c r="B217" s="39"/>
       <c r="C217" s="39"/>
@@ -8114,7 +8120,7 @@
       <c r="N217" s="39"/>
       <c r="O217" s="39"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A218" s="39"/>
       <c r="B218" s="39"/>
       <c r="C218" s="39"/>
@@ -8131,7 +8137,7 @@
       <c r="N218" s="39"/>
       <c r="O218" s="39"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A219" s="39"/>
       <c r="B219" s="39"/>
       <c r="C219" s="39"/>
@@ -8148,7 +8154,7 @@
       <c r="N219" s="39"/>
       <c r="O219" s="39"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A220" s="39"/>
       <c r="B220" s="39"/>
       <c r="C220" s="39"/>
@@ -8165,7 +8171,7 @@
       <c r="N220" s="39"/>
       <c r="O220" s="39"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A221" s="39"/>
       <c r="B221" s="39"/>
       <c r="C221" s="39"/>
@@ -8182,7 +8188,7 @@
       <c r="N221" s="39"/>
       <c r="O221" s="39"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A222" s="39"/>
       <c r="B222" s="39"/>
       <c r="C222" s="39"/>
@@ -8199,7 +8205,7 @@
       <c r="N222" s="39"/>
       <c r="O222" s="39"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A223" s="39"/>
       <c r="B223" s="39"/>
       <c r="C223" s="39"/>
@@ -8216,7 +8222,7 @@
       <c r="N223" s="39"/>
       <c r="O223" s="39"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A224" s="39"/>
       <c r="B224" s="39"/>
       <c r="C224" s="39"/>
@@ -8233,7 +8239,7 @@
       <c r="N224" s="39"/>
       <c r="O224" s="39"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A225" s="39"/>
       <c r="B225" s="39"/>
       <c r="C225" s="39"/>
@@ -8250,7 +8256,7 @@
       <c r="N225" s="39"/>
       <c r="O225" s="39"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A226" s="39"/>
       <c r="B226" s="39"/>
       <c r="C226" s="39"/>
@@ -8267,7 +8273,7 @@
       <c r="N226" s="39"/>
       <c r="O226" s="39"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A227" s="39"/>
       <c r="B227" s="39"/>
       <c r="C227" s="39"/>
@@ -8284,7 +8290,7 @@
       <c r="N227" s="39"/>
       <c r="O227" s="39"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="39"/>
       <c r="B228" s="39"/>
       <c r="C228" s="39"/>
@@ -8301,7 +8307,7 @@
       <c r="N228" s="39"/>
       <c r="O228" s="39"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A229" s="39"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
@@ -8318,7 +8324,7 @@
       <c r="N229" s="39"/>
       <c r="O229" s="39"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A230" s="39"/>
       <c r="B230" s="39"/>
       <c r="C230" s="39"/>
@@ -8335,7 +8341,7 @@
       <c r="N230" s="39"/>
       <c r="O230" s="39"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A231" s="39"/>
       <c r="B231" s="39"/>
       <c r="C231" s="39"/>
@@ -8352,7 +8358,7 @@
       <c r="N231" s="39"/>
       <c r="O231" s="39"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A232" s="39"/>
       <c r="B232" s="39"/>
       <c r="C232" s="39"/>
@@ -8369,7 +8375,7 @@
       <c r="N232" s="39"/>
       <c r="O232" s="39"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A233" s="39"/>
       <c r="B233" s="39"/>
       <c r="C233" s="39"/>
@@ -8386,7 +8392,7 @@
       <c r="N233" s="39"/>
       <c r="O233" s="39"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A234" s="39"/>
       <c r="B234" s="39"/>
       <c r="C234" s="39"/>
@@ -8403,7 +8409,7 @@
       <c r="N234" s="39"/>
       <c r="O234" s="39"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A235" s="39"/>
       <c r="B235" s="39"/>
       <c r="C235" s="39"/>
@@ -8420,7 +8426,7 @@
       <c r="N235" s="39"/>
       <c r="O235" s="39"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A236" s="39"/>
       <c r="B236" s="39"/>
       <c r="C236" s="39"/>
@@ -8437,7 +8443,7 @@
       <c r="N236" s="39"/>
       <c r="O236" s="39"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A237" s="39"/>
       <c r="B237" s="39"/>
       <c r="C237" s="39"/>
@@ -8454,7 +8460,7 @@
       <c r="N237" s="39"/>
       <c r="O237" s="39"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A238" s="39"/>
       <c r="B238" s="39"/>
       <c r="C238" s="39"/>
@@ -8471,7 +8477,7 @@
       <c r="N238" s="39"/>
       <c r="O238" s="39"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A239" s="39"/>
       <c r="B239" s="39"/>
       <c r="C239" s="39"/>
@@ -8488,7 +8494,7 @@
       <c r="N239" s="39"/>
       <c r="O239" s="39"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A240" s="39"/>
       <c r="B240" s="39"/>
       <c r="C240" s="39"/>
@@ -8505,7 +8511,7 @@
       <c r="N240" s="39"/>
       <c r="O240" s="39"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A241" s="39"/>
       <c r="B241" s="39"/>
       <c r="C241" s="39"/>
@@ -8522,7 +8528,7 @@
       <c r="N241" s="39"/>
       <c r="O241" s="39"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A242" s="39"/>
       <c r="B242" s="39"/>
       <c r="C242" s="39"/>
@@ -8539,7 +8545,7 @@
       <c r="N242" s="39"/>
       <c r="O242" s="39"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A243" s="39"/>
       <c r="B243" s="39"/>
       <c r="C243" s="39"/>
@@ -8556,7 +8562,7 @@
       <c r="N243" s="39"/>
       <c r="O243" s="39"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A244" s="39"/>
       <c r="B244" s="39"/>
       <c r="C244" s="39"/>
@@ -8573,7 +8579,7 @@
       <c r="N244" s="39"/>
       <c r="O244" s="39"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A245" s="39"/>
       <c r="B245" s="39"/>
       <c r="C245" s="39"/>
@@ -8590,7 +8596,7 @@
       <c r="N245" s="39"/>
       <c r="O245" s="39"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A246" s="39"/>
       <c r="B246" s="39"/>
       <c r="C246" s="39"/>
@@ -8607,7 +8613,7 @@
       <c r="N246" s="39"/>
       <c r="O246" s="39"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A247" s="39"/>
       <c r="B247" s="39"/>
       <c r="C247" s="39"/>
@@ -8624,7 +8630,7 @@
       <c r="N247" s="39"/>
       <c r="O247" s="39"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A248" s="39"/>
       <c r="B248" s="39"/>
       <c r="C248" s="39"/>
@@ -8641,7 +8647,7 @@
       <c r="N248" s="39"/>
       <c r="O248" s="39"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A249" s="39"/>
       <c r="B249" s="39"/>
       <c r="C249" s="39"/>
@@ -8658,7 +8664,7 @@
       <c r="N249" s="39"/>
       <c r="O249" s="39"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A250" s="39"/>
       <c r="B250" s="39"/>
       <c r="C250" s="39"/>
@@ -8675,7 +8681,7 @@
       <c r="N250" s="39"/>
       <c r="O250" s="39"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A251" s="39"/>
       <c r="B251" s="39"/>
       <c r="C251" s="39"/>
@@ -8692,7 +8698,7 @@
       <c r="N251" s="39"/>
       <c r="O251" s="39"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A252" s="39"/>
       <c r="B252" s="39"/>
       <c r="C252" s="39"/>
@@ -8709,7 +8715,7 @@
       <c r="N252" s="39"/>
       <c r="O252" s="39"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A253" s="39"/>
       <c r="B253" s="39"/>
       <c r="C253" s="39"/>
@@ -8726,7 +8732,7 @@
       <c r="N253" s="39"/>
       <c r="O253" s="39"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A254" s="39"/>
       <c r="B254" s="39"/>
       <c r="C254" s="39"/>
@@ -8743,7 +8749,7 @@
       <c r="N254" s="39"/>
       <c r="O254" s="39"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A255" s="39"/>
       <c r="B255" s="39"/>
       <c r="C255" s="39"/>
@@ -8760,7 +8766,7 @@
       <c r="N255" s="39"/>
       <c r="O255" s="39"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A256" s="39"/>
       <c r="B256" s="39"/>
       <c r="C256" s="39"/>
@@ -8777,7 +8783,7 @@
       <c r="N256" s="39"/>
       <c r="O256" s="39"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A257" s="39"/>
       <c r="B257" s="39"/>
       <c r="C257" s="39"/>
@@ -8794,7 +8800,7 @@
       <c r="N257" s="39"/>
       <c r="O257" s="39"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A258" s="39"/>
       <c r="B258" s="39"/>
       <c r="C258" s="39"/>
@@ -8811,7 +8817,7 @@
       <c r="N258" s="39"/>
       <c r="O258" s="39"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A259" s="39"/>
       <c r="B259" s="39"/>
       <c r="C259" s="39"/>
@@ -8828,7 +8834,7 @@
       <c r="N259" s="39"/>
       <c r="O259" s="39"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A260" s="39"/>
       <c r="B260" s="39"/>
       <c r="C260" s="39"/>
@@ -8845,7 +8851,7 @@
       <c r="N260" s="39"/>
       <c r="O260" s="39"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A261" s="39"/>
       <c r="B261" s="39"/>
       <c r="C261" s="39"/>
@@ -8862,7 +8868,7 @@
       <c r="N261" s="39"/>
       <c r="O261" s="39"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A262" s="39"/>
       <c r="B262" s="39"/>
       <c r="C262" s="39"/>
@@ -8879,7 +8885,7 @@
       <c r="N262" s="39"/>
       <c r="O262" s="39"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A263" s="39"/>
       <c r="B263" s="39"/>
       <c r="C263" s="39"/>
@@ -8896,7 +8902,7 @@
       <c r="N263" s="39"/>
       <c r="O263" s="39"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A264" s="39"/>
       <c r="B264" s="39"/>
       <c r="C264" s="39"/>
@@ -8913,7 +8919,7 @@
       <c r="N264" s="39"/>
       <c r="O264" s="39"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A265" s="39"/>
       <c r="B265" s="39"/>
       <c r="C265" s="39"/>
@@ -8930,7 +8936,7 @@
       <c r="N265" s="39"/>
       <c r="O265" s="39"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A266" s="39"/>
       <c r="B266" s="39"/>
       <c r="C266" s="39"/>
@@ -8947,7 +8953,7 @@
       <c r="N266" s="39"/>
       <c r="O266" s="39"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A267" s="39"/>
       <c r="B267" s="39"/>
       <c r="C267" s="39"/>
@@ -8964,7 +8970,7 @@
       <c r="N267" s="39"/>
       <c r="O267" s="39"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A268" s="39"/>
       <c r="B268" s="39"/>
       <c r="C268" s="39"/>
@@ -8981,7 +8987,7 @@
       <c r="N268" s="39"/>
       <c r="O268" s="39"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
@@ -8998,7 +9004,7 @@
       <c r="N269" s="39"/>
       <c r="O269" s="39"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A270" s="39"/>
       <c r="B270" s="39"/>
       <c r="C270" s="39"/>
@@ -9015,7 +9021,7 @@
       <c r="N270" s="39"/>
       <c r="O270" s="39"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A271" s="39"/>
       <c r="B271" s="39"/>
       <c r="C271" s="39"/>
@@ -9032,7 +9038,7 @@
       <c r="N271" s="39"/>
       <c r="O271" s="39"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A272" s="39"/>
       <c r="B272" s="39"/>
       <c r="C272" s="39"/>
@@ -9049,7 +9055,7 @@
       <c r="N272" s="39"/>
       <c r="O272" s="39"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A273" s="39"/>
       <c r="B273" s="39"/>
       <c r="C273" s="39"/>
@@ -9066,7 +9072,7 @@
       <c r="N273" s="39"/>
       <c r="O273" s="39"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A274" s="39"/>
       <c r="B274" s="39"/>
       <c r="C274" s="39"/>
@@ -9083,7 +9089,7 @@
       <c r="N274" s="39"/>
       <c r="O274" s="39"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A275" s="39"/>
       <c r="B275" s="39"/>
       <c r="C275" s="39"/>
@@ -9100,7 +9106,7 @@
       <c r="N275" s="39"/>
       <c r="O275" s="39"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A276" s="39"/>
       <c r="B276" s="39"/>
       <c r="C276" s="39"/>
@@ -9117,7 +9123,7 @@
       <c r="N276" s="39"/>
       <c r="O276" s="39"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A277" s="39"/>
       <c r="B277" s="39"/>
       <c r="C277" s="39"/>
@@ -9134,7 +9140,7 @@
       <c r="N277" s="39"/>
       <c r="O277" s="39"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A278" s="39"/>
       <c r="B278" s="39"/>
       <c r="C278" s="39"/>
@@ -9151,7 +9157,7 @@
       <c r="N278" s="39"/>
       <c r="O278" s="39"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A279" s="39"/>
       <c r="B279" s="39"/>
       <c r="C279" s="39"/>
@@ -9168,7 +9174,7 @@
       <c r="N279" s="39"/>
       <c r="O279" s="39"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A280" s="39"/>
       <c r="B280" s="39"/>
       <c r="C280" s="39"/>
@@ -9185,7 +9191,7 @@
       <c r="N280" s="39"/>
       <c r="O280" s="39"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A281" s="39"/>
       <c r="B281" s="39"/>
       <c r="C281" s="39"/>
@@ -9202,7 +9208,7 @@
       <c r="N281" s="39"/>
       <c r="O281" s="39"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A282" s="39"/>
       <c r="B282" s="39"/>
       <c r="C282" s="39"/>
@@ -9219,7 +9225,7 @@
       <c r="N282" s="39"/>
       <c r="O282" s="39"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A283" s="39"/>
       <c r="B283" s="39"/>
       <c r="C283" s="39"/>
@@ -9236,7 +9242,7 @@
       <c r="N283" s="39"/>
       <c r="O283" s="39"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A284" s="39"/>
       <c r="B284" s="39"/>
       <c r="C284" s="39"/>
@@ -9253,7 +9259,7 @@
       <c r="N284" s="39"/>
       <c r="O284" s="39"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A285" s="39"/>
       <c r="B285" s="39"/>
       <c r="C285" s="39"/>
@@ -9270,7 +9276,7 @@
       <c r="N285" s="39"/>
       <c r="O285" s="39"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A286" s="39"/>
       <c r="B286" s="39"/>
       <c r="C286" s="39"/>
@@ -9287,7 +9293,7 @@
       <c r="N286" s="39"/>
       <c r="O286" s="39"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A287" s="39"/>
       <c r="B287" s="39"/>
       <c r="C287" s="39"/>
@@ -9304,7 +9310,7 @@
       <c r="N287" s="39"/>
       <c r="O287" s="39"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A288" s="39"/>
       <c r="B288" s="39"/>
       <c r="C288" s="39"/>
@@ -9321,7 +9327,7 @@
       <c r="N288" s="39"/>
       <c r="O288" s="39"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A289" s="39"/>
       <c r="B289" s="39"/>
       <c r="C289" s="39"/>
@@ -9338,7 +9344,7 @@
       <c r="N289" s="39"/>
       <c r="O289" s="39"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A290" s="39"/>
       <c r="B290" s="39"/>
       <c r="C290" s="39"/>
@@ -9355,7 +9361,7 @@
       <c r="N290" s="39"/>
       <c r="O290" s="39"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A291" s="39"/>
       <c r="B291" s="39"/>
       <c r="C291" s="39"/>
@@ -9372,7 +9378,7 @@
       <c r="N291" s="39"/>
       <c r="O291" s="39"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A292" s="39"/>
       <c r="B292" s="39"/>
       <c r="C292" s="39"/>
@@ -9389,7 +9395,7 @@
       <c r="N292" s="39"/>
       <c r="O292" s="39"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A293" s="39"/>
       <c r="B293" s="39"/>
       <c r="C293" s="39"/>
@@ -9406,7 +9412,7 @@
       <c r="N293" s="39"/>
       <c r="O293" s="39"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A294" s="39"/>
       <c r="B294" s="39"/>
       <c r="C294" s="39"/>
@@ -9423,7 +9429,7 @@
       <c r="N294" s="39"/>
       <c r="O294" s="39"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A295" s="39"/>
       <c r="B295" s="39"/>
       <c r="C295" s="39"/>
@@ -9440,7 +9446,7 @@
       <c r="N295" s="39"/>
       <c r="O295" s="39"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A296" s="39"/>
       <c r="B296" s="39"/>
       <c r="C296" s="39"/>
@@ -9457,7 +9463,7 @@
       <c r="N296" s="39"/>
       <c r="O296" s="39"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A297" s="39"/>
       <c r="B297" s="39"/>
       <c r="C297" s="39"/>
@@ -9474,7 +9480,7 @@
       <c r="N297" s="39"/>
       <c r="O297" s="39"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A298" s="39"/>
       <c r="B298" s="39"/>
       <c r="C298" s="39"/>
@@ -9491,7 +9497,7 @@
       <c r="N298" s="39"/>
       <c r="O298" s="39"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A299" s="39"/>
       <c r="B299" s="39"/>
       <c r="C299" s="39"/>
@@ -9508,7 +9514,7 @@
       <c r="N299" s="39"/>
       <c r="O299" s="39"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A300" s="39"/>
       <c r="B300" s="39"/>
       <c r="C300" s="39"/>
@@ -9525,7 +9531,7 @@
       <c r="N300" s="39"/>
       <c r="O300" s="39"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A301" s="39"/>
       <c r="B301" s="39"/>
       <c r="C301" s="39"/>
@@ -9542,7 +9548,7 @@
       <c r="N301" s="39"/>
       <c r="O301" s="39"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A302" s="39"/>
       <c r="B302" s="39"/>
       <c r="C302" s="39"/>
@@ -9559,7 +9565,7 @@
       <c r="N302" s="39"/>
       <c r="O302" s="39"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A303" s="39"/>
       <c r="B303" s="39"/>
       <c r="C303" s="39"/>
@@ -9576,7 +9582,7 @@
       <c r="N303" s="39"/>
       <c r="O303" s="39"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A304" s="39"/>
       <c r="B304" s="39"/>
       <c r="C304" s="39"/>
@@ -9593,7 +9599,7 @@
       <c r="N304" s="39"/>
       <c r="O304" s="39"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A305" s="39"/>
       <c r="B305" s="39"/>
       <c r="C305" s="39"/>
@@ -9610,7 +9616,7 @@
       <c r="N305" s="39"/>
       <c r="O305" s="39"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A306" s="39"/>
       <c r="B306" s="39"/>
       <c r="C306" s="39"/>
@@ -9627,7 +9633,7 @@
       <c r="N306" s="39"/>
       <c r="O306" s="39"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A307" s="39"/>
       <c r="B307" s="39"/>
       <c r="C307" s="39"/>
@@ -9644,7 +9650,7 @@
       <c r="N307" s="39"/>
       <c r="O307" s="39"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A308" s="39"/>
       <c r="B308" s="39"/>
       <c r="C308" s="39"/>
@@ -9661,7 +9667,7 @@
       <c r="N308" s="39"/>
       <c r="O308" s="39"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A309" s="39"/>
       <c r="B309" s="39"/>
       <c r="C309" s="39"/>
@@ -9678,7 +9684,7 @@
       <c r="N309" s="39"/>
       <c r="O309" s="39"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A310" s="39"/>
       <c r="B310" s="39"/>
       <c r="C310" s="39"/>
@@ -9695,7 +9701,7 @@
       <c r="N310" s="39"/>
       <c r="O310" s="39"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A311" s="39"/>
       <c r="B311" s="39"/>
       <c r="C311" s="39"/>
@@ -9712,7 +9718,7 @@
       <c r="N311" s="39"/>
       <c r="O311" s="39"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A312" s="39"/>
       <c r="B312" s="39"/>
       <c r="C312" s="39"/>
@@ -9729,7 +9735,7 @@
       <c r="N312" s="39"/>
       <c r="O312" s="39"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A313" s="39"/>
       <c r="B313" s="39"/>
       <c r="C313" s="39"/>
@@ -9746,7 +9752,7 @@
       <c r="N313" s="39"/>
       <c r="O313" s="39"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A314" s="39"/>
       <c r="B314" s="39"/>
       <c r="C314" s="39"/>
@@ -9763,7 +9769,7 @@
       <c r="N314" s="39"/>
       <c r="O314" s="39"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A315" s="39"/>
       <c r="B315" s="39"/>
       <c r="C315" s="39"/>
@@ -9780,7 +9786,7 @@
       <c r="N315" s="39"/>
       <c r="O315" s="39"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A316" s="39"/>
       <c r="B316" s="39"/>
       <c r="C316" s="39"/>
@@ -9797,7 +9803,7 @@
       <c r="N316" s="39"/>
       <c r="O316" s="39"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A317" s="39"/>
       <c r="B317" s="39"/>
       <c r="C317" s="39"/>
@@ -9814,7 +9820,7 @@
       <c r="N317" s="39"/>
       <c r="O317" s="39"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A318" s="39"/>
       <c r="B318" s="39"/>
       <c r="C318" s="39"/>
@@ -9831,7 +9837,7 @@
       <c r="N318" s="39"/>
       <c r="O318" s="39"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A319" s="39"/>
       <c r="B319" s="39"/>
       <c r="C319" s="39"/>
@@ -9848,7 +9854,7 @@
       <c r="N319" s="39"/>
       <c r="O319" s="39"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A320" s="39"/>
       <c r="B320" s="39"/>
       <c r="C320" s="39"/>
@@ -9865,7 +9871,7 @@
       <c r="N320" s="39"/>
       <c r="O320" s="39"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A321" s="39"/>
       <c r="B321" s="39"/>
       <c r="C321" s="39"/>
@@ -9882,7 +9888,7 @@
       <c r="N321" s="39"/>
       <c r="O321" s="39"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A322" s="39"/>
       <c r="B322" s="39"/>
       <c r="C322" s="39"/>
@@ -9899,7 +9905,7 @@
       <c r="N322" s="39"/>
       <c r="O322" s="39"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A323" s="39"/>
       <c r="B323" s="39"/>
       <c r="C323" s="39"/>
@@ -9916,7 +9922,7 @@
       <c r="N323" s="39"/>
       <c r="O323" s="39"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A324" s="39"/>
       <c r="B324" s="39"/>
       <c r="C324" s="39"/>
@@ -9933,7 +9939,7 @@
       <c r="N324" s="39"/>
       <c r="O324" s="39"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A325" s="39"/>
       <c r="B325" s="39"/>
       <c r="C325" s="39"/>
@@ -9950,7 +9956,7 @@
       <c r="N325" s="39"/>
       <c r="O325" s="39"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A326" s="39"/>
       <c r="B326" s="39"/>
       <c r="C326" s="39"/>
@@ -9967,7 +9973,7 @@
       <c r="N326" s="39"/>
       <c r="O326" s="39"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
       <c r="C327" s="39"/>
@@ -9984,7 +9990,7 @@
       <c r="N327" s="39"/>
       <c r="O327" s="39"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A328" s="39"/>
       <c r="B328" s="39"/>
       <c r="C328" s="39"/>
@@ -10001,7 +10007,7 @@
       <c r="N328" s="39"/>
       <c r="O328" s="39"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A329" s="39"/>
       <c r="B329" s="39"/>
       <c r="C329" s="39"/>
@@ -10018,7 +10024,7 @@
       <c r="N329" s="39"/>
       <c r="O329" s="39"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A330" s="39"/>
       <c r="B330" s="39"/>
       <c r="C330" s="39"/>
@@ -10035,7 +10041,7 @@
       <c r="N330" s="39"/>
       <c r="O330" s="39"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A331" s="39"/>
       <c r="B331" s="39"/>
       <c r="C331" s="39"/>
@@ -10052,7 +10058,7 @@
       <c r="N331" s="39"/>
       <c r="O331" s="39"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A332" s="39"/>
       <c r="B332" s="39"/>
       <c r="C332" s="39"/>
@@ -10069,7 +10075,7 @@
       <c r="N332" s="39"/>
       <c r="O332" s="39"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A333" s="39"/>
       <c r="B333" s="39"/>
       <c r="C333" s="39"/>
@@ -10086,7 +10092,7 @@
       <c r="N333" s="39"/>
       <c r="O333" s="39"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A334" s="39"/>
       <c r="B334" s="39"/>
       <c r="C334" s="39"/>
@@ -10103,7 +10109,7 @@
       <c r="N334" s="39"/>
       <c r="O334" s="39"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A335" s="39"/>
       <c r="B335" s="39"/>
       <c r="C335" s="39"/>
@@ -10120,7 +10126,7 @@
       <c r="N335" s="39"/>
       <c r="O335" s="39"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A336" s="39"/>
       <c r="B336" s="39"/>
       <c r="C336" s="39"/>
@@ -10137,7 +10143,7 @@
       <c r="N336" s="39"/>
       <c r="O336" s="39"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A337" s="39"/>
       <c r="B337" s="39"/>
       <c r="C337" s="39"/>
@@ -10154,7 +10160,7 @@
       <c r="N337" s="39"/>
       <c r="O337" s="39"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A338" s="39"/>
       <c r="B338" s="39"/>
       <c r="C338" s="39"/>
@@ -10171,7 +10177,7 @@
       <c r="N338" s="39"/>
       <c r="O338" s="39"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A339" s="39"/>
       <c r="B339" s="39"/>
       <c r="C339" s="39"/>
@@ -10188,7 +10194,7 @@
       <c r="N339" s="39"/>
       <c r="O339" s="39"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A340" s="39"/>
       <c r="B340" s="39"/>
       <c r="C340" s="39"/>
@@ -10205,7 +10211,7 @@
       <c r="N340" s="39"/>
       <c r="O340" s="39"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A341" s="39"/>
       <c r="B341" s="39"/>
       <c r="C341" s="39"/>
@@ -10222,7 +10228,7 @@
       <c r="N341" s="39"/>
       <c r="O341" s="39"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A342" s="39"/>
       <c r="B342" s="39"/>
       <c r="C342" s="39"/>
@@ -10239,7 +10245,7 @@
       <c r="N342" s="39"/>
       <c r="O342" s="39"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A343" s="39"/>
       <c r="B343" s="39"/>
       <c r="C343" s="39"/>
@@ -10256,7 +10262,7 @@
       <c r="N343" s="39"/>
       <c r="O343" s="39"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A344" s="39"/>
       <c r="B344" s="39"/>
       <c r="C344" s="39"/>
@@ -10273,7 +10279,7 @@
       <c r="N344" s="39"/>
       <c r="O344" s="39"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A345" s="39"/>
       <c r="B345" s="39"/>
       <c r="C345" s="39"/>
@@ -10290,7 +10296,7 @@
       <c r="N345" s="39"/>
       <c r="O345" s="39"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="39"/>
@@ -10313,24 +10319,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
         <v>126</v>
       </c>
@@ -10347,7 +10353,7 @@
       <c r="J4" s="39"/>
       <c r="K4" s="39"/>
     </row>
-    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>43070</v>
       </c>
@@ -10364,7 +10370,7 @@
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
     </row>
-    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="39"/>
       <c r="B6" s="39" t="s">
         <v>112</v>
@@ -10379,7 +10385,7 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
     </row>
-    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="39"/>
       <c r="B7" s="39" t="s">
         <v>113</v>
@@ -10394,7 +10400,7 @@
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
     </row>
-    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="39"/>
       <c r="B8" s="39"/>
       <c r="C8" s="39"/>
@@ -10407,7 +10413,7 @@
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
     </row>
-    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>43091</v>
       </c>
@@ -10424,7 +10430,7 @@
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
     </row>
-    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="B10" s="39" t="s">
         <v>227</v>
@@ -10439,7 +10445,7 @@
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
     </row>
-    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="39"/>
       <c r="B11" s="39"/>
       <c r="C11" s="39"/>
@@ -10452,7 +10458,7 @@
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
     </row>
-    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39"/>
@@ -10465,7 +10471,7 @@
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
     </row>
-    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
@@ -10478,7 +10484,7 @@
       <c r="J13" s="39"/>
       <c r="K13" s="39"/>
     </row>
-    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
@@ -10491,7 +10497,7 @@
       <c r="J14" s="39"/>
       <c r="K14" s="39"/>
     </row>
-    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
@@ -10504,7 +10510,7 @@
       <c r="J15" s="39"/>
       <c r="K15" s="39"/>
     </row>
-    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
@@ -10517,7 +10523,7 @@
       <c r="J16" s="39"/>
       <c r="K16" s="39"/>
     </row>
-    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="39"/>
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
@@ -10530,7 +10536,7 @@
       <c r="J17" s="39"/>
       <c r="K17" s="39"/>
     </row>
-    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="39"/>
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
@@ -10543,7 +10549,7 @@
       <c r="J18" s="39"/>
       <c r="K18" s="39"/>
     </row>
-    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="39"/>
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>

</xml_diff>

<commit_message>
added pres.pptx and updated scrum.xls
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1953,8 +1953,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L53" sqref="L53"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3698,7 +3698,7 @@
         <v>4</v>
       </c>
       <c r="K49" s="78">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L49" s="78" t="s">
         <v>110</v>
@@ -3721,7 +3721,7 @@
         <v>94</v>
       </c>
       <c r="F50" s="78" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G50" s="78" t="s">
         <v>24</v>
@@ -3733,10 +3733,10 @@
         <v>4</v>
       </c>
       <c r="J50" s="78">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="K50" s="78">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="L50" s="78" t="s">
         <v>110</v>
@@ -3774,7 +3774,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="78">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L51" s="78" t="s">
         <v>110</v>
@@ -4021,11 +4021,11 @@
       </c>
       <c r="J61" s="1">
         <f>SUMIF(B2:B55,3,J2:J55)</f>
-        <v>74</v>
+        <v>73.5</v>
       </c>
       <c r="K61" s="1">
         <f>SUMIF(B2:B55,3,K2:K55)</f>
-        <v>42.25</v>
+        <v>54.75</v>
       </c>
     </row>
     <row r="64" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -4130,7 +4130,7 @@
       <c r="H69" s="95"/>
       <c r="I69" s="68">
         <f>SUMIFS(I$2:I$55,$B$2:$B$55,3,$F$2:$F$55,"gfels6")</f>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="J69" s="68">
         <f>SUMIFS(I$2:I$55,$B$2:$B$55,3,$F$2:$F$55,"ziegm")</f>
@@ -4138,7 +4138,7 @@
       </c>
       <c r="K69" s="68">
         <f>SUMIFS(I$2:I$55,$B$2:$B$55,3,$F$2:$F$55,"jntme")</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="L69" s="68">
         <f>SUMIFS(I$2:I$55,$B$2:$B$55,3,$F$2:$F$55,"kybup1")</f>
@@ -4255,7 +4255,7 @@
       <c r="H75" s="95"/>
       <c r="I75" s="68">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"gfels6")</f>
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="J75" s="68">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"ziegm")</f>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="K75" s="68">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"jntme")</f>
-        <v>20</v>
+        <v>23.5</v>
       </c>
       <c r="L75" s="68">
         <f>SUMIFS(J$2:J$55,$B$2:$B$55,3,$F$2:$F$55,"kybup1")</f>
@@ -4388,11 +4388,11 @@
       </c>
       <c r="K81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"jntme")</f>
-        <v>11</v>
+        <v>19.5</v>
       </c>
       <c r="L81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"kybup1")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"petim1")</f>

</xml_diff>

<commit_message>
Updated scrum.xlsx with sprint 3 time
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester 2017/bfh_software-engineering/Project/sohpboia_git/doc/04-ScrumSetup/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="24240" windowHeight="13740" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -22,11 +17,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$55</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1251,7 +1243,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1559,14 +1551,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1665,16 +1657,16 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.5" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="13" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1883,7 +1875,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1903,7 +1895,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1925,7 +1917,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1953,28 +1945,28 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.33203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="25" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.1640625" style="1"/>
-    <col min="16" max="16" width="8.1640625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="9.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" style="25" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="1"/>
+    <col min="16" max="16" width="8.140625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -3170,7 +3162,7 @@
         <v>4</v>
       </c>
       <c r="K35" s="78">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L35" s="78" t="s">
         <v>163</v>
@@ -3774,7 +3766,7 @@
         <v>4</v>
       </c>
       <c r="K51" s="78">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L51" s="78" t="s">
         <v>110</v>
@@ -4025,11 +4017,11 @@
       </c>
       <c r="K61" s="1">
         <f>SUMIF(B2:B55,3,K2:K55)</f>
-        <v>54.75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="7:14" x14ac:dyDescent="0.2">
+        <v>63.75</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G65" s="96" t="s">
         <v>54</v>
       </c>
@@ -4041,7 +4033,7 @@
       <c r="M65" s="97"/>
       <c r="N65" s="98"/>
     </row>
-    <row r="66" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G66" s="66"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
@@ -4063,7 +4055,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G67" s="92" t="s">
         <v>148</v>
       </c>
@@ -4093,7 +4085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G68" s="92" t="s">
         <v>149</v>
       </c>
@@ -4123,7 +4115,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G69" s="94" t="s">
         <v>150</v>
       </c>
@@ -4153,8 +4145,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G71" s="96" t="s">
         <v>55</v>
       </c>
@@ -4166,7 +4158,7 @@
       <c r="M71" s="97"/>
       <c r="N71" s="98"/>
     </row>
-    <row r="72" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G72" s="66"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18" t="s">
@@ -4188,7 +4180,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G73" s="92" t="s">
         <v>148</v>
       </c>
@@ -4218,7 +4210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G74" s="92" t="s">
         <v>149</v>
       </c>
@@ -4248,7 +4240,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G75" s="94" t="s">
         <v>150</v>
       </c>
@@ -4278,8 +4270,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G77" s="96" t="s">
         <v>56</v>
       </c>
@@ -4291,7 +4283,7 @@
       <c r="M77" s="97"/>
       <c r="N77" s="98"/>
     </row>
-    <row r="78" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G78" s="66"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18" t="s">
@@ -4313,7 +4305,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G79" s="92" t="s">
         <v>148</v>
       </c>
@@ -4343,7 +4335,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="7:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G80" s="92" t="s">
         <v>149</v>
       </c>
@@ -4373,7 +4365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G81" s="94" t="s">
         <v>150</v>
       </c>
@@ -4392,7 +4384,7 @@
       </c>
       <c r="L81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"kybup1")</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"petim1")</f>
@@ -4454,14 +4446,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -4495,12 +4487,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="29.1" x14ac:dyDescent="0.35">
       <c r="B1" s="23" t="s">
         <v>125</v>
       </c>
@@ -4539,7 +4531,7 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -4604,7 +4596,7 @@
       <c r="N11" s="39"/>
       <c r="O11" s="39"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39" t="s">
@@ -4839,7 +4831,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A25" s="40"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -4856,7 +4848,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="40"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -4873,7 +4865,7 @@
       <c r="N26" s="39"/>
       <c r="O26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A27" s="40"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
@@ -4890,7 +4882,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A28" s="40"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -4907,7 +4899,7 @@
       <c r="N28" s="39"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A29" s="40"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -4924,7 +4916,7 @@
       <c r="N29" s="39"/>
       <c r="O29" s="39"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="40"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -4941,7 +4933,7 @@
       <c r="N30" s="39"/>
       <c r="O30" s="39"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="40"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -4958,7 +4950,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="39"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A32" s="40"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -4975,7 +4967,7 @@
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A33" s="40"/>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -4992,7 +4984,7 @@
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="40"/>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -5009,7 +5001,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="40"/>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -5026,7 +5018,7 @@
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A36" s="40"/>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
@@ -5043,7 +5035,7 @@
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A37" s="40"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -5060,7 +5052,7 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="40"/>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
@@ -5077,7 +5069,7 @@
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="40"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -5094,7 +5086,7 @@
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A40" s="40"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -5111,7 +5103,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A41" s="40"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -5128,7 +5120,7 @@
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A42" s="40"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
@@ -5145,7 +5137,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A43" s="40"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -5162,7 +5154,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="40"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -5179,7 +5171,7 @@
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="40"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -5196,7 +5188,7 @@
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A46" s="40"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -5213,7 +5205,7 @@
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A47" s="40"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -5230,7 +5222,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A48" s="40"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -5247,7 +5239,7 @@
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A49" s="40"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -5264,7 +5256,7 @@
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A50" s="40"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -5281,7 +5273,7 @@
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A51" s="40"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -5298,7 +5290,7 @@
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A52" s="40"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -5315,7 +5307,7 @@
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A53" s="40"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -5332,7 +5324,7 @@
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A54" s="40"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -5349,7 +5341,7 @@
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A55" s="40"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -5366,7 +5358,7 @@
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A56" s="40"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -5383,7 +5375,7 @@
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A57" s="40"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -5400,7 +5392,7 @@
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -5417,7 +5409,7 @@
       <c r="N58" s="39"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -5434,7 +5426,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="39"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -5451,7 +5443,7 @@
       <c r="N60" s="39"/>
       <c r="O60" s="39"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -5468,7 +5460,7 @@
       <c r="N61" s="39"/>
       <c r="O61" s="39"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -5485,7 +5477,7 @@
       <c r="N62" s="39"/>
       <c r="O62" s="39"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -5502,7 +5494,7 @@
       <c r="N63" s="39"/>
       <c r="O63" s="39"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -5519,7 +5511,7 @@
       <c r="N64" s="39"/>
       <c r="O64" s="39"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -5536,7 +5528,7 @@
       <c r="N65" s="39"/>
       <c r="O65" s="39"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -5553,7 +5545,7 @@
       <c r="N66" s="39"/>
       <c r="O66" s="39"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -5570,7 +5562,7 @@
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -5587,7 +5579,7 @@
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -5604,7 +5596,7 @@
       <c r="N69" s="39"/>
       <c r="O69" s="39"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -5621,7 +5613,7 @@
       <c r="N70" s="39"/>
       <c r="O70" s="39"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -5638,7 +5630,7 @@
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -5655,7 +5647,7 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -5672,7 +5664,7 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -5689,7 +5681,7 @@
       <c r="N74" s="39"/>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -5706,7 +5698,7 @@
       <c r="N75" s="39"/>
       <c r="O75" s="39"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -5723,7 +5715,7 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -5740,7 +5732,7 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -5757,7 +5749,7 @@
       <c r="N78" s="39"/>
       <c r="O78" s="39"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -5774,7 +5766,7 @@
       <c r="N79" s="39"/>
       <c r="O79" s="39"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -5791,7 +5783,7 @@
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -5808,7 +5800,7 @@
       <c r="N81" s="39"/>
       <c r="O81" s="39"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -5825,7 +5817,7 @@
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -5842,7 +5834,7 @@
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -5859,7 +5851,7 @@
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -5876,7 +5868,7 @@
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -5893,7 +5885,7 @@
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -5910,7 +5902,7 @@
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -5927,7 +5919,7 @@
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -5944,7 +5936,7 @@
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -5961,7 +5953,7 @@
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -5978,7 +5970,7 @@
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -5995,7 +5987,7 @@
       <c r="N92" s="39"/>
       <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -6012,7 +6004,7 @@
       <c r="N93" s="39"/>
       <c r="O93" s="39"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -6029,7 +6021,7 @@
       <c r="N94" s="39"/>
       <c r="O94" s="39"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -6046,7 +6038,7 @@
       <c r="N95" s="39"/>
       <c r="O95" s="39"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -6063,7 +6055,7 @@
       <c r="N96" s="39"/>
       <c r="O96" s="39"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -6080,7 +6072,7 @@
       <c r="N97" s="39"/>
       <c r="O97" s="39"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -6097,7 +6089,7 @@
       <c r="N98" s="39"/>
       <c r="O98" s="39"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -6114,7 +6106,7 @@
       <c r="N99" s="39"/>
       <c r="O99" s="39"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A100" s="39"/>
       <c r="B100" s="39"/>
       <c r="C100" s="39"/>
@@ -6131,7 +6123,7 @@
       <c r="N100" s="39"/>
       <c r="O100" s="39"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A101" s="39"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -6148,7 +6140,7 @@
       <c r="N101" s="39"/>
       <c r="O101" s="39"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A102" s="39"/>
       <c r="B102" s="39"/>
       <c r="C102" s="39"/>
@@ -6165,7 +6157,7 @@
       <c r="N102" s="39"/>
       <c r="O102" s="39"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A103" s="39"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -6182,7 +6174,7 @@
       <c r="N103" s="39"/>
       <c r="O103" s="39"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -6199,7 +6191,7 @@
       <c r="N104" s="39"/>
       <c r="O104" s="39"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A105" s="39"/>
       <c r="B105" s="39"/>
       <c r="C105" s="39"/>
@@ -6216,7 +6208,7 @@
       <c r="N105" s="39"/>
       <c r="O105" s="39"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A106" s="39"/>
       <c r="B106" s="39"/>
       <c r="C106" s="39"/>
@@ -6233,7 +6225,7 @@
       <c r="N106" s="39"/>
       <c r="O106" s="39"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A107" s="39"/>
       <c r="B107" s="39"/>
       <c r="C107" s="39"/>
@@ -6250,7 +6242,7 @@
       <c r="N107" s="39"/>
       <c r="O107" s="39"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A108" s="39"/>
       <c r="B108" s="39"/>
       <c r="C108" s="39"/>
@@ -6267,7 +6259,7 @@
       <c r="N108" s="39"/>
       <c r="O108" s="39"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A109" s="39"/>
       <c r="B109" s="39"/>
       <c r="C109" s="39"/>
@@ -6284,7 +6276,7 @@
       <c r="N109" s="39"/>
       <c r="O109" s="39"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A110" s="39"/>
       <c r="B110" s="39"/>
       <c r="C110" s="39"/>
@@ -6301,7 +6293,7 @@
       <c r="N110" s="39"/>
       <c r="O110" s="39"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A111" s="39"/>
       <c r="B111" s="39"/>
       <c r="C111" s="39"/>
@@ -6318,7 +6310,7 @@
       <c r="N111" s="39"/>
       <c r="O111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A112" s="39"/>
       <c r="B112" s="39"/>
       <c r="C112" s="39"/>
@@ -6335,7 +6327,7 @@
       <c r="N112" s="39"/>
       <c r="O112" s="39"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="39"/>
       <c r="B113" s="39"/>
       <c r="C113" s="39"/>
@@ -6352,7 +6344,7 @@
       <c r="N113" s="39"/>
       <c r="O113" s="39"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A114" s="39"/>
       <c r="B114" s="39"/>
       <c r="C114" s="39"/>
@@ -6369,7 +6361,7 @@
       <c r="N114" s="39"/>
       <c r="O114" s="39"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A115" s="39"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
@@ -6386,7 +6378,7 @@
       <c r="N115" s="39"/>
       <c r="O115" s="39"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A116" s="39"/>
       <c r="B116" s="39"/>
       <c r="C116" s="39"/>
@@ -6403,7 +6395,7 @@
       <c r="N116" s="39"/>
       <c r="O116" s="39"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A117" s="39"/>
       <c r="B117" s="39"/>
       <c r="C117" s="39"/>
@@ -6420,7 +6412,7 @@
       <c r="N117" s="39"/>
       <c r="O117" s="39"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A118" s="39"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
@@ -6437,7 +6429,7 @@
       <c r="N118" s="39"/>
       <c r="O118" s="39"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A119" s="39"/>
       <c r="B119" s="39"/>
       <c r="C119" s="39"/>
@@ -6454,7 +6446,7 @@
       <c r="N119" s="39"/>
       <c r="O119" s="39"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -6471,7 +6463,7 @@
       <c r="N120" s="39"/>
       <c r="O120" s="39"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A121" s="39"/>
       <c r="B121" s="39"/>
       <c r="C121" s="39"/>
@@ -6488,7 +6480,7 @@
       <c r="N121" s="39"/>
       <c r="O121" s="39"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A122" s="39"/>
       <c r="B122" s="39"/>
       <c r="C122" s="39"/>
@@ -6505,7 +6497,7 @@
       <c r="N122" s="39"/>
       <c r="O122" s="39"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A123" s="39"/>
       <c r="B123" s="39"/>
       <c r="C123" s="39"/>
@@ -6522,7 +6514,7 @@
       <c r="N123" s="39"/>
       <c r="O123" s="39"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A124" s="39"/>
       <c r="B124" s="39"/>
       <c r="C124" s="39"/>
@@ -6539,7 +6531,7 @@
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A125" s="39"/>
       <c r="B125" s="39"/>
       <c r="C125" s="39"/>
@@ -6556,7 +6548,7 @@
       <c r="N125" s="39"/>
       <c r="O125" s="39"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A126" s="39"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -6573,7 +6565,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="39"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A127" s="39"/>
       <c r="B127" s="39"/>
       <c r="C127" s="39"/>
@@ -6590,7 +6582,7 @@
       <c r="N127" s="39"/>
       <c r="O127" s="39"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39"/>
@@ -6607,7 +6599,7 @@
       <c r="N128" s="39"/>
       <c r="O128" s="39"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39"/>
@@ -6624,7 +6616,7 @@
       <c r="N129" s="39"/>
       <c r="O129" s="39"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39"/>
@@ -6641,7 +6633,7 @@
       <c r="N130" s="39"/>
       <c r="O130" s="39"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -6658,7 +6650,7 @@
       <c r="N131" s="39"/>
       <c r="O131" s="39"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -6675,7 +6667,7 @@
       <c r="N132" s="39"/>
       <c r="O132" s="39"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A133" s="39"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
@@ -6692,7 +6684,7 @@
       <c r="N133" s="39"/>
       <c r="O133" s="39"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A134" s="39"/>
       <c r="B134" s="39"/>
       <c r="C134" s="39"/>
@@ -6709,7 +6701,7 @@
       <c r="N134" s="39"/>
       <c r="O134" s="39"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -6726,7 +6718,7 @@
       <c r="N135" s="39"/>
       <c r="O135" s="39"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A136" s="39"/>
       <c r="B136" s="39"/>
       <c r="C136" s="39"/>
@@ -6743,7 +6735,7 @@
       <c r="N136" s="39"/>
       <c r="O136" s="39"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A137" s="39"/>
       <c r="B137" s="39"/>
       <c r="C137" s="39"/>
@@ -6760,7 +6752,7 @@
       <c r="N137" s="39"/>
       <c r="O137" s="39"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A138" s="39"/>
       <c r="B138" s="39"/>
       <c r="C138" s="39"/>
@@ -6777,7 +6769,7 @@
       <c r="N138" s="39"/>
       <c r="O138" s="39"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A139" s="39"/>
       <c r="B139" s="39"/>
       <c r="C139" s="39"/>
@@ -6794,7 +6786,7 @@
       <c r="N139" s="39"/>
       <c r="O139" s="39"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A140" s="39"/>
       <c r="B140" s="39"/>
       <c r="C140" s="39"/>
@@ -6811,7 +6803,7 @@
       <c r="N140" s="39"/>
       <c r="O140" s="39"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A141" s="39"/>
       <c r="B141" s="39"/>
       <c r="C141" s="39"/>
@@ -6828,7 +6820,7 @@
       <c r="N141" s="39"/>
       <c r="O141" s="39"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A142" s="39"/>
       <c r="B142" s="39"/>
       <c r="C142" s="39"/>
@@ -6845,7 +6837,7 @@
       <c r="N142" s="39"/>
       <c r="O142" s="39"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A143" s="39"/>
       <c r="B143" s="39"/>
       <c r="C143" s="39"/>
@@ -6862,7 +6854,7 @@
       <c r="N143" s="39"/>
       <c r="O143" s="39"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A144" s="39"/>
       <c r="B144" s="39"/>
       <c r="C144" s="39"/>
@@ -6879,7 +6871,7 @@
       <c r="N144" s="39"/>
       <c r="O144" s="39"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A145" s="39"/>
       <c r="B145" s="39"/>
       <c r="C145" s="39"/>
@@ -6896,7 +6888,7 @@
       <c r="N145" s="39"/>
       <c r="O145" s="39"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A146" s="39"/>
       <c r="B146" s="39"/>
       <c r="C146" s="39"/>
@@ -6913,7 +6905,7 @@
       <c r="N146" s="39"/>
       <c r="O146" s="39"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A147" s="39"/>
       <c r="B147" s="39"/>
       <c r="C147" s="39"/>
@@ -6930,7 +6922,7 @@
       <c r="N147" s="39"/>
       <c r="O147" s="39"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A148" s="39"/>
       <c r="B148" s="39"/>
       <c r="C148" s="39"/>
@@ -6947,7 +6939,7 @@
       <c r="N148" s="39"/>
       <c r="O148" s="39"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A149" s="39"/>
       <c r="B149" s="39"/>
       <c r="C149" s="39"/>
@@ -6964,7 +6956,7 @@
       <c r="N149" s="39"/>
       <c r="O149" s="39"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A150" s="39"/>
       <c r="B150" s="39"/>
       <c r="C150" s="39"/>
@@ -6981,7 +6973,7 @@
       <c r="N150" s="39"/>
       <c r="O150" s="39"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A151" s="39"/>
       <c r="B151" s="39"/>
       <c r="C151" s="39"/>
@@ -6998,7 +6990,7 @@
       <c r="N151" s="39"/>
       <c r="O151" s="39"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A152" s="39"/>
       <c r="B152" s="39"/>
       <c r="C152" s="39"/>
@@ -7015,7 +7007,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A153" s="39"/>
       <c r="B153" s="39"/>
       <c r="C153" s="39"/>
@@ -7032,7 +7024,7 @@
       <c r="N153" s="39"/>
       <c r="O153" s="39"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A154" s="39"/>
       <c r="B154" s="39"/>
       <c r="C154" s="39"/>
@@ -7049,7 +7041,7 @@
       <c r="N154" s="39"/>
       <c r="O154" s="39"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A155" s="39"/>
       <c r="B155" s="39"/>
       <c r="C155" s="39"/>
@@ -7066,7 +7058,7 @@
       <c r="N155" s="39"/>
       <c r="O155" s="39"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A156" s="39"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
@@ -7083,7 +7075,7 @@
       <c r="N156" s="39"/>
       <c r="O156" s="39"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A157" s="39"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
@@ -7100,7 +7092,7 @@
       <c r="N157" s="39"/>
       <c r="O157" s="39"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A158" s="39"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -7117,7 +7109,7 @@
       <c r="N158" s="39"/>
       <c r="O158" s="39"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A159" s="39"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -7134,7 +7126,7 @@
       <c r="N159" s="39"/>
       <c r="O159" s="39"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A160" s="39"/>
       <c r="B160" s="39"/>
       <c r="C160" s="39"/>
@@ -7151,7 +7143,7 @@
       <c r="N160" s="39"/>
       <c r="O160" s="39"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A161" s="39"/>
       <c r="B161" s="39"/>
       <c r="C161" s="39"/>
@@ -7168,7 +7160,7 @@
       <c r="N161" s="39"/>
       <c r="O161" s="39"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A162" s="39"/>
       <c r="B162" s="39"/>
       <c r="C162" s="39"/>
@@ -7185,7 +7177,7 @@
       <c r="N162" s="39"/>
       <c r="O162" s="39"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A163" s="39"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
@@ -7202,7 +7194,7 @@
       <c r="N163" s="39"/>
       <c r="O163" s="39"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A164" s="39"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
@@ -7219,7 +7211,7 @@
       <c r="N164" s="39"/>
       <c r="O164" s="39"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A165" s="39"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
@@ -7236,7 +7228,7 @@
       <c r="N165" s="39"/>
       <c r="O165" s="39"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A166" s="39"/>
       <c r="B166" s="39"/>
       <c r="C166" s="39"/>
@@ -7253,7 +7245,7 @@
       <c r="N166" s="39"/>
       <c r="O166" s="39"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A167" s="39"/>
       <c r="B167" s="39"/>
       <c r="C167" s="39"/>
@@ -7270,7 +7262,7 @@
       <c r="N167" s="39"/>
       <c r="O167" s="39"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A168" s="39"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -7287,7 +7279,7 @@
       <c r="N168" s="39"/>
       <c r="O168" s="39"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A169" s="39"/>
       <c r="B169" s="39"/>
       <c r="C169" s="39"/>
@@ -7304,7 +7296,7 @@
       <c r="N169" s="39"/>
       <c r="O169" s="39"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A170" s="39"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
@@ -7321,7 +7313,7 @@
       <c r="N170" s="39"/>
       <c r="O170" s="39"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A171" s="39"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -7338,7 +7330,7 @@
       <c r="N171" s="39"/>
       <c r="O171" s="39"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A172" s="39"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
@@ -7355,7 +7347,7 @@
       <c r="N172" s="39"/>
       <c r="O172" s="39"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A173" s="39"/>
       <c r="B173" s="39"/>
       <c r="C173" s="39"/>
@@ -7372,7 +7364,7 @@
       <c r="N173" s="39"/>
       <c r="O173" s="39"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A174" s="39"/>
       <c r="B174" s="39"/>
       <c r="C174" s="39"/>
@@ -7389,7 +7381,7 @@
       <c r="N174" s="39"/>
       <c r="O174" s="39"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A175" s="39"/>
       <c r="B175" s="39"/>
       <c r="C175" s="39"/>
@@ -7406,7 +7398,7 @@
       <c r="N175" s="39"/>
       <c r="O175" s="39"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A176" s="39"/>
       <c r="B176" s="39"/>
       <c r="C176" s="39"/>
@@ -7423,7 +7415,7 @@
       <c r="N176" s="39"/>
       <c r="O176" s="39"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A177" s="39"/>
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
@@ -7440,7 +7432,7 @@
       <c r="N177" s="39"/>
       <c r="O177" s="39"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A178" s="39"/>
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
@@ -7457,7 +7449,7 @@
       <c r="N178" s="39"/>
       <c r="O178" s="39"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A179" s="39"/>
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
@@ -7474,7 +7466,7 @@
       <c r="N179" s="39"/>
       <c r="O179" s="39"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A180" s="39"/>
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
@@ -7491,7 +7483,7 @@
       <c r="N180" s="39"/>
       <c r="O180" s="39"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A181" s="39"/>
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
@@ -7508,7 +7500,7 @@
       <c r="N181" s="39"/>
       <c r="O181" s="39"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A182" s="39"/>
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
@@ -7525,7 +7517,7 @@
       <c r="N182" s="39"/>
       <c r="O182" s="39"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A183" s="39"/>
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
@@ -7542,7 +7534,7 @@
       <c r="N183" s="39"/>
       <c r="O183" s="39"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A184" s="39"/>
       <c r="B184" s="39"/>
       <c r="C184" s="39"/>
@@ -7559,7 +7551,7 @@
       <c r="N184" s="39"/>
       <c r="O184" s="39"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
       <c r="C185" s="39"/>
@@ -7576,7 +7568,7 @@
       <c r="N185" s="39"/>
       <c r="O185" s="39"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
       <c r="C186" s="39"/>
@@ -7593,7 +7585,7 @@
       <c r="N186" s="39"/>
       <c r="O186" s="39"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A187" s="39"/>
       <c r="B187" s="39"/>
       <c r="C187" s="39"/>
@@ -7610,7 +7602,7 @@
       <c r="N187" s="39"/>
       <c r="O187" s="39"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A188" s="39"/>
       <c r="B188" s="39"/>
       <c r="C188" s="39"/>
@@ -7627,7 +7619,7 @@
       <c r="N188" s="39"/>
       <c r="O188" s="39"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A189" s="39"/>
       <c r="B189" s="39"/>
       <c r="C189" s="39"/>
@@ -7644,7 +7636,7 @@
       <c r="N189" s="39"/>
       <c r="O189" s="39"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A190" s="39"/>
       <c r="B190" s="39"/>
       <c r="C190" s="39"/>
@@ -7661,7 +7653,7 @@
       <c r="N190" s="39"/>
       <c r="O190" s="39"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A191" s="39"/>
       <c r="B191" s="39"/>
       <c r="C191" s="39"/>
@@ -7678,7 +7670,7 @@
       <c r="N191" s="39"/>
       <c r="O191" s="39"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A192" s="39"/>
       <c r="B192" s="39"/>
       <c r="C192" s="39"/>
@@ -7695,7 +7687,7 @@
       <c r="N192" s="39"/>
       <c r="O192" s="39"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A193" s="39"/>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -7712,7 +7704,7 @@
       <c r="N193" s="39"/>
       <c r="O193" s="39"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A194" s="39"/>
       <c r="B194" s="39"/>
       <c r="C194" s="39"/>
@@ -7729,7 +7721,7 @@
       <c r="N194" s="39"/>
       <c r="O194" s="39"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A195" s="39"/>
       <c r="B195" s="39"/>
       <c r="C195" s="39"/>
@@ -7746,7 +7738,7 @@
       <c r="N195" s="39"/>
       <c r="O195" s="39"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A196" s="39"/>
       <c r="B196" s="39"/>
       <c r="C196" s="39"/>
@@ -7763,7 +7755,7 @@
       <c r="N196" s="39"/>
       <c r="O196" s="39"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A197" s="39"/>
       <c r="B197" s="39"/>
       <c r="C197" s="39"/>
@@ -7780,7 +7772,7 @@
       <c r="N197" s="39"/>
       <c r="O197" s="39"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A198" s="39"/>
       <c r="B198" s="39"/>
       <c r="C198" s="39"/>
@@ -7797,7 +7789,7 @@
       <c r="N198" s="39"/>
       <c r="O198" s="39"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A199" s="39"/>
       <c r="B199" s="39"/>
       <c r="C199" s="39"/>
@@ -7814,7 +7806,7 @@
       <c r="N199" s="39"/>
       <c r="O199" s="39"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A200" s="39"/>
       <c r="B200" s="39"/>
       <c r="C200" s="39"/>
@@ -7831,7 +7823,7 @@
       <c r="N200" s="39"/>
       <c r="O200" s="39"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A201" s="39"/>
       <c r="B201" s="39"/>
       <c r="C201" s="39"/>
@@ -7848,7 +7840,7 @@
       <c r="N201" s="39"/>
       <c r="O201" s="39"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A202" s="39"/>
       <c r="B202" s="39"/>
       <c r="C202" s="39"/>
@@ -7865,7 +7857,7 @@
       <c r="N202" s="39"/>
       <c r="O202" s="39"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A203" s="39"/>
       <c r="B203" s="39"/>
       <c r="C203" s="39"/>
@@ -7882,7 +7874,7 @@
       <c r="N203" s="39"/>
       <c r="O203" s="39"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A204" s="39"/>
       <c r="B204" s="39"/>
       <c r="C204" s="39"/>
@@ -7899,7 +7891,7 @@
       <c r="N204" s="39"/>
       <c r="O204" s="39"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A205" s="39"/>
       <c r="B205" s="39"/>
       <c r="C205" s="39"/>
@@ -7916,7 +7908,7 @@
       <c r="N205" s="39"/>
       <c r="O205" s="39"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A206" s="39"/>
       <c r="B206" s="39"/>
       <c r="C206" s="39"/>
@@ -7933,7 +7925,7 @@
       <c r="N206" s="39"/>
       <c r="O206" s="39"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A207" s="39"/>
       <c r="B207" s="39"/>
       <c r="C207" s="39"/>
@@ -7950,7 +7942,7 @@
       <c r="N207" s="39"/>
       <c r="O207" s="39"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A208" s="39"/>
       <c r="B208" s="39"/>
       <c r="C208" s="39"/>
@@ -7967,7 +7959,7 @@
       <c r="N208" s="39"/>
       <c r="O208" s="39"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A209" s="39"/>
       <c r="B209" s="39"/>
       <c r="C209" s="39"/>
@@ -7984,7 +7976,7 @@
       <c r="N209" s="39"/>
       <c r="O209" s="39"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A210" s="39"/>
       <c r="B210" s="39"/>
       <c r="C210" s="39"/>
@@ -8001,7 +7993,7 @@
       <c r="N210" s="39"/>
       <c r="O210" s="39"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A211" s="39"/>
       <c r="B211" s="39"/>
       <c r="C211" s="39"/>
@@ -8018,7 +8010,7 @@
       <c r="N211" s="39"/>
       <c r="O211" s="39"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A212" s="39"/>
       <c r="B212" s="39"/>
       <c r="C212" s="39"/>
@@ -8035,7 +8027,7 @@
       <c r="N212" s="39"/>
       <c r="O212" s="39"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A213" s="39"/>
       <c r="B213" s="39"/>
       <c r="C213" s="39"/>
@@ -8052,7 +8044,7 @@
       <c r="N213" s="39"/>
       <c r="O213" s="39"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A214" s="39"/>
       <c r="B214" s="39"/>
       <c r="C214" s="39"/>
@@ -8069,7 +8061,7 @@
       <c r="N214" s="39"/>
       <c r="O214" s="39"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A215" s="39"/>
       <c r="B215" s="39"/>
       <c r="C215" s="39"/>
@@ -8086,7 +8078,7 @@
       <c r="N215" s="39"/>
       <c r="O215" s="39"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A216" s="39"/>
       <c r="B216" s="39"/>
       <c r="C216" s="39"/>
@@ -8103,7 +8095,7 @@
       <c r="N216" s="39"/>
       <c r="O216" s="39"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A217" s="39"/>
       <c r="B217" s="39"/>
       <c r="C217" s="39"/>
@@ -8120,7 +8112,7 @@
       <c r="N217" s="39"/>
       <c r="O217" s="39"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A218" s="39"/>
       <c r="B218" s="39"/>
       <c r="C218" s="39"/>
@@ -8137,7 +8129,7 @@
       <c r="N218" s="39"/>
       <c r="O218" s="39"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A219" s="39"/>
       <c r="B219" s="39"/>
       <c r="C219" s="39"/>
@@ -8154,7 +8146,7 @@
       <c r="N219" s="39"/>
       <c r="O219" s="39"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A220" s="39"/>
       <c r="B220" s="39"/>
       <c r="C220" s="39"/>
@@ -8171,7 +8163,7 @@
       <c r="N220" s="39"/>
       <c r="O220" s="39"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A221" s="39"/>
       <c r="B221" s="39"/>
       <c r="C221" s="39"/>
@@ -8188,7 +8180,7 @@
       <c r="N221" s="39"/>
       <c r="O221" s="39"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A222" s="39"/>
       <c r="B222" s="39"/>
       <c r="C222" s="39"/>
@@ -8205,7 +8197,7 @@
       <c r="N222" s="39"/>
       <c r="O222" s="39"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A223" s="39"/>
       <c r="B223" s="39"/>
       <c r="C223" s="39"/>
@@ -8222,7 +8214,7 @@
       <c r="N223" s="39"/>
       <c r="O223" s="39"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A224" s="39"/>
       <c r="B224" s="39"/>
       <c r="C224" s="39"/>
@@ -8239,7 +8231,7 @@
       <c r="N224" s="39"/>
       <c r="O224" s="39"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A225" s="39"/>
       <c r="B225" s="39"/>
       <c r="C225" s="39"/>
@@ -8256,7 +8248,7 @@
       <c r="N225" s="39"/>
       <c r="O225" s="39"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A226" s="39"/>
       <c r="B226" s="39"/>
       <c r="C226" s="39"/>
@@ -8273,7 +8265,7 @@
       <c r="N226" s="39"/>
       <c r="O226" s="39"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A227" s="39"/>
       <c r="B227" s="39"/>
       <c r="C227" s="39"/>
@@ -8290,7 +8282,7 @@
       <c r="N227" s="39"/>
       <c r="O227" s="39"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A228" s="39"/>
       <c r="B228" s="39"/>
       <c r="C228" s="39"/>
@@ -8307,7 +8299,7 @@
       <c r="N228" s="39"/>
       <c r="O228" s="39"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A229" s="39"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
@@ -8324,7 +8316,7 @@
       <c r="N229" s="39"/>
       <c r="O229" s="39"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A230" s="39"/>
       <c r="B230" s="39"/>
       <c r="C230" s="39"/>
@@ -8341,7 +8333,7 @@
       <c r="N230" s="39"/>
       <c r="O230" s="39"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A231" s="39"/>
       <c r="B231" s="39"/>
       <c r="C231" s="39"/>
@@ -8358,7 +8350,7 @@
       <c r="N231" s="39"/>
       <c r="O231" s="39"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A232" s="39"/>
       <c r="B232" s="39"/>
       <c r="C232" s="39"/>
@@ -8375,7 +8367,7 @@
       <c r="N232" s="39"/>
       <c r="O232" s="39"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A233" s="39"/>
       <c r="B233" s="39"/>
       <c r="C233" s="39"/>
@@ -8392,7 +8384,7 @@
       <c r="N233" s="39"/>
       <c r="O233" s="39"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A234" s="39"/>
       <c r="B234" s="39"/>
       <c r="C234" s="39"/>
@@ -8409,7 +8401,7 @@
       <c r="N234" s="39"/>
       <c r="O234" s="39"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A235" s="39"/>
       <c r="B235" s="39"/>
       <c r="C235" s="39"/>
@@ -8426,7 +8418,7 @@
       <c r="N235" s="39"/>
       <c r="O235" s="39"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A236" s="39"/>
       <c r="B236" s="39"/>
       <c r="C236" s="39"/>
@@ -8443,7 +8435,7 @@
       <c r="N236" s="39"/>
       <c r="O236" s="39"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A237" s="39"/>
       <c r="B237" s="39"/>
       <c r="C237" s="39"/>
@@ -8460,7 +8452,7 @@
       <c r="N237" s="39"/>
       <c r="O237" s="39"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A238" s="39"/>
       <c r="B238" s="39"/>
       <c r="C238" s="39"/>
@@ -8477,7 +8469,7 @@
       <c r="N238" s="39"/>
       <c r="O238" s="39"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A239" s="39"/>
       <c r="B239" s="39"/>
       <c r="C239" s="39"/>
@@ -8494,7 +8486,7 @@
       <c r="N239" s="39"/>
       <c r="O239" s="39"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A240" s="39"/>
       <c r="B240" s="39"/>
       <c r="C240" s="39"/>
@@ -8511,7 +8503,7 @@
       <c r="N240" s="39"/>
       <c r="O240" s="39"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A241" s="39"/>
       <c r="B241" s="39"/>
       <c r="C241" s="39"/>
@@ -8528,7 +8520,7 @@
       <c r="N241" s="39"/>
       <c r="O241" s="39"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A242" s="39"/>
       <c r="B242" s="39"/>
       <c r="C242" s="39"/>
@@ -8545,7 +8537,7 @@
       <c r="N242" s="39"/>
       <c r="O242" s="39"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A243" s="39"/>
       <c r="B243" s="39"/>
       <c r="C243" s="39"/>
@@ -8562,7 +8554,7 @@
       <c r="N243" s="39"/>
       <c r="O243" s="39"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A244" s="39"/>
       <c r="B244" s="39"/>
       <c r="C244" s="39"/>
@@ -8579,7 +8571,7 @@
       <c r="N244" s="39"/>
       <c r="O244" s="39"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A245" s="39"/>
       <c r="B245" s="39"/>
       <c r="C245" s="39"/>
@@ -8596,7 +8588,7 @@
       <c r="N245" s="39"/>
       <c r="O245" s="39"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A246" s="39"/>
       <c r="B246" s="39"/>
       <c r="C246" s="39"/>
@@ -8613,7 +8605,7 @@
       <c r="N246" s="39"/>
       <c r="O246" s="39"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A247" s="39"/>
       <c r="B247" s="39"/>
       <c r="C247" s="39"/>
@@ -8630,7 +8622,7 @@
       <c r="N247" s="39"/>
       <c r="O247" s="39"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A248" s="39"/>
       <c r="B248" s="39"/>
       <c r="C248" s="39"/>
@@ -8647,7 +8639,7 @@
       <c r="N248" s="39"/>
       <c r="O248" s="39"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A249" s="39"/>
       <c r="B249" s="39"/>
       <c r="C249" s="39"/>
@@ -8664,7 +8656,7 @@
       <c r="N249" s="39"/>
       <c r="O249" s="39"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A250" s="39"/>
       <c r="B250" s="39"/>
       <c r="C250" s="39"/>
@@ -8681,7 +8673,7 @@
       <c r="N250" s="39"/>
       <c r="O250" s="39"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A251" s="39"/>
       <c r="B251" s="39"/>
       <c r="C251" s="39"/>
@@ -8698,7 +8690,7 @@
       <c r="N251" s="39"/>
       <c r="O251" s="39"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A252" s="39"/>
       <c r="B252" s="39"/>
       <c r="C252" s="39"/>
@@ -8715,7 +8707,7 @@
       <c r="N252" s="39"/>
       <c r="O252" s="39"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A253" s="39"/>
       <c r="B253" s="39"/>
       <c r="C253" s="39"/>
@@ -8732,7 +8724,7 @@
       <c r="N253" s="39"/>
       <c r="O253" s="39"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A254" s="39"/>
       <c r="B254" s="39"/>
       <c r="C254" s="39"/>
@@ -8749,7 +8741,7 @@
       <c r="N254" s="39"/>
       <c r="O254" s="39"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A255" s="39"/>
       <c r="B255" s="39"/>
       <c r="C255" s="39"/>
@@ -8766,7 +8758,7 @@
       <c r="N255" s="39"/>
       <c r="O255" s="39"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A256" s="39"/>
       <c r="B256" s="39"/>
       <c r="C256" s="39"/>
@@ -8783,7 +8775,7 @@
       <c r="N256" s="39"/>
       <c r="O256" s="39"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A257" s="39"/>
       <c r="B257" s="39"/>
       <c r="C257" s="39"/>
@@ -8800,7 +8792,7 @@
       <c r="N257" s="39"/>
       <c r="O257" s="39"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A258" s="39"/>
       <c r="B258" s="39"/>
       <c r="C258" s="39"/>
@@ -8817,7 +8809,7 @@
       <c r="N258" s="39"/>
       <c r="O258" s="39"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A259" s="39"/>
       <c r="B259" s="39"/>
       <c r="C259" s="39"/>
@@ -8834,7 +8826,7 @@
       <c r="N259" s="39"/>
       <c r="O259" s="39"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A260" s="39"/>
       <c r="B260" s="39"/>
       <c r="C260" s="39"/>
@@ -8851,7 +8843,7 @@
       <c r="N260" s="39"/>
       <c r="O260" s="39"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A261" s="39"/>
       <c r="B261" s="39"/>
       <c r="C261" s="39"/>
@@ -8868,7 +8860,7 @@
       <c r="N261" s="39"/>
       <c r="O261" s="39"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A262" s="39"/>
       <c r="B262" s="39"/>
       <c r="C262" s="39"/>
@@ -8885,7 +8877,7 @@
       <c r="N262" s="39"/>
       <c r="O262" s="39"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A263" s="39"/>
       <c r="B263" s="39"/>
       <c r="C263" s="39"/>
@@ -8902,7 +8894,7 @@
       <c r="N263" s="39"/>
       <c r="O263" s="39"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A264" s="39"/>
       <c r="B264" s="39"/>
       <c r="C264" s="39"/>
@@ -8919,7 +8911,7 @@
       <c r="N264" s="39"/>
       <c r="O264" s="39"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A265" s="39"/>
       <c r="B265" s="39"/>
       <c r="C265" s="39"/>
@@ -8936,7 +8928,7 @@
       <c r="N265" s="39"/>
       <c r="O265" s="39"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A266" s="39"/>
       <c r="B266" s="39"/>
       <c r="C266" s="39"/>
@@ -8953,7 +8945,7 @@
       <c r="N266" s="39"/>
       <c r="O266" s="39"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A267" s="39"/>
       <c r="B267" s="39"/>
       <c r="C267" s="39"/>
@@ -8970,7 +8962,7 @@
       <c r="N267" s="39"/>
       <c r="O267" s="39"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A268" s="39"/>
       <c r="B268" s="39"/>
       <c r="C268" s="39"/>
@@ -8987,7 +8979,7 @@
       <c r="N268" s="39"/>
       <c r="O268" s="39"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
@@ -9004,7 +8996,7 @@
       <c r="N269" s="39"/>
       <c r="O269" s="39"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A270" s="39"/>
       <c r="B270" s="39"/>
       <c r="C270" s="39"/>
@@ -9021,7 +9013,7 @@
       <c r="N270" s="39"/>
       <c r="O270" s="39"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A271" s="39"/>
       <c r="B271" s="39"/>
       <c r="C271" s="39"/>
@@ -9038,7 +9030,7 @@
       <c r="N271" s="39"/>
       <c r="O271" s="39"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A272" s="39"/>
       <c r="B272" s="39"/>
       <c r="C272" s="39"/>
@@ -9055,7 +9047,7 @@
       <c r="N272" s="39"/>
       <c r="O272" s="39"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A273" s="39"/>
       <c r="B273" s="39"/>
       <c r="C273" s="39"/>
@@ -9072,7 +9064,7 @@
       <c r="N273" s="39"/>
       <c r="O273" s="39"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A274" s="39"/>
       <c r="B274" s="39"/>
       <c r="C274" s="39"/>
@@ -9089,7 +9081,7 @@
       <c r="N274" s="39"/>
       <c r="O274" s="39"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A275" s="39"/>
       <c r="B275" s="39"/>
       <c r="C275" s="39"/>
@@ -9106,7 +9098,7 @@
       <c r="N275" s="39"/>
       <c r="O275" s="39"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A276" s="39"/>
       <c r="B276" s="39"/>
       <c r="C276" s="39"/>
@@ -9123,7 +9115,7 @@
       <c r="N276" s="39"/>
       <c r="O276" s="39"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A277" s="39"/>
       <c r="B277" s="39"/>
       <c r="C277" s="39"/>
@@ -9140,7 +9132,7 @@
       <c r="N277" s="39"/>
       <c r="O277" s="39"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A278" s="39"/>
       <c r="B278" s="39"/>
       <c r="C278" s="39"/>
@@ -9157,7 +9149,7 @@
       <c r="N278" s="39"/>
       <c r="O278" s="39"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A279" s="39"/>
       <c r="B279" s="39"/>
       <c r="C279" s="39"/>
@@ -9174,7 +9166,7 @@
       <c r="N279" s="39"/>
       <c r="O279" s="39"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A280" s="39"/>
       <c r="B280" s="39"/>
       <c r="C280" s="39"/>
@@ -9191,7 +9183,7 @@
       <c r="N280" s="39"/>
       <c r="O280" s="39"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A281" s="39"/>
       <c r="B281" s="39"/>
       <c r="C281" s="39"/>
@@ -9208,7 +9200,7 @@
       <c r="N281" s="39"/>
       <c r="O281" s="39"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A282" s="39"/>
       <c r="B282" s="39"/>
       <c r="C282" s="39"/>
@@ -9225,7 +9217,7 @@
       <c r="N282" s="39"/>
       <c r="O282" s="39"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A283" s="39"/>
       <c r="B283" s="39"/>
       <c r="C283" s="39"/>
@@ -9242,7 +9234,7 @@
       <c r="N283" s="39"/>
       <c r="O283" s="39"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A284" s="39"/>
       <c r="B284" s="39"/>
       <c r="C284" s="39"/>
@@ -9259,7 +9251,7 @@
       <c r="N284" s="39"/>
       <c r="O284" s="39"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A285" s="39"/>
       <c r="B285" s="39"/>
       <c r="C285" s="39"/>
@@ -9276,7 +9268,7 @@
       <c r="N285" s="39"/>
       <c r="O285" s="39"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A286" s="39"/>
       <c r="B286" s="39"/>
       <c r="C286" s="39"/>
@@ -9293,7 +9285,7 @@
       <c r="N286" s="39"/>
       <c r="O286" s="39"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A287" s="39"/>
       <c r="B287" s="39"/>
       <c r="C287" s="39"/>
@@ -9310,7 +9302,7 @@
       <c r="N287" s="39"/>
       <c r="O287" s="39"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A288" s="39"/>
       <c r="B288" s="39"/>
       <c r="C288" s="39"/>
@@ -9327,7 +9319,7 @@
       <c r="N288" s="39"/>
       <c r="O288" s="39"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A289" s="39"/>
       <c r="B289" s="39"/>
       <c r="C289" s="39"/>
@@ -9344,7 +9336,7 @@
       <c r="N289" s="39"/>
       <c r="O289" s="39"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A290" s="39"/>
       <c r="B290" s="39"/>
       <c r="C290" s="39"/>
@@ -9361,7 +9353,7 @@
       <c r="N290" s="39"/>
       <c r="O290" s="39"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A291" s="39"/>
       <c r="B291" s="39"/>
       <c r="C291" s="39"/>
@@ -9378,7 +9370,7 @@
       <c r="N291" s="39"/>
       <c r="O291" s="39"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A292" s="39"/>
       <c r="B292" s="39"/>
       <c r="C292" s="39"/>
@@ -9395,7 +9387,7 @@
       <c r="N292" s="39"/>
       <c r="O292" s="39"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A293" s="39"/>
       <c r="B293" s="39"/>
       <c r="C293" s="39"/>
@@ -9412,7 +9404,7 @@
       <c r="N293" s="39"/>
       <c r="O293" s="39"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A294" s="39"/>
       <c r="B294" s="39"/>
       <c r="C294" s="39"/>
@@ -9429,7 +9421,7 @@
       <c r="N294" s="39"/>
       <c r="O294" s="39"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A295" s="39"/>
       <c r="B295" s="39"/>
       <c r="C295" s="39"/>
@@ -9446,7 +9438,7 @@
       <c r="N295" s="39"/>
       <c r="O295" s="39"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A296" s="39"/>
       <c r="B296" s="39"/>
       <c r="C296" s="39"/>
@@ -9463,7 +9455,7 @@
       <c r="N296" s="39"/>
       <c r="O296" s="39"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A297" s="39"/>
       <c r="B297" s="39"/>
       <c r="C297" s="39"/>
@@ -9480,7 +9472,7 @@
       <c r="N297" s="39"/>
       <c r="O297" s="39"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A298" s="39"/>
       <c r="B298" s="39"/>
       <c r="C298" s="39"/>
@@ -9497,7 +9489,7 @@
       <c r="N298" s="39"/>
       <c r="O298" s="39"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A299" s="39"/>
       <c r="B299" s="39"/>
       <c r="C299" s="39"/>
@@ -9514,7 +9506,7 @@
       <c r="N299" s="39"/>
       <c r="O299" s="39"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A300" s="39"/>
       <c r="B300" s="39"/>
       <c r="C300" s="39"/>
@@ -9531,7 +9523,7 @@
       <c r="N300" s="39"/>
       <c r="O300" s="39"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A301" s="39"/>
       <c r="B301" s="39"/>
       <c r="C301" s="39"/>
@@ -9548,7 +9540,7 @@
       <c r="N301" s="39"/>
       <c r="O301" s="39"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A302" s="39"/>
       <c r="B302" s="39"/>
       <c r="C302" s="39"/>
@@ -9565,7 +9557,7 @@
       <c r="N302" s="39"/>
       <c r="O302" s="39"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A303" s="39"/>
       <c r="B303" s="39"/>
       <c r="C303" s="39"/>
@@ -9582,7 +9574,7 @@
       <c r="N303" s="39"/>
       <c r="O303" s="39"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A304" s="39"/>
       <c r="B304" s="39"/>
       <c r="C304" s="39"/>
@@ -9599,7 +9591,7 @@
       <c r="N304" s="39"/>
       <c r="O304" s="39"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A305" s="39"/>
       <c r="B305" s="39"/>
       <c r="C305" s="39"/>
@@ -9616,7 +9608,7 @@
       <c r="N305" s="39"/>
       <c r="O305" s="39"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A306" s="39"/>
       <c r="B306" s="39"/>
       <c r="C306" s="39"/>
@@ -9633,7 +9625,7 @@
       <c r="N306" s="39"/>
       <c r="O306" s="39"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A307" s="39"/>
       <c r="B307" s="39"/>
       <c r="C307" s="39"/>
@@ -9650,7 +9642,7 @@
       <c r="N307" s="39"/>
       <c r="O307" s="39"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A308" s="39"/>
       <c r="B308" s="39"/>
       <c r="C308" s="39"/>
@@ -9667,7 +9659,7 @@
       <c r="N308" s="39"/>
       <c r="O308" s="39"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A309" s="39"/>
       <c r="B309" s="39"/>
       <c r="C309" s="39"/>
@@ -9684,7 +9676,7 @@
       <c r="N309" s="39"/>
       <c r="O309" s="39"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A310" s="39"/>
       <c r="B310" s="39"/>
       <c r="C310" s="39"/>
@@ -9701,7 +9693,7 @@
       <c r="N310" s="39"/>
       <c r="O310" s="39"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A311" s="39"/>
       <c r="B311" s="39"/>
       <c r="C311" s="39"/>
@@ -9718,7 +9710,7 @@
       <c r="N311" s="39"/>
       <c r="O311" s="39"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A312" s="39"/>
       <c r="B312" s="39"/>
       <c r="C312" s="39"/>
@@ -9735,7 +9727,7 @@
       <c r="N312" s="39"/>
       <c r="O312" s="39"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A313" s="39"/>
       <c r="B313" s="39"/>
       <c r="C313" s="39"/>
@@ -9752,7 +9744,7 @@
       <c r="N313" s="39"/>
       <c r="O313" s="39"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A314" s="39"/>
       <c r="B314" s="39"/>
       <c r="C314" s="39"/>
@@ -9769,7 +9761,7 @@
       <c r="N314" s="39"/>
       <c r="O314" s="39"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A315" s="39"/>
       <c r="B315" s="39"/>
       <c r="C315" s="39"/>
@@ -9786,7 +9778,7 @@
       <c r="N315" s="39"/>
       <c r="O315" s="39"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A316" s="39"/>
       <c r="B316" s="39"/>
       <c r="C316" s="39"/>
@@ -9803,7 +9795,7 @@
       <c r="N316" s="39"/>
       <c r="O316" s="39"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A317" s="39"/>
       <c r="B317" s="39"/>
       <c r="C317" s="39"/>
@@ -9820,7 +9812,7 @@
       <c r="N317" s="39"/>
       <c r="O317" s="39"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A318" s="39"/>
       <c r="B318" s="39"/>
       <c r="C318" s="39"/>
@@ -9837,7 +9829,7 @@
       <c r="N318" s="39"/>
       <c r="O318" s="39"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A319" s="39"/>
       <c r="B319" s="39"/>
       <c r="C319" s="39"/>
@@ -9854,7 +9846,7 @@
       <c r="N319" s="39"/>
       <c r="O319" s="39"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A320" s="39"/>
       <c r="B320" s="39"/>
       <c r="C320" s="39"/>
@@ -9871,7 +9863,7 @@
       <c r="N320" s="39"/>
       <c r="O320" s="39"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A321" s="39"/>
       <c r="B321" s="39"/>
       <c r="C321" s="39"/>
@@ -9888,7 +9880,7 @@
       <c r="N321" s="39"/>
       <c r="O321" s="39"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A322" s="39"/>
       <c r="B322" s="39"/>
       <c r="C322" s="39"/>
@@ -9905,7 +9897,7 @@
       <c r="N322" s="39"/>
       <c r="O322" s="39"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A323" s="39"/>
       <c r="B323" s="39"/>
       <c r="C323" s="39"/>
@@ -9922,7 +9914,7 @@
       <c r="N323" s="39"/>
       <c r="O323" s="39"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A324" s="39"/>
       <c r="B324" s="39"/>
       <c r="C324" s="39"/>
@@ -9939,7 +9931,7 @@
       <c r="N324" s="39"/>
       <c r="O324" s="39"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A325" s="39"/>
       <c r="B325" s="39"/>
       <c r="C325" s="39"/>
@@ -9956,7 +9948,7 @@
       <c r="N325" s="39"/>
       <c r="O325" s="39"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A326" s="39"/>
       <c r="B326" s="39"/>
       <c r="C326" s="39"/>
@@ -9973,7 +9965,7 @@
       <c r="N326" s="39"/>
       <c r="O326" s="39"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
       <c r="C327" s="39"/>
@@ -9990,7 +9982,7 @@
       <c r="N327" s="39"/>
       <c r="O327" s="39"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A328" s="39"/>
       <c r="B328" s="39"/>
       <c r="C328" s="39"/>
@@ -10007,7 +9999,7 @@
       <c r="N328" s="39"/>
       <c r="O328" s="39"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A329" s="39"/>
       <c r="B329" s="39"/>
       <c r="C329" s="39"/>
@@ -10024,7 +10016,7 @@
       <c r="N329" s="39"/>
       <c r="O329" s="39"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A330" s="39"/>
       <c r="B330" s="39"/>
       <c r="C330" s="39"/>
@@ -10041,7 +10033,7 @@
       <c r="N330" s="39"/>
       <c r="O330" s="39"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A331" s="39"/>
       <c r="B331" s="39"/>
       <c r="C331" s="39"/>
@@ -10058,7 +10050,7 @@
       <c r="N331" s="39"/>
       <c r="O331" s="39"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A332" s="39"/>
       <c r="B332" s="39"/>
       <c r="C332" s="39"/>
@@ -10075,7 +10067,7 @@
       <c r="N332" s="39"/>
       <c r="O332" s="39"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A333" s="39"/>
       <c r="B333" s="39"/>
       <c r="C333" s="39"/>
@@ -10092,7 +10084,7 @@
       <c r="N333" s="39"/>
       <c r="O333" s="39"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A334" s="39"/>
       <c r="B334" s="39"/>
       <c r="C334" s="39"/>
@@ -10109,7 +10101,7 @@
       <c r="N334" s="39"/>
       <c r="O334" s="39"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A335" s="39"/>
       <c r="B335" s="39"/>
       <c r="C335" s="39"/>
@@ -10126,7 +10118,7 @@
       <c r="N335" s="39"/>
       <c r="O335" s="39"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A336" s="39"/>
       <c r="B336" s="39"/>
       <c r="C336" s="39"/>
@@ -10143,7 +10135,7 @@
       <c r="N336" s="39"/>
       <c r="O336" s="39"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A337" s="39"/>
       <c r="B337" s="39"/>
       <c r="C337" s="39"/>
@@ -10160,7 +10152,7 @@
       <c r="N337" s="39"/>
       <c r="O337" s="39"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A338" s="39"/>
       <c r="B338" s="39"/>
       <c r="C338" s="39"/>
@@ -10177,7 +10169,7 @@
       <c r="N338" s="39"/>
       <c r="O338" s="39"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A339" s="39"/>
       <c r="B339" s="39"/>
       <c r="C339" s="39"/>
@@ -10194,7 +10186,7 @@
       <c r="N339" s="39"/>
       <c r="O339" s="39"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A340" s="39"/>
       <c r="B340" s="39"/>
       <c r="C340" s="39"/>
@@ -10211,7 +10203,7 @@
       <c r="N340" s="39"/>
       <c r="O340" s="39"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A341" s="39"/>
       <c r="B341" s="39"/>
       <c r="C341" s="39"/>
@@ -10228,7 +10220,7 @@
       <c r="N341" s="39"/>
       <c r="O341" s="39"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A342" s="39"/>
       <c r="B342" s="39"/>
       <c r="C342" s="39"/>
@@ -10245,7 +10237,7 @@
       <c r="N342" s="39"/>
       <c r="O342" s="39"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A343" s="39"/>
       <c r="B343" s="39"/>
       <c r="C343" s="39"/>
@@ -10262,7 +10254,7 @@
       <c r="N343" s="39"/>
       <c r="O343" s="39"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A344" s="39"/>
       <c r="B344" s="39"/>
       <c r="C344" s="39"/>
@@ -10279,7 +10271,7 @@
       <c r="N344" s="39"/>
       <c r="O344" s="39"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A345" s="39"/>
       <c r="B345" s="39"/>
       <c r="C345" s="39"/>
@@ -10296,7 +10288,7 @@
       <c r="N345" s="39"/>
       <c r="O345" s="39"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="39"/>
@@ -10326,12 +10318,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29.1" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>

</xml_diff>

<commit_message>
updated scrum.xlsx and pres.pptx after last scrum meeting
</commit_message>
<xml_diff>
--- a/doc/04-ScrumSetup/scrum.xlsx
+++ b/doc/04-ScrumSetup/scrum.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mij2/Dropbox/01-BFH Student/06-Herbstsemester 2017/bfh_software-engineering/Project/sohpboia_git/doc/04-ScrumSetup/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="23256" windowHeight="13176" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -17,8 +22,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$B$1:$L$55</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -1243,7 +1251,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1551,14 +1559,14 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +1577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1580,7 +1588,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1602,7 +1610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1613,7 +1621,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1624,7 +1632,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1653,20 +1661,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="141" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="37.33203125" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1875,7 +1883,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="13">
         <v>7</v>
       </c>
@@ -1895,7 +1903,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
         <v>8</v>
       </c>
@@ -1917,7 +1925,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>60</v>
       </c>
@@ -1945,28 +1953,28 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="125" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" style="20" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="21" customWidth="1"/>
     <col min="3" max="3" width="44.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="25" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" style="1" customWidth="1"/>
-    <col min="14" max="15" width="9.109375" style="1"/>
-    <col min="16" max="16" width="8.109375" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="13" max="13" width="9.5" style="1" customWidth="1"/>
+    <col min="14" max="15" width="9.1640625" style="1"/>
+    <col min="16" max="16" width="8.1640625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -2045,7 +2053,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="70" t="s">
         <v>66</v>
       </c>
@@ -2069,7 +2077,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A4" s="79" t="s">
         <v>67</v>
       </c>
@@ -2145,7 +2153,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="79" t="s">
         <v>219</v>
       </c>
@@ -2183,7 +2191,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:12" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="75">
         <v>1.1000000000000001</v>
       </c>
@@ -2202,7 +2210,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="75">
         <v>1.2</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" s="74" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" s="74" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="70">
         <v>1.3</v>
       </c>
@@ -2245,7 +2253,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:12" s="30" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" s="30" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>63</v>
       </c>
@@ -2374,7 +2382,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="89" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" s="89" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="87">
         <v>2.2999999999999998</v>
       </c>
@@ -2431,7 +2439,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="28" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32">
         <v>3.2</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="79" t="s">
         <v>221</v>
       </c>
@@ -3016,7 +3024,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="79" t="s">
         <v>220</v>
       </c>
@@ -3054,7 +3062,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="79" t="s">
         <v>222</v>
       </c>
@@ -3092,7 +3100,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:12" s="78" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="79" t="s">
         <v>223</v>
       </c>
@@ -3165,7 +3173,7 @@
         <v>5</v>
       </c>
       <c r="L35" s="78" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -3200,10 +3208,10 @@
         <v>4</v>
       </c>
       <c r="K36" s="78">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="L36" s="78" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -3236,13 +3244,13 @@
         <v>4</v>
       </c>
       <c r="K37" s="78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="78" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="79"/>
       <c r="B38" s="80">
         <v>3</v>
@@ -3278,7 +3286,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" s="79" t="s">
         <v>212</v>
       </c>
@@ -3316,7 +3324,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:12" s="78" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" s="78" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A40" s="79" t="s">
         <v>213</v>
       </c>
@@ -3389,7 +3397,7 @@
         <v>1.5</v>
       </c>
       <c r="L41" s="82" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="78" customFormat="1" ht="90" x14ac:dyDescent="0.2">
@@ -3506,7 +3514,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:12" s="52" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:12" s="52" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="64" t="s">
         <v>133</v>
       </c>
@@ -3582,7 +3590,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:12" s="78" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A47" s="79" t="s">
         <v>218</v>
       </c>
@@ -3620,7 +3628,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:12" s="78" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:12" s="78" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="79" t="s">
         <v>233</v>
       </c>
@@ -3804,13 +3812,13 @@
         <v>5</v>
       </c>
       <c r="K52" s="82">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L52" s="82" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:17" s="82" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" s="82" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="84">
         <v>7.11</v>
       </c>
@@ -3845,10 +3853,10 @@
         <v>2.75</v>
       </c>
       <c r="L53" s="84" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" s="86" customFormat="1" ht="15" hidden="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="86" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="86">
         <v>7.12</v>
       </c>
@@ -3915,7 +3923,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="17"/>
       <c r="C56" s="18"/>
@@ -3929,7 +3937,7 @@
       <c r="K56" s="18"/>
       <c r="L56" s="18"/>
     </row>
-    <row r="57" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="17"/>
       <c r="C57" s="18"/>
@@ -3941,7 +3949,7 @@
       <c r="P57" s="91"/>
       <c r="Q57" s="91"/>
     </row>
-    <row r="58" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E58" s="18"/>
       <c r="F58" s="22"/>
       <c r="G58" s="18"/>
@@ -3957,7 +3965,7 @@
       </c>
       <c r="L58" s="18"/>
     </row>
-    <row r="59" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E59" s="1" t="s">
         <v>152</v>
       </c>
@@ -3978,7 +3986,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E60" s="1" t="s">
         <v>153</v>
       </c>
@@ -3999,7 +4007,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="E61" s="1" t="s">
         <v>154</v>
       </c>
@@ -4017,11 +4025,11 @@
       </c>
       <c r="K61" s="1">
         <f>SUMIF(B2:B55,3,K2:K55)</f>
-        <v>68.75</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+        <v>65.25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G65" s="96" t="s">
         <v>54</v>
       </c>
@@ -4033,7 +4041,7 @@
       <c r="M65" s="97"/>
       <c r="N65" s="98"/>
     </row>
-    <row r="66" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G66" s="66"/>
       <c r="H66" s="18"/>
       <c r="I66" s="18" t="s">
@@ -4055,7 +4063,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="67" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G67" s="92" t="s">
         <v>148</v>
       </c>
@@ -4085,7 +4093,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="68" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G68" s="92" t="s">
         <v>149</v>
       </c>
@@ -4115,7 +4123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G69" s="94" t="s">
         <v>150</v>
       </c>
@@ -4145,8 +4153,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G71" s="96" t="s">
         <v>55</v>
       </c>
@@ -4158,7 +4166,7 @@
       <c r="M71" s="97"/>
       <c r="N71" s="98"/>
     </row>
-    <row r="72" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G72" s="66"/>
       <c r="H72" s="18"/>
       <c r="I72" s="18" t="s">
@@ -4180,7 +4188,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G73" s="92" t="s">
         <v>148</v>
       </c>
@@ -4210,7 +4218,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="74" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G74" s="92" t="s">
         <v>149</v>
       </c>
@@ -4240,7 +4248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G75" s="94" t="s">
         <v>150</v>
       </c>
@@ -4270,8 +4278,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="7:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G77" s="96" t="s">
         <v>56</v>
       </c>
@@ -4283,7 +4291,7 @@
       <c r="M77" s="97"/>
       <c r="N77" s="98"/>
     </row>
-    <row r="78" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G78" s="66"/>
       <c r="H78" s="18"/>
       <c r="I78" s="18" t="s">
@@ -4305,7 +4313,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G79" s="92" t="s">
         <v>148</v>
       </c>
@@ -4335,7 +4343,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="7:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G80" s="92" t="s">
         <v>149</v>
       </c>
@@ -4365,14 +4373,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="7:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="7:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G81" s="94" t="s">
         <v>150</v>
       </c>
       <c r="H81" s="95"/>
       <c r="I81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"gfels6")</f>
-        <v>11.5</v>
+        <v>12.5</v>
       </c>
       <c r="J81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"ziegm")</f>
@@ -4380,7 +4388,7 @@
       </c>
       <c r="K81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"jntme")</f>
-        <v>19.5</v>
+        <v>20</v>
       </c>
       <c r="L81" s="68">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"kybup1")</f>
@@ -4392,7 +4400,7 @@
       </c>
       <c r="N81" s="69">
         <f>SUMIFS(K$2:K$55,$B$2:$B$55,3,$F$2:$F$55,"odaoj1")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4400,12 +4408,6 @@
     <filterColumn colId="0">
       <filters>
         <filter val="3"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="10">
-      <filters>
-        <filter val="pending"/>
-        <filter val="waiting"/>
       </filters>
     </filterColumn>
     <sortState ref="B4:L54">
@@ -4446,14 +4448,14 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -4467,10 +4469,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="6"/>
     </row>
   </sheetData>
@@ -4487,12 +4489,12 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="B1" s="23" t="s">
         <v>125</v>
       </c>
@@ -4531,7 +4533,7 @@
       <c r="N8" s="39"/>
       <c r="O8" s="39"/>
     </row>
-    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>1</v>
       </c>
@@ -4596,7 +4598,7 @@
       <c r="N11" s="39"/>
       <c r="O11" s="39"/>
     </row>
-    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="39"/>
       <c r="C12" s="39" t="s">
@@ -4831,7 +4833,7 @@
       <c r="N24" s="39"/>
       <c r="O24" s="39"/>
     </row>
-    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
@@ -4848,7 +4850,7 @@
       <c r="N25" s="39"/>
       <c r="O25" s="39"/>
     </row>
-    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
@@ -4865,7 +4867,7 @@
       <c r="N26" s="39"/>
       <c r="O26" s="39"/>
     </row>
-    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
@@ -4882,7 +4884,7 @@
       <c r="N27" s="39"/>
       <c r="O27" s="39"/>
     </row>
-    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
@@ -4899,7 +4901,7 @@
       <c r="N28" s="39"/>
       <c r="O28" s="39"/>
     </row>
-    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
@@ -4916,7 +4918,7 @@
       <c r="N29" s="39"/>
       <c r="O29" s="39"/>
     </row>
-    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
@@ -4933,7 +4935,7 @@
       <c r="N30" s="39"/>
       <c r="O30" s="39"/>
     </row>
-    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
@@ -4950,7 +4952,7 @@
       <c r="N31" s="39"/>
       <c r="O31" s="39"/>
     </row>
-    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="40"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
@@ -4967,7 +4969,7 @@
       <c r="N32" s="39"/>
       <c r="O32" s="39"/>
     </row>
-    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
@@ -4984,7 +4986,7 @@
       <c r="N33" s="39"/>
       <c r="O33" s="39"/>
     </row>
-    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
@@ -5001,7 +5003,7 @@
       <c r="N34" s="39"/>
       <c r="O34" s="39"/>
     </row>
-    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
@@ -5018,7 +5020,7 @@
       <c r="N35" s="39"/>
       <c r="O35" s="39"/>
     </row>
-    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="39"/>
       <c r="C36" s="39"/>
@@ -5035,7 +5037,7 @@
       <c r="N36" s="39"/>
       <c r="O36" s="39"/>
     </row>
-    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="39"/>
       <c r="C37" s="39"/>
@@ -5052,7 +5054,7 @@
       <c r="N37" s="39"/>
       <c r="O37" s="39"/>
     </row>
-    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="40"/>
       <c r="B38" s="39"/>
       <c r="C38" s="39"/>
@@ -5069,7 +5071,7 @@
       <c r="N38" s="39"/>
       <c r="O38" s="39"/>
     </row>
-    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="40"/>
       <c r="B39" s="39"/>
       <c r="C39" s="39"/>
@@ -5086,7 +5088,7 @@
       <c r="N39" s="39"/>
       <c r="O39" s="39"/>
     </row>
-    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="40"/>
       <c r="B40" s="39"/>
       <c r="C40" s="39"/>
@@ -5103,7 +5105,7 @@
       <c r="N40" s="39"/>
       <c r="O40" s="39"/>
     </row>
-    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="40"/>
       <c r="B41" s="39"/>
       <c r="C41" s="39"/>
@@ -5120,7 +5122,7 @@
       <c r="N41" s="39"/>
       <c r="O41" s="39"/>
     </row>
-    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="40"/>
       <c r="B42" s="39"/>
       <c r="C42" s="39"/>
@@ -5137,7 +5139,7 @@
       <c r="N42" s="39"/>
       <c r="O42" s="39"/>
     </row>
-    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="40"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -5154,7 +5156,7 @@
       <c r="N43" s="39"/>
       <c r="O43" s="39"/>
     </row>
-    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="40"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -5171,7 +5173,7 @@
       <c r="N44" s="39"/>
       <c r="O44" s="39"/>
     </row>
-    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="40"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -5188,7 +5190,7 @@
       <c r="N45" s="39"/>
       <c r="O45" s="39"/>
     </row>
-    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="40"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -5205,7 +5207,7 @@
       <c r="N46" s="39"/>
       <c r="O46" s="39"/>
     </row>
-    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="40"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -5222,7 +5224,7 @@
       <c r="N47" s="39"/>
       <c r="O47" s="39"/>
     </row>
-    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="40"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -5239,7 +5241,7 @@
       <c r="N48" s="39"/>
       <c r="O48" s="39"/>
     </row>
-    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="40"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -5256,7 +5258,7 @@
       <c r="N49" s="39"/>
       <c r="O49" s="39"/>
     </row>
-    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="40"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -5273,7 +5275,7 @@
       <c r="N50" s="39"/>
       <c r="O50" s="39"/>
     </row>
-    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="40"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -5290,7 +5292,7 @@
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
     </row>
-    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="40"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -5307,7 +5309,7 @@
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
     </row>
-    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="40"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -5324,7 +5326,7 @@
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
     </row>
-    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="40"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -5341,7 +5343,7 @@
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
     </row>
-    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="40"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -5358,7 +5360,7 @@
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
     </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="40"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -5375,7 +5377,7 @@
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
     </row>
-    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="40"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -5392,7 +5394,7 @@
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
     </row>
-    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -5409,7 +5411,7 @@
       <c r="N58" s="39"/>
       <c r="O58" s="39"/>
     </row>
-    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -5426,7 +5428,7 @@
       <c r="N59" s="39"/>
       <c r="O59" s="39"/>
     </row>
-    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -5443,7 +5445,7 @@
       <c r="N60" s="39"/>
       <c r="O60" s="39"/>
     </row>
-    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -5460,7 +5462,7 @@
       <c r="N61" s="39"/>
       <c r="O61" s="39"/>
     </row>
-    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -5477,7 +5479,7 @@
       <c r="N62" s="39"/>
       <c r="O62" s="39"/>
     </row>
-    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -5494,7 +5496,7 @@
       <c r="N63" s="39"/>
       <c r="O63" s="39"/>
     </row>
-    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -5511,7 +5513,7 @@
       <c r="N64" s="39"/>
       <c r="O64" s="39"/>
     </row>
-    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -5528,7 +5530,7 @@
       <c r="N65" s="39"/>
       <c r="O65" s="39"/>
     </row>
-    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -5545,7 +5547,7 @@
       <c r="N66" s="39"/>
       <c r="O66" s="39"/>
     </row>
-    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -5562,7 +5564,7 @@
       <c r="N67" s="39"/>
       <c r="O67" s="39"/>
     </row>
-    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -5579,7 +5581,7 @@
       <c r="N68" s="39"/>
       <c r="O68" s="39"/>
     </row>
-    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -5596,7 +5598,7 @@
       <c r="N69" s="39"/>
       <c r="O69" s="39"/>
     </row>
-    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -5613,7 +5615,7 @@
       <c r="N70" s="39"/>
       <c r="O70" s="39"/>
     </row>
-    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -5630,7 +5632,7 @@
       <c r="N71" s="39"/>
       <c r="O71" s="39"/>
     </row>
-    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -5647,7 +5649,7 @@
       <c r="N72" s="39"/>
       <c r="O72" s="39"/>
     </row>
-    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -5664,7 +5666,7 @@
       <c r="N73" s="39"/>
       <c r="O73" s="39"/>
     </row>
-    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -5681,7 +5683,7 @@
       <c r="N74" s="39"/>
       <c r="O74" s="39"/>
     </row>
-    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -5698,7 +5700,7 @@
       <c r="N75" s="39"/>
       <c r="O75" s="39"/>
     </row>
-    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -5715,7 +5717,7 @@
       <c r="N76" s="39"/>
       <c r="O76" s="39"/>
     </row>
-    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -5732,7 +5734,7 @@
       <c r="N77" s="39"/>
       <c r="O77" s="39"/>
     </row>
-    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -5749,7 +5751,7 @@
       <c r="N78" s="39"/>
       <c r="O78" s="39"/>
     </row>
-    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -5766,7 +5768,7 @@
       <c r="N79" s="39"/>
       <c r="O79" s="39"/>
     </row>
-    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -5783,7 +5785,7 @@
       <c r="N80" s="39"/>
       <c r="O80" s="39"/>
     </row>
-    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -5800,7 +5802,7 @@
       <c r="N81" s="39"/>
       <c r="O81" s="39"/>
     </row>
-    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -5817,7 +5819,7 @@
       <c r="N82" s="39"/>
       <c r="O82" s="39"/>
     </row>
-    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -5834,7 +5836,7 @@
       <c r="N83" s="39"/>
       <c r="O83" s="39"/>
     </row>
-    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -5851,7 +5853,7 @@
       <c r="N84" s="39"/>
       <c r="O84" s="39"/>
     </row>
-    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -5868,7 +5870,7 @@
       <c r="N85" s="39"/>
       <c r="O85" s="39"/>
     </row>
-    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -5885,7 +5887,7 @@
       <c r="N86" s="39"/>
       <c r="O86" s="39"/>
     </row>
-    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -5902,7 +5904,7 @@
       <c r="N87" s="39"/>
       <c r="O87" s="39"/>
     </row>
-    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -5919,7 +5921,7 @@
       <c r="N88" s="39"/>
       <c r="O88" s="39"/>
     </row>
-    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -5936,7 +5938,7 @@
       <c r="N89" s="39"/>
       <c r="O89" s="39"/>
     </row>
-    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -5953,7 +5955,7 @@
       <c r="N90" s="39"/>
       <c r="O90" s="39"/>
     </row>
-    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -5970,7 +5972,7 @@
       <c r="N91" s="39"/>
       <c r="O91" s="39"/>
     </row>
-    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -5987,7 +5989,7 @@
       <c r="N92" s="39"/>
       <c r="O92" s="39"/>
     </row>
-    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -6004,7 +6006,7 @@
       <c r="N93" s="39"/>
       <c r="O93" s="39"/>
     </row>
-    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -6021,7 +6023,7 @@
       <c r="N94" s="39"/>
       <c r="O94" s="39"/>
     </row>
-    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -6038,7 +6040,7 @@
       <c r="N95" s="39"/>
       <c r="O95" s="39"/>
     </row>
-    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -6055,7 +6057,7 @@
       <c r="N96" s="39"/>
       <c r="O96" s="39"/>
     </row>
-    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -6072,7 +6074,7 @@
       <c r="N97" s="39"/>
       <c r="O97" s="39"/>
     </row>
-    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -6089,7 +6091,7 @@
       <c r="N98" s="39"/>
       <c r="O98" s="39"/>
     </row>
-    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -6106,7 +6108,7 @@
       <c r="N99" s="39"/>
       <c r="O99" s="39"/>
     </row>
-    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A100" s="39"/>
       <c r="B100" s="39"/>
       <c r="C100" s="39"/>
@@ -6123,7 +6125,7 @@
       <c r="N100" s="39"/>
       <c r="O100" s="39"/>
     </row>
-    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A101" s="39"/>
       <c r="B101" s="39"/>
       <c r="C101" s="39"/>
@@ -6140,7 +6142,7 @@
       <c r="N101" s="39"/>
       <c r="O101" s="39"/>
     </row>
-    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A102" s="39"/>
       <c r="B102" s="39"/>
       <c r="C102" s="39"/>
@@ -6157,7 +6159,7 @@
       <c r="N102" s="39"/>
       <c r="O102" s="39"/>
     </row>
-    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A103" s="39"/>
       <c r="B103" s="39"/>
       <c r="C103" s="39"/>
@@ -6174,7 +6176,7 @@
       <c r="N103" s="39"/>
       <c r="O103" s="39"/>
     </row>
-    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -6191,7 +6193,7 @@
       <c r="N104" s="39"/>
       <c r="O104" s="39"/>
     </row>
-    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A105" s="39"/>
       <c r="B105" s="39"/>
       <c r="C105" s="39"/>
@@ -6208,7 +6210,7 @@
       <c r="N105" s="39"/>
       <c r="O105" s="39"/>
     </row>
-    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A106" s="39"/>
       <c r="B106" s="39"/>
       <c r="C106" s="39"/>
@@ -6225,7 +6227,7 @@
       <c r="N106" s="39"/>
       <c r="O106" s="39"/>
     </row>
-    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A107" s="39"/>
       <c r="B107" s="39"/>
       <c r="C107" s="39"/>
@@ -6242,7 +6244,7 @@
       <c r="N107" s="39"/>
       <c r="O107" s="39"/>
     </row>
-    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A108" s="39"/>
       <c r="B108" s="39"/>
       <c r="C108" s="39"/>
@@ -6259,7 +6261,7 @@
       <c r="N108" s="39"/>
       <c r="O108" s="39"/>
     </row>
-    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A109" s="39"/>
       <c r="B109" s="39"/>
       <c r="C109" s="39"/>
@@ -6276,7 +6278,7 @@
       <c r="N109" s="39"/>
       <c r="O109" s="39"/>
     </row>
-    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A110" s="39"/>
       <c r="B110" s="39"/>
       <c r="C110" s="39"/>
@@ -6293,7 +6295,7 @@
       <c r="N110" s="39"/>
       <c r="O110" s="39"/>
     </row>
-    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A111" s="39"/>
       <c r="B111" s="39"/>
       <c r="C111" s="39"/>
@@ -6310,7 +6312,7 @@
       <c r="N111" s="39"/>
       <c r="O111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A112" s="39"/>
       <c r="B112" s="39"/>
       <c r="C112" s="39"/>
@@ -6327,7 +6329,7 @@
       <c r="N112" s="39"/>
       <c r="O112" s="39"/>
     </row>
-    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A113" s="39"/>
       <c r="B113" s="39"/>
       <c r="C113" s="39"/>
@@ -6344,7 +6346,7 @@
       <c r="N113" s="39"/>
       <c r="O113" s="39"/>
     </row>
-    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A114" s="39"/>
       <c r="B114" s="39"/>
       <c r="C114" s="39"/>
@@ -6361,7 +6363,7 @@
       <c r="N114" s="39"/>
       <c r="O114" s="39"/>
     </row>
-    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A115" s="39"/>
       <c r="B115" s="39"/>
       <c r="C115" s="39"/>
@@ -6378,7 +6380,7 @@
       <c r="N115" s="39"/>
       <c r="O115" s="39"/>
     </row>
-    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A116" s="39"/>
       <c r="B116" s="39"/>
       <c r="C116" s="39"/>
@@ -6395,7 +6397,7 @@
       <c r="N116" s="39"/>
       <c r="O116" s="39"/>
     </row>
-    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A117" s="39"/>
       <c r="B117" s="39"/>
       <c r="C117" s="39"/>
@@ -6412,7 +6414,7 @@
       <c r="N117" s="39"/>
       <c r="O117" s="39"/>
     </row>
-    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A118" s="39"/>
       <c r="B118" s="39"/>
       <c r="C118" s="39"/>
@@ -6429,7 +6431,7 @@
       <c r="N118" s="39"/>
       <c r="O118" s="39"/>
     </row>
-    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A119" s="39"/>
       <c r="B119" s="39"/>
       <c r="C119" s="39"/>
@@ -6446,7 +6448,7 @@
       <c r="N119" s="39"/>
       <c r="O119" s="39"/>
     </row>
-    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A120" s="39"/>
       <c r="B120" s="39"/>
       <c r="C120" s="39"/>
@@ -6463,7 +6465,7 @@
       <c r="N120" s="39"/>
       <c r="O120" s="39"/>
     </row>
-    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A121" s="39"/>
       <c r="B121" s="39"/>
       <c r="C121" s="39"/>
@@ -6480,7 +6482,7 @@
       <c r="N121" s="39"/>
       <c r="O121" s="39"/>
     </row>
-    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A122" s="39"/>
       <c r="B122" s="39"/>
       <c r="C122" s="39"/>
@@ -6497,7 +6499,7 @@
       <c r="N122" s="39"/>
       <c r="O122" s="39"/>
     </row>
-    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A123" s="39"/>
       <c r="B123" s="39"/>
       <c r="C123" s="39"/>
@@ -6514,7 +6516,7 @@
       <c r="N123" s="39"/>
       <c r="O123" s="39"/>
     </row>
-    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A124" s="39"/>
       <c r="B124" s="39"/>
       <c r="C124" s="39"/>
@@ -6531,7 +6533,7 @@
       <c r="N124" s="39"/>
       <c r="O124" s="39"/>
     </row>
-    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A125" s="39"/>
       <c r="B125" s="39"/>
       <c r="C125" s="39"/>
@@ -6548,7 +6550,7 @@
       <c r="N125" s="39"/>
       <c r="O125" s="39"/>
     </row>
-    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A126" s="39"/>
       <c r="B126" s="39"/>
       <c r="C126" s="39"/>
@@ -6565,7 +6567,7 @@
       <c r="N126" s="39"/>
       <c r="O126" s="39"/>
     </row>
-    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A127" s="39"/>
       <c r="B127" s="39"/>
       <c r="C127" s="39"/>
@@ -6582,7 +6584,7 @@
       <c r="N127" s="39"/>
       <c r="O127" s="39"/>
     </row>
-    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A128" s="39"/>
       <c r="B128" s="39"/>
       <c r="C128" s="39"/>
@@ -6599,7 +6601,7 @@
       <c r="N128" s="39"/>
       <c r="O128" s="39"/>
     </row>
-    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A129" s="39"/>
       <c r="B129" s="39"/>
       <c r="C129" s="39"/>
@@ -6616,7 +6618,7 @@
       <c r="N129" s="39"/>
       <c r="O129" s="39"/>
     </row>
-    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A130" s="39"/>
       <c r="B130" s="39"/>
       <c r="C130" s="39"/>
@@ -6633,7 +6635,7 @@
       <c r="N130" s="39"/>
       <c r="O130" s="39"/>
     </row>
-    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A131" s="39"/>
       <c r="B131" s="39"/>
       <c r="C131" s="39"/>
@@ -6650,7 +6652,7 @@
       <c r="N131" s="39"/>
       <c r="O131" s="39"/>
     </row>
-    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A132" s="39"/>
       <c r="B132" s="39"/>
       <c r="C132" s="39"/>
@@ -6667,7 +6669,7 @@
       <c r="N132" s="39"/>
       <c r="O132" s="39"/>
     </row>
-    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A133" s="39"/>
       <c r="B133" s="39"/>
       <c r="C133" s="39"/>
@@ -6684,7 +6686,7 @@
       <c r="N133" s="39"/>
       <c r="O133" s="39"/>
     </row>
-    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A134" s="39"/>
       <c r="B134" s="39"/>
       <c r="C134" s="39"/>
@@ -6701,7 +6703,7 @@
       <c r="N134" s="39"/>
       <c r="O134" s="39"/>
     </row>
-    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A135" s="39"/>
       <c r="B135" s="39"/>
       <c r="C135" s="39"/>
@@ -6718,7 +6720,7 @@
       <c r="N135" s="39"/>
       <c r="O135" s="39"/>
     </row>
-    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A136" s="39"/>
       <c r="B136" s="39"/>
       <c r="C136" s="39"/>
@@ -6735,7 +6737,7 @@
       <c r="N136" s="39"/>
       <c r="O136" s="39"/>
     </row>
-    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A137" s="39"/>
       <c r="B137" s="39"/>
       <c r="C137" s="39"/>
@@ -6752,7 +6754,7 @@
       <c r="N137" s="39"/>
       <c r="O137" s="39"/>
     </row>
-    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A138" s="39"/>
       <c r="B138" s="39"/>
       <c r="C138" s="39"/>
@@ -6769,7 +6771,7 @@
       <c r="N138" s="39"/>
       <c r="O138" s="39"/>
     </row>
-    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A139" s="39"/>
       <c r="B139" s="39"/>
       <c r="C139" s="39"/>
@@ -6786,7 +6788,7 @@
       <c r="N139" s="39"/>
       <c r="O139" s="39"/>
     </row>
-    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A140" s="39"/>
       <c r="B140" s="39"/>
       <c r="C140" s="39"/>
@@ -6803,7 +6805,7 @@
       <c r="N140" s="39"/>
       <c r="O140" s="39"/>
     </row>
-    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A141" s="39"/>
       <c r="B141" s="39"/>
       <c r="C141" s="39"/>
@@ -6820,7 +6822,7 @@
       <c r="N141" s="39"/>
       <c r="O141" s="39"/>
     </row>
-    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A142" s="39"/>
       <c r="B142" s="39"/>
       <c r="C142" s="39"/>
@@ -6837,7 +6839,7 @@
       <c r="N142" s="39"/>
       <c r="O142" s="39"/>
     </row>
-    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A143" s="39"/>
       <c r="B143" s="39"/>
       <c r="C143" s="39"/>
@@ -6854,7 +6856,7 @@
       <c r="N143" s="39"/>
       <c r="O143" s="39"/>
     </row>
-    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A144" s="39"/>
       <c r="B144" s="39"/>
       <c r="C144" s="39"/>
@@ -6871,7 +6873,7 @@
       <c r="N144" s="39"/>
       <c r="O144" s="39"/>
     </row>
-    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A145" s="39"/>
       <c r="B145" s="39"/>
       <c r="C145" s="39"/>
@@ -6888,7 +6890,7 @@
       <c r="N145" s="39"/>
       <c r="O145" s="39"/>
     </row>
-    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A146" s="39"/>
       <c r="B146" s="39"/>
       <c r="C146" s="39"/>
@@ -6905,7 +6907,7 @@
       <c r="N146" s="39"/>
       <c r="O146" s="39"/>
     </row>
-    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A147" s="39"/>
       <c r="B147" s="39"/>
       <c r="C147" s="39"/>
@@ -6922,7 +6924,7 @@
       <c r="N147" s="39"/>
       <c r="O147" s="39"/>
     </row>
-    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A148" s="39"/>
       <c r="B148" s="39"/>
       <c r="C148" s="39"/>
@@ -6939,7 +6941,7 @@
       <c r="N148" s="39"/>
       <c r="O148" s="39"/>
     </row>
-    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A149" s="39"/>
       <c r="B149" s="39"/>
       <c r="C149" s="39"/>
@@ -6956,7 +6958,7 @@
       <c r="N149" s="39"/>
       <c r="O149" s="39"/>
     </row>
-    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A150" s="39"/>
       <c r="B150" s="39"/>
       <c r="C150" s="39"/>
@@ -6973,7 +6975,7 @@
       <c r="N150" s="39"/>
       <c r="O150" s="39"/>
     </row>
-    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A151" s="39"/>
       <c r="B151" s="39"/>
       <c r="C151" s="39"/>
@@ -6990,7 +6992,7 @@
       <c r="N151" s="39"/>
       <c r="O151" s="39"/>
     </row>
-    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A152" s="39"/>
       <c r="B152" s="39"/>
       <c r="C152" s="39"/>
@@ -7007,7 +7009,7 @@
       <c r="N152" s="39"/>
       <c r="O152" s="39"/>
     </row>
-    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A153" s="39"/>
       <c r="B153" s="39"/>
       <c r="C153" s="39"/>
@@ -7024,7 +7026,7 @@
       <c r="N153" s="39"/>
       <c r="O153" s="39"/>
     </row>
-    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A154" s="39"/>
       <c r="B154" s="39"/>
       <c r="C154" s="39"/>
@@ -7041,7 +7043,7 @@
       <c r="N154" s="39"/>
       <c r="O154" s="39"/>
     </row>
-    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A155" s="39"/>
       <c r="B155" s="39"/>
       <c r="C155" s="39"/>
@@ -7058,7 +7060,7 @@
       <c r="N155" s="39"/>
       <c r="O155" s="39"/>
     </row>
-    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A156" s="39"/>
       <c r="B156" s="39"/>
       <c r="C156" s="39"/>
@@ -7075,7 +7077,7 @@
       <c r="N156" s="39"/>
       <c r="O156" s="39"/>
     </row>
-    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A157" s="39"/>
       <c r="B157" s="39"/>
       <c r="C157" s="39"/>
@@ -7092,7 +7094,7 @@
       <c r="N157" s="39"/>
       <c r="O157" s="39"/>
     </row>
-    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A158" s="39"/>
       <c r="B158" s="39"/>
       <c r="C158" s="39"/>
@@ -7109,7 +7111,7 @@
       <c r="N158" s="39"/>
       <c r="O158" s="39"/>
     </row>
-    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A159" s="39"/>
       <c r="B159" s="39"/>
       <c r="C159" s="39"/>
@@ -7126,7 +7128,7 @@
       <c r="N159" s="39"/>
       <c r="O159" s="39"/>
     </row>
-    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A160" s="39"/>
       <c r="B160" s="39"/>
       <c r="C160" s="39"/>
@@ -7143,7 +7145,7 @@
       <c r="N160" s="39"/>
       <c r="O160" s="39"/>
     </row>
-    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A161" s="39"/>
       <c r="B161" s="39"/>
       <c r="C161" s="39"/>
@@ -7160,7 +7162,7 @@
       <c r="N161" s="39"/>
       <c r="O161" s="39"/>
     </row>
-    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A162" s="39"/>
       <c r="B162" s="39"/>
       <c r="C162" s="39"/>
@@ -7177,7 +7179,7 @@
       <c r="N162" s="39"/>
       <c r="O162" s="39"/>
     </row>
-    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A163" s="39"/>
       <c r="B163" s="39"/>
       <c r="C163" s="39"/>
@@ -7194,7 +7196,7 @@
       <c r="N163" s="39"/>
       <c r="O163" s="39"/>
     </row>
-    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A164" s="39"/>
       <c r="B164" s="39"/>
       <c r="C164" s="39"/>
@@ -7211,7 +7213,7 @@
       <c r="N164" s="39"/>
       <c r="O164" s="39"/>
     </row>
-    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A165" s="39"/>
       <c r="B165" s="39"/>
       <c r="C165" s="39"/>
@@ -7228,7 +7230,7 @@
       <c r="N165" s="39"/>
       <c r="O165" s="39"/>
     </row>
-    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A166" s="39"/>
       <c r="B166" s="39"/>
       <c r="C166" s="39"/>
@@ -7245,7 +7247,7 @@
       <c r="N166" s="39"/>
       <c r="O166" s="39"/>
     </row>
-    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A167" s="39"/>
       <c r="B167" s="39"/>
       <c r="C167" s="39"/>
@@ -7262,7 +7264,7 @@
       <c r="N167" s="39"/>
       <c r="O167" s="39"/>
     </row>
-    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A168" s="39"/>
       <c r="B168" s="39"/>
       <c r="C168" s="39"/>
@@ -7279,7 +7281,7 @@
       <c r="N168" s="39"/>
       <c r="O168" s="39"/>
     </row>
-    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A169" s="39"/>
       <c r="B169" s="39"/>
       <c r="C169" s="39"/>
@@ -7296,7 +7298,7 @@
       <c r="N169" s="39"/>
       <c r="O169" s="39"/>
     </row>
-    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A170" s="39"/>
       <c r="B170" s="39"/>
       <c r="C170" s="39"/>
@@ -7313,7 +7315,7 @@
       <c r="N170" s="39"/>
       <c r="O170" s="39"/>
     </row>
-    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A171" s="39"/>
       <c r="B171" s="39"/>
       <c r="C171" s="39"/>
@@ -7330,7 +7332,7 @@
       <c r="N171" s="39"/>
       <c r="O171" s="39"/>
     </row>
-    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A172" s="39"/>
       <c r="B172" s="39"/>
       <c r="C172" s="39"/>
@@ -7347,7 +7349,7 @@
       <c r="N172" s="39"/>
       <c r="O172" s="39"/>
     </row>
-    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A173" s="39"/>
       <c r="B173" s="39"/>
       <c r="C173" s="39"/>
@@ -7364,7 +7366,7 @@
       <c r="N173" s="39"/>
       <c r="O173" s="39"/>
     </row>
-    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A174" s="39"/>
       <c r="B174" s="39"/>
       <c r="C174" s="39"/>
@@ -7381,7 +7383,7 @@
       <c r="N174" s="39"/>
       <c r="O174" s="39"/>
     </row>
-    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A175" s="39"/>
       <c r="B175" s="39"/>
       <c r="C175" s="39"/>
@@ -7398,7 +7400,7 @@
       <c r="N175" s="39"/>
       <c r="O175" s="39"/>
     </row>
-    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A176" s="39"/>
       <c r="B176" s="39"/>
       <c r="C176" s="39"/>
@@ -7415,7 +7417,7 @@
       <c r="N176" s="39"/>
       <c r="O176" s="39"/>
     </row>
-    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A177" s="39"/>
       <c r="B177" s="39"/>
       <c r="C177" s="39"/>
@@ -7432,7 +7434,7 @@
       <c r="N177" s="39"/>
       <c r="O177" s="39"/>
     </row>
-    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A178" s="39"/>
       <c r="B178" s="39"/>
       <c r="C178" s="39"/>
@@ -7449,7 +7451,7 @@
       <c r="N178" s="39"/>
       <c r="O178" s="39"/>
     </row>
-    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A179" s="39"/>
       <c r="B179" s="39"/>
       <c r="C179" s="39"/>
@@ -7466,7 +7468,7 @@
       <c r="N179" s="39"/>
       <c r="O179" s="39"/>
     </row>
-    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A180" s="39"/>
       <c r="B180" s="39"/>
       <c r="C180" s="39"/>
@@ -7483,7 +7485,7 @@
       <c r="N180" s="39"/>
       <c r="O180" s="39"/>
     </row>
-    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A181" s="39"/>
       <c r="B181" s="39"/>
       <c r="C181" s="39"/>
@@ -7500,7 +7502,7 @@
       <c r="N181" s="39"/>
       <c r="O181" s="39"/>
     </row>
-    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A182" s="39"/>
       <c r="B182" s="39"/>
       <c r="C182" s="39"/>
@@ -7517,7 +7519,7 @@
       <c r="N182" s="39"/>
       <c r="O182" s="39"/>
     </row>
-    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A183" s="39"/>
       <c r="B183" s="39"/>
       <c r="C183" s="39"/>
@@ -7534,7 +7536,7 @@
       <c r="N183" s="39"/>
       <c r="O183" s="39"/>
     </row>
-    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A184" s="39"/>
       <c r="B184" s="39"/>
       <c r="C184" s="39"/>
@@ -7551,7 +7553,7 @@
       <c r="N184" s="39"/>
       <c r="O184" s="39"/>
     </row>
-    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A185" s="39"/>
       <c r="B185" s="39"/>
       <c r="C185" s="39"/>
@@ -7568,7 +7570,7 @@
       <c r="N185" s="39"/>
       <c r="O185" s="39"/>
     </row>
-    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A186" s="39"/>
       <c r="B186" s="39"/>
       <c r="C186" s="39"/>
@@ -7585,7 +7587,7 @@
       <c r="N186" s="39"/>
       <c r="O186" s="39"/>
     </row>
-    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A187" s="39"/>
       <c r="B187" s="39"/>
       <c r="C187" s="39"/>
@@ -7602,7 +7604,7 @@
       <c r="N187" s="39"/>
       <c r="O187" s="39"/>
     </row>
-    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A188" s="39"/>
       <c r="B188" s="39"/>
       <c r="C188" s="39"/>
@@ -7619,7 +7621,7 @@
       <c r="N188" s="39"/>
       <c r="O188" s="39"/>
     </row>
-    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A189" s="39"/>
       <c r="B189" s="39"/>
       <c r="C189" s="39"/>
@@ -7636,7 +7638,7 @@
       <c r="N189" s="39"/>
       <c r="O189" s="39"/>
     </row>
-    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A190" s="39"/>
       <c r="B190" s="39"/>
       <c r="C190" s="39"/>
@@ -7653,7 +7655,7 @@
       <c r="N190" s="39"/>
       <c r="O190" s="39"/>
     </row>
-    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A191" s="39"/>
       <c r="B191" s="39"/>
       <c r="C191" s="39"/>
@@ -7670,7 +7672,7 @@
       <c r="N191" s="39"/>
       <c r="O191" s="39"/>
     </row>
-    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A192" s="39"/>
       <c r="B192" s="39"/>
       <c r="C192" s="39"/>
@@ -7687,7 +7689,7 @@
       <c r="N192" s="39"/>
       <c r="O192" s="39"/>
     </row>
-    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A193" s="39"/>
       <c r="B193" s="39"/>
       <c r="C193" s="39"/>
@@ -7704,7 +7706,7 @@
       <c r="N193" s="39"/>
       <c r="O193" s="39"/>
     </row>
-    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A194" s="39"/>
       <c r="B194" s="39"/>
       <c r="C194" s="39"/>
@@ -7721,7 +7723,7 @@
       <c r="N194" s="39"/>
       <c r="O194" s="39"/>
     </row>
-    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A195" s="39"/>
       <c r="B195" s="39"/>
       <c r="C195" s="39"/>
@@ -7738,7 +7740,7 @@
       <c r="N195" s="39"/>
       <c r="O195" s="39"/>
     </row>
-    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A196" s="39"/>
       <c r="B196" s="39"/>
       <c r="C196" s="39"/>
@@ -7755,7 +7757,7 @@
       <c r="N196" s="39"/>
       <c r="O196" s="39"/>
     </row>
-    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A197" s="39"/>
       <c r="B197" s="39"/>
       <c r="C197" s="39"/>
@@ -7772,7 +7774,7 @@
       <c r="N197" s="39"/>
       <c r="O197" s="39"/>
     </row>
-    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A198" s="39"/>
       <c r="B198" s="39"/>
       <c r="C198" s="39"/>
@@ -7789,7 +7791,7 @@
       <c r="N198" s="39"/>
       <c r="O198" s="39"/>
     </row>
-    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A199" s="39"/>
       <c r="B199" s="39"/>
       <c r="C199" s="39"/>
@@ -7806,7 +7808,7 @@
       <c r="N199" s="39"/>
       <c r="O199" s="39"/>
     </row>
-    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A200" s="39"/>
       <c r="B200" s="39"/>
       <c r="C200" s="39"/>
@@ -7823,7 +7825,7 @@
       <c r="N200" s="39"/>
       <c r="O200" s="39"/>
     </row>
-    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A201" s="39"/>
       <c r="B201" s="39"/>
       <c r="C201" s="39"/>
@@ -7840,7 +7842,7 @@
       <c r="N201" s="39"/>
       <c r="O201" s="39"/>
     </row>
-    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A202" s="39"/>
       <c r="B202" s="39"/>
       <c r="C202" s="39"/>
@@ -7857,7 +7859,7 @@
       <c r="N202" s="39"/>
       <c r="O202" s="39"/>
     </row>
-    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A203" s="39"/>
       <c r="B203" s="39"/>
       <c r="C203" s="39"/>
@@ -7874,7 +7876,7 @@
       <c r="N203" s="39"/>
       <c r="O203" s="39"/>
     </row>
-    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A204" s="39"/>
       <c r="B204" s="39"/>
       <c r="C204" s="39"/>
@@ -7891,7 +7893,7 @@
       <c r="N204" s="39"/>
       <c r="O204" s="39"/>
     </row>
-    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="205" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A205" s="39"/>
       <c r="B205" s="39"/>
       <c r="C205" s="39"/>
@@ -7908,7 +7910,7 @@
       <c r="N205" s="39"/>
       <c r="O205" s="39"/>
     </row>
-    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A206" s="39"/>
       <c r="B206" s="39"/>
       <c r="C206" s="39"/>
@@ -7925,7 +7927,7 @@
       <c r="N206" s="39"/>
       <c r="O206" s="39"/>
     </row>
-    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A207" s="39"/>
       <c r="B207" s="39"/>
       <c r="C207" s="39"/>
@@ -7942,7 +7944,7 @@
       <c r="N207" s="39"/>
       <c r="O207" s="39"/>
     </row>
-    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="208" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A208" s="39"/>
       <c r="B208" s="39"/>
       <c r="C208" s="39"/>
@@ -7959,7 +7961,7 @@
       <c r="N208" s="39"/>
       <c r="O208" s="39"/>
     </row>
-    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="209" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A209" s="39"/>
       <c r="B209" s="39"/>
       <c r="C209" s="39"/>
@@ -7976,7 +7978,7 @@
       <c r="N209" s="39"/>
       <c r="O209" s="39"/>
     </row>
-    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="210" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A210" s="39"/>
       <c r="B210" s="39"/>
       <c r="C210" s="39"/>
@@ -7993,7 +7995,7 @@
       <c r="N210" s="39"/>
       <c r="O210" s="39"/>
     </row>
-    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="211" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A211" s="39"/>
       <c r="B211" s="39"/>
       <c r="C211" s="39"/>
@@ -8010,7 +8012,7 @@
       <c r="N211" s="39"/>
       <c r="O211" s="39"/>
     </row>
-    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="212" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A212" s="39"/>
       <c r="B212" s="39"/>
       <c r="C212" s="39"/>
@@ -8027,7 +8029,7 @@
       <c r="N212" s="39"/>
       <c r="O212" s="39"/>
     </row>
-    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="213" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A213" s="39"/>
       <c r="B213" s="39"/>
       <c r="C213" s="39"/>
@@ -8044,7 +8046,7 @@
       <c r="N213" s="39"/>
       <c r="O213" s="39"/>
     </row>
-    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="214" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A214" s="39"/>
       <c r="B214" s="39"/>
       <c r="C214" s="39"/>
@@ -8061,7 +8063,7 @@
       <c r="N214" s="39"/>
       <c r="O214" s="39"/>
     </row>
-    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="215" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A215" s="39"/>
       <c r="B215" s="39"/>
       <c r="C215" s="39"/>
@@ -8078,7 +8080,7 @@
       <c r="N215" s="39"/>
       <c r="O215" s="39"/>
     </row>
-    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="216" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A216" s="39"/>
       <c r="B216" s="39"/>
       <c r="C216" s="39"/>
@@ -8095,7 +8097,7 @@
       <c r="N216" s="39"/>
       <c r="O216" s="39"/>
     </row>
-    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="217" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A217" s="39"/>
       <c r="B217" s="39"/>
       <c r="C217" s="39"/>
@@ -8112,7 +8114,7 @@
       <c r="N217" s="39"/>
       <c r="O217" s="39"/>
     </row>
-    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="218" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A218" s="39"/>
       <c r="B218" s="39"/>
       <c r="C218" s="39"/>
@@ -8129,7 +8131,7 @@
       <c r="N218" s="39"/>
       <c r="O218" s="39"/>
     </row>
-    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="219" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A219" s="39"/>
       <c r="B219" s="39"/>
       <c r="C219" s="39"/>
@@ -8146,7 +8148,7 @@
       <c r="N219" s="39"/>
       <c r="O219" s="39"/>
     </row>
-    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="220" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A220" s="39"/>
       <c r="B220" s="39"/>
       <c r="C220" s="39"/>
@@ -8163,7 +8165,7 @@
       <c r="N220" s="39"/>
       <c r="O220" s="39"/>
     </row>
-    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="221" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A221" s="39"/>
       <c r="B221" s="39"/>
       <c r="C221" s="39"/>
@@ -8180,7 +8182,7 @@
       <c r="N221" s="39"/>
       <c r="O221" s="39"/>
     </row>
-    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="222" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A222" s="39"/>
       <c r="B222" s="39"/>
       <c r="C222" s="39"/>
@@ -8197,7 +8199,7 @@
       <c r="N222" s="39"/>
       <c r="O222" s="39"/>
     </row>
-    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="223" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A223" s="39"/>
       <c r="B223" s="39"/>
       <c r="C223" s="39"/>
@@ -8214,7 +8216,7 @@
       <c r="N223" s="39"/>
       <c r="O223" s="39"/>
     </row>
-    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="224" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A224" s="39"/>
       <c r="B224" s="39"/>
       <c r="C224" s="39"/>
@@ -8231,7 +8233,7 @@
       <c r="N224" s="39"/>
       <c r="O224" s="39"/>
     </row>
-    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="225" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A225" s="39"/>
       <c r="B225" s="39"/>
       <c r="C225" s="39"/>
@@ -8248,7 +8250,7 @@
       <c r="N225" s="39"/>
       <c r="O225" s="39"/>
     </row>
-    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="226" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A226" s="39"/>
       <c r="B226" s="39"/>
       <c r="C226" s="39"/>
@@ -8265,7 +8267,7 @@
       <c r="N226" s="39"/>
       <c r="O226" s="39"/>
     </row>
-    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="227" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A227" s="39"/>
       <c r="B227" s="39"/>
       <c r="C227" s="39"/>
@@ -8282,7 +8284,7 @@
       <c r="N227" s="39"/>
       <c r="O227" s="39"/>
     </row>
-    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="228" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A228" s="39"/>
       <c r="B228" s="39"/>
       <c r="C228" s="39"/>
@@ -8299,7 +8301,7 @@
       <c r="N228" s="39"/>
       <c r="O228" s="39"/>
     </row>
-    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="229" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A229" s="39"/>
       <c r="B229" s="39"/>
       <c r="C229" s="39"/>
@@ -8316,7 +8318,7 @@
       <c r="N229" s="39"/>
       <c r="O229" s="39"/>
     </row>
-    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="230" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A230" s="39"/>
       <c r="B230" s="39"/>
       <c r="C230" s="39"/>
@@ -8333,7 +8335,7 @@
       <c r="N230" s="39"/>
       <c r="O230" s="39"/>
     </row>
-    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="231" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A231" s="39"/>
       <c r="B231" s="39"/>
       <c r="C231" s="39"/>
@@ -8350,7 +8352,7 @@
       <c r="N231" s="39"/>
       <c r="O231" s="39"/>
     </row>
-    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="232" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A232" s="39"/>
       <c r="B232" s="39"/>
       <c r="C232" s="39"/>
@@ -8367,7 +8369,7 @@
       <c r="N232" s="39"/>
       <c r="O232" s="39"/>
     </row>
-    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="233" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A233" s="39"/>
       <c r="B233" s="39"/>
       <c r="C233" s="39"/>
@@ -8384,7 +8386,7 @@
       <c r="N233" s="39"/>
       <c r="O233" s="39"/>
     </row>
-    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="234" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A234" s="39"/>
       <c r="B234" s="39"/>
       <c r="C234" s="39"/>
@@ -8401,7 +8403,7 @@
       <c r="N234" s="39"/>
       <c r="O234" s="39"/>
     </row>
-    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="235" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A235" s="39"/>
       <c r="B235" s="39"/>
       <c r="C235" s="39"/>
@@ -8418,7 +8420,7 @@
       <c r="N235" s="39"/>
       <c r="O235" s="39"/>
     </row>
-    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="236" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A236" s="39"/>
       <c r="B236" s="39"/>
       <c r="C236" s="39"/>
@@ -8435,7 +8437,7 @@
       <c r="N236" s="39"/>
       <c r="O236" s="39"/>
     </row>
-    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="237" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A237" s="39"/>
       <c r="B237" s="39"/>
       <c r="C237" s="39"/>
@@ -8452,7 +8454,7 @@
       <c r="N237" s="39"/>
       <c r="O237" s="39"/>
     </row>
-    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="238" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A238" s="39"/>
       <c r="B238" s="39"/>
       <c r="C238" s="39"/>
@@ -8469,7 +8471,7 @@
       <c r="N238" s="39"/>
       <c r="O238" s="39"/>
     </row>
-    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="239" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A239" s="39"/>
       <c r="B239" s="39"/>
       <c r="C239" s="39"/>
@@ -8486,7 +8488,7 @@
       <c r="N239" s="39"/>
       <c r="O239" s="39"/>
     </row>
-    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="240" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A240" s="39"/>
       <c r="B240" s="39"/>
       <c r="C240" s="39"/>
@@ -8503,7 +8505,7 @@
       <c r="N240" s="39"/>
       <c r="O240" s="39"/>
     </row>
-    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="241" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A241" s="39"/>
       <c r="B241" s="39"/>
       <c r="C241" s="39"/>
@@ -8520,7 +8522,7 @@
       <c r="N241" s="39"/>
       <c r="O241" s="39"/>
     </row>
-    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="242" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A242" s="39"/>
       <c r="B242" s="39"/>
       <c r="C242" s="39"/>
@@ -8537,7 +8539,7 @@
       <c r="N242" s="39"/>
       <c r="O242" s="39"/>
     </row>
-    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="243" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A243" s="39"/>
       <c r="B243" s="39"/>
       <c r="C243" s="39"/>
@@ -8554,7 +8556,7 @@
       <c r="N243" s="39"/>
       <c r="O243" s="39"/>
     </row>
-    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="244" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A244" s="39"/>
       <c r="B244" s="39"/>
       <c r="C244" s="39"/>
@@ -8571,7 +8573,7 @@
       <c r="N244" s="39"/>
       <c r="O244" s="39"/>
     </row>
-    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="245" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A245" s="39"/>
       <c r="B245" s="39"/>
       <c r="C245" s="39"/>
@@ -8588,7 +8590,7 @@
       <c r="N245" s="39"/>
       <c r="O245" s="39"/>
     </row>
-    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="246" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A246" s="39"/>
       <c r="B246" s="39"/>
       <c r="C246" s="39"/>
@@ -8605,7 +8607,7 @@
       <c r="N246" s="39"/>
       <c r="O246" s="39"/>
     </row>
-    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="247" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A247" s="39"/>
       <c r="B247" s="39"/>
       <c r="C247" s="39"/>
@@ -8622,7 +8624,7 @@
       <c r="N247" s="39"/>
       <c r="O247" s="39"/>
     </row>
-    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="248" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A248" s="39"/>
       <c r="B248" s="39"/>
       <c r="C248" s="39"/>
@@ -8639,7 +8641,7 @@
       <c r="N248" s="39"/>
       <c r="O248" s="39"/>
     </row>
-    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="249" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A249" s="39"/>
       <c r="B249" s="39"/>
       <c r="C249" s="39"/>
@@ -8656,7 +8658,7 @@
       <c r="N249" s="39"/>
       <c r="O249" s="39"/>
     </row>
-    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="250" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A250" s="39"/>
       <c r="B250" s="39"/>
       <c r="C250" s="39"/>
@@ -8673,7 +8675,7 @@
       <c r="N250" s="39"/>
       <c r="O250" s="39"/>
     </row>
-    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="251" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A251" s="39"/>
       <c r="B251" s="39"/>
       <c r="C251" s="39"/>
@@ -8690,7 +8692,7 @@
       <c r="N251" s="39"/>
       <c r="O251" s="39"/>
     </row>
-    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="252" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A252" s="39"/>
       <c r="B252" s="39"/>
       <c r="C252" s="39"/>
@@ -8707,7 +8709,7 @@
       <c r="N252" s="39"/>
       <c r="O252" s="39"/>
     </row>
-    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="253" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A253" s="39"/>
       <c r="B253" s="39"/>
       <c r="C253" s="39"/>
@@ -8724,7 +8726,7 @@
       <c r="N253" s="39"/>
       <c r="O253" s="39"/>
     </row>
-    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="254" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A254" s="39"/>
       <c r="B254" s="39"/>
       <c r="C254" s="39"/>
@@ -8741,7 +8743,7 @@
       <c r="N254" s="39"/>
       <c r="O254" s="39"/>
     </row>
-    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="255" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A255" s="39"/>
       <c r="B255" s="39"/>
       <c r="C255" s="39"/>
@@ -8758,7 +8760,7 @@
       <c r="N255" s="39"/>
       <c r="O255" s="39"/>
     </row>
-    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="256" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A256" s="39"/>
       <c r="B256" s="39"/>
       <c r="C256" s="39"/>
@@ -8775,7 +8777,7 @@
       <c r="N256" s="39"/>
       <c r="O256" s="39"/>
     </row>
-    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="257" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A257" s="39"/>
       <c r="B257" s="39"/>
       <c r="C257" s="39"/>
@@ -8792,7 +8794,7 @@
       <c r="N257" s="39"/>
       <c r="O257" s="39"/>
     </row>
-    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="258" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A258" s="39"/>
       <c r="B258" s="39"/>
       <c r="C258" s="39"/>
@@ -8809,7 +8811,7 @@
       <c r="N258" s="39"/>
       <c r="O258" s="39"/>
     </row>
-    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="259" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A259" s="39"/>
       <c r="B259" s="39"/>
       <c r="C259" s="39"/>
@@ -8826,7 +8828,7 @@
       <c r="N259" s="39"/>
       <c r="O259" s="39"/>
     </row>
-    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="260" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A260" s="39"/>
       <c r="B260" s="39"/>
       <c r="C260" s="39"/>
@@ -8843,7 +8845,7 @@
       <c r="N260" s="39"/>
       <c r="O260" s="39"/>
     </row>
-    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="261" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A261" s="39"/>
       <c r="B261" s="39"/>
       <c r="C261" s="39"/>
@@ -8860,7 +8862,7 @@
       <c r="N261" s="39"/>
       <c r="O261" s="39"/>
     </row>
-    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="262" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A262" s="39"/>
       <c r="B262" s="39"/>
       <c r="C262" s="39"/>
@@ -8877,7 +8879,7 @@
       <c r="N262" s="39"/>
       <c r="O262" s="39"/>
     </row>
-    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="263" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A263" s="39"/>
       <c r="B263" s="39"/>
       <c r="C263" s="39"/>
@@ -8894,7 +8896,7 @@
       <c r="N263" s="39"/>
       <c r="O263" s="39"/>
     </row>
-    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="264" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A264" s="39"/>
       <c r="B264" s="39"/>
       <c r="C264" s="39"/>
@@ -8911,7 +8913,7 @@
       <c r="N264" s="39"/>
       <c r="O264" s="39"/>
     </row>
-    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="265" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A265" s="39"/>
       <c r="B265" s="39"/>
       <c r="C265" s="39"/>
@@ -8928,7 +8930,7 @@
       <c r="N265" s="39"/>
       <c r="O265" s="39"/>
     </row>
-    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="266" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A266" s="39"/>
       <c r="B266" s="39"/>
       <c r="C266" s="39"/>
@@ -8945,7 +8947,7 @@
       <c r="N266" s="39"/>
       <c r="O266" s="39"/>
     </row>
-    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="267" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A267" s="39"/>
       <c r="B267" s="39"/>
       <c r="C267" s="39"/>
@@ -8962,7 +8964,7 @@
       <c r="N267" s="39"/>
       <c r="O267" s="39"/>
     </row>
-    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="268" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A268" s="39"/>
       <c r="B268" s="39"/>
       <c r="C268" s="39"/>
@@ -8979,7 +8981,7 @@
       <c r="N268" s="39"/>
       <c r="O268" s="39"/>
     </row>
-    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="269" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A269" s="39"/>
       <c r="B269" s="39"/>
       <c r="C269" s="39"/>
@@ -8996,7 +8998,7 @@
       <c r="N269" s="39"/>
       <c r="O269" s="39"/>
     </row>
-    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="270" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A270" s="39"/>
       <c r="B270" s="39"/>
       <c r="C270" s="39"/>
@@ -9013,7 +9015,7 @@
       <c r="N270" s="39"/>
       <c r="O270" s="39"/>
     </row>
-    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="271" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A271" s="39"/>
       <c r="B271" s="39"/>
       <c r="C271" s="39"/>
@@ -9030,7 +9032,7 @@
       <c r="N271" s="39"/>
       <c r="O271" s="39"/>
     </row>
-    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="272" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A272" s="39"/>
       <c r="B272" s="39"/>
       <c r="C272" s="39"/>
@@ -9047,7 +9049,7 @@
       <c r="N272" s="39"/>
       <c r="O272" s="39"/>
     </row>
-    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="273" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A273" s="39"/>
       <c r="B273" s="39"/>
       <c r="C273" s="39"/>
@@ -9064,7 +9066,7 @@
       <c r="N273" s="39"/>
       <c r="O273" s="39"/>
     </row>
-    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="274" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A274" s="39"/>
       <c r="B274" s="39"/>
       <c r="C274" s="39"/>
@@ -9081,7 +9083,7 @@
       <c r="N274" s="39"/>
       <c r="O274" s="39"/>
     </row>
-    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="275" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A275" s="39"/>
       <c r="B275" s="39"/>
       <c r="C275" s="39"/>
@@ -9098,7 +9100,7 @@
       <c r="N275" s="39"/>
       <c r="O275" s="39"/>
     </row>
-    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="276" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A276" s="39"/>
       <c r="B276" s="39"/>
       <c r="C276" s="39"/>
@@ -9115,7 +9117,7 @@
       <c r="N276" s="39"/>
       <c r="O276" s="39"/>
     </row>
-    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="277" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A277" s="39"/>
       <c r="B277" s="39"/>
       <c r="C277" s="39"/>
@@ -9132,7 +9134,7 @@
       <c r="N277" s="39"/>
       <c r="O277" s="39"/>
     </row>
-    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="278" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A278" s="39"/>
       <c r="B278" s="39"/>
       <c r="C278" s="39"/>
@@ -9149,7 +9151,7 @@
       <c r="N278" s="39"/>
       <c r="O278" s="39"/>
     </row>
-    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="279" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A279" s="39"/>
       <c r="B279" s="39"/>
       <c r="C279" s="39"/>
@@ -9166,7 +9168,7 @@
       <c r="N279" s="39"/>
       <c r="O279" s="39"/>
     </row>
-    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="280" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A280" s="39"/>
       <c r="B280" s="39"/>
       <c r="C280" s="39"/>
@@ -9183,7 +9185,7 @@
       <c r="N280" s="39"/>
       <c r="O280" s="39"/>
     </row>
-    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="281" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A281" s="39"/>
       <c r="B281" s="39"/>
       <c r="C281" s="39"/>
@@ -9200,7 +9202,7 @@
       <c r="N281" s="39"/>
       <c r="O281" s="39"/>
     </row>
-    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="282" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A282" s="39"/>
       <c r="B282" s="39"/>
       <c r="C282" s="39"/>
@@ -9217,7 +9219,7 @@
       <c r="N282" s="39"/>
       <c r="O282" s="39"/>
     </row>
-    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="283" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A283" s="39"/>
       <c r="B283" s="39"/>
       <c r="C283" s="39"/>
@@ -9234,7 +9236,7 @@
       <c r="N283" s="39"/>
       <c r="O283" s="39"/>
     </row>
-    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="284" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A284" s="39"/>
       <c r="B284" s="39"/>
       <c r="C284" s="39"/>
@@ -9251,7 +9253,7 @@
       <c r="N284" s="39"/>
       <c r="O284" s="39"/>
     </row>
-    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="285" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A285" s="39"/>
       <c r="B285" s="39"/>
       <c r="C285" s="39"/>
@@ -9268,7 +9270,7 @@
       <c r="N285" s="39"/>
       <c r="O285" s="39"/>
     </row>
-    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="286" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A286" s="39"/>
       <c r="B286" s="39"/>
       <c r="C286" s="39"/>
@@ -9285,7 +9287,7 @@
       <c r="N286" s="39"/>
       <c r="O286" s="39"/>
     </row>
-    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="287" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A287" s="39"/>
       <c r="B287" s="39"/>
       <c r="C287" s="39"/>
@@ -9302,7 +9304,7 @@
       <c r="N287" s="39"/>
       <c r="O287" s="39"/>
     </row>
-    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="288" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A288" s="39"/>
       <c r="B288" s="39"/>
       <c r="C288" s="39"/>
@@ -9319,7 +9321,7 @@
       <c r="N288" s="39"/>
       <c r="O288" s="39"/>
     </row>
-    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A289" s="39"/>
       <c r="B289" s="39"/>
       <c r="C289" s="39"/>
@@ -9336,7 +9338,7 @@
       <c r="N289" s="39"/>
       <c r="O289" s="39"/>
     </row>
-    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="290" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A290" s="39"/>
       <c r="B290" s="39"/>
       <c r="C290" s="39"/>
@@ -9353,7 +9355,7 @@
       <c r="N290" s="39"/>
       <c r="O290" s="39"/>
     </row>
-    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="291" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A291" s="39"/>
       <c r="B291" s="39"/>
       <c r="C291" s="39"/>
@@ -9370,7 +9372,7 @@
       <c r="N291" s="39"/>
       <c r="O291" s="39"/>
     </row>
-    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="292" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A292" s="39"/>
       <c r="B292" s="39"/>
       <c r="C292" s="39"/>
@@ -9387,7 +9389,7 @@
       <c r="N292" s="39"/>
       <c r="O292" s="39"/>
     </row>
-    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="293" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A293" s="39"/>
       <c r="B293" s="39"/>
       <c r="C293" s="39"/>
@@ -9404,7 +9406,7 @@
       <c r="N293" s="39"/>
       <c r="O293" s="39"/>
     </row>
-    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="294" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A294" s="39"/>
       <c r="B294" s="39"/>
       <c r="C294" s="39"/>
@@ -9421,7 +9423,7 @@
       <c r="N294" s="39"/>
       <c r="O294" s="39"/>
     </row>
-    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A295" s="39"/>
       <c r="B295" s="39"/>
       <c r="C295" s="39"/>
@@ -9438,7 +9440,7 @@
       <c r="N295" s="39"/>
       <c r="O295" s="39"/>
     </row>
-    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="296" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A296" s="39"/>
       <c r="B296" s="39"/>
       <c r="C296" s="39"/>
@@ -9455,7 +9457,7 @@
       <c r="N296" s="39"/>
       <c r="O296" s="39"/>
     </row>
-    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="297" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A297" s="39"/>
       <c r="B297" s="39"/>
       <c r="C297" s="39"/>
@@ -9472,7 +9474,7 @@
       <c r="N297" s="39"/>
       <c r="O297" s="39"/>
     </row>
-    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="298" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A298" s="39"/>
       <c r="B298" s="39"/>
       <c r="C298" s="39"/>
@@ -9489,7 +9491,7 @@
       <c r="N298" s="39"/>
       <c r="O298" s="39"/>
     </row>
-    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A299" s="39"/>
       <c r="B299" s="39"/>
       <c r="C299" s="39"/>
@@ -9506,7 +9508,7 @@
       <c r="N299" s="39"/>
       <c r="O299" s="39"/>
     </row>
-    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="300" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A300" s="39"/>
       <c r="B300" s="39"/>
       <c r="C300" s="39"/>
@@ -9523,7 +9525,7 @@
       <c r="N300" s="39"/>
       <c r="O300" s="39"/>
     </row>
-    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="301" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A301" s="39"/>
       <c r="B301" s="39"/>
       <c r="C301" s="39"/>
@@ -9540,7 +9542,7 @@
       <c r="N301" s="39"/>
       <c r="O301" s="39"/>
     </row>
-    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="302" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A302" s="39"/>
       <c r="B302" s="39"/>
       <c r="C302" s="39"/>
@@ -9557,7 +9559,7 @@
       <c r="N302" s="39"/>
       <c r="O302" s="39"/>
     </row>
-    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="303" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A303" s="39"/>
       <c r="B303" s="39"/>
       <c r="C303" s="39"/>
@@ -9574,7 +9576,7 @@
       <c r="N303" s="39"/>
       <c r="O303" s="39"/>
     </row>
-    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="304" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A304" s="39"/>
       <c r="B304" s="39"/>
       <c r="C304" s="39"/>
@@ -9591,7 +9593,7 @@
       <c r="N304" s="39"/>
       <c r="O304" s="39"/>
     </row>
-    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="305" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A305" s="39"/>
       <c r="B305" s="39"/>
       <c r="C305" s="39"/>
@@ -9608,7 +9610,7 @@
       <c r="N305" s="39"/>
       <c r="O305" s="39"/>
     </row>
-    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="306" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A306" s="39"/>
       <c r="B306" s="39"/>
       <c r="C306" s="39"/>
@@ -9625,7 +9627,7 @@
       <c r="N306" s="39"/>
       <c r="O306" s="39"/>
     </row>
-    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="307" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A307" s="39"/>
       <c r="B307" s="39"/>
       <c r="C307" s="39"/>
@@ -9642,7 +9644,7 @@
       <c r="N307" s="39"/>
       <c r="O307" s="39"/>
     </row>
-    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="308" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A308" s="39"/>
       <c r="B308" s="39"/>
       <c r="C308" s="39"/>
@@ -9659,7 +9661,7 @@
       <c r="N308" s="39"/>
       <c r="O308" s="39"/>
     </row>
-    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="309" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A309" s="39"/>
       <c r="B309" s="39"/>
       <c r="C309" s="39"/>
@@ -9676,7 +9678,7 @@
       <c r="N309" s="39"/>
       <c r="O309" s="39"/>
     </row>
-    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="310" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A310" s="39"/>
       <c r="B310" s="39"/>
       <c r="C310" s="39"/>
@@ -9693,7 +9695,7 @@
       <c r="N310" s="39"/>
       <c r="O310" s="39"/>
     </row>
-    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="311" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A311" s="39"/>
       <c r="B311" s="39"/>
       <c r="C311" s="39"/>
@@ -9710,7 +9712,7 @@
       <c r="N311" s="39"/>
       <c r="O311" s="39"/>
     </row>
-    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="312" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A312" s="39"/>
       <c r="B312" s="39"/>
       <c r="C312" s="39"/>
@@ -9727,7 +9729,7 @@
       <c r="N312" s="39"/>
       <c r="O312" s="39"/>
     </row>
-    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="313" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A313" s="39"/>
       <c r="B313" s="39"/>
       <c r="C313" s="39"/>
@@ -9744,7 +9746,7 @@
       <c r="N313" s="39"/>
       <c r="O313" s="39"/>
     </row>
-    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="314" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A314" s="39"/>
       <c r="B314" s="39"/>
       <c r="C314" s="39"/>
@@ -9761,7 +9763,7 @@
       <c r="N314" s="39"/>
       <c r="O314" s="39"/>
     </row>
-    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="315" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A315" s="39"/>
       <c r="B315" s="39"/>
       <c r="C315" s="39"/>
@@ -9778,7 +9780,7 @@
       <c r="N315" s="39"/>
       <c r="O315" s="39"/>
     </row>
-    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="316" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A316" s="39"/>
       <c r="B316" s="39"/>
       <c r="C316" s="39"/>
@@ -9795,7 +9797,7 @@
       <c r="N316" s="39"/>
       <c r="O316" s="39"/>
     </row>
-    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="317" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A317" s="39"/>
       <c r="B317" s="39"/>
       <c r="C317" s="39"/>
@@ -9812,7 +9814,7 @@
       <c r="N317" s="39"/>
       <c r="O317" s="39"/>
     </row>
-    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="318" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A318" s="39"/>
       <c r="B318" s="39"/>
       <c r="C318" s="39"/>
@@ -9829,7 +9831,7 @@
       <c r="N318" s="39"/>
       <c r="O318" s="39"/>
     </row>
-    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="319" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A319" s="39"/>
       <c r="B319" s="39"/>
       <c r="C319" s="39"/>
@@ -9846,7 +9848,7 @@
       <c r="N319" s="39"/>
       <c r="O319" s="39"/>
     </row>
-    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="320" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A320" s="39"/>
       <c r="B320" s="39"/>
       <c r="C320" s="39"/>
@@ -9863,7 +9865,7 @@
       <c r="N320" s="39"/>
       <c r="O320" s="39"/>
     </row>
-    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="321" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A321" s="39"/>
       <c r="B321" s="39"/>
       <c r="C321" s="39"/>
@@ -9880,7 +9882,7 @@
       <c r="N321" s="39"/>
       <c r="O321" s="39"/>
     </row>
-    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="322" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A322" s="39"/>
       <c r="B322" s="39"/>
       <c r="C322" s="39"/>
@@ -9897,7 +9899,7 @@
       <c r="N322" s="39"/>
       <c r="O322" s="39"/>
     </row>
-    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="323" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A323" s="39"/>
       <c r="B323" s="39"/>
       <c r="C323" s="39"/>
@@ -9914,7 +9916,7 @@
       <c r="N323" s="39"/>
       <c r="O323" s="39"/>
     </row>
-    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="324" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A324" s="39"/>
       <c r="B324" s="39"/>
       <c r="C324" s="39"/>
@@ -9931,7 +9933,7 @@
       <c r="N324" s="39"/>
       <c r="O324" s="39"/>
     </row>
-    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="325" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A325" s="39"/>
       <c r="B325" s="39"/>
       <c r="C325" s="39"/>
@@ -9948,7 +9950,7 @@
       <c r="N325" s="39"/>
       <c r="O325" s="39"/>
     </row>
-    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="326" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A326" s="39"/>
       <c r="B326" s="39"/>
       <c r="C326" s="39"/>
@@ -9965,7 +9967,7 @@
       <c r="N326" s="39"/>
       <c r="O326" s="39"/>
     </row>
-    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="327" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
       <c r="C327" s="39"/>
@@ -9982,7 +9984,7 @@
       <c r="N327" s="39"/>
       <c r="O327" s="39"/>
     </row>
-    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="328" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A328" s="39"/>
       <c r="B328" s="39"/>
       <c r="C328" s="39"/>
@@ -9999,7 +10001,7 @@
       <c r="N328" s="39"/>
       <c r="O328" s="39"/>
     </row>
-    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="329" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A329" s="39"/>
       <c r="B329" s="39"/>
       <c r="C329" s="39"/>
@@ -10016,7 +10018,7 @@
       <c r="N329" s="39"/>
       <c r="O329" s="39"/>
     </row>
-    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="330" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A330" s="39"/>
       <c r="B330" s="39"/>
       <c r="C330" s="39"/>
@@ -10033,7 +10035,7 @@
       <c r="N330" s="39"/>
       <c r="O330" s="39"/>
     </row>
-    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="331" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A331" s="39"/>
       <c r="B331" s="39"/>
       <c r="C331" s="39"/>
@@ -10050,7 +10052,7 @@
       <c r="N331" s="39"/>
       <c r="O331" s="39"/>
     </row>
-    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="332" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A332" s="39"/>
       <c r="B332" s="39"/>
       <c r="C332" s="39"/>
@@ -10067,7 +10069,7 @@
       <c r="N332" s="39"/>
       <c r="O332" s="39"/>
     </row>
-    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="333" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A333" s="39"/>
       <c r="B333" s="39"/>
       <c r="C333" s="39"/>
@@ -10084,7 +10086,7 @@
       <c r="N333" s="39"/>
       <c r="O333" s="39"/>
     </row>
-    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="334" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A334" s="39"/>
       <c r="B334" s="39"/>
       <c r="C334" s="39"/>
@@ -10101,7 +10103,7 @@
       <c r="N334" s="39"/>
       <c r="O334" s="39"/>
     </row>
-    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="335" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A335" s="39"/>
       <c r="B335" s="39"/>
       <c r="C335" s="39"/>
@@ -10118,7 +10120,7 @@
       <c r="N335" s="39"/>
       <c r="O335" s="39"/>
     </row>
-    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="336" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A336" s="39"/>
       <c r="B336" s="39"/>
       <c r="C336" s="39"/>
@@ -10135,7 +10137,7 @@
       <c r="N336" s="39"/>
       <c r="O336" s="39"/>
     </row>
-    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="337" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A337" s="39"/>
       <c r="B337" s="39"/>
       <c r="C337" s="39"/>
@@ -10152,7 +10154,7 @@
       <c r="N337" s="39"/>
       <c r="O337" s="39"/>
     </row>
-    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="338" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A338" s="39"/>
       <c r="B338" s="39"/>
       <c r="C338" s="39"/>
@@ -10169,7 +10171,7 @@
       <c r="N338" s="39"/>
       <c r="O338" s="39"/>
     </row>
-    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="339" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A339" s="39"/>
       <c r="B339" s="39"/>
       <c r="C339" s="39"/>
@@ -10186,7 +10188,7 @@
       <c r="N339" s="39"/>
       <c r="O339" s="39"/>
     </row>
-    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="340" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A340" s="39"/>
       <c r="B340" s="39"/>
       <c r="C340" s="39"/>
@@ -10203,7 +10205,7 @@
       <c r="N340" s="39"/>
       <c r="O340" s="39"/>
     </row>
-    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="341" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A341" s="39"/>
       <c r="B341" s="39"/>
       <c r="C341" s="39"/>
@@ -10220,7 +10222,7 @@
       <c r="N341" s="39"/>
       <c r="O341" s="39"/>
     </row>
-    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="342" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A342" s="39"/>
       <c r="B342" s="39"/>
       <c r="C342" s="39"/>
@@ -10237,7 +10239,7 @@
       <c r="N342" s="39"/>
       <c r="O342" s="39"/>
     </row>
-    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="343" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A343" s="39"/>
       <c r="B343" s="39"/>
       <c r="C343" s="39"/>
@@ -10254,7 +10256,7 @@
       <c r="N343" s="39"/>
       <c r="O343" s="39"/>
     </row>
-    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="344" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A344" s="39"/>
       <c r="B344" s="39"/>
       <c r="C344" s="39"/>
@@ -10271,7 +10273,7 @@
       <c r="N344" s="39"/>
       <c r="O344" s="39"/>
     </row>
-    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="345" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A345" s="39"/>
       <c r="B345" s="39"/>
       <c r="C345" s="39"/>
@@ -10288,7 +10290,7 @@
       <c r="N345" s="39"/>
       <c r="O345" s="39"/>
     </row>
-    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="346" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="39"/>
@@ -10318,12 +10320,12 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="38" t="s">
         <v>114</v>
       </c>

</xml_diff>